<commit_message>
formula and smartphone notes
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0525FCA5-32E9-5340-A502-447BF084C35D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C361AF2F-E430-704E-9260-30D907872642}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="943">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="945">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -2848,9 +2848,6 @@
     <t>Luke Dormehl</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>Sleeping with Your Smartphone: How to Break the 24/7 Habit and Change the Way You Work</t>
   </si>
   <si>
@@ -2861,6 +2858,15 @@
   </si>
   <si>
     <t>Austin Kleon</t>
+  </si>
+  <si>
+    <t>I had been waiting to listen to this for awhile since it looked interesting, but it didn't live up to expectations. It felt quite rambling without a coherent (or effective) overall thesis, included some weird stuff about online dating and such that makees me wonder why the author included it, and just wansn't as good as other books on similar topics like *Life 3.0*, *Weapons of Math Destruction*, *Signal and the Noise*, etc.: save you time for those.</t>
+  </si>
+  <si>
+    <t>This was recommended quite some time ago by Cal Newport. He recommended it in a newsletter about email when discussing her "Cycle of Responsiveness" (6) where the pressure to always "be on" leads to a vicious cycle of always being on. The rest of the book is a discussion of how she implemented PTO (**PTO = predictability + teaming + open communication) at BCG, and then instructions to implement it in your own organization. These are effective strategies to manage work life balance especially in absurd jobs, and certainly some of them can be applied in less-extreme jobs. However, I think a first step is to *avoid* a culture of work like this in the first place, and to *set expectations from day 1* that you don't check your email at home, work on the weekends, etc.</t>
+  </si>
+  <si>
+    <t>This had been on my radar for quite some time and I decided to read it while on this Alan Jacobs and sharing on the internet reading kick. This is a quick and actionable read.</t>
   </si>
 </sst>
 </file>
@@ -7565,7 +7571,7 @@
   <dimension ref="A1:H498"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A465" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A471" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A499" sqref="A499"/>
     </sheetView>
   </sheetViews>
@@ -15062,10 +15068,10 @@
     </row>
     <row r="496" spans="1:8">
       <c r="A496" s="6" t="s">
+        <v>938</v>
+      </c>
+      <c r="B496" s="6" t="s">
         <v>939</v>
-      </c>
-      <c r="B496" s="6" t="s">
-        <v>940</v>
       </c>
       <c r="C496" s="6" t="s">
         <v>201</v>
@@ -15080,10 +15086,10 @@
         <v>288</v>
       </c>
       <c r="G496" s="9" t="s">
-        <v>938</v>
+        <v>243</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>938</v>
+        <v>943</v>
       </c>
     </row>
     <row r="497" spans="1:8">
@@ -15106,18 +15112,18 @@
         <v>288</v>
       </c>
       <c r="G497" s="9" t="s">
-        <v>938</v>
+        <v>243</v>
       </c>
       <c r="H497" s="6" t="s">
-        <v>938</v>
+        <v>942</v>
       </c>
     </row>
     <row r="498" spans="1:8">
       <c r="A498" s="6" t="s">
+        <v>940</v>
+      </c>
+      <c r="B498" s="6" t="s">
         <v>941</v>
-      </c>
-      <c r="B498" s="6" t="s">
-        <v>942</v>
       </c>
       <c r="C498" s="6" t="s">
         <v>935</v>
@@ -15135,7 +15141,7 @@
         <v>243</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>938</v>
+        <v>944</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Steal Like an Artist
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{561136F5-E69C-7644-ACDA-5AEBDDE3177B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F7A7B00F-23A0-1E4E-95F1-67D2FA13BE3D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="951">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="953">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -2885,6 +2885,12 @@
   </si>
   <si>
     <t>I came across this after finding the resources page on his website, and this is a great overview of reproducible research. I have added it to the "essential" reading list along with Tidy Data, etc. He uses EMCAS, R, pandoc, which are tools I haven't used but am interested in learning. More important, as he acknowledges, is the *process*: backups, version control, plain-text, reproducibility.</t>
+  </si>
+  <si>
+    <t>Steal Like an Artist</t>
+  </si>
+  <si>
+    <t>Quick, full of good advice, and fun.</t>
   </si>
 </sst>
 </file>
@@ -7586,11 +7592,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H500"/>
+  <dimension ref="A1:H501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A471" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A501" sqref="A501"/>
+      <selection pane="bottomLeft" activeCell="A502" sqref="A502"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -15212,6 +15218,32 @@
       </c>
       <c r="H500" s="6" t="s">
         <v>950</v>
+      </c>
+    </row>
+    <row r="501" spans="1:8">
+      <c r="A501" s="6" t="s">
+        <v>951</v>
+      </c>
+      <c r="B501" s="6" t="s">
+        <v>941</v>
+      </c>
+      <c r="C501" s="6" t="s">
+        <v>935</v>
+      </c>
+      <c r="D501" s="9">
+        <v>2018</v>
+      </c>
+      <c r="E501" s="9">
+        <v>2012</v>
+      </c>
+      <c r="F501" s="9">
+        <v>140</v>
+      </c>
+      <c r="G501" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="H501" s="6" t="s">
+        <v>952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Jazz and Hahn
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,38 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10319"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr hidePivotFieldList="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F7A7B00F-23A0-1E4E-95F1-67D2FA13BE3D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26840" yWindow="4420" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
     <sheet name="Pivot" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="953">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="957">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -2839,9 +2833,6 @@
     <t>I listened to this over a weekend or so. It echoes of Matthew Crawford and the growing loss of tech-idealism. He chronicles analog through music, writing, reading, work, board games, etc. This book speaks to the truth that humans have bodies and this is a sacramental world we live in.</t>
   </si>
   <si>
-    <t>LIbrary</t>
-  </si>
-  <si>
     <t>The Formula: How Algorithms Solve All Our Problems . . . and Create More</t>
   </si>
   <si>
@@ -2891,13 +2882,28 @@
   </si>
   <si>
     <t>Quick, full of good advice, and fun.</t>
+  </si>
+  <si>
+    <t>Consuming the Word: The New Testament and The Eucharist in the Early Church</t>
+  </si>
+  <si>
+    <t>Being Jazz: My Life as a (Transgender) Teen</t>
+  </si>
+  <si>
+    <t>Jazz Jennings</t>
+  </si>
+  <si>
+    <t>Scott Hahn is characteristically cogent and devout in this description of the New Testament (or covenant as he explains) and the Eucharist. This book is a tour of the early church and the language of the scriptures. Reading Hahn always engenders a deeper love and respect for scripture. Some tidbits I enjoyed inlcude the discussion of his personal library in the preface and Christians popularizing the Codex in Chapter 9, which I read about previously from Turner and Jacobs. He also mentions how the 1969 lectionary was a significant ecumentical milestone, and how Jesus' mind was so saturated with the scriptures. This is a beautiful book to read and reflect on.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I read this to balance my reading of Ryan Anderson and to give a pro-transgender voice an audience, certainly not by way of providing a philosophical argument but through the story of a self-described happy transgender individual. Putting aside the politicized and simplistic description of transgenderism ("I'm have a girl brain in a boy body") I tried to be open-minded in learning about Jazz's story, how Jazz's parents have responded to the situation, how Jazz deals with ongoing depression, and how Jazz has become a transgender activist. Reading both Jennings and Anderson has given me new appreciation for the need for sensativity toward people with gender dysphoria as well as the larger context surrounding transgenderism. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2968,7 +2974,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="557">
+  <cellStyleXfs count="565">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3455,6 +3461,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3561,7 +3575,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="557">
+  <cellStyles count="565">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4083,6 +4097,10 @@
     <cellStyle name="Followed Hyperlink" xfId="552" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="489" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="491" builtinId="8" hidden="1"/>
@@ -4118,6 +4136,10 @@
     <cellStyle name="Hyperlink" xfId="551" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4134,7 +4156,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4181,26 +4203,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -4229,121 +4231,121 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>-399</c:v>
+                  <c:v>-399.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>426</c:v>
+                  <c:v>426.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1808</c:v>
+                  <c:v>1808.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1813</c:v>
+                  <c:v>1813.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1898</c:v>
+                  <c:v>1898.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1902</c:v>
+                  <c:v>1902.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1908</c:v>
+                  <c:v>1908.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1911</c:v>
+                  <c:v>1911.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1936</c:v>
+                  <c:v>1936.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1947</c:v>
+                  <c:v>1947.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1949</c:v>
+                  <c:v>1949.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1950</c:v>
+                  <c:v>1950.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1953</c:v>
+                  <c:v>1953.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1956</c:v>
+                  <c:v>1956.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1959</c:v>
+                  <c:v>1959.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1964</c:v>
+                  <c:v>1964.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1966</c:v>
+                  <c:v>1966.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1968</c:v>
+                  <c:v>1968.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1970</c:v>
+                  <c:v>1970.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1979</c:v>
+                  <c:v>1979.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1982</c:v>
+                  <c:v>1982.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1987</c:v>
+                  <c:v>1987.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1992</c:v>
+                  <c:v>1992.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1994</c:v>
+                  <c:v>1994.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1997</c:v>
+                  <c:v>1997.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2002</c:v>
+                  <c:v>2002.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2004</c:v>
+                  <c:v>2004.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2006</c:v>
+                  <c:v>2006.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2007</c:v>
+                  <c:v>2007.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2009</c:v>
+                  <c:v>2009.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2010</c:v>
+                  <c:v>2010.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2011</c:v>
+                  <c:v>2011.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2012</c:v>
+                  <c:v>2012.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2013</c:v>
+                  <c:v>2013.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2014</c:v>
+                  <c:v>2014.0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2015</c:v>
+                  <c:v>2015.0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2016</c:v>
+                  <c:v>2016.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2017</c:v>
+                  <c:v>2017.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4355,126 +4357,126 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0624-D142-B189-136781839F18}"/>
             </c:ext>
@@ -4490,11 +4492,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2087936264"/>
-        <c:axId val="2087914776"/>
+        <c:axId val="2083500296"/>
+        <c:axId val="2082547528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2087936264"/>
+        <c:axId val="2083500296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4537,7 +4539,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2087914776"/>
+        <c:crossAx val="2082547528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4545,7 +4547,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2087914776"/>
+        <c:axId val="2082547528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4596,7 +4598,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2087936264"/>
+        <c:crossAx val="2083500296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4646,7 +4648,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4693,26 +4695,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="50" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -4744,7 +4726,7 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-1BFB-5148-B23A-9164704C5FA6}"/>
               </c:ext>
@@ -4772,7 +4754,7 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-1BFB-5148-B23A-9164704C5FA6}"/>
               </c:ext>
@@ -4800,7 +4782,7 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-1BFB-5148-B23A-9164704C5FA6}"/>
               </c:ext>
@@ -4828,7 +4810,7 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-1BFB-5148-B23A-9164704C5FA6}"/>
               </c:ext>
@@ -4856,7 +4838,7 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-1BFB-5148-B23A-9164704C5FA6}"/>
               </c:ext>
@@ -4911,7 +4893,7 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -4945,24 +4927,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>52</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000A-1BFB-5148-B23A-9164704C5FA6}"/>
             </c:ext>
@@ -6145,7 +6127,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6181,7 +6163,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6203,7 +6185,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="43091.62880486111" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="100" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="43091.62880486111" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="100">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F467" sheet="Books"/>
   </cacheSource>
@@ -7152,7 +7134,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -7581,25 +7563,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H501"/>
+  <dimension ref="A1:H503"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A471" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A502" sqref="A502"/>
+      <pane ySplit="1" topLeftCell="A492" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A504" sqref="A504"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="79.33203125" style="6" customWidth="1"/>
     <col min="2" max="2" width="28.83203125" style="6" bestFit="1" customWidth="1"/>
@@ -7634,7 +7616,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="12" customFormat="1" ht="16">
+    <row r="2" spans="1:8" s="12" customFormat="1">
       <c r="A2" s="12" t="s">
         <v>260</v>
       </c>
@@ -7647,7 +7629,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
     </row>
-    <row r="3" spans="1:8" customFormat="1" ht="16">
+    <row r="3" spans="1:8" customFormat="1">
       <c r="A3" t="s">
         <v>261</v>
       </c>
@@ -7660,7 +7642,7 @@
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:8" customFormat="1" ht="16">
+    <row r="4" spans="1:8" customFormat="1">
       <c r="A4" t="s">
         <v>262</v>
       </c>
@@ -7673,7 +7655,7 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
     </row>
-    <row r="5" spans="1:8" customFormat="1" ht="16">
+    <row r="5" spans="1:8" customFormat="1">
       <c r="A5" t="s">
         <v>263</v>
       </c>
@@ -7686,7 +7668,7 @@
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
     </row>
-    <row r="6" spans="1:8" customFormat="1" ht="16">
+    <row r="6" spans="1:8" customFormat="1">
       <c r="A6" t="s">
         <v>264</v>
       </c>
@@ -7699,7 +7681,7 @@
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
     </row>
-    <row r="7" spans="1:8" customFormat="1" ht="16">
+    <row r="7" spans="1:8" customFormat="1">
       <c r="A7" t="s">
         <v>265</v>
       </c>
@@ -7712,7 +7694,7 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="1:8" customFormat="1" ht="16">
+    <row r="8" spans="1:8" customFormat="1">
       <c r="A8" t="s">
         <v>266</v>
       </c>
@@ -7725,7 +7707,7 @@
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:8" customFormat="1" ht="16">
+    <row r="9" spans="1:8" customFormat="1">
       <c r="A9" t="s">
         <v>267</v>
       </c>
@@ -7738,7 +7720,7 @@
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
     </row>
-    <row r="10" spans="1:8" customFormat="1" ht="16">
+    <row r="10" spans="1:8" customFormat="1">
       <c r="A10" t="s">
         <v>268</v>
       </c>
@@ -7751,7 +7733,7 @@
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
     </row>
-    <row r="11" spans="1:8" customFormat="1" ht="16">
+    <row r="11" spans="1:8" customFormat="1">
       <c r="A11" t="s">
         <v>269</v>
       </c>
@@ -7764,7 +7746,7 @@
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
     </row>
-    <row r="12" spans="1:8" customFormat="1" ht="16">
+    <row r="12" spans="1:8" customFormat="1">
       <c r="A12" t="s">
         <v>270</v>
       </c>
@@ -7777,7 +7759,7 @@
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
     </row>
-    <row r="13" spans="1:8" customFormat="1" ht="16">
+    <row r="13" spans="1:8" customFormat="1">
       <c r="A13" t="s">
         <v>271</v>
       </c>
@@ -7787,7 +7769,7 @@
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
     </row>
-    <row r="14" spans="1:8" customFormat="1" ht="16">
+    <row r="14" spans="1:8" customFormat="1">
       <c r="A14" t="s">
         <v>272</v>
       </c>
@@ -7800,7 +7782,7 @@
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="1:8" s="12" customFormat="1" ht="16">
+    <row r="15" spans="1:8" s="12" customFormat="1">
       <c r="A15" s="12" t="s">
         <v>273</v>
       </c>
@@ -7813,7 +7795,7 @@
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:8" customFormat="1" ht="16">
+    <row r="16" spans="1:8" customFormat="1">
       <c r="A16" t="s">
         <v>274</v>
       </c>
@@ -7826,7 +7808,7 @@
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
     </row>
-    <row r="17" spans="1:6" customFormat="1" ht="16">
+    <row r="17" spans="1:6" customFormat="1">
       <c r="A17" s="15" t="s">
         <v>887</v>
       </c>
@@ -7839,7 +7821,7 @@
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="1:6" customFormat="1" ht="16">
+    <row r="18" spans="1:6" customFormat="1">
       <c r="A18" t="s">
         <v>275</v>
       </c>
@@ -7852,7 +7834,7 @@
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:6" customFormat="1" ht="16">
+    <row r="19" spans="1:6" customFormat="1">
       <c r="A19" t="s">
         <v>276</v>
       </c>
@@ -7865,7 +7847,7 @@
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
     </row>
-    <row r="20" spans="1:6" customFormat="1" ht="16">
+    <row r="20" spans="1:6" customFormat="1">
       <c r="A20" t="s">
         <v>277</v>
       </c>
@@ -7878,7 +7860,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
     </row>
-    <row r="21" spans="1:6" customFormat="1" ht="16">
+    <row r="21" spans="1:6" customFormat="1">
       <c r="A21" t="s">
         <v>278</v>
       </c>
@@ -7891,7 +7873,7 @@
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
     </row>
-    <row r="22" spans="1:6" customFormat="1" ht="16">
+    <row r="22" spans="1:6" customFormat="1">
       <c r="A22" t="s">
         <v>279</v>
       </c>
@@ -7904,7 +7886,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="1:6" customFormat="1" ht="16">
+    <row r="23" spans="1:6" customFormat="1">
       <c r="A23" t="s">
         <v>280</v>
       </c>
@@ -7917,7 +7899,7 @@
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
     </row>
-    <row r="24" spans="1:6" customFormat="1" ht="16">
+    <row r="24" spans="1:6" customFormat="1">
       <c r="A24" t="s">
         <v>281</v>
       </c>
@@ -7930,7 +7912,7 @@
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
     </row>
-    <row r="25" spans="1:6" customFormat="1" ht="16">
+    <row r="25" spans="1:6" customFormat="1">
       <c r="A25" t="s">
         <v>282</v>
       </c>
@@ -7943,7 +7925,7 @@
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
     </row>
-    <row r="26" spans="1:6" customFormat="1" ht="16">
+    <row r="26" spans="1:6" customFormat="1">
       <c r="A26" t="s">
         <v>283</v>
       </c>
@@ -7956,7 +7938,7 @@
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
     </row>
-    <row r="27" spans="1:6" customFormat="1" ht="16">
+    <row r="27" spans="1:6" customFormat="1">
       <c r="A27" t="s">
         <v>284</v>
       </c>
@@ -7969,7 +7951,7 @@
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
     </row>
-    <row r="28" spans="1:6" customFormat="1" ht="16">
+    <row r="28" spans="1:6" customFormat="1">
       <c r="A28" t="s">
         <v>285</v>
       </c>
@@ -7982,7 +7964,7 @@
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
     </row>
-    <row r="29" spans="1:6" s="12" customFormat="1" ht="16">
+    <row r="29" spans="1:6" s="12" customFormat="1">
       <c r="A29" s="12" t="s">
         <v>286</v>
       </c>
@@ -7995,7 +7977,7 @@
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:6" customFormat="1" ht="16">
+    <row r="30" spans="1:6" customFormat="1">
       <c r="A30" t="s">
         <v>287</v>
       </c>
@@ -8008,7 +7990,7 @@
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
     </row>
-    <row r="31" spans="1:6" customFormat="1" ht="16">
+    <row r="31" spans="1:6" customFormat="1">
       <c r="A31" t="s">
         <v>288</v>
       </c>
@@ -8021,7 +8003,7 @@
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
     </row>
-    <row r="32" spans="1:6" customFormat="1" ht="16">
+    <row r="32" spans="1:6" customFormat="1">
       <c r="A32" t="s">
         <v>289</v>
       </c>
@@ -8034,7 +8016,7 @@
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
     </row>
-    <row r="33" spans="1:6" customFormat="1" ht="16">
+    <row r="33" spans="1:6" customFormat="1">
       <c r="A33" t="s">
         <v>290</v>
       </c>
@@ -8047,7 +8029,7 @@
       <c r="E33" s="14"/>
       <c r="F33" s="14"/>
     </row>
-    <row r="34" spans="1:6" customFormat="1" ht="16">
+    <row r="34" spans="1:6" customFormat="1">
       <c r="A34" t="s">
         <v>291</v>
       </c>
@@ -8060,7 +8042,7 @@
       <c r="E34" s="14"/>
       <c r="F34" s="14"/>
     </row>
-    <row r="35" spans="1:6" customFormat="1" ht="16">
+    <row r="35" spans="1:6" customFormat="1">
       <c r="A35" t="s">
         <v>279</v>
       </c>
@@ -8073,7 +8055,7 @@
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
     </row>
-    <row r="36" spans="1:6" customFormat="1" ht="16">
+    <row r="36" spans="1:6" customFormat="1">
       <c r="A36" t="s">
         <v>292</v>
       </c>
@@ -8086,7 +8068,7 @@
       <c r="E36" s="14"/>
       <c r="F36" s="14"/>
     </row>
-    <row r="37" spans="1:6" customFormat="1" ht="16">
+    <row r="37" spans="1:6" customFormat="1">
       <c r="A37" t="s">
         <v>293</v>
       </c>
@@ -8099,7 +8081,7 @@
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
     </row>
-    <row r="38" spans="1:6" customFormat="1" ht="16">
+    <row r="38" spans="1:6" customFormat="1">
       <c r="A38" t="s">
         <v>294</v>
       </c>
@@ -8112,7 +8094,7 @@
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
     </row>
-    <row r="39" spans="1:6" customFormat="1" ht="16">
+    <row r="39" spans="1:6" customFormat="1">
       <c r="A39" t="s">
         <v>295</v>
       </c>
@@ -8125,7 +8107,7 @@
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
     </row>
-    <row r="40" spans="1:6" customFormat="1" ht="16">
+    <row r="40" spans="1:6" customFormat="1">
       <c r="A40" t="s">
         <v>296</v>
       </c>
@@ -8138,7 +8120,7 @@
       <c r="E40" s="14"/>
       <c r="F40" s="14"/>
     </row>
-    <row r="41" spans="1:6" customFormat="1" ht="16">
+    <row r="41" spans="1:6" customFormat="1">
       <c r="A41" t="s">
         <v>297</v>
       </c>
@@ -8151,7 +8133,7 @@
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
     </row>
-    <row r="42" spans="1:6" customFormat="1" ht="16">
+    <row r="42" spans="1:6" customFormat="1">
       <c r="A42" t="s">
         <v>298</v>
       </c>
@@ -8164,7 +8146,7 @@
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
     </row>
-    <row r="43" spans="1:6" customFormat="1" ht="16">
+    <row r="43" spans="1:6" customFormat="1">
       <c r="A43" t="s">
         <v>299</v>
       </c>
@@ -8177,7 +8159,7 @@
       <c r="E43" s="14"/>
       <c r="F43" s="14"/>
     </row>
-    <row r="44" spans="1:6" customFormat="1" ht="16">
+    <row r="44" spans="1:6" customFormat="1">
       <c r="A44" t="s">
         <v>300</v>
       </c>
@@ -8190,7 +8172,7 @@
       <c r="E44" s="14"/>
       <c r="F44" s="14"/>
     </row>
-    <row r="45" spans="1:6" customFormat="1" ht="16">
+    <row r="45" spans="1:6" customFormat="1">
       <c r="A45" t="s">
         <v>301</v>
       </c>
@@ -8203,7 +8185,7 @@
       <c r="E45" s="14"/>
       <c r="F45" s="14"/>
     </row>
-    <row r="46" spans="1:6" s="12" customFormat="1" ht="16">
+    <row r="46" spans="1:6" s="12" customFormat="1">
       <c r="A46" s="12" t="s">
         <v>302</v>
       </c>
@@ -8216,7 +8198,7 @@
       <c r="E46" s="13"/>
       <c r="F46" s="13"/>
     </row>
-    <row r="47" spans="1:6" customFormat="1" ht="16">
+    <row r="47" spans="1:6" customFormat="1">
       <c r="A47" t="s">
         <v>303</v>
       </c>
@@ -8229,7 +8211,7 @@
       <c r="E47" s="14"/>
       <c r="F47" s="14"/>
     </row>
-    <row r="48" spans="1:6" customFormat="1" ht="16">
+    <row r="48" spans="1:6" customFormat="1">
       <c r="A48" t="s">
         <v>304</v>
       </c>
@@ -8242,7 +8224,7 @@
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
     </row>
-    <row r="49" spans="1:6" customFormat="1" ht="16">
+    <row r="49" spans="1:6" customFormat="1">
       <c r="A49" t="s">
         <v>305</v>
       </c>
@@ -8255,7 +8237,7 @@
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
     </row>
-    <row r="50" spans="1:6" customFormat="1" ht="16">
+    <row r="50" spans="1:6" customFormat="1">
       <c r="A50" t="s">
         <v>306</v>
       </c>
@@ -8268,7 +8250,7 @@
       <c r="E50" s="14"/>
       <c r="F50" s="14"/>
     </row>
-    <row r="51" spans="1:6" customFormat="1" ht="16">
+    <row r="51" spans="1:6" customFormat="1">
       <c r="A51" t="s">
         <v>307</v>
       </c>
@@ -8281,7 +8263,7 @@
       <c r="E51" s="14"/>
       <c r="F51" s="14"/>
     </row>
-    <row r="52" spans="1:6" customFormat="1" ht="16">
+    <row r="52" spans="1:6" customFormat="1">
       <c r="A52" t="s">
         <v>308</v>
       </c>
@@ -8294,7 +8276,7 @@
       <c r="E52" s="14"/>
       <c r="F52" s="14"/>
     </row>
-    <row r="53" spans="1:6" customFormat="1" ht="16">
+    <row r="53" spans="1:6" customFormat="1">
       <c r="A53" t="s">
         <v>309</v>
       </c>
@@ -8307,7 +8289,7 @@
       <c r="E53" s="14"/>
       <c r="F53" s="14"/>
     </row>
-    <row r="54" spans="1:6" customFormat="1" ht="16">
+    <row r="54" spans="1:6" customFormat="1">
       <c r="A54" t="s">
         <v>310</v>
       </c>
@@ -8320,7 +8302,7 @@
       <c r="E54" s="14"/>
       <c r="F54" s="14"/>
     </row>
-    <row r="55" spans="1:6" customFormat="1" ht="16">
+    <row r="55" spans="1:6" customFormat="1">
       <c r="A55" t="s">
         <v>311</v>
       </c>
@@ -8333,7 +8315,7 @@
       <c r="E55" s="14"/>
       <c r="F55" s="14"/>
     </row>
-    <row r="56" spans="1:6" customFormat="1" ht="16">
+    <row r="56" spans="1:6" customFormat="1">
       <c r="A56" t="s">
         <v>312</v>
       </c>
@@ -8346,7 +8328,7 @@
       <c r="E56" s="14"/>
       <c r="F56" s="14"/>
     </row>
-    <row r="57" spans="1:6" customFormat="1" ht="16">
+    <row r="57" spans="1:6" customFormat="1">
       <c r="A57" t="s">
         <v>313</v>
       </c>
@@ -8359,7 +8341,7 @@
       <c r="E57" s="14"/>
       <c r="F57" s="14"/>
     </row>
-    <row r="58" spans="1:6" customFormat="1" ht="16">
+    <row r="58" spans="1:6" customFormat="1">
       <c r="A58" t="s">
         <v>314</v>
       </c>
@@ -8372,7 +8354,7 @@
       <c r="E58" s="14"/>
       <c r="F58" s="14"/>
     </row>
-    <row r="59" spans="1:6" customFormat="1" ht="16">
+    <row r="59" spans="1:6" customFormat="1">
       <c r="A59" t="s">
         <v>315</v>
       </c>
@@ -8385,7 +8367,7 @@
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
     </row>
-    <row r="60" spans="1:6" customFormat="1" ht="16">
+    <row r="60" spans="1:6" customFormat="1">
       <c r="A60" t="s">
         <v>316</v>
       </c>
@@ -8398,7 +8380,7 @@
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
     </row>
-    <row r="61" spans="1:6" customFormat="1" ht="16">
+    <row r="61" spans="1:6" customFormat="1">
       <c r="A61" t="s">
         <v>317</v>
       </c>
@@ -8411,7 +8393,7 @@
       <c r="E61" s="14"/>
       <c r="F61" s="14"/>
     </row>
-    <row r="62" spans="1:6" customFormat="1" ht="16">
+    <row r="62" spans="1:6" customFormat="1">
       <c r="A62" t="s">
         <v>318</v>
       </c>
@@ -8424,7 +8406,7 @@
       <c r="E62" s="14"/>
       <c r="F62" s="14"/>
     </row>
-    <row r="63" spans="1:6" customFormat="1" ht="16">
+    <row r="63" spans="1:6" customFormat="1">
       <c r="A63" t="s">
         <v>319</v>
       </c>
@@ -8437,7 +8419,7 @@
       <c r="E63" s="14"/>
       <c r="F63" s="14"/>
     </row>
-    <row r="64" spans="1:6" customFormat="1" ht="16">
+    <row r="64" spans="1:6" customFormat="1">
       <c r="A64" t="s">
         <v>320</v>
       </c>
@@ -8450,7 +8432,7 @@
       <c r="E64" s="14"/>
       <c r="F64" s="14"/>
     </row>
-    <row r="65" spans="1:6" customFormat="1" ht="16">
+    <row r="65" spans="1:6" customFormat="1">
       <c r="A65" t="s">
         <v>321</v>
       </c>
@@ -8463,7 +8445,7 @@
       <c r="E65" s="14"/>
       <c r="F65" s="14"/>
     </row>
-    <row r="66" spans="1:6" customFormat="1" ht="16">
+    <row r="66" spans="1:6" customFormat="1">
       <c r="A66" t="s">
         <v>322</v>
       </c>
@@ -8476,7 +8458,7 @@
       <c r="E66" s="14"/>
       <c r="F66" s="14"/>
     </row>
-    <row r="67" spans="1:6" customFormat="1" ht="16">
+    <row r="67" spans="1:6" customFormat="1">
       <c r="A67" t="s">
         <v>323</v>
       </c>
@@ -8489,7 +8471,7 @@
       <c r="E67" s="14"/>
       <c r="F67" s="14"/>
     </row>
-    <row r="68" spans="1:6" s="12" customFormat="1" ht="16">
+    <row r="68" spans="1:6" s="12" customFormat="1">
       <c r="A68" s="12" t="s">
         <v>324</v>
       </c>
@@ -8499,7 +8481,7 @@
       <c r="E68" s="13"/>
       <c r="F68" s="13"/>
     </row>
-    <row r="69" spans="1:6" customFormat="1" ht="16">
+    <row r="69" spans="1:6" customFormat="1">
       <c r="A69" t="s">
         <v>325</v>
       </c>
@@ -8512,7 +8494,7 @@
       <c r="E69" s="14"/>
       <c r="F69" s="14"/>
     </row>
-    <row r="70" spans="1:6" customFormat="1" ht="16">
+    <row r="70" spans="1:6" customFormat="1">
       <c r="A70" t="s">
         <v>326</v>
       </c>
@@ -8525,7 +8507,7 @@
       <c r="E70" s="14"/>
       <c r="F70" s="14"/>
     </row>
-    <row r="71" spans="1:6" customFormat="1" ht="16">
+    <row r="71" spans="1:6" customFormat="1">
       <c r="A71" t="s">
         <v>318</v>
       </c>
@@ -8538,7 +8520,7 @@
       <c r="E71" s="14"/>
       <c r="F71" s="14"/>
     </row>
-    <row r="72" spans="1:6" customFormat="1" ht="16">
+    <row r="72" spans="1:6" customFormat="1">
       <c r="A72" t="s">
         <v>327</v>
       </c>
@@ -8551,7 +8533,7 @@
       <c r="E72" s="14"/>
       <c r="F72" s="14"/>
     </row>
-    <row r="73" spans="1:6" customFormat="1" ht="16">
+    <row r="73" spans="1:6" customFormat="1">
       <c r="A73" t="s">
         <v>328</v>
       </c>
@@ -8564,7 +8546,7 @@
       <c r="E73" s="14"/>
       <c r="F73" s="14"/>
     </row>
-    <row r="74" spans="1:6" customFormat="1" ht="16">
+    <row r="74" spans="1:6" customFormat="1">
       <c r="A74" t="s">
         <v>329</v>
       </c>
@@ -8577,7 +8559,7 @@
       <c r="E74" s="14"/>
       <c r="F74" s="14"/>
     </row>
-    <row r="75" spans="1:6" customFormat="1" ht="16">
+    <row r="75" spans="1:6" customFormat="1">
       <c r="A75" t="s">
         <v>330</v>
       </c>
@@ -8590,7 +8572,7 @@
       <c r="E75" s="14"/>
       <c r="F75" s="14"/>
     </row>
-    <row r="76" spans="1:6" customFormat="1" ht="16">
+    <row r="76" spans="1:6" customFormat="1">
       <c r="A76" t="s">
         <v>331</v>
       </c>
@@ -8603,7 +8585,7 @@
       <c r="E76" s="14"/>
       <c r="F76" s="14"/>
     </row>
-    <row r="77" spans="1:6" customFormat="1" ht="16">
+    <row r="77" spans="1:6" customFormat="1">
       <c r="A77" t="s">
         <v>332</v>
       </c>
@@ -8616,7 +8598,7 @@
       <c r="E77" s="14"/>
       <c r="F77" s="14"/>
     </row>
-    <row r="78" spans="1:6" customFormat="1" ht="16">
+    <row r="78" spans="1:6" customFormat="1">
       <c r="A78" t="s">
         <v>333</v>
       </c>
@@ -8629,7 +8611,7 @@
       <c r="E78" s="14"/>
       <c r="F78" s="14"/>
     </row>
-    <row r="79" spans="1:6" customFormat="1" ht="16">
+    <row r="79" spans="1:6" customFormat="1">
       <c r="A79" t="s">
         <v>334</v>
       </c>
@@ -8639,7 +8621,7 @@
       <c r="E79" s="14"/>
       <c r="F79" s="14"/>
     </row>
-    <row r="80" spans="1:6" customFormat="1" ht="16">
+    <row r="80" spans="1:6" customFormat="1">
       <c r="A80" t="s">
         <v>335</v>
       </c>
@@ -8652,7 +8634,7 @@
       <c r="E80" s="14"/>
       <c r="F80" s="14"/>
     </row>
-    <row r="81" spans="1:6" customFormat="1" ht="16">
+    <row r="81" spans="1:6" customFormat="1">
       <c r="A81" t="s">
         <v>336</v>
       </c>
@@ -8665,7 +8647,7 @@
       <c r="E81" s="14"/>
       <c r="F81" s="14"/>
     </row>
-    <row r="82" spans="1:6" customFormat="1" ht="16">
+    <row r="82" spans="1:6" customFormat="1">
       <c r="A82" t="s">
         <v>337</v>
       </c>
@@ -8678,7 +8660,7 @@
       <c r="E82" s="14"/>
       <c r="F82" s="14"/>
     </row>
-    <row r="83" spans="1:6" customFormat="1" ht="16">
+    <row r="83" spans="1:6" customFormat="1">
       <c r="A83" t="s">
         <v>338</v>
       </c>
@@ -8691,7 +8673,7 @@
       <c r="E83" s="14"/>
       <c r="F83" s="14"/>
     </row>
-    <row r="84" spans="1:6" customFormat="1" ht="16">
+    <row r="84" spans="1:6" customFormat="1">
       <c r="A84" t="s">
         <v>339</v>
       </c>
@@ -8704,7 +8686,7 @@
       <c r="E84" s="14"/>
       <c r="F84" s="14"/>
     </row>
-    <row r="85" spans="1:6" customFormat="1" ht="16">
+    <row r="85" spans="1:6" customFormat="1">
       <c r="A85" t="s">
         <v>340</v>
       </c>
@@ -8717,7 +8699,7 @@
       <c r="E85" s="14"/>
       <c r="F85" s="14"/>
     </row>
-    <row r="86" spans="1:6" customFormat="1" ht="16">
+    <row r="86" spans="1:6" customFormat="1">
       <c r="A86" t="s">
         <v>341</v>
       </c>
@@ -8727,7 +8709,7 @@
       <c r="E86" s="14"/>
       <c r="F86" s="14"/>
     </row>
-    <row r="87" spans="1:6" customFormat="1" ht="16">
+    <row r="87" spans="1:6" customFormat="1">
       <c r="A87" t="s">
         <v>342</v>
       </c>
@@ -8740,7 +8722,7 @@
       <c r="E87" s="14"/>
       <c r="F87" s="14"/>
     </row>
-    <row r="88" spans="1:6" customFormat="1" ht="16">
+    <row r="88" spans="1:6" customFormat="1">
       <c r="A88" t="s">
         <v>343</v>
       </c>
@@ -8753,7 +8735,7 @@
       <c r="E88" s="14"/>
       <c r="F88" s="14"/>
     </row>
-    <row r="89" spans="1:6" customFormat="1" ht="16">
+    <row r="89" spans="1:6" customFormat="1">
       <c r="A89" t="s">
         <v>344</v>
       </c>
@@ -8766,7 +8748,7 @@
       <c r="E89" s="14"/>
       <c r="F89" s="14"/>
     </row>
-    <row r="90" spans="1:6" customFormat="1" ht="16">
+    <row r="90" spans="1:6" customFormat="1">
       <c r="A90" t="s">
         <v>345</v>
       </c>
@@ -8779,7 +8761,7 @@
       <c r="E90" s="14"/>
       <c r="F90" s="14"/>
     </row>
-    <row r="91" spans="1:6" customFormat="1" ht="16">
+    <row r="91" spans="1:6" customFormat="1">
       <c r="A91" t="s">
         <v>346</v>
       </c>
@@ -8792,7 +8774,7 @@
       <c r="E91" s="14"/>
       <c r="F91" s="14"/>
     </row>
-    <row r="92" spans="1:6" customFormat="1" ht="16">
+    <row r="92" spans="1:6" customFormat="1">
       <c r="A92" t="s">
         <v>347</v>
       </c>
@@ -8805,7 +8787,7 @@
       <c r="E92" s="14"/>
       <c r="F92" s="14"/>
     </row>
-    <row r="93" spans="1:6" customFormat="1" ht="16">
+    <row r="93" spans="1:6" customFormat="1">
       <c r="A93" t="s">
         <v>348</v>
       </c>
@@ -8818,7 +8800,7 @@
       <c r="E93" s="14"/>
       <c r="F93" s="14"/>
     </row>
-    <row r="94" spans="1:6" s="12" customFormat="1" ht="16">
+    <row r="94" spans="1:6" s="12" customFormat="1">
       <c r="A94" s="12" t="s">
         <v>349</v>
       </c>
@@ -8831,7 +8813,7 @@
       <c r="E94" s="13"/>
       <c r="F94" s="13"/>
     </row>
-    <row r="95" spans="1:6" customFormat="1" ht="16">
+    <row r="95" spans="1:6" customFormat="1">
       <c r="A95" t="s">
         <v>350</v>
       </c>
@@ -8844,7 +8826,7 @@
       <c r="E95" s="14"/>
       <c r="F95" s="14"/>
     </row>
-    <row r="96" spans="1:6" customFormat="1" ht="16">
+    <row r="96" spans="1:6" customFormat="1">
       <c r="A96" t="s">
         <v>351</v>
       </c>
@@ -8857,7 +8839,7 @@
       <c r="E96" s="14"/>
       <c r="F96" s="14"/>
     </row>
-    <row r="97" spans="1:6" customFormat="1" ht="16">
+    <row r="97" spans="1:6" customFormat="1">
       <c r="A97" t="s">
         <v>352</v>
       </c>
@@ -8870,7 +8852,7 @@
       <c r="E97" s="14"/>
       <c r="F97" s="14"/>
     </row>
-    <row r="98" spans="1:6" customFormat="1" ht="16">
+    <row r="98" spans="1:6" customFormat="1">
       <c r="A98" t="s">
         <v>353</v>
       </c>
@@ -8883,7 +8865,7 @@
       <c r="E98" s="14"/>
       <c r="F98" s="14"/>
     </row>
-    <row r="99" spans="1:6" customFormat="1" ht="16">
+    <row r="99" spans="1:6" customFormat="1">
       <c r="A99" t="s">
         <v>354</v>
       </c>
@@ -8896,7 +8878,7 @@
       <c r="E99" s="14"/>
       <c r="F99" s="14"/>
     </row>
-    <row r="100" spans="1:6" customFormat="1" ht="16">
+    <row r="100" spans="1:6" customFormat="1">
       <c r="A100" t="s">
         <v>355</v>
       </c>
@@ -8909,7 +8891,7 @@
       <c r="E100" s="14"/>
       <c r="F100" s="14"/>
     </row>
-    <row r="101" spans="1:6" customFormat="1" ht="16">
+    <row r="101" spans="1:6" customFormat="1">
       <c r="A101" t="s">
         <v>356</v>
       </c>
@@ -8922,7 +8904,7 @@
       <c r="E101" s="14"/>
       <c r="F101" s="14"/>
     </row>
-    <row r="102" spans="1:6" customFormat="1" ht="16">
+    <row r="102" spans="1:6" customFormat="1">
       <c r="A102" t="s">
         <v>357</v>
       </c>
@@ -8935,7 +8917,7 @@
       <c r="E102" s="14"/>
       <c r="F102" s="14"/>
     </row>
-    <row r="103" spans="1:6" customFormat="1" ht="16">
+    <row r="103" spans="1:6" customFormat="1">
       <c r="A103" t="s">
         <v>358</v>
       </c>
@@ -8948,7 +8930,7 @@
       <c r="E103" s="14"/>
       <c r="F103" s="14"/>
     </row>
-    <row r="104" spans="1:6" customFormat="1" ht="16">
+    <row r="104" spans="1:6" customFormat="1">
       <c r="A104" t="s">
         <v>359</v>
       </c>
@@ -8961,7 +8943,7 @@
       <c r="E104" s="14"/>
       <c r="F104" s="14"/>
     </row>
-    <row r="105" spans="1:6" customFormat="1" ht="16">
+    <row r="105" spans="1:6" customFormat="1">
       <c r="A105" t="s">
         <v>360</v>
       </c>
@@ -8974,7 +8956,7 @@
       <c r="E105" s="14"/>
       <c r="F105" s="14"/>
     </row>
-    <row r="106" spans="1:6" customFormat="1" ht="16">
+    <row r="106" spans="1:6" customFormat="1">
       <c r="A106" t="s">
         <v>361</v>
       </c>
@@ -8987,7 +8969,7 @@
       <c r="E106" s="14"/>
       <c r="F106" s="14"/>
     </row>
-    <row r="107" spans="1:6" customFormat="1" ht="16">
+    <row r="107" spans="1:6" customFormat="1">
       <c r="A107" t="s">
         <v>362</v>
       </c>
@@ -9000,7 +8982,7 @@
       <c r="E107" s="14"/>
       <c r="F107" s="14"/>
     </row>
-    <row r="108" spans="1:6" customFormat="1" ht="16">
+    <row r="108" spans="1:6" customFormat="1">
       <c r="A108" t="s">
         <v>363</v>
       </c>
@@ -9013,7 +8995,7 @@
       <c r="E108" s="14"/>
       <c r="F108" s="14"/>
     </row>
-    <row r="109" spans="1:6" customFormat="1" ht="16">
+    <row r="109" spans="1:6" customFormat="1">
       <c r="A109" t="s">
         <v>364</v>
       </c>
@@ -9026,7 +9008,7 @@
       <c r="E109" s="14"/>
       <c r="F109" s="14"/>
     </row>
-    <row r="110" spans="1:6" customFormat="1" ht="16">
+    <row r="110" spans="1:6" customFormat="1">
       <c r="A110" t="s">
         <v>365</v>
       </c>
@@ -9039,7 +9021,7 @@
       <c r="E110" s="14"/>
       <c r="F110" s="14"/>
     </row>
-    <row r="111" spans="1:6" customFormat="1" ht="16">
+    <row r="111" spans="1:6" customFormat="1">
       <c r="A111" t="s">
         <v>366</v>
       </c>
@@ -9052,7 +9034,7 @@
       <c r="E111" s="14"/>
       <c r="F111" s="14"/>
     </row>
-    <row r="112" spans="1:6" customFormat="1" ht="16">
+    <row r="112" spans="1:6" customFormat="1">
       <c r="A112" t="s">
         <v>367</v>
       </c>
@@ -9062,7 +9044,7 @@
       <c r="E112" s="14"/>
       <c r="F112" s="14"/>
     </row>
-    <row r="113" spans="1:6" customFormat="1" ht="16">
+    <row r="113" spans="1:6" customFormat="1">
       <c r="A113" t="s">
         <v>368</v>
       </c>
@@ -9075,7 +9057,7 @@
       <c r="E113" s="14"/>
       <c r="F113" s="14"/>
     </row>
-    <row r="114" spans="1:6" customFormat="1" ht="16">
+    <row r="114" spans="1:6" customFormat="1">
       <c r="A114" t="s">
         <v>369</v>
       </c>
@@ -9088,7 +9070,7 @@
       <c r="E114" s="14"/>
       <c r="F114" s="14"/>
     </row>
-    <row r="115" spans="1:6" customFormat="1" ht="16">
+    <row r="115" spans="1:6" customFormat="1">
       <c r="A115" t="s">
         <v>370</v>
       </c>
@@ -9101,7 +9083,7 @@
       <c r="E115" s="14"/>
       <c r="F115" s="14"/>
     </row>
-    <row r="116" spans="1:6" customFormat="1" ht="16">
+    <row r="116" spans="1:6" customFormat="1">
       <c r="A116" t="s">
         <v>371</v>
       </c>
@@ -9114,7 +9096,7 @@
       <c r="E116" s="14"/>
       <c r="F116" s="14"/>
     </row>
-    <row r="117" spans="1:6" customFormat="1" ht="16">
+    <row r="117" spans="1:6" customFormat="1">
       <c r="A117" t="s">
         <v>372</v>
       </c>
@@ -9127,7 +9109,7 @@
       <c r="E117" s="14"/>
       <c r="F117" s="14"/>
     </row>
-    <row r="118" spans="1:6" s="12" customFormat="1" ht="16">
+    <row r="118" spans="1:6" s="12" customFormat="1">
       <c r="A118" s="12" t="s">
         <v>373</v>
       </c>
@@ -9140,7 +9122,7 @@
       <c r="E118" s="13"/>
       <c r="F118" s="13"/>
     </row>
-    <row r="119" spans="1:6" customFormat="1" ht="16">
+    <row r="119" spans="1:6" customFormat="1">
       <c r="A119" t="s">
         <v>374</v>
       </c>
@@ -9153,7 +9135,7 @@
       <c r="E119" s="14"/>
       <c r="F119" s="14"/>
     </row>
-    <row r="120" spans="1:6" customFormat="1" ht="16">
+    <row r="120" spans="1:6" customFormat="1">
       <c r="A120" t="s">
         <v>375</v>
       </c>
@@ -9166,7 +9148,7 @@
       <c r="E120" s="14"/>
       <c r="F120" s="14"/>
     </row>
-    <row r="121" spans="1:6" customFormat="1" ht="16">
+    <row r="121" spans="1:6" customFormat="1">
       <c r="A121" t="s">
         <v>376</v>
       </c>
@@ -9179,7 +9161,7 @@
       <c r="E121" s="14"/>
       <c r="F121" s="14"/>
     </row>
-    <row r="122" spans="1:6" customFormat="1" ht="16">
+    <row r="122" spans="1:6" customFormat="1">
       <c r="A122" t="s">
         <v>377</v>
       </c>
@@ -9192,7 +9174,7 @@
       <c r="E122" s="14"/>
       <c r="F122" s="14"/>
     </row>
-    <row r="123" spans="1:6" customFormat="1" ht="16">
+    <row r="123" spans="1:6" customFormat="1">
       <c r="A123" t="s">
         <v>378</v>
       </c>
@@ -9205,7 +9187,7 @@
       <c r="E123" s="14"/>
       <c r="F123" s="14"/>
     </row>
-    <row r="124" spans="1:6" customFormat="1" ht="16">
+    <row r="124" spans="1:6" customFormat="1">
       <c r="A124" t="s">
         <v>379</v>
       </c>
@@ -9218,7 +9200,7 @@
       <c r="E124" s="14"/>
       <c r="F124" s="14"/>
     </row>
-    <row r="125" spans="1:6" customFormat="1" ht="16">
+    <row r="125" spans="1:6" customFormat="1">
       <c r="A125" t="s">
         <v>380</v>
       </c>
@@ -9231,7 +9213,7 @@
       <c r="E125" s="14"/>
       <c r="F125" s="14"/>
     </row>
-    <row r="126" spans="1:6" customFormat="1" ht="16">
+    <row r="126" spans="1:6" customFormat="1">
       <c r="A126" t="s">
         <v>381</v>
       </c>
@@ -9244,7 +9226,7 @@
       <c r="E126" s="14"/>
       <c r="F126" s="14"/>
     </row>
-    <row r="127" spans="1:6" customFormat="1" ht="16">
+    <row r="127" spans="1:6" customFormat="1">
       <c r="A127" t="s">
         <v>382</v>
       </c>
@@ -9257,7 +9239,7 @@
       <c r="E127" s="14"/>
       <c r="F127" s="14"/>
     </row>
-    <row r="128" spans="1:6" customFormat="1" ht="16">
+    <row r="128" spans="1:6" customFormat="1">
       <c r="A128" t="s">
         <v>383</v>
       </c>
@@ -9270,7 +9252,7 @@
       <c r="E128" s="14"/>
       <c r="F128" s="14"/>
     </row>
-    <row r="129" spans="1:6" customFormat="1" ht="16">
+    <row r="129" spans="1:6" customFormat="1">
       <c r="A129" t="s">
         <v>67</v>
       </c>
@@ -9283,7 +9265,7 @@
       <c r="E129" s="14"/>
       <c r="F129" s="14"/>
     </row>
-    <row r="130" spans="1:6" customFormat="1" ht="16">
+    <row r="130" spans="1:6" customFormat="1">
       <c r="A130" t="s">
         <v>384</v>
       </c>
@@ -9296,7 +9278,7 @@
       <c r="E130" s="14"/>
       <c r="F130" s="14"/>
     </row>
-    <row r="131" spans="1:6" customFormat="1" ht="16">
+    <row r="131" spans="1:6" customFormat="1">
       <c r="A131" t="s">
         <v>385</v>
       </c>
@@ -9309,7 +9291,7 @@
       <c r="E131" s="14"/>
       <c r="F131" s="14"/>
     </row>
-    <row r="132" spans="1:6" customFormat="1" ht="16">
+    <row r="132" spans="1:6" customFormat="1">
       <c r="A132" t="s">
         <v>386</v>
       </c>
@@ -9322,7 +9304,7 @@
       <c r="E132" s="14"/>
       <c r="F132" s="14"/>
     </row>
-    <row r="133" spans="1:6" customFormat="1" ht="16">
+    <row r="133" spans="1:6" customFormat="1">
       <c r="A133" t="s">
         <v>387</v>
       </c>
@@ -9335,7 +9317,7 @@
       <c r="E133" s="14"/>
       <c r="F133" s="14"/>
     </row>
-    <row r="134" spans="1:6" customFormat="1" ht="16">
+    <row r="134" spans="1:6" customFormat="1">
       <c r="A134" t="s">
         <v>388</v>
       </c>
@@ -9348,7 +9330,7 @@
       <c r="E134" s="14"/>
       <c r="F134" s="14"/>
     </row>
-    <row r="135" spans="1:6" customFormat="1" ht="16">
+    <row r="135" spans="1:6" customFormat="1">
       <c r="A135" t="s">
         <v>389</v>
       </c>
@@ -9361,7 +9343,7 @@
       <c r="E135" s="14"/>
       <c r="F135" s="14"/>
     </row>
-    <row r="136" spans="1:6" customFormat="1" ht="16">
+    <row r="136" spans="1:6" customFormat="1">
       <c r="A136" t="s">
         <v>390</v>
       </c>
@@ -9374,7 +9356,7 @@
       <c r="E136" s="14"/>
       <c r="F136" s="14"/>
     </row>
-    <row r="137" spans="1:6" customFormat="1" ht="16">
+    <row r="137" spans="1:6" customFormat="1">
       <c r="A137" t="s">
         <v>391</v>
       </c>
@@ -9387,7 +9369,7 @@
       <c r="E137" s="14"/>
       <c r="F137" s="14"/>
     </row>
-    <row r="138" spans="1:6" customFormat="1" ht="16">
+    <row r="138" spans="1:6" customFormat="1">
       <c r="A138" t="s">
         <v>392</v>
       </c>
@@ -9400,7 +9382,7 @@
       <c r="E138" s="14"/>
       <c r="F138" s="14"/>
     </row>
-    <row r="139" spans="1:6" customFormat="1" ht="16">
+    <row r="139" spans="1:6" customFormat="1">
       <c r="A139" t="s">
         <v>393</v>
       </c>
@@ -9413,7 +9395,7 @@
       <c r="E139" s="14"/>
       <c r="F139" s="14"/>
     </row>
-    <row r="140" spans="1:6" customFormat="1" ht="16">
+    <row r="140" spans="1:6" customFormat="1">
       <c r="A140" t="s">
         <v>394</v>
       </c>
@@ -9426,7 +9408,7 @@
       <c r="E140" s="14"/>
       <c r="F140" s="14"/>
     </row>
-    <row r="141" spans="1:6" customFormat="1" ht="16">
+    <row r="141" spans="1:6" customFormat="1">
       <c r="A141" t="s">
         <v>395</v>
       </c>
@@ -9439,7 +9421,7 @@
       <c r="E141" s="14"/>
       <c r="F141" s="14"/>
     </row>
-    <row r="142" spans="1:6" customFormat="1" ht="16">
+    <row r="142" spans="1:6" customFormat="1">
       <c r="A142" t="s">
         <v>396</v>
       </c>
@@ -9452,7 +9434,7 @@
       <c r="E142" s="14"/>
       <c r="F142" s="14"/>
     </row>
-    <row r="143" spans="1:6" customFormat="1" ht="16">
+    <row r="143" spans="1:6" customFormat="1">
       <c r="A143" t="s">
         <v>397</v>
       </c>
@@ -9465,7 +9447,7 @@
       <c r="E143" s="14"/>
       <c r="F143" s="14"/>
     </row>
-    <row r="144" spans="1:6" customFormat="1" ht="16">
+    <row r="144" spans="1:6" customFormat="1">
       <c r="A144" t="s">
         <v>398</v>
       </c>
@@ -9478,7 +9460,7 @@
       <c r="E144" s="14"/>
       <c r="F144" s="14"/>
     </row>
-    <row r="145" spans="1:6" customFormat="1" ht="16">
+    <row r="145" spans="1:6" customFormat="1">
       <c r="A145" t="s">
         <v>399</v>
       </c>
@@ -9491,7 +9473,7 @@
       <c r="E145" s="14"/>
       <c r="F145" s="14"/>
     </row>
-    <row r="146" spans="1:6" customFormat="1" ht="16">
+    <row r="146" spans="1:6" customFormat="1">
       <c r="A146" t="s">
         <v>400</v>
       </c>
@@ -9504,7 +9486,7 @@
       <c r="E146" s="14"/>
       <c r="F146" s="14"/>
     </row>
-    <row r="147" spans="1:6" customFormat="1" ht="16">
+    <row r="147" spans="1:6" customFormat="1">
       <c r="A147" t="s">
         <v>401</v>
       </c>
@@ -9517,7 +9499,7 @@
       <c r="E147" s="14"/>
       <c r="F147" s="14"/>
     </row>
-    <row r="148" spans="1:6" customFormat="1" ht="16">
+    <row r="148" spans="1:6" customFormat="1">
       <c r="A148" t="s">
         <v>402</v>
       </c>
@@ -9530,7 +9512,7 @@
       <c r="E148" s="14"/>
       <c r="F148" s="14"/>
     </row>
-    <row r="149" spans="1:6" s="12" customFormat="1" ht="16">
+    <row r="149" spans="1:6" s="12" customFormat="1">
       <c r="A149" s="12" t="s">
         <v>403</v>
       </c>
@@ -9543,7 +9525,7 @@
       <c r="E149" s="13"/>
       <c r="F149" s="13"/>
     </row>
-    <row r="150" spans="1:6" customFormat="1" ht="16">
+    <row r="150" spans="1:6" customFormat="1">
       <c r="A150" t="s">
         <v>404</v>
       </c>
@@ -9556,7 +9538,7 @@
       <c r="E150" s="14"/>
       <c r="F150" s="14"/>
     </row>
-    <row r="151" spans="1:6" customFormat="1" ht="16">
+    <row r="151" spans="1:6" customFormat="1">
       <c r="A151" t="s">
         <v>405</v>
       </c>
@@ -9569,7 +9551,7 @@
       <c r="E151" s="14"/>
       <c r="F151" s="14"/>
     </row>
-    <row r="152" spans="1:6" customFormat="1" ht="16">
+    <row r="152" spans="1:6" customFormat="1">
       <c r="A152" t="s">
         <v>406</v>
       </c>
@@ -9582,7 +9564,7 @@
       <c r="E152" s="14"/>
       <c r="F152" s="14"/>
     </row>
-    <row r="153" spans="1:6" customFormat="1" ht="16">
+    <row r="153" spans="1:6" customFormat="1">
       <c r="A153" t="s">
         <v>407</v>
       </c>
@@ -9595,7 +9577,7 @@
       <c r="E153" s="14"/>
       <c r="F153" s="14"/>
     </row>
-    <row r="154" spans="1:6" customFormat="1" ht="16">
+    <row r="154" spans="1:6" customFormat="1">
       <c r="A154" t="s">
         <v>408</v>
       </c>
@@ -9608,7 +9590,7 @@
       <c r="E154" s="14"/>
       <c r="F154" s="14"/>
     </row>
-    <row r="155" spans="1:6" customFormat="1" ht="16">
+    <row r="155" spans="1:6" customFormat="1">
       <c r="A155" t="s">
         <v>409</v>
       </c>
@@ -9621,7 +9603,7 @@
       <c r="E155" s="14"/>
       <c r="F155" s="14"/>
     </row>
-    <row r="156" spans="1:6" customFormat="1" ht="16">
+    <row r="156" spans="1:6" customFormat="1">
       <c r="A156" t="s">
         <v>410</v>
       </c>
@@ -9634,7 +9616,7 @@
       <c r="E156" s="14"/>
       <c r="F156" s="14"/>
     </row>
-    <row r="157" spans="1:6" customFormat="1" ht="16">
+    <row r="157" spans="1:6" customFormat="1">
       <c r="A157" t="s">
         <v>411</v>
       </c>
@@ -9647,7 +9629,7 @@
       <c r="E157" s="14"/>
       <c r="F157" s="14"/>
     </row>
-    <row r="158" spans="1:6" customFormat="1" ht="16">
+    <row r="158" spans="1:6" customFormat="1">
       <c r="A158" t="s">
         <v>412</v>
       </c>
@@ -9657,7 +9639,7 @@
       <c r="E158" s="14"/>
       <c r="F158" s="14"/>
     </row>
-    <row r="159" spans="1:6" customFormat="1" ht="16">
+    <row r="159" spans="1:6" customFormat="1">
       <c r="A159" t="s">
         <v>413</v>
       </c>
@@ -9670,7 +9652,7 @@
       <c r="E159" s="14"/>
       <c r="F159" s="14"/>
     </row>
-    <row r="160" spans="1:6" customFormat="1" ht="16">
+    <row r="160" spans="1:6" customFormat="1">
       <c r="A160" t="s">
         <v>414</v>
       </c>
@@ -9683,7 +9665,7 @@
       <c r="E160" s="14"/>
       <c r="F160" s="14"/>
     </row>
-    <row r="161" spans="1:6" customFormat="1" ht="16">
+    <row r="161" spans="1:6" customFormat="1">
       <c r="A161" t="s">
         <v>415</v>
       </c>
@@ -9696,7 +9678,7 @@
       <c r="E161" s="14"/>
       <c r="F161" s="14"/>
     </row>
-    <row r="162" spans="1:6" customFormat="1" ht="16">
+    <row r="162" spans="1:6" customFormat="1">
       <c r="A162" t="s">
         <v>416</v>
       </c>
@@ -9709,7 +9691,7 @@
       <c r="E162" s="14"/>
       <c r="F162" s="14"/>
     </row>
-    <row r="163" spans="1:6" customFormat="1" ht="16">
+    <row r="163" spans="1:6" customFormat="1">
       <c r="A163" t="s">
         <v>417</v>
       </c>
@@ -9722,7 +9704,7 @@
       <c r="E163" s="14"/>
       <c r="F163" s="14"/>
     </row>
-    <row r="164" spans="1:6" customFormat="1" ht="16">
+    <row r="164" spans="1:6" customFormat="1">
       <c r="A164" t="s">
         <v>418</v>
       </c>
@@ -9735,7 +9717,7 @@
       <c r="E164" s="14"/>
       <c r="F164" s="14"/>
     </row>
-    <row r="165" spans="1:6" customFormat="1" ht="16">
+    <row r="165" spans="1:6" customFormat="1">
       <c r="A165" t="s">
         <v>419</v>
       </c>
@@ -9748,7 +9730,7 @@
       <c r="E165" s="14"/>
       <c r="F165" s="14"/>
     </row>
-    <row r="166" spans="1:6" customFormat="1" ht="16">
+    <row r="166" spans="1:6" customFormat="1">
       <c r="A166" t="s">
         <v>420</v>
       </c>
@@ -9761,7 +9743,7 @@
       <c r="E166" s="14"/>
       <c r="F166" s="14"/>
     </row>
-    <row r="167" spans="1:6" customFormat="1" ht="16">
+    <row r="167" spans="1:6" customFormat="1">
       <c r="A167" t="s">
         <v>421</v>
       </c>
@@ -9774,7 +9756,7 @@
       <c r="E167" s="14"/>
       <c r="F167" s="14"/>
     </row>
-    <row r="168" spans="1:6" customFormat="1" ht="16">
+    <row r="168" spans="1:6" customFormat="1">
       <c r="A168" t="s">
         <v>422</v>
       </c>
@@ -9787,7 +9769,7 @@
       <c r="E168" s="14"/>
       <c r="F168" s="14"/>
     </row>
-    <row r="169" spans="1:6" customFormat="1" ht="16">
+    <row r="169" spans="1:6" customFormat="1">
       <c r="A169" t="s">
         <v>423</v>
       </c>
@@ -9800,7 +9782,7 @@
       <c r="E169" s="14"/>
       <c r="F169" s="14"/>
     </row>
-    <row r="170" spans="1:6" customFormat="1" ht="16">
+    <row r="170" spans="1:6" customFormat="1">
       <c r="A170" t="s">
         <v>424</v>
       </c>
@@ -9810,7 +9792,7 @@
       <c r="E170" s="14"/>
       <c r="F170" s="14"/>
     </row>
-    <row r="171" spans="1:6" customFormat="1" ht="16">
+    <row r="171" spans="1:6" customFormat="1">
       <c r="A171" t="s">
         <v>425</v>
       </c>
@@ -9823,7 +9805,7 @@
       <c r="E171" s="14"/>
       <c r="F171" s="14"/>
     </row>
-    <row r="172" spans="1:6" customFormat="1" ht="16">
+    <row r="172" spans="1:6" customFormat="1">
       <c r="A172" t="s">
         <v>426</v>
       </c>
@@ -9836,7 +9818,7 @@
       <c r="E172" s="14"/>
       <c r="F172" s="14"/>
     </row>
-    <row r="173" spans="1:6" customFormat="1" ht="16">
+    <row r="173" spans="1:6" customFormat="1">
       <c r="A173" t="s">
         <v>427</v>
       </c>
@@ -9846,7 +9828,7 @@
       <c r="E173" s="14"/>
       <c r="F173" s="14"/>
     </row>
-    <row r="174" spans="1:6" customFormat="1" ht="16">
+    <row r="174" spans="1:6" customFormat="1">
       <c r="A174" t="s">
         <v>428</v>
       </c>
@@ -9859,7 +9841,7 @@
       <c r="E174" s="14"/>
       <c r="F174" s="14"/>
     </row>
-    <row r="175" spans="1:6" customFormat="1" ht="16">
+    <row r="175" spans="1:6" customFormat="1">
       <c r="A175" t="s">
         <v>429</v>
       </c>
@@ -9872,7 +9854,7 @@
       <c r="E175" s="14"/>
       <c r="F175" s="14"/>
     </row>
-    <row r="176" spans="1:6" customFormat="1" ht="16">
+    <row r="176" spans="1:6" customFormat="1">
       <c r="A176" t="s">
         <v>430</v>
       </c>
@@ -9885,7 +9867,7 @@
       <c r="E176" s="14"/>
       <c r="F176" s="14"/>
     </row>
-    <row r="177" spans="1:6" customFormat="1" ht="16">
+    <row r="177" spans="1:6" customFormat="1">
       <c r="A177" t="s">
         <v>431</v>
       </c>
@@ -9898,7 +9880,7 @@
       <c r="E177" s="14"/>
       <c r="F177" s="14"/>
     </row>
-    <row r="178" spans="1:6" customFormat="1" ht="16">
+    <row r="178" spans="1:6" customFormat="1">
       <c r="A178" t="s">
         <v>432</v>
       </c>
@@ -9911,7 +9893,7 @@
       <c r="E178" s="14"/>
       <c r="F178" s="14"/>
     </row>
-    <row r="179" spans="1:6" customFormat="1" ht="16">
+    <row r="179" spans="1:6" customFormat="1">
       <c r="A179" t="s">
         <v>433</v>
       </c>
@@ -9924,7 +9906,7 @@
       <c r="E179" s="14"/>
       <c r="F179" s="14"/>
     </row>
-    <row r="180" spans="1:6" customFormat="1" ht="16">
+    <row r="180" spans="1:6" customFormat="1">
       <c r="A180" t="s">
         <v>434</v>
       </c>
@@ -9937,7 +9919,7 @@
       <c r="E180" s="14"/>
       <c r="F180" s="14"/>
     </row>
-    <row r="181" spans="1:6" customFormat="1" ht="16">
+    <row r="181" spans="1:6" customFormat="1">
       <c r="A181" t="s">
         <v>435</v>
       </c>
@@ -9950,7 +9932,7 @@
       <c r="E181" s="14"/>
       <c r="F181" s="14"/>
     </row>
-    <row r="182" spans="1:6" customFormat="1" ht="16">
+    <row r="182" spans="1:6" customFormat="1">
       <c r="A182" t="s">
         <v>436</v>
       </c>
@@ -9963,7 +9945,7 @@
       <c r="E182" s="14"/>
       <c r="F182" s="14"/>
     </row>
-    <row r="183" spans="1:6" customFormat="1" ht="16">
+    <row r="183" spans="1:6" customFormat="1">
       <c r="A183" t="s">
         <v>437</v>
       </c>
@@ -9976,7 +9958,7 @@
       <c r="E183" s="14"/>
       <c r="F183" s="14"/>
     </row>
-    <row r="184" spans="1:6" customFormat="1" ht="16">
+    <row r="184" spans="1:6" customFormat="1">
       <c r="A184" t="s">
         <v>438</v>
       </c>
@@ -9989,7 +9971,7 @@
       <c r="E184" s="14"/>
       <c r="F184" s="14"/>
     </row>
-    <row r="185" spans="1:6" customFormat="1" ht="16">
+    <row r="185" spans="1:6" customFormat="1">
       <c r="A185" t="s">
         <v>439</v>
       </c>
@@ -10002,7 +9984,7 @@
       <c r="E185" s="14"/>
       <c r="F185" s="14"/>
     </row>
-    <row r="186" spans="1:6" customFormat="1" ht="16">
+    <row r="186" spans="1:6" customFormat="1">
       <c r="A186" t="s">
         <v>440</v>
       </c>
@@ -10015,7 +9997,7 @@
       <c r="E186" s="14"/>
       <c r="F186" s="14"/>
     </row>
-    <row r="187" spans="1:6" customFormat="1" ht="16">
+    <row r="187" spans="1:6" customFormat="1">
       <c r="A187" t="s">
         <v>441</v>
       </c>
@@ -10028,7 +10010,7 @@
       <c r="E187" s="14"/>
       <c r="F187" s="14"/>
     </row>
-    <row r="188" spans="1:6" customFormat="1" ht="16">
+    <row r="188" spans="1:6" customFormat="1">
       <c r="A188" t="s">
         <v>442</v>
       </c>
@@ -10041,7 +10023,7 @@
       <c r="E188" s="14"/>
       <c r="F188" s="14"/>
     </row>
-    <row r="189" spans="1:6" customFormat="1" ht="16">
+    <row r="189" spans="1:6" customFormat="1">
       <c r="A189" t="s">
         <v>443</v>
       </c>
@@ -10054,7 +10036,7 @@
       <c r="E189" s="14"/>
       <c r="F189" s="14"/>
     </row>
-    <row r="190" spans="1:6" customFormat="1" ht="16">
+    <row r="190" spans="1:6" customFormat="1">
       <c r="A190" t="s">
         <v>444</v>
       </c>
@@ -10067,7 +10049,7 @@
       <c r="E190" s="14"/>
       <c r="F190" s="14"/>
     </row>
-    <row r="191" spans="1:6" s="12" customFormat="1" ht="16">
+    <row r="191" spans="1:6" s="12" customFormat="1">
       <c r="A191" s="12" t="s">
         <v>445</v>
       </c>
@@ -10080,7 +10062,7 @@
       <c r="E191" s="13"/>
       <c r="F191" s="13"/>
     </row>
-    <row r="192" spans="1:6" customFormat="1" ht="16">
+    <row r="192" spans="1:6" customFormat="1">
       <c r="A192" t="s">
         <v>446</v>
       </c>
@@ -10093,7 +10075,7 @@
       <c r="E192" s="14"/>
       <c r="F192" s="14"/>
     </row>
-    <row r="193" spans="1:6" customFormat="1" ht="16">
+    <row r="193" spans="1:6" customFormat="1">
       <c r="A193" t="s">
         <v>447</v>
       </c>
@@ -10103,7 +10085,7 @@
       <c r="E193" s="14"/>
       <c r="F193" s="14"/>
     </row>
-    <row r="194" spans="1:6" customFormat="1" ht="16">
+    <row r="194" spans="1:6" customFormat="1">
       <c r="A194" t="s">
         <v>448</v>
       </c>
@@ -10113,7 +10095,7 @@
       <c r="E194" s="14"/>
       <c r="F194" s="14"/>
     </row>
-    <row r="195" spans="1:6" customFormat="1" ht="16">
+    <row r="195" spans="1:6" customFormat="1">
       <c r="A195" t="s">
         <v>449</v>
       </c>
@@ -10123,7 +10105,7 @@
       <c r="E195" s="14"/>
       <c r="F195" s="14"/>
     </row>
-    <row r="196" spans="1:6" customFormat="1" ht="16">
+    <row r="196" spans="1:6" customFormat="1">
       <c r="A196" t="s">
         <v>618</v>
       </c>
@@ -10136,7 +10118,7 @@
       <c r="E196" s="14"/>
       <c r="F196" s="14"/>
     </row>
-    <row r="197" spans="1:6" customFormat="1" ht="16">
+    <row r="197" spans="1:6" customFormat="1">
       <c r="A197" t="s">
         <v>450</v>
       </c>
@@ -10149,7 +10131,7 @@
       <c r="E197" s="14"/>
       <c r="F197" s="14"/>
     </row>
-    <row r="198" spans="1:6" customFormat="1" ht="16">
+    <row r="198" spans="1:6" customFormat="1">
       <c r="A198" t="s">
         <v>451</v>
       </c>
@@ -10162,7 +10144,7 @@
       <c r="E198" s="14"/>
       <c r="F198" s="14"/>
     </row>
-    <row r="199" spans="1:6" customFormat="1" ht="16">
+    <row r="199" spans="1:6" customFormat="1">
       <c r="A199" t="s">
         <v>452</v>
       </c>
@@ -10175,7 +10157,7 @@
       <c r="E199" s="14"/>
       <c r="F199" s="14"/>
     </row>
-    <row r="200" spans="1:6" customFormat="1" ht="16">
+    <row r="200" spans="1:6" customFormat="1">
       <c r="A200" t="s">
         <v>453</v>
       </c>
@@ -10188,7 +10170,7 @@
       <c r="E200" s="14"/>
       <c r="F200" s="14"/>
     </row>
-    <row r="201" spans="1:6" customFormat="1" ht="16">
+    <row r="201" spans="1:6" customFormat="1">
       <c r="A201" t="s">
         <v>454</v>
       </c>
@@ -10201,7 +10183,7 @@
       <c r="E201" s="14"/>
       <c r="F201" s="14"/>
     </row>
-    <row r="202" spans="1:6" customFormat="1" ht="16">
+    <row r="202" spans="1:6" customFormat="1">
       <c r="A202" t="s">
         <v>455</v>
       </c>
@@ -10214,7 +10196,7 @@
       <c r="E202" s="14"/>
       <c r="F202" s="14"/>
     </row>
-    <row r="203" spans="1:6" customFormat="1" ht="16">
+    <row r="203" spans="1:6" customFormat="1">
       <c r="A203" t="s">
         <v>456</v>
       </c>
@@ -10227,7 +10209,7 @@
       <c r="E203" s="14"/>
       <c r="F203" s="14"/>
     </row>
-    <row r="204" spans="1:6" customFormat="1" ht="16">
+    <row r="204" spans="1:6" customFormat="1">
       <c r="A204" t="s">
         <v>457</v>
       </c>
@@ -10240,7 +10222,7 @@
       <c r="E204" s="14"/>
       <c r="F204" s="14"/>
     </row>
-    <row r="205" spans="1:6" customFormat="1" ht="16">
+    <row r="205" spans="1:6" customFormat="1">
       <c r="A205" t="s">
         <v>458</v>
       </c>
@@ -10253,7 +10235,7 @@
       <c r="E205" s="14"/>
       <c r="F205" s="14"/>
     </row>
-    <row r="206" spans="1:6" customFormat="1" ht="16">
+    <row r="206" spans="1:6" customFormat="1">
       <c r="A206" t="s">
         <v>459</v>
       </c>
@@ -10266,7 +10248,7 @@
       <c r="E206" s="14"/>
       <c r="F206" s="14"/>
     </row>
-    <row r="207" spans="1:6" customFormat="1" ht="16">
+    <row r="207" spans="1:6" customFormat="1">
       <c r="A207" t="s">
         <v>460</v>
       </c>
@@ -10279,7 +10261,7 @@
       <c r="E207" s="14"/>
       <c r="F207" s="14"/>
     </row>
-    <row r="208" spans="1:6" customFormat="1" ht="16">
+    <row r="208" spans="1:6" customFormat="1">
       <c r="A208" t="s">
         <v>461</v>
       </c>
@@ -10292,7 +10274,7 @@
       <c r="E208" s="14"/>
       <c r="F208" s="14"/>
     </row>
-    <row r="209" spans="1:6" customFormat="1" ht="16">
+    <row r="209" spans="1:6" customFormat="1">
       <c r="A209" t="s">
         <v>462</v>
       </c>
@@ -10305,7 +10287,7 @@
       <c r="E209" s="14"/>
       <c r="F209" s="14"/>
     </row>
-    <row r="210" spans="1:6" customFormat="1" ht="16">
+    <row r="210" spans="1:6" customFormat="1">
       <c r="A210" t="s">
         <v>463</v>
       </c>
@@ -10318,7 +10300,7 @@
       <c r="E210" s="14"/>
       <c r="F210" s="14"/>
     </row>
-    <row r="211" spans="1:6" customFormat="1" ht="16">
+    <row r="211" spans="1:6" customFormat="1">
       <c r="A211" t="s">
         <v>464</v>
       </c>
@@ -10331,7 +10313,7 @@
       <c r="E211" s="14"/>
       <c r="F211" s="14"/>
     </row>
-    <row r="212" spans="1:6" customFormat="1" ht="16">
+    <row r="212" spans="1:6" customFormat="1">
       <c r="A212" t="s">
         <v>465</v>
       </c>
@@ -10344,7 +10326,7 @@
       <c r="E212" s="14"/>
       <c r="F212" s="14"/>
     </row>
-    <row r="213" spans="1:6" customFormat="1" ht="16">
+    <row r="213" spans="1:6" customFormat="1">
       <c r="A213" t="s">
         <v>466</v>
       </c>
@@ -10357,7 +10339,7 @@
       <c r="E213" s="14"/>
       <c r="F213" s="14"/>
     </row>
-    <row r="214" spans="1:6" customFormat="1" ht="16">
+    <row r="214" spans="1:6" customFormat="1">
       <c r="A214" t="s">
         <v>467</v>
       </c>
@@ -10370,7 +10352,7 @@
       <c r="E214" s="14"/>
       <c r="F214" s="14"/>
     </row>
-    <row r="215" spans="1:6" customFormat="1" ht="16">
+    <row r="215" spans="1:6" customFormat="1">
       <c r="A215" t="s">
         <v>468</v>
       </c>
@@ -10383,7 +10365,7 @@
       <c r="E215" s="14"/>
       <c r="F215" s="14"/>
     </row>
-    <row r="216" spans="1:6" customFormat="1" ht="16">
+    <row r="216" spans="1:6" customFormat="1">
       <c r="A216" t="s">
         <v>469</v>
       </c>
@@ -10396,7 +10378,7 @@
       <c r="E216" s="14"/>
       <c r="F216" s="14"/>
     </row>
-    <row r="217" spans="1:6" customFormat="1" ht="16">
+    <row r="217" spans="1:6" customFormat="1">
       <c r="A217" t="s">
         <v>470</v>
       </c>
@@ -10409,7 +10391,7 @@
       <c r="E217" s="14"/>
       <c r="F217" s="14"/>
     </row>
-    <row r="218" spans="1:6" customFormat="1" ht="16">
+    <row r="218" spans="1:6" customFormat="1">
       <c r="A218" t="s">
         <v>471</v>
       </c>
@@ -10422,7 +10404,7 @@
       <c r="E218" s="14"/>
       <c r="F218" s="14"/>
     </row>
-    <row r="219" spans="1:6" customFormat="1" ht="16">
+    <row r="219" spans="1:6" customFormat="1">
       <c r="A219" t="s">
         <v>472</v>
       </c>
@@ -10435,7 +10417,7 @@
       <c r="E219" s="14"/>
       <c r="F219" s="14"/>
     </row>
-    <row r="220" spans="1:6" customFormat="1" ht="16">
+    <row r="220" spans="1:6" customFormat="1">
       <c r="A220" t="s">
         <v>473</v>
       </c>
@@ -10448,7 +10430,7 @@
       <c r="E220" s="14"/>
       <c r="F220" s="14"/>
     </row>
-    <row r="221" spans="1:6" customFormat="1" ht="16">
+    <row r="221" spans="1:6" customFormat="1">
       <c r="A221" t="s">
         <v>474</v>
       </c>
@@ -10461,7 +10443,7 @@
       <c r="E221" s="14"/>
       <c r="F221" s="14"/>
     </row>
-    <row r="222" spans="1:6" customFormat="1" ht="16">
+    <row r="222" spans="1:6" customFormat="1">
       <c r="A222" t="s">
         <v>475</v>
       </c>
@@ -10474,7 +10456,7 @@
       <c r="E222" s="14"/>
       <c r="F222" s="14"/>
     </row>
-    <row r="223" spans="1:6" customFormat="1" ht="16">
+    <row r="223" spans="1:6" customFormat="1">
       <c r="A223" t="s">
         <v>476</v>
       </c>
@@ -10487,7 +10469,7 @@
       <c r="E223" s="14"/>
       <c r="F223" s="14"/>
     </row>
-    <row r="224" spans="1:6" customFormat="1" ht="16">
+    <row r="224" spans="1:6" customFormat="1">
       <c r="A224" t="s">
         <v>477</v>
       </c>
@@ -10500,7 +10482,7 @@
       <c r="E224" s="14"/>
       <c r="F224" s="14"/>
     </row>
-    <row r="225" spans="1:6" customFormat="1" ht="16">
+    <row r="225" spans="1:6" customFormat="1">
       <c r="A225" t="s">
         <v>478</v>
       </c>
@@ -10513,7 +10495,7 @@
       <c r="E225" s="14"/>
       <c r="F225" s="14"/>
     </row>
-    <row r="226" spans="1:6" customFormat="1" ht="16">
+    <row r="226" spans="1:6" customFormat="1">
       <c r="A226" t="s">
         <v>479</v>
       </c>
@@ -10526,7 +10508,7 @@
       <c r="E226" s="14"/>
       <c r="F226" s="14"/>
     </row>
-    <row r="227" spans="1:6" customFormat="1" ht="16">
+    <row r="227" spans="1:6" customFormat="1">
       <c r="A227" t="s">
         <v>480</v>
       </c>
@@ -10539,7 +10521,7 @@
       <c r="E227" s="14"/>
       <c r="F227" s="14"/>
     </row>
-    <row r="228" spans="1:6" customFormat="1" ht="16">
+    <row r="228" spans="1:6" customFormat="1">
       <c r="A228" t="s">
         <v>481</v>
       </c>
@@ -10552,7 +10534,7 @@
       <c r="E228" s="14"/>
       <c r="F228" s="14"/>
     </row>
-    <row r="229" spans="1:6" customFormat="1" ht="16">
+    <row r="229" spans="1:6" customFormat="1">
       <c r="A229" t="s">
         <v>482</v>
       </c>
@@ -10565,7 +10547,7 @@
       <c r="E229" s="14"/>
       <c r="F229" s="14"/>
     </row>
-    <row r="230" spans="1:6" customFormat="1" ht="16">
+    <row r="230" spans="1:6" customFormat="1">
       <c r="A230" t="s">
         <v>483</v>
       </c>
@@ -10578,7 +10560,7 @@
       <c r="E230" s="14"/>
       <c r="F230" s="14"/>
     </row>
-    <row r="231" spans="1:6" customFormat="1" ht="16">
+    <row r="231" spans="1:6" customFormat="1">
       <c r="A231" t="s">
         <v>484</v>
       </c>
@@ -10591,7 +10573,7 @@
       <c r="E231" s="14"/>
       <c r="F231" s="14"/>
     </row>
-    <row r="232" spans="1:6" customFormat="1" ht="16">
+    <row r="232" spans="1:6" customFormat="1">
       <c r="A232" t="s">
         <v>485</v>
       </c>
@@ -10604,7 +10586,7 @@
       <c r="E232" s="14"/>
       <c r="F232" s="14"/>
     </row>
-    <row r="233" spans="1:6" customFormat="1" ht="16">
+    <row r="233" spans="1:6" customFormat="1">
       <c r="A233" t="s">
         <v>486</v>
       </c>
@@ -10617,7 +10599,7 @@
       <c r="E233" s="14"/>
       <c r="F233" s="14"/>
     </row>
-    <row r="234" spans="1:6" customFormat="1" ht="16">
+    <row r="234" spans="1:6" customFormat="1">
       <c r="A234" t="s">
         <v>487</v>
       </c>
@@ -10630,7 +10612,7 @@
       <c r="E234" s="14"/>
       <c r="F234" s="14"/>
     </row>
-    <row r="235" spans="1:6" customFormat="1" ht="16">
+    <row r="235" spans="1:6" customFormat="1">
       <c r="A235" t="s">
         <v>488</v>
       </c>
@@ -10643,7 +10625,7 @@
       <c r="E235" s="14"/>
       <c r="F235" s="14"/>
     </row>
-    <row r="236" spans="1:6" customFormat="1" ht="16">
+    <row r="236" spans="1:6" customFormat="1">
       <c r="A236" t="s">
         <v>489</v>
       </c>
@@ -10656,7 +10638,7 @@
       <c r="E236" s="14"/>
       <c r="F236" s="14"/>
     </row>
-    <row r="237" spans="1:6" customFormat="1" ht="16">
+    <row r="237" spans="1:6" customFormat="1">
       <c r="A237" t="s">
         <v>490</v>
       </c>
@@ -10669,7 +10651,7 @@
       <c r="E237" s="14"/>
       <c r="F237" s="14"/>
     </row>
-    <row r="238" spans="1:6" customFormat="1" ht="16">
+    <row r="238" spans="1:6" customFormat="1">
       <c r="A238" t="s">
         <v>491</v>
       </c>
@@ -10682,7 +10664,7 @@
       <c r="E238" s="14"/>
       <c r="F238" s="14"/>
     </row>
-    <row r="239" spans="1:6" s="12" customFormat="1" ht="16">
+    <row r="239" spans="1:6" s="12" customFormat="1">
       <c r="A239" s="12" t="s">
         <v>492</v>
       </c>
@@ -10695,7 +10677,7 @@
       <c r="E239" s="13"/>
       <c r="F239" s="13"/>
     </row>
-    <row r="240" spans="1:6" customFormat="1" ht="16">
+    <row r="240" spans="1:6" customFormat="1">
       <c r="A240" t="s">
         <v>311</v>
       </c>
@@ -10708,7 +10690,7 @@
       <c r="E240" s="14"/>
       <c r="F240" s="14"/>
     </row>
-    <row r="241" spans="1:6" customFormat="1" ht="16">
+    <row r="241" spans="1:6" customFormat="1">
       <c r="A241" t="s">
         <v>493</v>
       </c>
@@ -10721,7 +10703,7 @@
       <c r="E241" s="14"/>
       <c r="F241" s="14"/>
     </row>
-    <row r="242" spans="1:6" customFormat="1" ht="16">
+    <row r="242" spans="1:6" customFormat="1">
       <c r="A242" t="s">
         <v>494</v>
       </c>
@@ -10734,7 +10716,7 @@
       <c r="E242" s="14"/>
       <c r="F242" s="14"/>
     </row>
-    <row r="243" spans="1:6" customFormat="1" ht="16">
+    <row r="243" spans="1:6" customFormat="1">
       <c r="A243" t="s">
         <v>495</v>
       </c>
@@ -10747,7 +10729,7 @@
       <c r="E243" s="14"/>
       <c r="F243" s="14"/>
     </row>
-    <row r="244" spans="1:6" customFormat="1" ht="16">
+    <row r="244" spans="1:6" customFormat="1">
       <c r="A244" t="s">
         <v>496</v>
       </c>
@@ -10760,7 +10742,7 @@
       <c r="E244" s="14"/>
       <c r="F244" s="14"/>
     </row>
-    <row r="245" spans="1:6" customFormat="1" ht="16">
+    <row r="245" spans="1:6" customFormat="1">
       <c r="A245" t="s">
         <v>497</v>
       </c>
@@ -10773,7 +10755,7 @@
       <c r="E245" s="14"/>
       <c r="F245" s="14"/>
     </row>
-    <row r="246" spans="1:6" customFormat="1" ht="16">
+    <row r="246" spans="1:6" customFormat="1">
       <c r="A246" t="s">
         <v>498</v>
       </c>
@@ -10786,7 +10768,7 @@
       <c r="E246" s="14"/>
       <c r="F246" s="14"/>
     </row>
-    <row r="247" spans="1:6" customFormat="1" ht="16">
+    <row r="247" spans="1:6" customFormat="1">
       <c r="A247" t="s">
         <v>499</v>
       </c>
@@ -10799,7 +10781,7 @@
       <c r="E247" s="14"/>
       <c r="F247" s="14"/>
     </row>
-    <row r="248" spans="1:6" customFormat="1" ht="16">
+    <row r="248" spans="1:6" customFormat="1">
       <c r="A248" t="s">
         <v>500</v>
       </c>
@@ -10812,7 +10794,7 @@
       <c r="E248" s="14"/>
       <c r="F248" s="14"/>
     </row>
-    <row r="249" spans="1:6" customFormat="1" ht="16">
+    <row r="249" spans="1:6" customFormat="1">
       <c r="A249" t="s">
         <v>501</v>
       </c>
@@ -10825,7 +10807,7 @@
       <c r="E249" s="14"/>
       <c r="F249" s="14"/>
     </row>
-    <row r="250" spans="1:6" customFormat="1" ht="16">
+    <row r="250" spans="1:6" customFormat="1">
       <c r="A250" t="s">
         <v>502</v>
       </c>
@@ -10838,7 +10820,7 @@
       <c r="E250" s="14"/>
       <c r="F250" s="14"/>
     </row>
-    <row r="251" spans="1:6" customFormat="1" ht="16">
+    <row r="251" spans="1:6" customFormat="1">
       <c r="A251" t="s">
         <v>503</v>
       </c>
@@ -10851,7 +10833,7 @@
       <c r="E251" s="14"/>
       <c r="F251" s="14"/>
     </row>
-    <row r="252" spans="1:6" customFormat="1" ht="16">
+    <row r="252" spans="1:6" customFormat="1">
       <c r="A252" t="s">
         <v>504</v>
       </c>
@@ -10864,7 +10846,7 @@
       <c r="E252" s="14"/>
       <c r="F252" s="14"/>
     </row>
-    <row r="253" spans="1:6" customFormat="1" ht="16">
+    <row r="253" spans="1:6" customFormat="1">
       <c r="A253" t="s">
         <v>505</v>
       </c>
@@ -10877,7 +10859,7 @@
       <c r="E253" s="14"/>
       <c r="F253" s="14"/>
     </row>
-    <row r="254" spans="1:6" customFormat="1" ht="16">
+    <row r="254" spans="1:6" customFormat="1">
       <c r="A254" t="s">
         <v>506</v>
       </c>
@@ -10890,7 +10872,7 @@
       <c r="E254" s="14"/>
       <c r="F254" s="14"/>
     </row>
-    <row r="255" spans="1:6" customFormat="1" ht="16">
+    <row r="255" spans="1:6" customFormat="1">
       <c r="A255" t="s">
         <v>507</v>
       </c>
@@ -10903,7 +10885,7 @@
       <c r="E255" s="14"/>
       <c r="F255" s="14"/>
     </row>
-    <row r="256" spans="1:6" customFormat="1" ht="16">
+    <row r="256" spans="1:6" customFormat="1">
       <c r="A256" t="s">
         <v>508</v>
       </c>
@@ -10916,7 +10898,7 @@
       <c r="E256" s="14"/>
       <c r="F256" s="14"/>
     </row>
-    <row r="257" spans="1:6" customFormat="1" ht="16">
+    <row r="257" spans="1:6" customFormat="1">
       <c r="A257" t="s">
         <v>509</v>
       </c>
@@ -10929,7 +10911,7 @@
       <c r="E257" s="14"/>
       <c r="F257" s="14"/>
     </row>
-    <row r="258" spans="1:6" customFormat="1" ht="16">
+    <row r="258" spans="1:6" customFormat="1">
       <c r="A258" t="s">
         <v>510</v>
       </c>
@@ -10942,7 +10924,7 @@
       <c r="E258" s="14"/>
       <c r="F258" s="14"/>
     </row>
-    <row r="259" spans="1:6" customFormat="1" ht="16">
+    <row r="259" spans="1:6" customFormat="1">
       <c r="A259" t="s">
         <v>511</v>
       </c>
@@ -10955,7 +10937,7 @@
       <c r="E259" s="14"/>
       <c r="F259" s="14"/>
     </row>
-    <row r="260" spans="1:6" customFormat="1" ht="16">
+    <row r="260" spans="1:6" customFormat="1">
       <c r="A260" t="s">
         <v>512</v>
       </c>
@@ -10968,7 +10950,7 @@
       <c r="E260" s="14"/>
       <c r="F260" s="14"/>
     </row>
-    <row r="261" spans="1:6" customFormat="1" ht="16">
+    <row r="261" spans="1:6" customFormat="1">
       <c r="A261" t="s">
         <v>513</v>
       </c>
@@ -10981,7 +10963,7 @@
       <c r="E261" s="14"/>
       <c r="F261" s="14"/>
     </row>
-    <row r="262" spans="1:6" customFormat="1" ht="16">
+    <row r="262" spans="1:6" customFormat="1">
       <c r="A262" t="s">
         <v>514</v>
       </c>
@@ -10994,7 +10976,7 @@
       <c r="E262" s="14"/>
       <c r="F262" s="14"/>
     </row>
-    <row r="263" spans="1:6" customFormat="1" ht="16">
+    <row r="263" spans="1:6" customFormat="1">
       <c r="A263" t="s">
         <v>515</v>
       </c>
@@ -11007,7 +10989,7 @@
       <c r="E263" s="14"/>
       <c r="F263" s="14"/>
     </row>
-    <row r="264" spans="1:6" customFormat="1" ht="16">
+    <row r="264" spans="1:6" customFormat="1">
       <c r="A264" t="s">
         <v>516</v>
       </c>
@@ -11020,7 +11002,7 @@
       <c r="E264" s="14"/>
       <c r="F264" s="14"/>
     </row>
-    <row r="265" spans="1:6" customFormat="1" ht="16">
+    <row r="265" spans="1:6" customFormat="1">
       <c r="A265" t="s">
         <v>517</v>
       </c>
@@ -11033,7 +11015,7 @@
       <c r="E265" s="14"/>
       <c r="F265" s="14"/>
     </row>
-    <row r="266" spans="1:6" customFormat="1" ht="16">
+    <row r="266" spans="1:6" customFormat="1">
       <c r="A266" t="s">
         <v>518</v>
       </c>
@@ -11046,7 +11028,7 @@
       <c r="E266" s="14"/>
       <c r="F266" s="14"/>
     </row>
-    <row r="267" spans="1:6" customFormat="1" ht="16">
+    <row r="267" spans="1:6" customFormat="1">
       <c r="A267" t="s">
         <v>519</v>
       </c>
@@ -11059,7 +11041,7 @@
       <c r="E267" s="14"/>
       <c r="F267" s="14"/>
     </row>
-    <row r="268" spans="1:6" customFormat="1" ht="16">
+    <row r="268" spans="1:6" customFormat="1">
       <c r="A268" t="s">
         <v>520</v>
       </c>
@@ -11072,7 +11054,7 @@
       <c r="E268" s="14"/>
       <c r="F268" s="14"/>
     </row>
-    <row r="269" spans="1:6" customFormat="1" ht="16">
+    <row r="269" spans="1:6" customFormat="1">
       <c r="A269" t="s">
         <v>521</v>
       </c>
@@ -11085,7 +11067,7 @@
       <c r="E269" s="14"/>
       <c r="F269" s="14"/>
     </row>
-    <row r="270" spans="1:6" customFormat="1" ht="16">
+    <row r="270" spans="1:6" customFormat="1">
       <c r="A270" t="s">
         <v>522</v>
       </c>
@@ -11098,7 +11080,7 @@
       <c r="E270" s="14"/>
       <c r="F270" s="14"/>
     </row>
-    <row r="271" spans="1:6" customFormat="1" ht="16">
+    <row r="271" spans="1:6" customFormat="1">
       <c r="A271" t="s">
         <v>523</v>
       </c>
@@ -11111,7 +11093,7 @@
       <c r="E271" s="14"/>
       <c r="F271" s="14"/>
     </row>
-    <row r="272" spans="1:6" customFormat="1" ht="16">
+    <row r="272" spans="1:6" customFormat="1">
       <c r="A272" t="s">
         <v>524</v>
       </c>
@@ -11124,7 +11106,7 @@
       <c r="E272" s="14"/>
       <c r="F272" s="14"/>
     </row>
-    <row r="273" spans="1:6" customFormat="1" ht="16">
+    <row r="273" spans="1:6" customFormat="1">
       <c r="A273" t="s">
         <v>525</v>
       </c>
@@ -11137,7 +11119,7 @@
       <c r="E273" s="14"/>
       <c r="F273" s="14"/>
     </row>
-    <row r="274" spans="1:6" customFormat="1" ht="16">
+    <row r="274" spans="1:6" customFormat="1">
       <c r="A274" t="s">
         <v>526</v>
       </c>
@@ -11150,7 +11132,7 @@
       <c r="E274" s="14"/>
       <c r="F274" s="14"/>
     </row>
-    <row r="275" spans="1:6" customFormat="1" ht="16">
+    <row r="275" spans="1:6" customFormat="1">
       <c r="A275" t="s">
         <v>527</v>
       </c>
@@ -11163,7 +11145,7 @@
       <c r="E275" s="14"/>
       <c r="F275" s="14"/>
     </row>
-    <row r="276" spans="1:6" customFormat="1" ht="16">
+    <row r="276" spans="1:6" customFormat="1">
       <c r="A276" t="s">
         <v>210</v>
       </c>
@@ -11176,7 +11158,7 @@
       <c r="E276" s="14"/>
       <c r="F276" s="14"/>
     </row>
-    <row r="277" spans="1:6" customFormat="1" ht="16">
+    <row r="277" spans="1:6" customFormat="1">
       <c r="A277" t="s">
         <v>528</v>
       </c>
@@ -11189,7 +11171,7 @@
       <c r="E277" s="14"/>
       <c r="F277" s="14"/>
     </row>
-    <row r="278" spans="1:6" customFormat="1" ht="16">
+    <row r="278" spans="1:6" customFormat="1">
       <c r="A278" t="s">
         <v>529</v>
       </c>
@@ -11199,7 +11181,7 @@
       <c r="E278" s="14"/>
       <c r="F278" s="14"/>
     </row>
-    <row r="279" spans="1:6" customFormat="1" ht="16">
+    <row r="279" spans="1:6" customFormat="1">
       <c r="A279" t="s">
         <v>530</v>
       </c>
@@ -11209,7 +11191,7 @@
       <c r="E279" s="14"/>
       <c r="F279" s="14"/>
     </row>
-    <row r="280" spans="1:6" s="12" customFormat="1" ht="16">
+    <row r="280" spans="1:6" s="12" customFormat="1">
       <c r="A280" s="12" t="s">
         <v>531</v>
       </c>
@@ -11222,7 +11204,7 @@
       <c r="E280" s="13"/>
       <c r="F280" s="13"/>
     </row>
-    <row r="281" spans="1:6" customFormat="1" ht="16">
+    <row r="281" spans="1:6" customFormat="1">
       <c r="A281" t="s">
         <v>532</v>
       </c>
@@ -11235,7 +11217,7 @@
       <c r="E281" s="14"/>
       <c r="F281" s="14"/>
     </row>
-    <row r="282" spans="1:6" customFormat="1" ht="16">
+    <row r="282" spans="1:6" customFormat="1">
       <c r="A282" t="s">
         <v>533</v>
       </c>
@@ -11248,7 +11230,7 @@
       <c r="E282" s="14"/>
       <c r="F282" s="14"/>
     </row>
-    <row r="283" spans="1:6" customFormat="1" ht="16">
+    <row r="283" spans="1:6" customFormat="1">
       <c r="A283" t="s">
         <v>534</v>
       </c>
@@ -11261,7 +11243,7 @@
       <c r="E283" s="14"/>
       <c r="F283" s="14"/>
     </row>
-    <row r="284" spans="1:6" customFormat="1" ht="16">
+    <row r="284" spans="1:6" customFormat="1">
       <c r="A284" t="s">
         <v>535</v>
       </c>
@@ -11274,7 +11256,7 @@
       <c r="E284" s="14"/>
       <c r="F284" s="14"/>
     </row>
-    <row r="285" spans="1:6" customFormat="1" ht="16">
+    <row r="285" spans="1:6" customFormat="1">
       <c r="A285" t="s">
         <v>536</v>
       </c>
@@ -11287,7 +11269,7 @@
       <c r="E285" s="14"/>
       <c r="F285" s="14"/>
     </row>
-    <row r="286" spans="1:6" customFormat="1" ht="16">
+    <row r="286" spans="1:6" customFormat="1">
       <c r="A286" t="s">
         <v>537</v>
       </c>
@@ -11300,7 +11282,7 @@
       <c r="E286" s="14"/>
       <c r="F286" s="14"/>
     </row>
-    <row r="287" spans="1:6" customFormat="1" ht="16">
+    <row r="287" spans="1:6" customFormat="1">
       <c r="A287" t="s">
         <v>538</v>
       </c>
@@ -11310,7 +11292,7 @@
       <c r="E287" s="14"/>
       <c r="F287" s="14"/>
     </row>
-    <row r="288" spans="1:6" customFormat="1" ht="16">
+    <row r="288" spans="1:6" customFormat="1">
       <c r="A288" t="s">
         <v>539</v>
       </c>
@@ -11323,7 +11305,7 @@
       <c r="E288" s="14"/>
       <c r="F288" s="14"/>
     </row>
-    <row r="289" spans="1:6" customFormat="1" ht="16">
+    <row r="289" spans="1:6" customFormat="1">
       <c r="A289" t="s">
         <v>540</v>
       </c>
@@ -11336,7 +11318,7 @@
       <c r="E289" s="14"/>
       <c r="F289" s="14"/>
     </row>
-    <row r="290" spans="1:6" customFormat="1" ht="16">
+    <row r="290" spans="1:6" customFormat="1">
       <c r="A290" t="s">
         <v>541</v>
       </c>
@@ -11349,7 +11331,7 @@
       <c r="E290" s="14"/>
       <c r="F290" s="14"/>
     </row>
-    <row r="291" spans="1:6" customFormat="1" ht="16">
+    <row r="291" spans="1:6" customFormat="1">
       <c r="A291" t="s">
         <v>542</v>
       </c>
@@ -11362,7 +11344,7 @@
       <c r="E291" s="14"/>
       <c r="F291" s="14"/>
     </row>
-    <row r="292" spans="1:6" customFormat="1" ht="16">
+    <row r="292" spans="1:6" customFormat="1">
       <c r="A292" t="s">
         <v>543</v>
       </c>
@@ -11375,7 +11357,7 @@
       <c r="E292" s="14"/>
       <c r="F292" s="14"/>
     </row>
-    <row r="293" spans="1:6" customFormat="1" ht="16">
+    <row r="293" spans="1:6" customFormat="1">
       <c r="A293" t="s">
         <v>544</v>
       </c>
@@ -11388,7 +11370,7 @@
       <c r="E293" s="14"/>
       <c r="F293" s="14"/>
     </row>
-    <row r="294" spans="1:6" customFormat="1" ht="16">
+    <row r="294" spans="1:6" customFormat="1">
       <c r="A294" t="s">
         <v>545</v>
       </c>
@@ -11401,7 +11383,7 @@
       <c r="E294" s="14"/>
       <c r="F294" s="14"/>
     </row>
-    <row r="295" spans="1:6" customFormat="1" ht="16">
+    <row r="295" spans="1:6" customFormat="1">
       <c r="A295" t="s">
         <v>546</v>
       </c>
@@ -11414,7 +11396,7 @@
       <c r="E295" s="14"/>
       <c r="F295" s="14"/>
     </row>
-    <row r="296" spans="1:6" customFormat="1" ht="16">
+    <row r="296" spans="1:6" customFormat="1">
       <c r="A296" t="s">
         <v>547</v>
       </c>
@@ -11427,7 +11409,7 @@
       <c r="E296" s="14"/>
       <c r="F296" s="14"/>
     </row>
-    <row r="297" spans="1:6" customFormat="1" ht="16">
+    <row r="297" spans="1:6" customFormat="1">
       <c r="A297" t="s">
         <v>548</v>
       </c>
@@ -11440,7 +11422,7 @@
       <c r="E297" s="14"/>
       <c r="F297" s="14"/>
     </row>
-    <row r="298" spans="1:6" customFormat="1" ht="16">
+    <row r="298" spans="1:6" customFormat="1">
       <c r="A298" t="s">
         <v>549</v>
       </c>
@@ -11453,7 +11435,7 @@
       <c r="E298" s="14"/>
       <c r="F298" s="14"/>
     </row>
-    <row r="299" spans="1:6" customFormat="1" ht="16">
+    <row r="299" spans="1:6" customFormat="1">
       <c r="A299" t="s">
         <v>550</v>
       </c>
@@ -11466,7 +11448,7 @@
       <c r="E299" s="14"/>
       <c r="F299" s="14"/>
     </row>
-    <row r="300" spans="1:6" customFormat="1" ht="16">
+    <row r="300" spans="1:6" customFormat="1">
       <c r="A300" t="s">
         <v>551</v>
       </c>
@@ -11479,7 +11461,7 @@
       <c r="E300" s="14"/>
       <c r="F300" s="14"/>
     </row>
-    <row r="301" spans="1:6" customFormat="1" ht="16">
+    <row r="301" spans="1:6" customFormat="1">
       <c r="A301" t="s">
         <v>552</v>
       </c>
@@ -11492,7 +11474,7 @@
       <c r="E301" s="14"/>
       <c r="F301" s="14"/>
     </row>
-    <row r="302" spans="1:6" customFormat="1" ht="16">
+    <row r="302" spans="1:6" customFormat="1">
       <c r="A302" t="s">
         <v>553</v>
       </c>
@@ -11502,7 +11484,7 @@
       <c r="E302" s="14"/>
       <c r="F302" s="14"/>
     </row>
-    <row r="303" spans="1:6" customFormat="1" ht="16">
+    <row r="303" spans="1:6" customFormat="1">
       <c r="A303" t="s">
         <v>554</v>
       </c>
@@ -11515,7 +11497,7 @@
       <c r="E303" s="14"/>
       <c r="F303" s="14"/>
     </row>
-    <row r="304" spans="1:6" customFormat="1" ht="16">
+    <row r="304" spans="1:6" customFormat="1">
       <c r="A304" t="s">
         <v>555</v>
       </c>
@@ -11528,7 +11510,7 @@
       <c r="E304" s="14"/>
       <c r="F304" s="14"/>
     </row>
-    <row r="305" spans="1:6" customFormat="1" ht="16">
+    <row r="305" spans="1:6" customFormat="1">
       <c r="A305" t="s">
         <v>556</v>
       </c>
@@ -11541,7 +11523,7 @@
       <c r="E305" s="14"/>
       <c r="F305" s="14"/>
     </row>
-    <row r="306" spans="1:6" customFormat="1" ht="16">
+    <row r="306" spans="1:6" customFormat="1">
       <c r="A306" t="s">
         <v>557</v>
       </c>
@@ -11554,7 +11536,7 @@
       <c r="E306" s="14"/>
       <c r="F306" s="14"/>
     </row>
-    <row r="307" spans="1:6" customFormat="1" ht="16">
+    <row r="307" spans="1:6" customFormat="1">
       <c r="A307" t="s">
         <v>558</v>
       </c>
@@ -11567,7 +11549,7 @@
       <c r="E307" s="14"/>
       <c r="F307" s="14"/>
     </row>
-    <row r="308" spans="1:6" customFormat="1" ht="16">
+    <row r="308" spans="1:6" customFormat="1">
       <c r="A308" t="s">
         <v>559</v>
       </c>
@@ -11580,7 +11562,7 @@
       <c r="E308" s="14"/>
       <c r="F308" s="14"/>
     </row>
-    <row r="309" spans="1:6" customFormat="1" ht="16">
+    <row r="309" spans="1:6" customFormat="1">
       <c r="A309" t="s">
         <v>560</v>
       </c>
@@ -11590,7 +11572,7 @@
       <c r="E309" s="14"/>
       <c r="F309" s="14"/>
     </row>
-    <row r="310" spans="1:6" customFormat="1" ht="16">
+    <row r="310" spans="1:6" customFormat="1">
       <c r="A310" t="s">
         <v>561</v>
       </c>
@@ -11603,7 +11585,7 @@
       <c r="E310" s="14"/>
       <c r="F310" s="14"/>
     </row>
-    <row r="311" spans="1:6" customFormat="1" ht="16">
+    <row r="311" spans="1:6" customFormat="1">
       <c r="A311" t="s">
         <v>562</v>
       </c>
@@ -11616,7 +11598,7 @@
       <c r="E311" s="14"/>
       <c r="F311" s="14"/>
     </row>
-    <row r="312" spans="1:6" customFormat="1" ht="16">
+    <row r="312" spans="1:6" customFormat="1">
       <c r="A312" t="s">
         <v>563</v>
       </c>
@@ -11629,7 +11611,7 @@
       <c r="E312" s="14"/>
       <c r="F312" s="14"/>
     </row>
-    <row r="313" spans="1:6" customFormat="1" ht="16">
+    <row r="313" spans="1:6" customFormat="1">
       <c r="A313" t="s">
         <v>564</v>
       </c>
@@ -11642,7 +11624,7 @@
       <c r="E313" s="14"/>
       <c r="F313" s="14"/>
     </row>
-    <row r="314" spans="1:6" customFormat="1" ht="16">
+    <row r="314" spans="1:6" customFormat="1">
       <c r="A314" t="s">
         <v>565</v>
       </c>
@@ -11655,7 +11637,7 @@
       <c r="E314" s="14"/>
       <c r="F314" s="14"/>
     </row>
-    <row r="315" spans="1:6" customFormat="1" ht="16">
+    <row r="315" spans="1:6" customFormat="1">
       <c r="A315" t="s">
         <v>566</v>
       </c>
@@ -11668,7 +11650,7 @@
       <c r="E315" s="14"/>
       <c r="F315" s="14"/>
     </row>
-    <row r="316" spans="1:6" customFormat="1" ht="16">
+    <row r="316" spans="1:6" customFormat="1">
       <c r="A316" t="s">
         <v>567</v>
       </c>
@@ -11681,7 +11663,7 @@
       <c r="E316" s="14"/>
       <c r="F316" s="14"/>
     </row>
-    <row r="317" spans="1:6" customFormat="1" ht="16">
+    <row r="317" spans="1:6" customFormat="1">
       <c r="A317" t="s">
         <v>568</v>
       </c>
@@ -11694,7 +11676,7 @@
       <c r="E317" s="14"/>
       <c r="F317" s="14"/>
     </row>
-    <row r="318" spans="1:6" customFormat="1" ht="16">
+    <row r="318" spans="1:6" customFormat="1">
       <c r="A318" t="s">
         <v>569</v>
       </c>
@@ -11707,7 +11689,7 @@
       <c r="E318" s="14"/>
       <c r="F318" s="14"/>
     </row>
-    <row r="319" spans="1:6" customFormat="1" ht="16">
+    <row r="319" spans="1:6" customFormat="1">
       <c r="A319" t="s">
         <v>570</v>
       </c>
@@ -11720,7 +11702,7 @@
       <c r="E319" s="14"/>
       <c r="F319" s="14"/>
     </row>
-    <row r="320" spans="1:6" customFormat="1" ht="16">
+    <row r="320" spans="1:6" customFormat="1">
       <c r="A320" t="s">
         <v>571</v>
       </c>
@@ -11733,7 +11715,7 @@
       <c r="E320" s="14"/>
       <c r="F320" s="14"/>
     </row>
-    <row r="321" spans="1:6" customFormat="1" ht="16">
+    <row r="321" spans="1:6" customFormat="1">
       <c r="A321" t="s">
         <v>572</v>
       </c>
@@ -11746,7 +11728,7 @@
       <c r="E321" s="14"/>
       <c r="F321" s="14"/>
     </row>
-    <row r="322" spans="1:6" customFormat="1" ht="16">
+    <row r="322" spans="1:6" customFormat="1">
       <c r="A322" t="s">
         <v>573</v>
       </c>
@@ -11759,7 +11741,7 @@
       <c r="E322" s="14"/>
       <c r="F322" s="14"/>
     </row>
-    <row r="323" spans="1:6" customFormat="1" ht="16">
+    <row r="323" spans="1:6" customFormat="1">
       <c r="A323" t="s">
         <v>574</v>
       </c>
@@ -11772,7 +11754,7 @@
       <c r="E323" s="14"/>
       <c r="F323" s="14"/>
     </row>
-    <row r="324" spans="1:6" customFormat="1" ht="16">
+    <row r="324" spans="1:6" customFormat="1">
       <c r="A324" t="s">
         <v>575</v>
       </c>
@@ -11785,7 +11767,7 @@
       <c r="E324" s="14"/>
       <c r="F324" s="14"/>
     </row>
-    <row r="325" spans="1:6" customFormat="1" ht="16">
+    <row r="325" spans="1:6" customFormat="1">
       <c r="A325" t="s">
         <v>576</v>
       </c>
@@ -11798,7 +11780,7 @@
       <c r="E325" s="14"/>
       <c r="F325" s="14"/>
     </row>
-    <row r="326" spans="1:6" customFormat="1" ht="16">
+    <row r="326" spans="1:6" customFormat="1">
       <c r="A326" t="s">
         <v>577</v>
       </c>
@@ -11811,7 +11793,7 @@
       <c r="E326" s="14"/>
       <c r="F326" s="14"/>
     </row>
-    <row r="327" spans="1:6" customFormat="1" ht="16">
+    <row r="327" spans="1:6" customFormat="1">
       <c r="A327" t="s">
         <v>578</v>
       </c>
@@ -11824,7 +11806,7 @@
       <c r="E327" s="14"/>
       <c r="F327" s="14"/>
     </row>
-    <row r="328" spans="1:6" customFormat="1" ht="16">
+    <row r="328" spans="1:6" customFormat="1">
       <c r="A328" t="s">
         <v>579</v>
       </c>
@@ -11837,7 +11819,7 @@
       <c r="E328" s="14"/>
       <c r="F328" s="14"/>
     </row>
-    <row r="329" spans="1:6" customFormat="1" ht="16">
+    <row r="329" spans="1:6" customFormat="1">
       <c r="A329" t="s">
         <v>580</v>
       </c>
@@ -11850,7 +11832,7 @@
       <c r="E329" s="14"/>
       <c r="F329" s="14"/>
     </row>
-    <row r="330" spans="1:6" customFormat="1" ht="16">
+    <row r="330" spans="1:6" customFormat="1">
       <c r="A330" t="s">
         <v>581</v>
       </c>
@@ -11863,7 +11845,7 @@
       <c r="E330" s="14"/>
       <c r="F330" s="14"/>
     </row>
-    <row r="331" spans="1:6" customFormat="1" ht="16">
+    <row r="331" spans="1:6" customFormat="1">
       <c r="A331" t="s">
         <v>582</v>
       </c>
@@ -11876,7 +11858,7 @@
       <c r="E331" s="14"/>
       <c r="F331" s="14"/>
     </row>
-    <row r="332" spans="1:6" customFormat="1" ht="16">
+    <row r="332" spans="1:6" customFormat="1">
       <c r="A332" t="s">
         <v>583</v>
       </c>
@@ -11889,7 +11871,7 @@
       <c r="E332" s="14"/>
       <c r="F332" s="14"/>
     </row>
-    <row r="333" spans="1:6" customFormat="1" ht="16">
+    <row r="333" spans="1:6" customFormat="1">
       <c r="A333" t="s">
         <v>584</v>
       </c>
@@ -11902,7 +11884,7 @@
       <c r="E333" s="14"/>
       <c r="F333" s="14"/>
     </row>
-    <row r="334" spans="1:6" customFormat="1" ht="16">
+    <row r="334" spans="1:6" customFormat="1">
       <c r="A334" t="s">
         <v>585</v>
       </c>
@@ -11915,7 +11897,7 @@
       <c r="E334" s="14"/>
       <c r="F334" s="14"/>
     </row>
-    <row r="335" spans="1:6" customFormat="1" ht="16">
+    <row r="335" spans="1:6" customFormat="1">
       <c r="A335" t="s">
         <v>586</v>
       </c>
@@ -11928,7 +11910,7 @@
       <c r="E335" s="14"/>
       <c r="F335" s="14"/>
     </row>
-    <row r="336" spans="1:6" customFormat="1" ht="16">
+    <row r="336" spans="1:6" customFormat="1">
       <c r="A336" t="s">
         <v>587</v>
       </c>
@@ -11941,7 +11923,7 @@
       <c r="E336" s="14"/>
       <c r="F336" s="14"/>
     </row>
-    <row r="337" spans="1:6" customFormat="1" ht="16">
+    <row r="337" spans="1:6" customFormat="1">
       <c r="A337" t="s">
         <v>588</v>
       </c>
@@ -11954,7 +11936,7 @@
       <c r="E337" s="14"/>
       <c r="F337" s="14"/>
     </row>
-    <row r="338" spans="1:6" customFormat="1" ht="16">
+    <row r="338" spans="1:6" customFormat="1">
       <c r="A338" t="s">
         <v>589</v>
       </c>
@@ -11964,7 +11946,7 @@
       <c r="E338" s="14"/>
       <c r="F338" s="14"/>
     </row>
-    <row r="339" spans="1:6" customFormat="1" ht="16">
+    <row r="339" spans="1:6" customFormat="1">
       <c r="A339" t="s">
         <v>590</v>
       </c>
@@ -11977,7 +11959,7 @@
       <c r="E339" s="14"/>
       <c r="F339" s="14"/>
     </row>
-    <row r="340" spans="1:6" customFormat="1" ht="16">
+    <row r="340" spans="1:6" customFormat="1">
       <c r="A340" t="s">
         <v>591</v>
       </c>
@@ -11990,7 +11972,7 @@
       <c r="E340" s="14"/>
       <c r="F340" s="14"/>
     </row>
-    <row r="341" spans="1:6" customFormat="1" ht="16">
+    <row r="341" spans="1:6" customFormat="1">
       <c r="A341" t="s">
         <v>592</v>
       </c>
@@ -12003,7 +11985,7 @@
       <c r="E341" s="14"/>
       <c r="F341" s="14"/>
     </row>
-    <row r="342" spans="1:6" customFormat="1" ht="16">
+    <row r="342" spans="1:6" customFormat="1">
       <c r="A342" t="s">
         <v>593</v>
       </c>
@@ -12016,7 +11998,7 @@
       <c r="E342" s="14"/>
       <c r="F342" s="14"/>
     </row>
-    <row r="343" spans="1:6" customFormat="1" ht="16">
+    <row r="343" spans="1:6" customFormat="1">
       <c r="A343" t="s">
         <v>594</v>
       </c>
@@ -12029,7 +12011,7 @@
       <c r="E343" s="14"/>
       <c r="F343" s="14"/>
     </row>
-    <row r="344" spans="1:6" customFormat="1" ht="16">
+    <row r="344" spans="1:6" customFormat="1">
       <c r="A344" t="s">
         <v>595</v>
       </c>
@@ -12042,7 +12024,7 @@
       <c r="E344" s="14"/>
       <c r="F344" s="14"/>
     </row>
-    <row r="345" spans="1:6" customFormat="1" ht="16">
+    <row r="345" spans="1:6" customFormat="1">
       <c r="A345" t="s">
         <v>596</v>
       </c>
@@ -12055,7 +12037,7 @@
       <c r="E345" s="14"/>
       <c r="F345" s="14"/>
     </row>
-    <row r="346" spans="1:6" customFormat="1" ht="16">
+    <row r="346" spans="1:6" customFormat="1">
       <c r="A346" t="s">
         <v>597</v>
       </c>
@@ -12068,7 +12050,7 @@
       <c r="E346" s="14"/>
       <c r="F346" s="14"/>
     </row>
-    <row r="347" spans="1:6" customFormat="1" ht="16">
+    <row r="347" spans="1:6" customFormat="1">
       <c r="A347" t="s">
         <v>598</v>
       </c>
@@ -12081,7 +12063,7 @@
       <c r="E347" s="14"/>
       <c r="F347" s="14"/>
     </row>
-    <row r="348" spans="1:6" customFormat="1" ht="16">
+    <row r="348" spans="1:6" customFormat="1">
       <c r="A348" t="s">
         <v>599</v>
       </c>
@@ -12094,7 +12076,7 @@
       <c r="E348" s="14"/>
       <c r="F348" s="14"/>
     </row>
-    <row r="349" spans="1:6" customFormat="1" ht="16">
+    <row r="349" spans="1:6" customFormat="1">
       <c r="A349" t="s">
         <v>600</v>
       </c>
@@ -12107,7 +12089,7 @@
       <c r="E349" s="14"/>
       <c r="F349" s="14"/>
     </row>
-    <row r="350" spans="1:6" customFormat="1" ht="16">
+    <row r="350" spans="1:6" customFormat="1">
       <c r="A350" t="s">
         <v>601</v>
       </c>
@@ -12120,7 +12102,7 @@
       <c r="E350" s="14"/>
       <c r="F350" s="14"/>
     </row>
-    <row r="351" spans="1:6" customFormat="1" ht="16">
+    <row r="351" spans="1:6" customFormat="1">
       <c r="A351" t="s">
         <v>602</v>
       </c>
@@ -12133,7 +12115,7 @@
       <c r="E351" s="14"/>
       <c r="F351" s="14"/>
     </row>
-    <row r="352" spans="1:6" customFormat="1" ht="16">
+    <row r="352" spans="1:6" customFormat="1">
       <c r="A352" t="s">
         <v>603</v>
       </c>
@@ -12146,7 +12128,7 @@
       <c r="E352" s="14"/>
       <c r="F352" s="14"/>
     </row>
-    <row r="353" spans="1:7" customFormat="1" ht="16">
+    <row r="353" spans="1:7" customFormat="1">
       <c r="A353" t="s">
         <v>604</v>
       </c>
@@ -12159,7 +12141,7 @@
       <c r="E353" s="14"/>
       <c r="F353" s="14"/>
     </row>
-    <row r="354" spans="1:7" customFormat="1" ht="16">
+    <row r="354" spans="1:7" customFormat="1">
       <c r="A354" t="s">
         <v>605</v>
       </c>
@@ -12172,7 +12154,7 @@
       <c r="E354" s="14"/>
       <c r="F354" s="14"/>
     </row>
-    <row r="355" spans="1:7" customFormat="1" ht="16">
+    <row r="355" spans="1:7" customFormat="1">
       <c r="A355" t="s">
         <v>606</v>
       </c>
@@ -12185,7 +12167,7 @@
       <c r="E355" s="14"/>
       <c r="F355" s="14"/>
     </row>
-    <row r="356" spans="1:7" customFormat="1" ht="16">
+    <row r="356" spans="1:7" customFormat="1">
       <c r="A356" t="s">
         <v>607</v>
       </c>
@@ -12198,7 +12180,7 @@
       <c r="E356" s="14"/>
       <c r="F356" s="14"/>
     </row>
-    <row r="357" spans="1:7" customFormat="1" ht="16">
+    <row r="357" spans="1:7" customFormat="1">
       <c r="A357" t="s">
         <v>608</v>
       </c>
@@ -12211,7 +12193,7 @@
       <c r="E357" s="14"/>
       <c r="F357" s="14"/>
     </row>
-    <row r="358" spans="1:7" customFormat="1" ht="16">
+    <row r="358" spans="1:7" customFormat="1">
       <c r="A358" t="s">
         <v>609</v>
       </c>
@@ -12224,7 +12206,7 @@
       <c r="E358" s="14"/>
       <c r="F358" s="14"/>
     </row>
-    <row r="359" spans="1:7" customFormat="1" ht="16">
+    <row r="359" spans="1:7" customFormat="1">
       <c r="A359" t="s">
         <v>610</v>
       </c>
@@ -12237,7 +12219,7 @@
       <c r="E359" s="14"/>
       <c r="F359" s="14"/>
     </row>
-    <row r="360" spans="1:7" customFormat="1" ht="16">
+    <row r="360" spans="1:7" customFormat="1">
       <c r="A360" t="s">
         <v>611</v>
       </c>
@@ -12250,7 +12232,7 @@
       <c r="E360" s="14"/>
       <c r="F360" s="14"/>
     </row>
-    <row r="361" spans="1:7" customFormat="1" ht="16">
+    <row r="361" spans="1:7" customFormat="1">
       <c r="A361" t="s">
         <v>612</v>
       </c>
@@ -12263,7 +12245,7 @@
       <c r="E361" s="14"/>
       <c r="F361" s="14"/>
     </row>
-    <row r="362" spans="1:7" customFormat="1" ht="16">
+    <row r="362" spans="1:7" customFormat="1">
       <c r="A362" t="s">
         <v>613</v>
       </c>
@@ -12276,7 +12258,7 @@
       <c r="E362" s="14"/>
       <c r="F362" s="14"/>
     </row>
-    <row r="363" spans="1:7" customFormat="1" ht="16">
+    <row r="363" spans="1:7" customFormat="1">
       <c r="A363" t="s">
         <v>614</v>
       </c>
@@ -12289,7 +12271,7 @@
       <c r="E363" s="14"/>
       <c r="F363" s="14"/>
     </row>
-    <row r="364" spans="1:7" customFormat="1" ht="16">
+    <row r="364" spans="1:7" customFormat="1">
       <c r="A364" t="s">
         <v>615</v>
       </c>
@@ -12302,7 +12284,7 @@
       <c r="E364" s="14"/>
       <c r="F364" s="14"/>
     </row>
-    <row r="365" spans="1:7" customFormat="1" ht="16">
+    <row r="365" spans="1:7" customFormat="1">
       <c r="A365" t="s">
         <v>616</v>
       </c>
@@ -12315,7 +12297,7 @@
       <c r="E365" s="14"/>
       <c r="F365" s="14"/>
     </row>
-    <row r="366" spans="1:7" customFormat="1" ht="16">
+    <row r="366" spans="1:7" customFormat="1">
       <c r="A366" t="s">
         <v>617</v>
       </c>
@@ -12328,7 +12310,7 @@
       <c r="E366" s="14"/>
       <c r="F366" s="14"/>
     </row>
-    <row r="367" spans="1:7" customFormat="1" ht="16">
+    <row r="367" spans="1:7" customFormat="1">
       <c r="A367" t="s">
         <v>622</v>
       </c>
@@ -15092,10 +15074,10 @@
     </row>
     <row r="496" spans="1:8">
       <c r="A496" s="6" t="s">
+        <v>937</v>
+      </c>
+      <c r="B496" s="6" t="s">
         <v>938</v>
-      </c>
-      <c r="B496" s="6" t="s">
-        <v>939</v>
       </c>
       <c r="C496" s="6" t="s">
         <v>201</v>
@@ -15113,15 +15095,15 @@
         <v>243</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="497" spans="1:8">
       <c r="A497" s="6" t="s">
+        <v>935</v>
+      </c>
+      <c r="B497" s="6" t="s">
         <v>936</v>
-      </c>
-      <c r="B497" s="6" t="s">
-        <v>937</v>
       </c>
       <c r="C497" s="6" t="s">
         <v>201</v>
@@ -15139,18 +15121,18 @@
         <v>243</v>
       </c>
       <c r="H497" s="6" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="498" spans="1:8">
       <c r="A498" s="6" t="s">
+        <v>939</v>
+      </c>
+      <c r="B498" s="6" t="s">
         <v>940</v>
       </c>
-      <c r="B498" s="6" t="s">
-        <v>941</v>
-      </c>
       <c r="C498" s="6" t="s">
-        <v>935</v>
+        <v>202</v>
       </c>
       <c r="D498" s="9">
         <v>2018</v>
@@ -15165,15 +15147,15 @@
         <v>243</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="499" spans="1:8">
       <c r="A499" s="6" t="s">
+        <v>944</v>
+      </c>
+      <c r="B499" s="6" t="s">
         <v>945</v>
-      </c>
-      <c r="B499" s="6" t="s">
-        <v>946</v>
       </c>
       <c r="C499" s="6" t="s">
         <v>202</v>
@@ -15191,15 +15173,15 @@
         <v>243</v>
       </c>
       <c r="H499" s="6" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="500" spans="1:8">
       <c r="A500" s="6" t="s">
+        <v>947</v>
+      </c>
+      <c r="B500" s="6" t="s">
         <v>948</v>
-      </c>
-      <c r="B500" s="6" t="s">
-        <v>949</v>
       </c>
       <c r="C500" s="6" t="s">
         <v>244</v>
@@ -15217,18 +15199,18 @@
         <v>245</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="501" spans="1:8">
       <c r="A501" s="6" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B501" s="6" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C501" s="6" t="s">
-        <v>935</v>
+        <v>202</v>
       </c>
       <c r="D501" s="9">
         <v>2018</v>
@@ -15243,7 +15225,59 @@
         <v>243</v>
       </c>
       <c r="H501" s="6" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="502" spans="1:8">
+      <c r="A502" s="6" t="s">
         <v>952</v>
+      </c>
+      <c r="B502" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C502" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D502" s="9">
+        <v>2018</v>
+      </c>
+      <c r="E502" s="9">
+        <v>2013</v>
+      </c>
+      <c r="F502" s="9">
+        <v>176</v>
+      </c>
+      <c r="G502" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="H502" s="6" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="503" spans="1:8">
+      <c r="A503" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="B503" s="6" t="s">
+        <v>954</v>
+      </c>
+      <c r="C503" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D503" s="9">
+        <v>2018</v>
+      </c>
+      <c r="E503" s="9">
+        <v>2017</v>
+      </c>
+      <c r="F503" s="9">
+        <v>272</v>
+      </c>
+      <c r="G503" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="H503" s="6" t="s">
+        <v>956</v>
       </c>
     </row>
   </sheetData>
@@ -15259,14 +15293,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:Q41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>

</xml_diff>

<commit_message>
*When Harry Became Sally*
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="957">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="959">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -2897,6 +2897,12 @@
   </si>
   <si>
     <t xml:space="preserve">I read this to balance my reading of Ryan Anderson and to give a pro-transgender voice an audience, certainly not by way of providing a philosophical argument but through the story of a self-described happy transgender individual. Putting aside the politicized and simplistic description of transgenderism ("I'm have a girl brain in a boy body") I tried to be open-minded in learning about Jazz's story, how Jazz's parents have responded to the situation, how Jazz deals with ongoing depression, and how Jazz has become a transgender activist. Reading both Jennings and Anderson has given me new appreciation for the need for sensativity toward people with gender dysphoria as well as the larger context surrounding transgenderism. </t>
+  </si>
+  <si>
+    <t>When Harry Became Sally: Responding to the Transgender Moment</t>
+  </si>
+  <si>
+    <t>Anderson provides a thorough examination of transgender ideology and its consequences, motivated by a love for the truth and sympathy for victims of the transgender agenda. His writing is characteristically intellectually rigorous and honest in a way lacking from that of the views I have read of those who disagree with him. This book is a helpful for understanding and responding to transgender activists and individuals with gender dysphoria.</t>
   </si>
 </sst>
 </file>
@@ -4492,11 +4498,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2083500296"/>
-        <c:axId val="2082547528"/>
+        <c:axId val="2109802808"/>
+        <c:axId val="2109798952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2083500296"/>
+        <c:axId val="2109802808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4539,7 +4545,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2082547528"/>
+        <c:crossAx val="2109798952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4547,7 +4553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2082547528"/>
+        <c:axId val="2109798952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4598,7 +4604,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083500296"/>
+        <c:crossAx val="2109802808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6127,7 +6133,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6163,7 +6169,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7134,7 +7140,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -7563,7 +7569,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7574,11 +7580,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H503"/>
+  <dimension ref="A1:H504"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A492" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A504" sqref="A504"/>
+      <selection pane="bottomLeft" activeCell="A505" sqref="A505"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -15278,6 +15284,32 @@
       </c>
       <c r="H503" s="6" t="s">
         <v>956</v>
+      </c>
+    </row>
+    <row r="504" spans="1:8">
+      <c r="A504" s="6" t="s">
+        <v>957</v>
+      </c>
+      <c r="B504" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C504" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D504" s="9">
+        <v>2018</v>
+      </c>
+      <c r="E504" s="9">
+        <v>2018</v>
+      </c>
+      <c r="F504" s="9">
+        <v>213</v>
+      </c>
+      <c r="G504" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="H504" s="6" t="s">
+        <v>958</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add constitution of ireland
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{55419AAA-110B-DB47-B1D7-C0FAFF9ADF4C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1B830FE9-4C26-6946-A2EE-7A55145D8185}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="1880" windowWidth="25600" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9500" yWindow="460" windowWidth="19200" windowHeight="17440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="981">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -2974,6 +2974,15 @@
   </si>
   <si>
     <t>This story is incredible. First their ship gets stuck in ice, then sinks, then they drift through the south Atlantic on an ice flow, then they sail to Elephant Island, then a group sails to an island with whalers, and finally they complete the first crossing of said island to get help. It is incredible to think about the suffering they went through and the resolve required to get out.</t>
+  </si>
+  <si>
+    <t>The Constitution of Ireland</t>
+  </si>
+  <si>
+    <t>I was in Ireland shortly before the national referendum about whether or not to repeal the 8th amendment to the Irish Constitution to allow for legislation of abortion. I chose to read most of the Constitution, which is a beautiful document in how it orients positive law beneath natural law and supports the family.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -10158,7 +10167,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -10536,11 +10545,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H510"/>
+  <dimension ref="A1:H511"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A490" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A511" sqref="A511"/>
+      <pane ySplit="1" topLeftCell="A488" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B512" sqref="B512"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19524,6 +19533,32 @@
       </c>
       <c r="H510" s="6" t="s">
         <v>977</v>
+      </c>
+    </row>
+    <row r="511" spans="1:8">
+      <c r="A511" s="6" t="s">
+        <v>978</v>
+      </c>
+      <c r="B511" s="6" t="s">
+        <v>980</v>
+      </c>
+      <c r="C511" s="6" t="s">
+        <v>959</v>
+      </c>
+      <c r="D511" s="14">
+        <v>2018</v>
+      </c>
+      <c r="E511" s="14">
+        <v>1937</v>
+      </c>
+      <c r="F511" s="14">
+        <v>44</v>
+      </c>
+      <c r="G511" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="H511" s="6" t="s">
+        <v>979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The Island of the World
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10513"/>
   <workbookPr hidePivotFieldList="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1B830FE9-4C26-6946-A2EE-7A55145D8185}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C06D139A-0892-3F49-A96E-7A713D65BDFE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9500" yWindow="460" windowWidth="19200" windowHeight="17440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="3" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="984">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -2983,6 +2983,15 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>The Island of the World</t>
+  </si>
+  <si>
+    <t>Michael D. O'Brien</t>
+  </si>
+  <si>
+    <t>The most beautiful prose I have ever read.</t>
   </si>
 </sst>
 </file>
@@ -10167,7 +10176,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -10545,11 +10554,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H511"/>
+  <dimension ref="A1:H512"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A488" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B512" sqref="B512"/>
+      <selection pane="bottomLeft" activeCell="A513" sqref="A513"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19559,6 +19568,32 @@
       </c>
       <c r="H511" s="6" t="s">
         <v>979</v>
+      </c>
+    </row>
+    <row r="512" spans="1:8">
+      <c r="A512" s="6" t="s">
+        <v>981</v>
+      </c>
+      <c r="B512" s="6" t="s">
+        <v>982</v>
+      </c>
+      <c r="C512" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D512" s="14">
+        <v>2018</v>
+      </c>
+      <c r="E512" s="14">
+        <v>2007</v>
+      </c>
+      <c r="F512" s="14">
+        <v>813</v>
+      </c>
+      <c r="G512" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="H512" s="6" t="s">
+        <v>983</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Endurance by Scott Kelly
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr hidePivotFieldList="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6D4F177B-47C9-164E-B99E-EC4D006B6D80}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{840DB0B0-3224-7F43-8533-027958019693}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="460" windowWidth="28080" windowHeight="17440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId3"/>
+    <pivotCache cacheId="27" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="999">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3028,6 +3028,15 @@
   </si>
   <si>
     <t>Some good wisdom, a lot of fluff, and not my favorite from Matthew Kelly. Also I thought I heard enough about Southwest Airlines in business school…but some actionable points if you need that.</t>
+  </si>
+  <si>
+    <t>Endurance: A Year in Space, A Lifetime of Discovery</t>
+  </si>
+  <si>
+    <t>Scott Kelly</t>
+  </si>
+  <si>
+    <t>This is another epic story of exploration, hearing first hand about living on ISS for a year. I know more than most about space but this impressed upon me how amazing ISS really is and the struggles that come with living there, especially for a long period of time. I liked how Kelly structured his book, interspersing his year-long mission with bits about his life leading up to then starting as a kit and moving through becoming a Navy pilot, test pilot, and his previous space missions.</t>
   </si>
 </sst>
 </file>
@@ -10212,7 +10221,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable4" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable4" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -10590,11 +10599,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H517"/>
+  <dimension ref="A1:H518"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A488" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A518" sqref="A518"/>
+      <selection pane="bottomLeft" activeCell="A519" sqref="A519"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19760,6 +19769,32 @@
       </c>
       <c r="H517" s="6" t="s">
         <v>995</v>
+      </c>
+    </row>
+    <row r="518" spans="1:8">
+      <c r="A518" s="6" t="s">
+        <v>996</v>
+      </c>
+      <c r="B518" s="6" t="s">
+        <v>997</v>
+      </c>
+      <c r="C518" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D518" s="14">
+        <v>2018</v>
+      </c>
+      <c r="E518" s="14">
+        <v>2017</v>
+      </c>
+      <c r="F518" s="14">
+        <v>400</v>
+      </c>
+      <c r="G518" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="H518" s="6" t="s">
+        <v>998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a place on earth
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0B333284-7BA3-BA4F-B4EB-2EF6DFDBE581}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8F9FE50C-708E-8C43-80CB-8A7B6BCB5D16}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="460" windowWidth="28080" windowHeight="17440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="15" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1716" uniqueCount="1028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="1031">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3124,6 +3124,15 @@
   </si>
   <si>
     <t>This was a favorite of mine as a kid and I got it from the library many times. In going through books for baby I rediscovered it and it is even cooler now! I especially like the castle, cathedral (Chartres!!), galleon, and helicopter.</t>
+  </si>
+  <si>
+    <t>A Place on Earth</t>
+  </si>
+  <si>
+    <t>Wendell Berry</t>
+  </si>
+  <si>
+    <t>I was alterted of Wendell Berry by Deneen in *Why Liberalism Failed*, and this is one in a series about life in Port William during WWII. This story is beautiful for the simplicity of small town life, living close to nature, enduring death and loss, but surviving as a community.</t>
   </si>
 </sst>
 </file>
@@ -10308,7 +10317,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable4" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -10686,11 +10695,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H528"/>
+  <dimension ref="A1:H529"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A509" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A529" sqref="A529"/>
+      <selection pane="bottomLeft" activeCell="A530" sqref="A530"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20142,6 +20151,32 @@
       </c>
       <c r="H528" s="6" t="s">
         <v>1027</v>
+      </c>
+    </row>
+    <row r="529" spans="1:8">
+      <c r="A529" s="6" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B529" s="6" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C529" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D529" s="14">
+        <v>2018</v>
+      </c>
+      <c r="E529" s="14">
+        <v>1967</v>
+      </c>
+      <c r="F529" s="14">
+        <v>320</v>
+      </c>
+      <c r="G529" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="H529" s="6" t="s">
+        <v>1030</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
From Islam to Christ
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{10B41979-A8F4-BA44-9E96-0A6B8B6BFE2C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6E8FF00C-F0C4-064E-935D-824873D8C2CE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="460" windowWidth="28080" windowHeight="17440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="5" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="1042">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3157,6 +3157,15 @@
   </si>
   <si>
     <t>It was lovely to re-read this, which I read originally in 2010, and then read a few sections of in 2015 in LA. Lewis is so insightful about the ways we are tempted to sin—reading this makes you feel guilty but you know it is true. One of my favorite lines in this book is about stumbles: "He wants them to learn to walk and must therefore take away His hand; and if only the will to walk is really there He is pleased even with their stumbles." (47).</t>
+  </si>
+  <si>
+    <t>From Islam to Christ</t>
+  </si>
+  <si>
+    <t>Derya Little</t>
+  </si>
+  <si>
+    <t>This is a beautiful conversion story. I appreciated an insider's view on Islam, as well as the convert's well-reasoned views on Islam, Evangelical Protestantism, and Catholicism. Her story is filled with grace and a beautiful witness.</t>
   </si>
 </sst>
 </file>
@@ -10382,7 +10391,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D7C14FFC-0A7D-094B-8E63-9A42C2B18BA1}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D7C14FFC-0A7D-094B-8E63-9A42C2B18BA1}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField dataField="1" showAll="0">
@@ -11300,11 +11309,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H533"/>
+  <dimension ref="A1:H534"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A508" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A534" sqref="A534"/>
+      <selection pane="bottomLeft" activeCell="A535" sqref="A535"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20886,6 +20895,32 @@
       </c>
       <c r="H533" s="6" t="s">
         <v>1038</v>
+      </c>
+    </row>
+    <row r="534" spans="1:8">
+      <c r="A534" s="6" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B534" s="6" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C534" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D534" s="14">
+        <v>2018</v>
+      </c>
+      <c r="E534" s="14">
+        <v>2017</v>
+      </c>
+      <c r="F534" s="14">
+        <v>204</v>
+      </c>
+      <c r="G534" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="H534" s="6" t="s">
+        <v>1041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The Practice of the Presence of God
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C75EE4-BEC8-8F44-AEB0-692645753687}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
     <sheet name="Pivot" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1777" uniqueCount="1063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1782" uniqueCount="1066">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3210,13 +3209,22 @@
   </si>
   <si>
     <t>I read this after Jordan did and it is a beautiful and inspiring story. I love how authentic they are and how entrepreneurial and hard-working they are. They take risks and trust in God and create things. Very inspirational.</t>
+  </si>
+  <si>
+    <t>The Practice of the Presence of God (Paraclete Essentials)</t>
+  </si>
+  <si>
+    <t>Brother Lawrence &amp; Hal M. Helms (Editor), Robert J. Edmonson (Translator)</t>
+  </si>
+  <si>
+    <t>Brother Lawrence offers a beautifully simple faith and way of life: to always put yourself in the presence of God and to want to know Him and love Him.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3275,7 +3283,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="569">
+  <cellStyleXfs count="573">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3762,6 +3770,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3878,7 +3890,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="569">
+  <cellStyles count="573">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4406,6 +4418,8 @@
     <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="489" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="491" builtinId="8" hidden="1"/>
@@ -4447,6 +4461,8 @@
     <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4505,7 +4521,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -4557,7 +4573,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -4751,27 +4767,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H541"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H542"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A514" workbookViewId="0">
-      <selection activeCell="A542" sqref="A542"/>
+      <selection activeCell="A543" sqref="A543"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="98" customWidth="1"/>
     <col min="2" max="2" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="16">
       <c r="A1" s="4" t="s">
         <v>195</v>
       </c>
@@ -7884,7 +7900,7 @@
       <c r="E196" s="10"/>
       <c r="F196" s="10"/>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:6" ht="16">
       <c r="A197" s="9" t="s">
         <v>448</v>
       </c>
@@ -10599,7 +10615,7 @@
       <c r="E367" s="10"/>
       <c r="F367" s="10"/>
     </row>
-    <row r="368" spans="1:7">
+    <row r="368" spans="1:7" ht="16">
       <c r="A368" s="12" t="s">
         <v>0</v>
       </c>
@@ -10620,7 +10636,7 @@
       </c>
       <c r="G368" s="13"/>
     </row>
-    <row r="369" spans="1:8">
+    <row r="369" spans="1:8" ht="16">
       <c r="A369" s="6" t="s">
         <v>1</v>
       </c>
@@ -10643,7 +10659,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="370" spans="1:8">
+    <row r="370" spans="1:8" ht="16">
       <c r="A370" s="6" t="s">
         <v>2</v>
       </c>
@@ -10663,7 +10679,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="371" spans="1:8">
+    <row r="371" spans="1:8" ht="16">
       <c r="A371" s="6" t="s">
         <v>3</v>
       </c>
@@ -10683,7 +10699,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="372" spans="1:8">
+    <row r="372" spans="1:8" ht="16">
       <c r="A372" s="6" t="s">
         <v>4</v>
       </c>
@@ -10706,7 +10722,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="373" spans="1:8">
+    <row r="373" spans="1:8" ht="16">
       <c r="A373" s="6" t="s">
         <v>5</v>
       </c>
@@ -10729,7 +10745,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="374" spans="1:8">
+    <row r="374" spans="1:8" ht="16">
       <c r="A374" s="6" t="s">
         <v>6</v>
       </c>
@@ -10749,7 +10765,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="375" spans="1:8">
+    <row r="375" spans="1:8" ht="16">
       <c r="A375" s="6" t="s">
         <v>7</v>
       </c>
@@ -10769,7 +10785,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="376" spans="1:8">
+    <row r="376" spans="1:8" ht="16">
       <c r="A376" s="6" t="s">
         <v>8</v>
       </c>
@@ -10789,7 +10805,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="377" spans="1:8">
+    <row r="377" spans="1:8" ht="16">
       <c r="A377" s="6" t="s">
         <v>9</v>
       </c>
@@ -10809,7 +10825,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="378" spans="1:8">
+    <row r="378" spans="1:8" ht="16">
       <c r="A378" s="6" t="s">
         <v>10</v>
       </c>
@@ -10829,7 +10845,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="379" spans="1:8">
+    <row r="379" spans="1:8" ht="16">
       <c r="A379" s="6" t="s">
         <v>11</v>
       </c>
@@ -10849,7 +10865,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="380" spans="1:8">
+    <row r="380" spans="1:8" ht="16">
       <c r="A380" s="6" t="s">
         <v>12</v>
       </c>
@@ -10869,7 +10885,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="381" spans="1:8">
+    <row r="381" spans="1:8" ht="16">
       <c r="A381" s="6" t="s">
         <v>13</v>
       </c>
@@ -10889,7 +10905,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="382" spans="1:8">
+    <row r="382" spans="1:8" ht="16">
       <c r="A382" s="6" t="s">
         <v>14</v>
       </c>
@@ -10912,7 +10928,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="383" spans="1:8">
+    <row r="383" spans="1:8" ht="16">
       <c r="A383" s="6" t="s">
         <v>15</v>
       </c>
@@ -10932,7 +10948,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="384" spans="1:8">
+    <row r="384" spans="1:8" ht="16">
       <c r="A384" s="6" t="s">
         <v>16</v>
       </c>
@@ -10952,7 +10968,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="385" spans="1:8">
+    <row r="385" spans="1:8" ht="16">
       <c r="A385" s="6" t="s">
         <v>17</v>
       </c>
@@ -10972,7 +10988,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="386" spans="1:8">
+    <row r="386" spans="1:8" ht="16">
       <c r="A386" s="6" t="s">
         <v>18</v>
       </c>
@@ -10992,7 +11008,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="387" spans="1:8">
+    <row r="387" spans="1:8" ht="16">
       <c r="A387" s="6" t="s">
         <v>19</v>
       </c>
@@ -11012,7 +11028,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="388" spans="1:8">
+    <row r="388" spans="1:8" ht="16">
       <c r="A388" s="6" t="s">
         <v>20</v>
       </c>
@@ -11032,7 +11048,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="389" spans="1:8">
+    <row r="389" spans="1:8" ht="16">
       <c r="A389" s="6" t="s">
         <v>21</v>
       </c>
@@ -11052,7 +11068,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="390" spans="1:8">
+    <row r="390" spans="1:8" ht="16">
       <c r="A390" s="6" t="s">
         <v>22</v>
       </c>
@@ -11072,7 +11088,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="391" spans="1:8">
+    <row r="391" spans="1:8" ht="16">
       <c r="A391" s="6" t="s">
         <v>23</v>
       </c>
@@ -11096,7 +11112,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="392" spans="1:8">
+    <row r="392" spans="1:8" ht="16">
       <c r="A392" s="6" t="s">
         <v>24</v>
       </c>
@@ -11116,7 +11132,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="393" spans="1:8">
+    <row r="393" spans="1:8" ht="16">
       <c r="A393" s="6" t="s">
         <v>25</v>
       </c>
@@ -11136,7 +11152,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="394" spans="1:8">
+    <row r="394" spans="1:8" ht="16">
       <c r="A394" s="6" t="s">
         <v>26</v>
       </c>
@@ -11156,7 +11172,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="395" spans="1:8">
+    <row r="395" spans="1:8" ht="16">
       <c r="A395" s="6" t="s">
         <v>27</v>
       </c>
@@ -11176,7 +11192,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="396" spans="1:8">
+    <row r="396" spans="1:8" ht="16">
       <c r="A396" s="6" t="s">
         <v>28</v>
       </c>
@@ -11196,7 +11212,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="397" spans="1:8">
+    <row r="397" spans="1:8" ht="16">
       <c r="A397" s="6" t="s">
         <v>29</v>
       </c>
@@ -11216,7 +11232,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="398" spans="1:8">
+    <row r="398" spans="1:8" ht="16">
       <c r="A398" s="6" t="s">
         <v>30</v>
       </c>
@@ -11236,7 +11252,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="399" spans="1:8">
+    <row r="399" spans="1:8" ht="16">
       <c r="A399" s="6" t="s">
         <v>31</v>
       </c>
@@ -11256,7 +11272,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="400" spans="1:8">
+    <row r="400" spans="1:8" ht="16">
       <c r="A400" s="6" t="s">
         <v>32</v>
       </c>
@@ -11276,7 +11292,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="401" spans="1:8">
+    <row r="401" spans="1:8" ht="16">
       <c r="A401" s="6" t="s">
         <v>33</v>
       </c>
@@ -11296,7 +11312,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="402" spans="1:8">
+    <row r="402" spans="1:8" ht="16">
       <c r="A402" s="6" t="s">
         <v>34</v>
       </c>
@@ -11316,7 +11332,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="403" spans="1:8">
+    <row r="403" spans="1:8" ht="16">
       <c r="A403" s="6" t="s">
         <v>35</v>
       </c>
@@ -11336,7 +11352,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="404" spans="1:8">
+    <row r="404" spans="1:8" ht="16">
       <c r="A404" s="6" t="s">
         <v>36</v>
       </c>
@@ -11359,7 +11375,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="405" spans="1:8">
+    <row r="405" spans="1:8" ht="16">
       <c r="A405" s="6" t="s">
         <v>37</v>
       </c>
@@ -11379,7 +11395,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="406" spans="1:8">
+    <row r="406" spans="1:8" ht="16">
       <c r="A406" s="6" t="s">
         <v>38</v>
       </c>
@@ -11402,7 +11418,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="407" spans="1:8">
+    <row r="407" spans="1:8" ht="16">
       <c r="A407" s="6" t="s">
         <v>39</v>
       </c>
@@ -11422,7 +11438,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="408" spans="1:8">
+    <row r="408" spans="1:8" ht="16">
       <c r="A408" s="6" t="s">
         <v>40</v>
       </c>
@@ -11442,7 +11458,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="409" spans="1:8">
+    <row r="409" spans="1:8" ht="16">
       <c r="A409" s="6" t="s">
         <v>41</v>
       </c>
@@ -11462,7 +11478,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="410" spans="1:8">
+    <row r="410" spans="1:8" ht="16">
       <c r="A410" s="6" t="s">
         <v>42</v>
       </c>
@@ -11482,7 +11498,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="411" spans="1:8">
+    <row r="411" spans="1:8" ht="16">
       <c r="A411" s="6" t="s">
         <v>43</v>
       </c>
@@ -11502,7 +11518,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="412" spans="1:8">
+    <row r="412" spans="1:8" ht="16">
       <c r="A412" s="6" t="s">
         <v>44</v>
       </c>
@@ -11522,7 +11538,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="413" spans="1:8">
+    <row r="413" spans="1:8" ht="16">
       <c r="A413" s="6" t="s">
         <v>45</v>
       </c>
@@ -11542,7 +11558,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="414" spans="1:8">
+    <row r="414" spans="1:8" ht="16">
       <c r="A414" s="6" t="s">
         <v>46</v>
       </c>
@@ -11562,7 +11578,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="415" spans="1:8">
+    <row r="415" spans="1:8" ht="16">
       <c r="A415" s="6" t="s">
         <v>47</v>
       </c>
@@ -11582,7 +11598,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="416" spans="1:8">
+    <row r="416" spans="1:8" ht="16">
       <c r="A416" s="6" t="s">
         <v>48</v>
       </c>
@@ -11602,7 +11618,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="417" spans="1:6">
+    <row r="417" spans="1:6" ht="16">
       <c r="A417" s="6" t="s">
         <v>49</v>
       </c>
@@ -11622,7 +11638,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="418" spans="1:6">
+    <row r="418" spans="1:6" ht="16">
       <c r="A418" s="6" t="s">
         <v>50</v>
       </c>
@@ -11642,7 +11658,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="419" spans="1:6">
+    <row r="419" spans="1:6" ht="16">
       <c r="A419" s="6" t="s">
         <v>51</v>
       </c>
@@ -11662,7 +11678,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="420" spans="1:6">
+    <row r="420" spans="1:6" ht="16">
       <c r="A420" s="6" t="s">
         <v>52</v>
       </c>
@@ -11682,7 +11698,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="421" spans="1:6">
+    <row r="421" spans="1:6" ht="16">
       <c r="A421" s="6" t="s">
         <v>53</v>
       </c>
@@ -11702,7 +11718,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="422" spans="1:6">
+    <row r="422" spans="1:6" ht="16">
       <c r="A422" s="6" t="s">
         <v>54</v>
       </c>
@@ -11722,7 +11738,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="423" spans="1:6">
+    <row r="423" spans="1:6" ht="16">
       <c r="A423" s="6" t="s">
         <v>55</v>
       </c>
@@ -11742,7 +11758,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="424" spans="1:6">
+    <row r="424" spans="1:6" ht="16">
       <c r="A424" s="6" t="s">
         <v>56</v>
       </c>
@@ -11762,7 +11778,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="425" spans="1:6">
+    <row r="425" spans="1:6" ht="16">
       <c r="A425" s="6" t="s">
         <v>57</v>
       </c>
@@ -11782,7 +11798,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="426" spans="1:6">
+    <row r="426" spans="1:6" ht="16">
       <c r="A426" s="6" t="s">
         <v>58</v>
       </c>
@@ -11802,7 +11818,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="427" spans="1:6">
+    <row r="427" spans="1:6" ht="16">
       <c r="A427" s="6" t="s">
         <v>59</v>
       </c>
@@ -11822,7 +11838,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="428" spans="1:6">
+    <row r="428" spans="1:6" ht="16">
       <c r="A428" s="6" t="s">
         <v>60</v>
       </c>
@@ -11842,7 +11858,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="429" spans="1:6">
+    <row r="429" spans="1:6" ht="16">
       <c r="A429" s="6" t="s">
         <v>61</v>
       </c>
@@ -11862,7 +11878,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="430" spans="1:6">
+    <row r="430" spans="1:6" ht="16">
       <c r="A430" s="6" t="s">
         <v>62</v>
       </c>
@@ -11882,7 +11898,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="431" spans="1:6">
+    <row r="431" spans="1:6" ht="16">
       <c r="A431" s="6" t="s">
         <v>63</v>
       </c>
@@ -11902,7 +11918,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="432" spans="1:6">
+    <row r="432" spans="1:6" ht="16">
       <c r="A432" s="6" t="s">
         <v>64</v>
       </c>
@@ -11922,7 +11938,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="433" spans="1:8">
+    <row r="433" spans="1:8" ht="16">
       <c r="A433" s="6" t="s">
         <v>65</v>
       </c>
@@ -11945,7 +11961,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="434" spans="1:8">
+    <row r="434" spans="1:8" ht="16">
       <c r="A434" s="6" t="s">
         <v>66</v>
       </c>
@@ -11965,7 +11981,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="435" spans="1:8">
+    <row r="435" spans="1:8" ht="16">
       <c r="A435" s="6" t="s">
         <v>67</v>
       </c>
@@ -11988,7 +12004,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="436" spans="1:8">
+    <row r="436" spans="1:8" ht="16">
       <c r="A436" s="6" t="s">
         <v>68</v>
       </c>
@@ -12008,7 +12024,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="437" spans="1:8">
+    <row r="437" spans="1:8" ht="16">
       <c r="A437" s="6" t="s">
         <v>69</v>
       </c>
@@ -12028,7 +12044,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="438" spans="1:8">
+    <row r="438" spans="1:8" ht="16">
       <c r="A438" s="6" t="s">
         <v>70</v>
       </c>
@@ -12051,7 +12067,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="439" spans="1:8">
+    <row r="439" spans="1:8" ht="16">
       <c r="A439" s="6" t="s">
         <v>71</v>
       </c>
@@ -12071,7 +12087,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="440" spans="1:8">
+    <row r="440" spans="1:8" ht="16">
       <c r="A440" s="6" t="s">
         <v>72</v>
       </c>
@@ -12092,7 +12108,7 @@
       </c>
       <c r="G440" s="15"/>
     </row>
-    <row r="441" spans="1:8">
+    <row r="441" spans="1:8" ht="16">
       <c r="A441" s="6" t="s">
         <v>73</v>
       </c>
@@ -12112,7 +12128,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="442" spans="1:8">
+    <row r="442" spans="1:8" ht="16">
       <c r="A442" s="6" t="s">
         <v>74</v>
       </c>
@@ -12132,7 +12148,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="443" spans="1:8">
+    <row r="443" spans="1:8" ht="16">
       <c r="A443" s="6" t="s">
         <v>75</v>
       </c>
@@ -12152,7 +12168,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="444" spans="1:8">
+    <row r="444" spans="1:8" ht="16">
       <c r="A444" s="6" t="s">
         <v>76</v>
       </c>
@@ -12172,7 +12188,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="445" spans="1:8">
+    <row r="445" spans="1:8" ht="16">
       <c r="A445" s="6" t="s">
         <v>77</v>
       </c>
@@ -12192,7 +12208,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="446" spans="1:8">
+    <row r="446" spans="1:8" ht="16">
       <c r="A446" s="6" t="s">
         <v>78</v>
       </c>
@@ -12212,7 +12228,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="447" spans="1:8">
+    <row r="447" spans="1:8" ht="16">
       <c r="A447" s="6" t="s">
         <v>79</v>
       </c>
@@ -12232,7 +12248,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="448" spans="1:8">
+    <row r="448" spans="1:8" ht="16">
       <c r="A448" s="6" t="s">
         <v>80</v>
       </c>
@@ -12252,7 +12268,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="449" spans="1:8">
+    <row r="449" spans="1:8" ht="16">
       <c r="A449" s="6" t="s">
         <v>81</v>
       </c>
@@ -12272,7 +12288,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="450" spans="1:8">
+    <row r="450" spans="1:8" ht="16">
       <c r="A450" s="6" t="s">
         <v>82</v>
       </c>
@@ -12292,7 +12308,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="451" spans="1:8">
+    <row r="451" spans="1:8" ht="16">
       <c r="A451" s="6" t="s">
         <v>83</v>
       </c>
@@ -12312,7 +12328,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="452" spans="1:8">
+    <row r="452" spans="1:8" ht="16">
       <c r="A452" s="6" t="s">
         <v>84</v>
       </c>
@@ -12333,7 +12349,7 @@
       </c>
       <c r="G452" s="15"/>
     </row>
-    <row r="453" spans="1:8">
+    <row r="453" spans="1:8" ht="16">
       <c r="A453" s="6" t="s">
         <v>85</v>
       </c>
@@ -12353,7 +12369,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="454" spans="1:8">
+    <row r="454" spans="1:8" ht="16">
       <c r="A454" s="6" t="s">
         <v>86</v>
       </c>
@@ -12376,7 +12392,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="455" spans="1:8">
+    <row r="455" spans="1:8" ht="16">
       <c r="A455" s="6" t="s">
         <v>87</v>
       </c>
@@ -12396,7 +12412,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="456" spans="1:8">
+    <row r="456" spans="1:8" ht="16">
       <c r="A456" s="6" t="s">
         <v>88</v>
       </c>
@@ -12417,7 +12433,7 @@
       </c>
       <c r="G456" s="15"/>
     </row>
-    <row r="457" spans="1:8">
+    <row r="457" spans="1:8" ht="16">
       <c r="A457" s="6" t="s">
         <v>89</v>
       </c>
@@ -12437,7 +12453,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="458" spans="1:8">
+    <row r="458" spans="1:8" ht="16">
       <c r="A458" s="6" t="s">
         <v>90</v>
       </c>
@@ -12457,7 +12473,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="459" spans="1:8">
+    <row r="459" spans="1:8" ht="16">
       <c r="A459" s="6" t="s">
         <v>91</v>
       </c>
@@ -12477,7 +12493,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="460" spans="1:8">
+    <row r="460" spans="1:8" ht="16">
       <c r="A460" s="6" t="s">
         <v>92</v>
       </c>
@@ -12497,7 +12513,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="461" spans="1:8">
+    <row r="461" spans="1:8" ht="16">
       <c r="A461" s="6" t="s">
         <v>93</v>
       </c>
@@ -12517,7 +12533,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="462" spans="1:8">
+    <row r="462" spans="1:8" ht="16">
       <c r="A462" s="6" t="s">
         <v>94</v>
       </c>
@@ -12537,7 +12553,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="463" spans="1:8">
+    <row r="463" spans="1:8" ht="16">
       <c r="A463" s="6" t="s">
         <v>95</v>
       </c>
@@ -12560,7 +12576,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="464" spans="1:8">
+    <row r="464" spans="1:8" ht="16">
       <c r="A464" s="6" t="s">
         <v>96</v>
       </c>
@@ -12580,7 +12596,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="465" spans="1:8">
+    <row r="465" spans="1:8" ht="16">
       <c r="A465" s="6" t="s">
         <v>97</v>
       </c>
@@ -12600,7 +12616,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="466" spans="1:8">
+    <row r="466" spans="1:8" ht="16">
       <c r="A466" s="6" t="s">
         <v>98</v>
       </c>
@@ -12623,7 +12639,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="467" spans="1:8">
+    <row r="467" spans="1:8" ht="16">
       <c r="A467" s="6" t="s">
         <v>99</v>
       </c>
@@ -12646,7 +12662,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="468" spans="1:8">
+    <row r="468" spans="1:8" ht="16">
       <c r="A468" s="6" t="s">
         <v>208</v>
       </c>
@@ -12670,7 +12686,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="469" spans="1:8">
+    <row r="469" spans="1:8" ht="16">
       <c r="A469" s="6" t="s">
         <v>210</v>
       </c>
@@ -12694,7 +12710,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="470" spans="1:8">
+    <row r="470" spans="1:8" ht="16">
       <c r="A470" s="6" t="s">
         <v>212</v>
       </c>
@@ -12705,7 +12721,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="471" spans="1:8">
+    <row r="471" spans="1:8" ht="16">
       <c r="A471" s="12" t="s">
         <v>223</v>
       </c>
@@ -12731,7 +12747,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="472" spans="1:8">
+    <row r="472" spans="1:8" ht="16">
       <c r="A472" s="6" t="s">
         <v>225</v>
       </c>
@@ -12757,7 +12773,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="473" spans="1:8">
+    <row r="473" spans="1:8" ht="16">
       <c r="A473" s="6" t="s">
         <v>231</v>
       </c>
@@ -12783,7 +12799,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="474" spans="1:8">
+    <row r="474" spans="1:8" ht="16">
       <c r="A474" s="6" t="s">
         <v>234</v>
       </c>
@@ -12809,7 +12825,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="475" spans="1:8">
+    <row r="475" spans="1:8" ht="16">
       <c r="A475" s="6" t="s">
         <v>235</v>
       </c>
@@ -12835,7 +12851,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="476" spans="1:8">
+    <row r="476" spans="1:8" ht="16">
       <c r="A476" s="6" t="s">
         <v>237</v>
       </c>
@@ -12861,7 +12877,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="477" spans="1:8">
+    <row r="477" spans="1:8" ht="16">
       <c r="A477" s="6" t="s">
         <v>249</v>
       </c>
@@ -12887,7 +12903,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="478" spans="1:8">
+    <row r="478" spans="1:8" ht="16">
       <c r="A478" s="6" t="s">
         <v>251</v>
       </c>
@@ -12913,7 +12929,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="479" spans="1:8">
+    <row r="479" spans="1:8" ht="16">
       <c r="A479" s="6" t="s">
         <v>255</v>
       </c>
@@ -12939,7 +12955,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="480" spans="1:8">
+    <row r="480" spans="1:8" ht="16">
       <c r="A480" s="6" t="s">
         <v>885</v>
       </c>
@@ -12965,7 +12981,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="481" spans="1:8">
+    <row r="481" spans="1:8" ht="16">
       <c r="A481" s="6" t="s">
         <v>889</v>
       </c>
@@ -12991,7 +13007,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="482" spans="1:8">
+    <row r="482" spans="1:8" ht="16">
       <c r="A482" s="6" t="s">
         <v>892</v>
       </c>
@@ -13017,7 +13033,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="483" spans="1:8">
+    <row r="483" spans="1:8" ht="16">
       <c r="A483" s="6" t="s">
         <v>509</v>
       </c>
@@ -13043,7 +13059,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="484" spans="1:8">
+    <row r="484" spans="1:8" ht="16">
       <c r="A484" s="6" t="s">
         <v>895</v>
       </c>
@@ -13069,7 +13085,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="485" spans="1:8">
+    <row r="485" spans="1:8" ht="16">
       <c r="A485" s="6" t="s">
         <v>899</v>
       </c>
@@ -13095,7 +13111,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="486" spans="1:8">
+    <row r="486" spans="1:8" ht="16">
       <c r="A486" s="6" t="s">
         <v>902</v>
       </c>
@@ -13121,7 +13137,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="487" spans="1:8">
+    <row r="487" spans="1:8" ht="16">
       <c r="A487" s="6" t="s">
         <v>905</v>
       </c>
@@ -13147,7 +13163,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="488" spans="1:8">
+    <row r="488" spans="1:8" ht="16">
       <c r="A488" s="6" t="s">
         <v>908</v>
       </c>
@@ -13173,7 +13189,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="489" spans="1:8">
+    <row r="489" spans="1:8" ht="16">
       <c r="A489" s="6" t="s">
         <v>910</v>
       </c>
@@ -13199,7 +13215,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="490" spans="1:8">
+    <row r="490" spans="1:8" ht="16">
       <c r="A490" s="6" t="s">
         <v>912</v>
       </c>
@@ -13225,7 +13241,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="491" spans="1:8">
+    <row r="491" spans="1:8" ht="16">
       <c r="A491" s="6" t="s">
         <v>915</v>
       </c>
@@ -13251,7 +13267,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="492" spans="1:8">
+    <row r="492" spans="1:8" ht="16">
       <c r="A492" s="6" t="s">
         <v>917</v>
       </c>
@@ -13277,7 +13293,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="493" spans="1:8">
+    <row r="493" spans="1:8" ht="16">
       <c r="A493" s="6" t="s">
         <v>921</v>
       </c>
@@ -13303,7 +13319,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="494" spans="1:8">
+    <row r="494" spans="1:8" ht="16">
       <c r="A494" s="6" t="s">
         <v>923</v>
       </c>
@@ -13329,7 +13345,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="495" spans="1:8">
+    <row r="495" spans="1:8" ht="16">
       <c r="A495" s="6" t="s">
         <v>926</v>
       </c>
@@ -13355,7 +13371,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="496" spans="1:8">
+    <row r="496" spans="1:8" ht="16">
       <c r="A496" s="6" t="s">
         <v>934</v>
       </c>
@@ -13381,7 +13397,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="497" spans="1:8">
+    <row r="497" spans="1:8" ht="16">
       <c r="A497" s="6" t="s">
         <v>932</v>
       </c>
@@ -13407,7 +13423,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="498" spans="1:8">
+    <row r="498" spans="1:8" ht="16">
       <c r="A498" s="6" t="s">
         <v>936</v>
       </c>
@@ -13433,7 +13449,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="499" spans="1:8">
+    <row r="499" spans="1:8" ht="16">
       <c r="A499" s="6" t="s">
         <v>941</v>
       </c>
@@ -13459,7 +13475,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="500" spans="1:8">
+    <row r="500" spans="1:8" ht="16">
       <c r="A500" s="6" t="s">
         <v>944</v>
       </c>
@@ -13485,7 +13501,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="501" spans="1:8">
+    <row r="501" spans="1:8" ht="16">
       <c r="A501" s="6" t="s">
         <v>947</v>
       </c>
@@ -13511,7 +13527,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="502" spans="1:8">
+    <row r="502" spans="1:8" ht="16">
       <c r="A502" s="6" t="s">
         <v>949</v>
       </c>
@@ -13537,7 +13553,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="503" spans="1:8">
+    <row r="503" spans="1:8" ht="16">
       <c r="A503" s="6" t="s">
         <v>950</v>
       </c>
@@ -13563,7 +13579,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="504" spans="1:8">
+    <row r="504" spans="1:8" ht="16">
       <c r="A504" s="6" t="s">
         <v>954</v>
       </c>
@@ -13589,7 +13605,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="505" spans="1:8">
+    <row r="505" spans="1:8" ht="16">
       <c r="A505" s="6" t="s">
         <v>956</v>
       </c>
@@ -13615,7 +13631,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="506" spans="1:8">
+    <row r="506" spans="1:8" ht="16">
       <c r="A506" s="6" t="s">
         <v>959</v>
       </c>
@@ -13641,7 +13657,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="507" spans="1:8">
+    <row r="507" spans="1:8" ht="16">
       <c r="A507" s="6" t="s">
         <v>963</v>
       </c>
@@ -13667,7 +13683,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="508" spans="1:8">
+    <row r="508" spans="1:8" ht="16">
       <c r="A508" s="6" t="s">
         <v>966</v>
       </c>
@@ -13693,7 +13709,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="509" spans="1:8">
+    <row r="509" spans="1:8" ht="16">
       <c r="A509" s="6" t="s">
         <v>969</v>
       </c>
@@ -13719,7 +13735,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="510" spans="1:8">
+    <row r="510" spans="1:8" ht="16">
       <c r="A510" s="6" t="s">
         <v>972</v>
       </c>
@@ -13745,7 +13761,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="511" spans="1:8">
+    <row r="511" spans="1:8" ht="16">
       <c r="A511" s="6" t="s">
         <v>975</v>
       </c>
@@ -13771,7 +13787,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="512" spans="1:8">
+    <row r="512" spans="1:8" ht="16">
       <c r="A512" s="6" t="s">
         <v>978</v>
       </c>
@@ -13797,7 +13813,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="513" spans="1:8">
+    <row r="513" spans="1:8" ht="16">
       <c r="A513" s="6" t="s">
         <v>981</v>
       </c>
@@ -13823,7 +13839,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="514" spans="1:8">
+    <row r="514" spans="1:8" ht="16">
       <c r="A514" s="6" t="s">
         <v>982</v>
       </c>
@@ -13849,7 +13865,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="515" spans="1:8">
+    <row r="515" spans="1:8" ht="16">
       <c r="A515" s="6" t="s">
         <v>983</v>
       </c>
@@ -13875,7 +13891,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="516" spans="1:8">
+    <row r="516" spans="1:8" ht="16">
       <c r="A516" s="6" t="s">
         <v>984</v>
       </c>
@@ -13901,7 +13917,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="517" spans="1:8">
+    <row r="517" spans="1:8" ht="16">
       <c r="A517" s="6" t="s">
         <v>991</v>
       </c>
@@ -13927,7 +13943,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="518" spans="1:8">
+    <row r="518" spans="1:8" ht="16">
       <c r="A518" s="6" t="s">
         <v>993</v>
       </c>
@@ -13953,7 +13969,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="519" spans="1:8">
+    <row r="519" spans="1:8" ht="16">
       <c r="A519" s="6" t="s">
         <v>996</v>
       </c>
@@ -13979,7 +13995,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="520" spans="1:8">
+    <row r="520" spans="1:8" ht="16">
       <c r="A520" s="6" t="s">
         <v>999</v>
       </c>
@@ -14005,7 +14021,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="521" spans="1:8">
+    <row r="521" spans="1:8" ht="16">
       <c r="A521" s="6" t="s">
         <v>1002</v>
       </c>
@@ -14031,7 +14047,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="522" spans="1:8">
+    <row r="522" spans="1:8" ht="16">
       <c r="A522" s="6" t="s">
         <v>1005</v>
       </c>
@@ -14057,7 +14073,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="523" spans="1:8">
+    <row r="523" spans="1:8" ht="16">
       <c r="A523" s="6" t="s">
         <v>1008</v>
       </c>
@@ -14083,7 +14099,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="524" spans="1:8">
+    <row r="524" spans="1:8" ht="16">
       <c r="A524" s="6" t="s">
         <v>1011</v>
       </c>
@@ -14109,7 +14125,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="525" spans="1:8">
+    <row r="525" spans="1:8" ht="16">
       <c r="A525" s="6" t="s">
         <v>1014</v>
       </c>
@@ -14135,7 +14151,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="526" spans="1:8">
+    <row r="526" spans="1:8" ht="16">
       <c r="A526" s="6" t="s">
         <v>1017</v>
       </c>
@@ -14161,7 +14177,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="527" spans="1:8">
+    <row r="527" spans="1:8" ht="16">
       <c r="A527" s="6" t="s">
         <v>1020</v>
       </c>
@@ -14187,7 +14203,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="528" spans="1:8">
+    <row r="528" spans="1:8" ht="16">
       <c r="A528" s="6" t="s">
         <v>1022</v>
       </c>
@@ -14213,7 +14229,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="529" spans="1:8">
+    <row r="529" spans="1:8" ht="16">
       <c r="A529" s="6" t="s">
         <v>1025</v>
       </c>
@@ -14239,7 +14255,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="530" spans="1:8">
+    <row r="530" spans="1:8" ht="16">
       <c r="A530" s="6" t="s">
         <v>1028</v>
       </c>
@@ -14265,7 +14281,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="531" spans="1:8">
+    <row r="531" spans="1:8" ht="16">
       <c r="A531" s="6" t="s">
         <v>1031</v>
       </c>
@@ -14291,7 +14307,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="532" spans="1:8">
+    <row r="532" spans="1:8" ht="16">
       <c r="A532" s="6" t="s">
         <v>1033</v>
       </c>
@@ -14317,7 +14333,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="533" spans="1:8">
+    <row r="533" spans="1:8" ht="16">
       <c r="A533" s="6" t="s">
         <v>337</v>
       </c>
@@ -14343,7 +14359,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="534" spans="1:8">
+    <row r="534" spans="1:8" ht="16">
       <c r="A534" s="6" t="s">
         <v>1039</v>
       </c>
@@ -14369,7 +14385,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="535" spans="1:8">
+    <row r="535" spans="1:8" ht="16">
       <c r="A535" s="6" t="s">
         <v>1042</v>
       </c>
@@ -14395,7 +14411,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="536" spans="1:8">
+    <row r="536" spans="1:8" ht="16">
       <c r="A536" s="6" t="s">
         <v>1045</v>
       </c>
@@ -14421,7 +14437,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="537" spans="1:8">
+    <row r="537" spans="1:8" ht="16">
       <c r="A537" s="6" t="s">
         <v>1048</v>
       </c>
@@ -14447,7 +14463,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="538" spans="1:8">
+    <row r="538" spans="1:8" ht="16">
       <c r="A538" s="6" t="s">
         <v>1051</v>
       </c>
@@ -14473,7 +14489,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="539" spans="1:8">
+    <row r="539" spans="1:8" ht="16">
       <c r="A539" s="6" t="s">
         <v>1054</v>
       </c>
@@ -14499,7 +14515,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="540" spans="1:8">
+    <row r="540" spans="1:8" ht="16">
       <c r="A540" s="6" t="s">
         <v>1057</v>
       </c>
@@ -14525,7 +14541,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="541" spans="1:8">
+    <row r="541" spans="1:8" ht="16">
       <c r="A541" s="6" t="s">
         <v>1060</v>
       </c>
@@ -14551,18 +14567,50 @@
         <v>1062</v>
       </c>
     </row>
+    <row r="542" spans="1:8" ht="16">
+      <c r="A542" s="6" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B542" s="6" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C542" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D542" s="14">
+        <v>2018</v>
+      </c>
+      <c r="E542" s="14">
+        <v>1693</v>
+      </c>
+      <c r="F542" s="14">
+        <v>127</v>
+      </c>
+      <c r="G542" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="H542" s="6" t="s">
+        <v>1065</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
@@ -14635,5 +14683,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
The End of Big
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AA0413-0529-4A4A-984D-F72AB61586F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9803B9DD-9331-7C49-8B02-8F627E9B859B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1881" uniqueCount="1115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="1117">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3371,6 +3371,12 @@
   </si>
   <si>
     <t>New American Bible, Revised Edition (Matthew, Mark, Luke, John, Acts of the Apostles, Revelation, Job, Isaiah, Wisdom, Matthew, James, 1-2 Peter, 1-3 John, Jude)</t>
+  </si>
+  <si>
+    <t>The End of Big: How the Internet Makes David the New Goliath</t>
+  </si>
+  <si>
+    <t>Nicco Mele</t>
   </si>
 </sst>
 </file>
@@ -4674,7 +4680,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -4726,7 +4732,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -4928,10 +4934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H575"/>
+  <dimension ref="A1:H576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A560" workbookViewId="0">
-      <selection activeCell="A576" sqref="A576"/>
+      <selection activeCell="A577" sqref="A577"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15339,6 +15345,29 @@
       </c>
       <c r="H575" s="6" t="s">
         <v>1062</v>
+      </c>
+    </row>
+    <row r="576" spans="1:8">
+      <c r="A576" s="6" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B576" s="6" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C576" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D576" s="14">
+        <v>2018</v>
+      </c>
+      <c r="E576" s="14">
+        <v>2013</v>
+      </c>
+      <c r="F576" s="14">
+        <v>321</v>
+      </c>
+      <c r="G576" s="14" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shop Class as Soulcraft
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9803B9DD-9331-7C49-8B02-8F627E9B859B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1324E498-77F0-534C-9F54-64C37B53473F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="1117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1891" uniqueCount="1120">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3377,6 +3377,15 @@
   </si>
   <si>
     <t>Nicco Mele</t>
+  </si>
+  <si>
+    <t>Shop Class as Soulcraft: An Inquiry into the Value of Work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mele's basic premise is that internet-based technologies are in the process of reversing the trend of large institutions and moving us back toward smaller players in news, politics, entertianment, government, military, and business. He said toward the beginning that the book would be a bit all over the place which it was. He has some interesting experience but plenty of anecdotes that could have been omitted. I appreciated his calling out "nerd disease" or the tendency to make things overly complicated for the sake of doing so or to cement authority. I also found his description of "Digital Feudalism" to be compelling and important for thinking about our use of the internet so that we be more than just serfs on the turf of Facebook, Twitter, etc. cultivating their fields. </t>
+  </si>
+  <si>
+    <t>I read Crawford's other book last year, and he continues to impress me with his deep thinking about the very practical and ordinary. This book is in part a manifesto against the false dichotomy between "thinking" white-collar work for which college is required and "non-thinking" work that includes all the trades: he demonstrates the deep intellectual engagement required in the trades and how that very intellectual engagement is being lost in many professional jobs. His writing about owning your stuff and having control over your life is compelling, and all of his stories about working on motocycles is fascinating. His ability to bring deep philosophy to bear on orginary work is impressive.</t>
   </si>
 </sst>
 </file>
@@ -4934,10 +4943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H576"/>
+  <dimension ref="A1:H577"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A560" workbookViewId="0">
-      <selection activeCell="A577" sqref="A577"/>
+      <selection activeCell="A578" sqref="A578"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15368,6 +15377,35 @@
       </c>
       <c r="G576" s="14" t="s">
         <v>240</v>
+      </c>
+      <c r="H576" s="6" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="577" spans="1:8">
+      <c r="A577" s="6" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B577" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C577" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D577" s="14">
+        <v>2018</v>
+      </c>
+      <c r="E577" s="14">
+        <v>2009</v>
+      </c>
+      <c r="F577" s="14">
+        <v>256</v>
+      </c>
+      <c r="G577" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="H577" s="6" t="s">
+        <v>1119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commercial Real Estate Investing
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4225295-DB22-9C43-801B-167E3265B37C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15040"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
     <sheet name="Pivot" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="1132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="1135">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3422,13 +3416,22 @@
   </si>
   <si>
     <t>Dad recommended this and I thought this was a great and important corrolary to the chapter on probability in The Organized Mind. Mathematical and probabilistic thinking and decision making is important and something I want to become more natural for myself.</t>
+  </si>
+  <si>
+    <t>Commercial Real Estate Investing</t>
+  </si>
+  <si>
+    <t>Dolf de Roos</t>
+  </si>
+  <si>
+    <t>My first real estate book, and a helpful overview of commercial real estate investing with some interesting stories. This book is intended for investors who want to find a property with a twist they can use to their advantage to create massive value.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4963,21 +4966,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A568" workbookViewId="0">
-      <selection activeCell="G584" sqref="G584"/>
+      <selection activeCell="A585" sqref="A585"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="98" style="6" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="6" customWidth="1"/>
@@ -15594,10 +15597,30 @@
       </c>
     </row>
     <row r="584" spans="1:8">
-      <c r="D584" s="9"/>
-      <c r="E584" s="9"/>
-      <c r="F584" s="9"/>
-      <c r="G584" s="9"/>
+      <c r="A584" s="6" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B584" s="6" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C584" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D584" s="9">
+        <v>2018</v>
+      </c>
+      <c r="E584" s="9">
+        <v>2008</v>
+      </c>
+      <c r="F584" s="9">
+        <v>268</v>
+      </c>
+      <c r="G584" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="H584" s="6" t="s">
+        <v>1134</v>
+      </c>
     </row>
     <row r="585" spans="1:8">
       <c r="D585" s="9"/>
@@ -19145,12 +19168,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Monuments, Scarlet Pimpernel, Chip
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781F8222-F7DD-2341-8602-0AC884F3A25A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C000D9-4460-2C41-BDDC-A1065F21FAC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="25120" windowHeight="15040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
     <sheet name="Pivot" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1930" uniqueCount="1137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="1143">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3437,6 +3437,24 @@
   </si>
   <si>
     <t>Robert M. Edsel and Bret Witter</t>
+  </si>
+  <si>
+    <t>The Scarlet Pimpernel</t>
+  </si>
+  <si>
+    <t>Baroness Emma Orczy</t>
+  </si>
+  <si>
+    <t>Capital Gaines: Smart Things I Learned Doing Stupid Stuff</t>
+  </si>
+  <si>
+    <t>Chip Gaines</t>
+  </si>
+  <si>
+    <t>I watched the movie when it came out several years ago and it was great to hear all of the detail that went behind this amazing group of men and women—both American Monuments Men as well as noble Germans—who took it upon themselves to save so much of Western Civilization that could have been lost in the war. I loved the scene at the end of Chapter 17 showing how true beauty in art speaks to people across time and class and situation: how it speaks to the truth.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Much of what I think people are attracted to in Chip and Joanna Gaines is their authenticity, and that comes out very much in his book. He is a real man doing real work, raising a family, and building real businesses. To say they are inspiring is an understatement. </t>
   </si>
 </sst>
 </file>
@@ -4988,8 +5006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A568" workbookViewId="0">
-      <selection activeCell="C587" sqref="C587"/>
+    <sheetView tabSelected="1" topLeftCell="A563" workbookViewId="0">
+      <selection activeCell="A588" sqref="A588"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15656,18 +15674,58 @@
       <c r="G585" s="9" t="s">
         <v>242</v>
       </c>
+      <c r="H585" s="6" t="s">
+        <v>1141</v>
+      </c>
     </row>
     <row r="586" spans="1:8">
-      <c r="D586" s="9"/>
-      <c r="E586" s="9"/>
-      <c r="F586" s="9"/>
-      <c r="G586" s="9"/>
+      <c r="A586" s="6" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B586" s="6" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C586" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D586" s="9">
+        <v>2018</v>
+      </c>
+      <c r="E586" s="9">
+        <v>1905</v>
+      </c>
+      <c r="F586" s="9">
+        <v>319</v>
+      </c>
+      <c r="G586" s="9" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="587" spans="1:8">
-      <c r="D587" s="9"/>
-      <c r="E587" s="9"/>
-      <c r="F587" s="9"/>
-      <c r="G587" s="9"/>
+      <c r="A587" s="6" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B587" s="6" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C587" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D587" s="9">
+        <v>2018</v>
+      </c>
+      <c r="E587" s="9">
+        <v>2017</v>
+      </c>
+      <c r="F587" s="9">
+        <v>208</v>
+      </c>
+      <c r="G587" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="H587" s="6" t="s">
+        <v>1142</v>
+      </c>
     </row>
     <row r="588" spans="1:8">
       <c r="D588" s="9"/>

</xml_diff>

<commit_message>
Making Room For God (declutter)
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F12059B-D56C-874C-B106-2513777FA260}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFF428A-6520-0C4D-AEF6-A08B27F12CA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="25120" windowHeight="15040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1946" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="1150">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3467,6 +3467,15 @@
   </si>
   <si>
     <t>The Vatican Diaries: A Behind-the-Scenes Look at the Power, Personalities, and Politics at the Heart of the Catholic Church</t>
+  </si>
+  <si>
+    <t>Making Room for God: Decluttering and the Spiritual Life</t>
+  </si>
+  <si>
+    <t>Mary Elizabeth Sperry</t>
+  </si>
+  <si>
+    <t>I read this after Jordan and appreciated her notes. One very insightful thing Sperry mentions is how clutter in our lives if often the symptom of sin, and in fixing the clutter we need to dig down to the root of the sin.</t>
   </si>
 </sst>
 </file>
@@ -5018,8 +5027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A439" workbookViewId="0">
-      <selection activeCell="A456" sqref="A456"/>
+    <sheetView tabSelected="1" topLeftCell="A579" workbookViewId="0">
+      <selection activeCell="A590" sqref="A590"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15769,10 +15778,30 @@
       </c>
     </row>
     <row r="589" spans="1:8">
-      <c r="D589" s="9"/>
-      <c r="E589" s="9"/>
-      <c r="F589" s="9"/>
-      <c r="G589" s="9"/>
+      <c r="A589" s="6" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B589" s="6" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C589" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D589" s="9">
+        <v>2018</v>
+      </c>
+      <c r="E589" s="9">
+        <v>2018</v>
+      </c>
+      <c r="F589" s="9">
+        <v>129</v>
+      </c>
+      <c r="G589" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="H589" s="6" t="s">
+        <v>1149</v>
+      </c>
     </row>
     <row r="590" spans="1:8">
       <c r="D590" s="9"/>

</xml_diff>

<commit_message>
Them by Ben Sasse
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814440D0-D78D-6A4D-B6DA-CBE0D5E39090}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660D3B19-F88A-664F-968D-99B8C4DB53E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1966" uniqueCount="1157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1971" uniqueCount="1159">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3497,6 +3497,12 @@
   </si>
   <si>
     <t xml:space="preserve">Adam recommended this at Nos Lumine. In some ways a very "self-helpy" book but he advocates taking about an hour each morning for silence, affirmation, visualization, exercise, reading, and journaling. </t>
+  </si>
+  <si>
+    <t>Them: Why We Hate Each Other—and How to Heal</t>
+  </si>
+  <si>
+    <t>Ben Sasse is a boss. His argument: focus on the what unites us above (civics) and upstream (culture) of politics, and build strong communities.</t>
   </si>
 </sst>
 </file>
@@ -4792,7 +4798,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -4844,7 +4850,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -5049,7 +5055,7 @@
   <dimension ref="A1:H1173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A579" workbookViewId="0">
-      <selection activeCell="A593" sqref="A593"/>
+      <selection activeCell="A594" sqref="A594"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15902,97 +15908,117 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="593" spans="4:7">
-      <c r="D593" s="9"/>
-      <c r="E593" s="9"/>
-      <c r="F593" s="9"/>
-      <c r="G593" s="9"/>
-    </row>
-    <row r="594" spans="4:7">
+    <row r="593" spans="1:8">
+      <c r="A593" s="6" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B593" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C593" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D593" s="9">
+        <v>2018</v>
+      </c>
+      <c r="E593" s="9">
+        <v>2018</v>
+      </c>
+      <c r="F593" s="9">
+        <v>256</v>
+      </c>
+      <c r="G593" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="H593" s="6" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="594" spans="1:8">
       <c r="D594" s="9"/>
       <c r="E594" s="9"/>
       <c r="F594" s="9"/>
       <c r="G594" s="9"/>
     </row>
-    <row r="595" spans="4:7">
+    <row r="595" spans="1:8">
       <c r="D595" s="9"/>
       <c r="E595" s="9"/>
       <c r="F595" s="9"/>
       <c r="G595" s="9"/>
     </row>
-    <row r="596" spans="4:7">
+    <row r="596" spans="1:8">
       <c r="D596" s="9"/>
       <c r="E596" s="9"/>
       <c r="F596" s="9"/>
       <c r="G596" s="9"/>
     </row>
-    <row r="597" spans="4:7">
+    <row r="597" spans="1:8">
       <c r="D597" s="9"/>
       <c r="E597" s="9"/>
       <c r="F597" s="9"/>
       <c r="G597" s="9"/>
     </row>
-    <row r="598" spans="4:7">
+    <row r="598" spans="1:8">
       <c r="D598" s="9"/>
       <c r="E598" s="9"/>
       <c r="F598" s="9"/>
       <c r="G598" s="9"/>
     </row>
-    <row r="599" spans="4:7">
+    <row r="599" spans="1:8">
       <c r="D599" s="9"/>
       <c r="E599" s="9"/>
       <c r="F599" s="9"/>
       <c r="G599" s="9"/>
     </row>
-    <row r="600" spans="4:7">
+    <row r="600" spans="1:8">
       <c r="D600" s="9"/>
       <c r="E600" s="9"/>
       <c r="F600" s="9"/>
       <c r="G600" s="9"/>
     </row>
-    <row r="601" spans="4:7">
+    <row r="601" spans="1:8">
       <c r="D601" s="9"/>
       <c r="E601" s="9"/>
       <c r="F601" s="9"/>
       <c r="G601" s="9"/>
     </row>
-    <row r="602" spans="4:7">
+    <row r="602" spans="1:8">
       <c r="D602" s="9"/>
       <c r="E602" s="9"/>
       <c r="F602" s="9"/>
       <c r="G602" s="9"/>
     </row>
-    <row r="603" spans="4:7">
+    <row r="603" spans="1:8">
       <c r="D603" s="9"/>
       <c r="E603" s="9"/>
       <c r="F603" s="9"/>
       <c r="G603" s="9"/>
     </row>
-    <row r="604" spans="4:7">
+    <row r="604" spans="1:8">
       <c r="D604" s="9"/>
       <c r="E604" s="9"/>
       <c r="F604" s="9"/>
       <c r="G604" s="9"/>
     </row>
-    <row r="605" spans="4:7">
+    <row r="605" spans="1:8">
       <c r="D605" s="9"/>
       <c r="E605" s="9"/>
       <c r="F605" s="9"/>
       <c r="G605" s="9"/>
     </row>
-    <row r="606" spans="4:7">
+    <row r="606" spans="1:8">
       <c r="D606" s="9"/>
       <c r="E606" s="9"/>
       <c r="F606" s="9"/>
       <c r="G606" s="9"/>
     </row>
-    <row r="607" spans="4:7">
+    <row r="607" spans="1:8">
       <c r="D607" s="9"/>
       <c r="E607" s="9"/>
       <c r="F607" s="9"/>
       <c r="G607" s="9"/>
     </row>
-    <row r="608" spans="4:7">
+    <row r="608" spans="1:8">
       <c r="D608" s="9"/>
       <c r="E608" s="9"/>
       <c r="F608" s="9"/>

</xml_diff>

<commit_message>
Them & Real Estate
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660D3B19-F88A-664F-968D-99B8C4DB53E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F150FEA-1D73-CF4A-9F8E-A90E3934615B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1971" uniqueCount="1159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="1162">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3503,6 +3503,15 @@
   </si>
   <si>
     <t>Ben Sasse is a boss. His argument: focus on the what unites us above (civics) and upstream (culture) of politics, and build strong communities.</t>
+  </si>
+  <si>
+    <t>How to Get Started in Real Estate</t>
+  </si>
+  <si>
+    <t>Robert Irwin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I listened to this quickly to increase my familiarity with real estate investing terms and topics. It is a broad overview without much detail but outlines some additional topics to learn about. </t>
   </si>
 </sst>
 </file>
@@ -5055,7 +5064,7 @@
   <dimension ref="A1:H1173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A579" workbookViewId="0">
-      <selection activeCell="A594" sqref="A594"/>
+      <selection activeCell="A595" sqref="A595"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15935,10 +15944,30 @@
       </c>
     </row>
     <row r="594" spans="1:8">
-      <c r="D594" s="9"/>
-      <c r="E594" s="9"/>
-      <c r="F594" s="9"/>
-      <c r="G594" s="9"/>
+      <c r="A594" s="6" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B594" s="6" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C594" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D594" s="9">
+        <v>2018</v>
+      </c>
+      <c r="E594" s="9">
+        <v>2008</v>
+      </c>
+      <c r="F594" s="9">
+        <v>100</v>
+      </c>
+      <c r="G594" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="H594" s="6" t="s">
+        <v>1161</v>
+      </c>
     </row>
     <row r="595" spans="1:8">
       <c r="D595" s="9"/>

</xml_diff>

<commit_message>
Secrets of the Millionaire Mind
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F150FEA-1D73-CF4A-9F8E-A90E3934615B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
     <sheet name="Pivot" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="1162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="1165">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3512,13 +3506,22 @@
   </si>
   <si>
     <t xml:space="preserve">I listened to this quickly to increase my familiarity with real estate investing terms and topics. It is a broad overview without much detail but outlines some additional topics to learn about. </t>
+  </si>
+  <si>
+    <t>Secrets of the Millionaire Mind: Mastering the Inner Game of Wealth</t>
+  </si>
+  <si>
+    <t>T. Harv Eker</t>
+  </si>
+  <si>
+    <t>This book was recommended in The Miracle Morning and naturally had a similar "self-helpy" feel. But his rules for understanding and emulating how rich people think are helpful.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4807,7 +4810,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -4859,7 +4862,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -5053,21 +5056,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A579" workbookViewId="0">
-      <selection activeCell="A595" sqref="A595"/>
+      <selection activeCell="A596" sqref="A596"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="98" style="6" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="6" customWidth="1"/>
@@ -15970,10 +15973,30 @@
       </c>
     </row>
     <row r="595" spans="1:8">
-      <c r="D595" s="9"/>
-      <c r="E595" s="9"/>
-      <c r="F595" s="9"/>
-      <c r="G595" s="9"/>
+      <c r="A595" s="6" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B595" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C595" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D595" s="9">
+        <v>2018</v>
+      </c>
+      <c r="E595" s="9">
+        <v>2005</v>
+      </c>
+      <c r="F595" s="9">
+        <v>210</v>
+      </c>
+      <c r="G595" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="H595" s="6" t="s">
+        <v>1164</v>
+      </c>
     </row>
     <row r="596" spans="1:8">
       <c r="D596" s="9"/>
@@ -19455,12 +19478,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Barking up the wrong tree
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C019933-0195-2C4E-A51C-CCA2155D08C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
     <sheet name="Pivot" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -3520,8 +3526,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5056,21 +5062,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A579" workbookViewId="0">
       <selection activeCell="A596" sqref="A596"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="98" style="6" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="6" customWidth="1"/>
@@ -15888,7 +15894,7 @@
         <v>320</v>
       </c>
       <c r="G591" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H591" s="6" t="s">
         <v>1153</v>
@@ -19478,12 +19484,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Loopholes of Real Estate
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FC4DEB-0B3E-F841-A0A3-EC62938E87AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677B84D4-DD85-7C4A-BEA8-079A4255A34A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="440" windowWidth="25360" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2006" uniqueCount="1178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2011" uniqueCount="1181">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3560,6 +3560,15 @@
   </si>
   <si>
     <t>While many aspects of Trump's character and behavior are deeply concerning, I don't think he is a tyrant in a similar way as the tyrants of the 20th Century Snyder compares him to. Nevertheless, this is a short and thought-provoking look at what we can actively do to secure liberty and learn from the horrific events of the 20th Century.</t>
+  </si>
+  <si>
+    <t>Loopholes of Real Estate</t>
+  </si>
+  <si>
+    <t>Garrett Sutton</t>
+  </si>
+  <si>
+    <t>A great overview of many aspects of real estate taxes and legal considerations, presented with helpful case studies. I will definitely be reffering back to this often. I came across this when litsening to a podcast on 1031 exchanges.</t>
   </si>
 </sst>
 </file>
@@ -4855,7 +4864,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -4907,7 +4916,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -5112,7 +5121,7 @@
   <dimension ref="A1:H1173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A576" workbookViewId="0">
-      <selection activeCell="A601" sqref="A601"/>
+      <selection activeCell="A602" sqref="A602"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -16174,10 +16183,30 @@
       </c>
     </row>
     <row r="601" spans="1:8">
-      <c r="D601" s="9"/>
-      <c r="E601" s="9"/>
-      <c r="F601" s="9"/>
-      <c r="G601" s="9"/>
+      <c r="A601" s="6" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B601" s="6" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C601" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D601" s="9">
+        <v>2018</v>
+      </c>
+      <c r="E601" s="9">
+        <v>2013</v>
+      </c>
+      <c r="F601" s="9">
+        <v>352</v>
+      </c>
+      <c r="G601" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="H601" s="6" t="s">
+        <v>1180</v>
+      </c>
     </row>
     <row r="602" spans="1:8">
       <c r="D602" s="9"/>

</xml_diff>

<commit_message>
Barking to the Choir
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4987576-C914-ED42-BBE1-67FE060E86FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379629D4-85DD-6B45-809A-E2AFFE0C43C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="1182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="1185">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3572,6 +3572,15 @@
   </si>
   <si>
     <t>I read this in preparation for beginning spiritual direction again. A wonderful guide to examining and growing in your spiritual life.</t>
+  </si>
+  <si>
+    <t>Barking to the Choir: The Power of Radical Kinship</t>
+  </si>
+  <si>
+    <t>Gregory Boyle</t>
+  </si>
+  <si>
+    <t>With Fr. Greg Boyle's books it is best to listen to them. He is a wonderful storyteller and his message of simple love is beautiful.</t>
   </si>
 </sst>
 </file>
@@ -5124,7 +5133,7 @@
   <dimension ref="A1:H1173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A576" workbookViewId="0">
-      <selection activeCell="A603" sqref="A603"/>
+      <selection activeCell="A604" sqref="A604"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -16238,10 +16247,30 @@
       </c>
     </row>
     <row r="603" spans="1:8">
-      <c r="D603" s="9"/>
-      <c r="E603" s="9"/>
-      <c r="F603" s="9"/>
-      <c r="G603" s="9"/>
+      <c r="A603" s="6" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B603" s="6" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C603" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D603" s="9">
+        <v>2018</v>
+      </c>
+      <c r="E603" s="9">
+        <v>2017</v>
+      </c>
+      <c r="F603" s="9">
+        <v>224</v>
+      </c>
+      <c r="G603" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="H603" s="6" t="s">
+        <v>1184</v>
+      </c>
     </row>
     <row r="604" spans="1:8">
       <c r="D604" s="9"/>

</xml_diff>

<commit_message>
Start Your Own Corporation
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCE249D-06C8-674B-A9E2-612D1633089B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92E474C-E857-6345-8EC1-64A61F11DD5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="1187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="1190">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3587,6 +3587,15 @@
   </si>
   <si>
     <t>Mark Owen</t>
+  </si>
+  <si>
+    <t>Start Your Own Corporation: Why the Rich Own Their Own Companies and Everyone Else Works for Them</t>
+  </si>
+  <si>
+    <t>Apparently the author was forced to pay back the over $6m he received in royalties for writing this book. It was an interesting view into the life of a Navy Seal and the mission to kill Bin Laden.</t>
+  </si>
+  <si>
+    <t>This was a helpful book with great information to familiarize yourself with the reasons to form a corporate entity and advantages of the options.</t>
   </si>
 </sst>
 </file>
@@ -5139,7 +5148,7 @@
   <dimension ref="A1:H1173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A576" workbookViewId="0">
-      <selection activeCell="H604" sqref="H604"/>
+      <selection activeCell="A606" sqref="A606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -16300,12 +16309,35 @@
       <c r="G604" s="9" t="s">
         <v>241</v>
       </c>
+      <c r="H604" s="6" t="s">
+        <v>1188</v>
+      </c>
     </row>
     <row r="605" spans="1:8">
-      <c r="D605" s="9"/>
-      <c r="E605" s="9"/>
-      <c r="F605" s="9"/>
-      <c r="G605" s="9"/>
+      <c r="A605" s="6" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B605" s="6" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C605" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D605" s="9">
+        <v>2018</v>
+      </c>
+      <c r="E605" s="9">
+        <v>2001</v>
+      </c>
+      <c r="F605" s="9">
+        <v>250</v>
+      </c>
+      <c r="G605" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="H605" s="6" t="s">
+        <v>1189</v>
+      </c>
     </row>
     <row r="606" spans="1:8">
       <c r="D606" s="9"/>

</xml_diff>

<commit_message>
No Hero and Measure What Matters
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299A251C-F6EB-D648-8962-688552F7F7F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2058F42-38D5-924B-AD09-6D3859E60CEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2039" uniqueCount="1194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="1198">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3608,6 +3608,18 @@
   </si>
   <si>
     <t>Simcha Fisher</t>
+  </si>
+  <si>
+    <t>No Hero: The Evolution of a Navy Seal</t>
+  </si>
+  <si>
+    <t>This book is all about OKR's (objectives and key results), structured goal setting, continuous performance review, and how tech companies like Intel and Google have used them to great effect. As with most pop business books there is plenty of fluff and people taking themselves way too seriously—including the discussion of robotic pizzas—but the concept of structured goal setting is helpful and well-described.</t>
+  </si>
+  <si>
+    <t>This is a quick and easy read talking about the real-life challenges of practicing NFP.</t>
+  </si>
+  <si>
+    <t>This is Owen's second book and tells stories about his time as a Navy Seal while relating the lessons he learned to everday life. The most striking to me was to "stay in your 3-foot bubble" or to only focus on those things you can control and prioritize how you deal with them.</t>
   </si>
 </sst>
 </file>
@@ -5160,7 +5172,7 @@
   <dimension ref="A1:H1173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A576" workbookViewId="0">
-      <selection activeCell="A608" sqref="A608"/>
+      <selection activeCell="A609" sqref="A609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -16371,7 +16383,10 @@
         <v>320</v>
       </c>
       <c r="G606" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
+      </c>
+      <c r="H606" s="6" t="s">
+        <v>1195</v>
       </c>
     </row>
     <row r="607" spans="1:8">
@@ -16396,12 +16411,35 @@
       <c r="G607" s="9" t="s">
         <v>241</v>
       </c>
+      <c r="H607" s="6" t="s">
+        <v>1196</v>
+      </c>
     </row>
     <row r="608" spans="1:8">
-      <c r="D608" s="9"/>
-      <c r="E608" s="9"/>
-      <c r="F608" s="9"/>
-      <c r="G608" s="9"/>
+      <c r="A608" s="6" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B608" s="6" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C608" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D608" s="9">
+        <v>2018</v>
+      </c>
+      <c r="E608" s="9">
+        <v>2015</v>
+      </c>
+      <c r="F608" s="9">
+        <v>304</v>
+      </c>
+      <c r="G608" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="H608" s="6" t="s">
+        <v>1197</v>
+      </c>
     </row>
     <row r="609" spans="4:7">
       <c r="D609" s="9"/>

</xml_diff>

<commit_message>
Thomas Aquinas in 90 Minutes
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C77B84-66BD-614B-9439-7DC8CBF3FF0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A802BF-C31C-474A-8CE7-B733DE8B9D2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2068" uniqueCount="1211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2073" uniqueCount="1214">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3658,6 +3658,15 @@
   </si>
   <si>
     <t>It's crazy that this was my first time reading Thomas, and Kreeft does a great job introducing him, explaining him, and centextualizing his work for the modern reader. He has a deep love and respect for Aquinas which comes through in his thorough explanations. Reading Aquinas is beautiful.</t>
+  </si>
+  <si>
+    <t>Thomas Aquinas in 90 Minutes</t>
+  </si>
+  <si>
+    <t>Paul Strathern</t>
+  </si>
+  <si>
+    <t>Strathern is not a big Aquinas fan which comes through (he should be "swept away like cobwebs"), but he has to admit the huge impact he had and the weight of his thinking. This was interesting background on the context of Aquinas.</t>
   </si>
 </sst>
 </file>
@@ -5213,7 +5222,7 @@
   <dimension ref="A1:H1173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A605" workbookViewId="0">
-      <selection activeCell="E616" sqref="E616"/>
+      <selection activeCell="A616" sqref="A616"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -16653,12 +16662,30 @@
       </c>
     </row>
     <row r="616" spans="1:8">
+      <c r="A616" s="3" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B616" s="3" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C616" s="3" t="s">
+        <v>201</v>
+      </c>
       <c r="D616" s="6">
         <v>2019</v>
       </c>
-      <c r="E616" s="6"/>
-      <c r="F616" s="6"/>
-      <c r="G616" s="6"/>
+      <c r="E616" s="6">
+        <v>1998</v>
+      </c>
+      <c r="F616" s="6">
+        <v>88</v>
+      </c>
+      <c r="G616" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H616" s="3" t="s">
+        <v>1213</v>
+      </c>
     </row>
     <row r="617" spans="1:8">
       <c r="D617" s="6"/>

</xml_diff>

<commit_message>
A Tale of Two Cities
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A697AC-9274-054E-B33B-D58E0E9803DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterate="1" iterateCount="20"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2078" uniqueCount="1217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="1220">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3381,9 +3387,6 @@
     <t>Since I got into a bit of a Tolkien kick by reading the Hobbit, I decided to listen to this. It is full of great wisdom culled from Tolkien's works, focusing on living the simple life of the Shire.</t>
   </si>
   <si>
-    <t>This was our first book for our "Classics" book group. It makes you think: about tyrrany, free speech, and being educated as a citizen.</t>
-  </si>
-  <si>
     <t>I started reading this to Henry while he was still in the womb and we finished it just before he turned 2 months! Always a beautiful read.</t>
   </si>
   <si>
@@ -3441,9 +3444,6 @@
     <t>This is a quick read and a beautiful reflection on living simply and living the ordinary life well. She ends each chapter with helpful practical tips.</t>
   </si>
   <si>
-    <t xml:space="preserve">We read this for our classics book group and while a little slow to get started I really enjoyed the story. I wish people still spoke like this! </t>
-  </si>
-  <si>
     <t>The Vatican Diaries: A Behind-the-Scenes Look at the Power, Personalities, and Politics at the Heart of the Catholic Church</t>
   </si>
   <si>
@@ -3456,9 +3456,6 @@
     <t>I read this after Jordan and appreciated her notes. One very insightful thing Sperry mentions is how clutter in our lives if often the symptom of sin, and in fixing the clutter we need to dig down to the root of the sin.</t>
   </si>
   <si>
-    <t>We read this for our classics book club (that no one came to). It is a tragic tale but a lesson about priorities and the ability of money to ruin your lives, and a reminder to be grateful for what we have.</t>
-  </si>
-  <si>
     <t>Barking Up the Wrong Tree: The Surprising Science Behind Why Everything You Know About Success Is (Mostly) Wrong</t>
   </si>
   <si>
@@ -3670,13 +3667,31 @@
   </si>
   <si>
     <t>This is the modern IT version of *The Goal*, an entertaining read, and an insightful look at how to do DevOps properly to help the business succeed. I only wish I worked on a team big enough to employ these principles.</t>
+  </si>
+  <si>
+    <t>A Tale of Two Cities</t>
+  </si>
+  <si>
+    <t>Charles Dickens</t>
+  </si>
+  <si>
+    <t>BC1: This was our first book for our "Classics" book group. It makes you think: about tyrrany, free speech, and being educated as a citizen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BC2: We read this for our classics book group and while a little slow to get started I really enjoyed the story. I wish people still spoke like this! </t>
+  </si>
+  <si>
+    <t>BC3: We read this for our classics book club (that no one came to). It is a tragic tale but a lesson about priorities and the ability of money to ruin your lives, and a reminder to be grateful for what we have.</t>
+  </si>
+  <si>
+    <t>BC4: This was a struggle to get through but a beautiful story of love, resurrection, and sacrifice. The language is beautiful, the French Revolution is repulsive, and my difficulty with it points to the distraction of my mind and our age. We had a wonderful disucssion with Mrs. Russell, Ben and Johanna, Terry and Kate, Ashley, and Adam!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4968,7 +4983,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -5020,7 +5035,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -5214,21 +5229,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A605" workbookViewId="0">
-      <selection activeCell="A618" sqref="A618"/>
+    <sheetView tabSelected="1" topLeftCell="A598" workbookViewId="0">
+      <selection activeCell="A619" sqref="A619"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="98" style="3" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="3" customWidth="1"/>
@@ -8541,7 +8556,7 @@
     </row>
     <row r="204" spans="1:6">
       <c r="A204" s="3" t="s">
-        <v>1176</v>
+        <v>1173</v>
       </c>
       <c r="B204" s="3" t="s">
         <v>739</v>
@@ -10661,7 +10676,7 @@
     </row>
     <row r="338" spans="1:6">
       <c r="A338" s="3" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="B338" s="3" t="s">
         <v>830</v>
@@ -12763,7 +12778,7 @@
     </row>
     <row r="455" spans="1:6">
       <c r="A455" s="3" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="B455" s="3" t="s">
         <v>153</v>
@@ -15711,7 +15726,7 @@
         <v>239</v>
       </c>
       <c r="H578" s="3" t="s">
-        <v>1120</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="579" spans="1:8">
@@ -15815,15 +15830,15 @@
         <v>239</v>
       </c>
       <c r="H582" s="3" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="583" spans="1:8">
       <c r="A583" s="3" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B583" s="3" t="s">
         <v>1122</v>
-      </c>
-      <c r="B583" s="3" t="s">
-        <v>1123</v>
       </c>
       <c r="C583" s="3" t="s">
         <v>200</v>
@@ -15841,15 +15856,15 @@
         <v>239</v>
       </c>
       <c r="H583" s="3" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="584" spans="1:8">
       <c r="A584" s="3" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B584" s="3" t="s">
         <v>1125</v>
-      </c>
-      <c r="B584" s="3" t="s">
-        <v>1126</v>
       </c>
       <c r="C584" s="3" t="s">
         <v>199</v>
@@ -15867,15 +15882,15 @@
         <v>237</v>
       </c>
       <c r="H584" s="3" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="585" spans="1:8">
       <c r="A585" s="3" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B585" s="3" t="s">
         <v>1128</v>
-      </c>
-      <c r="B585" s="3" t="s">
-        <v>1129</v>
       </c>
       <c r="C585" s="3" t="s">
         <v>200</v>
@@ -15893,15 +15908,15 @@
         <v>239</v>
       </c>
       <c r="H585" s="3" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="586" spans="1:8">
       <c r="A586" s="3" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B586" s="3" t="s">
         <v>1130</v>
-      </c>
-      <c r="B586" s="3" t="s">
-        <v>1131</v>
       </c>
       <c r="C586" s="3" t="s">
         <v>199</v>
@@ -15919,15 +15934,15 @@
         <v>237</v>
       </c>
       <c r="H586" s="3" t="s">
-        <v>1140</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="587" spans="1:8">
       <c r="A587" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B587" s="3" t="s">
         <v>1132</v>
-      </c>
-      <c r="B587" s="3" t="s">
-        <v>1133</v>
       </c>
       <c r="C587" s="3" t="s">
         <v>200</v>
@@ -15945,15 +15960,15 @@
         <v>239</v>
       </c>
       <c r="H587" s="3" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="588" spans="1:8">
       <c r="A588" s="3" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B588" s="3" t="s">
         <v>1137</v>
-      </c>
-      <c r="B588" s="3" t="s">
-        <v>1138</v>
       </c>
       <c r="C588" s="3" t="s">
         <v>199</v>
@@ -15971,15 +15986,15 @@
         <v>239</v>
       </c>
       <c r="H588" s="3" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="589" spans="1:8">
       <c r="A589" s="3" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="C589" s="3" t="s">
         <v>201</v>
@@ -15997,7 +16012,7 @@
         <v>237</v>
       </c>
       <c r="H589" s="3" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="590" spans="1:8">
@@ -16023,15 +16038,15 @@
         <v>239</v>
       </c>
       <c r="H590" s="3" t="s">
-        <v>1145</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="591" spans="1:8">
       <c r="A591" s="3" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
       <c r="B591" s="3" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="C591" s="3" t="s">
         <v>200</v>
@@ -16049,15 +16064,15 @@
         <v>237</v>
       </c>
       <c r="H591" s="3" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="592" spans="1:8">
       <c r="A592" s="3" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="B592" s="3" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
       <c r="C592" s="3" t="s">
         <v>201</v>
@@ -16075,12 +16090,12 @@
         <v>237</v>
       </c>
       <c r="H592" s="3" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="593" spans="1:8">
       <c r="A593" s="3" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
       <c r="B593" s="3" t="s">
         <v>179</v>
@@ -16101,15 +16116,15 @@
         <v>237</v>
       </c>
       <c r="H593" s="3" t="s">
-        <v>1153</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="594" spans="1:8">
       <c r="A594" s="3" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="B594" s="3" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="C594" s="3" t="s">
         <v>200</v>
@@ -16127,15 +16142,15 @@
         <v>239</v>
       </c>
       <c r="H594" s="3" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="595" spans="1:8">
       <c r="A595" s="3" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="B595" s="3" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="C595" s="3" t="s">
         <v>200</v>
@@ -16153,7 +16168,7 @@
         <v>237</v>
       </c>
       <c r="H595" s="3" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="596" spans="1:8">
@@ -16179,15 +16194,15 @@
         <v>239</v>
       </c>
       <c r="H596" s="3" t="s">
-        <v>1162</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="597" spans="1:8">
       <c r="A597" s="3" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
       <c r="B597" s="3" t="s">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="C597" s="3" t="s">
         <v>200</v>
@@ -16205,15 +16220,15 @@
         <v>239</v>
       </c>
       <c r="H597" s="3" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="598" spans="1:8">
       <c r="A598" s="3" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="B598" s="3" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="C598" s="3" t="s">
         <v>201</v>
@@ -16231,15 +16246,15 @@
         <v>237</v>
       </c>
       <c r="H598" s="3" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="599" spans="1:8">
       <c r="A599" s="3" t="s">
-        <v>1167</v>
+        <v>1164</v>
       </c>
       <c r="B599" s="3" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
       <c r="C599" s="3" t="s">
         <v>201</v>
@@ -16257,15 +16272,15 @@
         <v>237</v>
       </c>
       <c r="H599" s="3" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="600" spans="1:8">
       <c r="A600" s="3" t="s">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="B600" s="3" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="C600" s="3" t="s">
         <v>200</v>
@@ -16283,15 +16298,15 @@
         <v>237</v>
       </c>
       <c r="H600" s="3" t="s">
-        <v>1172</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="601" spans="1:8">
       <c r="A601" s="3" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
       <c r="B601" s="3" t="s">
-        <v>1174</v>
+        <v>1171</v>
       </c>
       <c r="C601" s="3" t="s">
         <v>199</v>
@@ -16309,12 +16324,12 @@
         <v>239</v>
       </c>
       <c r="H601" s="3" t="s">
-        <v>1175</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="602" spans="1:8">
       <c r="A602" s="3" t="s">
-        <v>1176</v>
+        <v>1173</v>
       </c>
       <c r="B602" s="3" t="s">
         <v>739</v>
@@ -16335,15 +16350,15 @@
         <v>239</v>
       </c>
       <c r="H602" s="3" t="s">
-        <v>1177</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="603" spans="1:8">
       <c r="A603" s="3" t="s">
-        <v>1178</v>
+        <v>1175</v>
       </c>
       <c r="B603" s="3" t="s">
-        <v>1179</v>
+        <v>1176</v>
       </c>
       <c r="C603" s="3" t="s">
         <v>200</v>
@@ -16361,15 +16376,15 @@
         <v>239</v>
       </c>
       <c r="H603" s="3" t="s">
-        <v>1180</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="604" spans="1:8">
       <c r="A604" s="3" t="s">
-        <v>1181</v>
+        <v>1178</v>
       </c>
       <c r="B604" s="3" t="s">
-        <v>1182</v>
+        <v>1179</v>
       </c>
       <c r="C604" s="3" t="s">
         <v>200</v>
@@ -16387,15 +16402,15 @@
         <v>239</v>
       </c>
       <c r="H604" s="3" t="s">
-        <v>1184</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="605" spans="1:8">
       <c r="A605" s="3" t="s">
-        <v>1183</v>
+        <v>1180</v>
       </c>
       <c r="B605" s="3" t="s">
-        <v>1174</v>
+        <v>1171</v>
       </c>
       <c r="C605" s="3" t="s">
         <v>201</v>
@@ -16413,15 +16428,15 @@
         <v>237</v>
       </c>
       <c r="H605" s="3" t="s">
-        <v>1185</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="606" spans="1:8">
       <c r="A606" s="3" t="s">
-        <v>1186</v>
+        <v>1183</v>
       </c>
       <c r="B606" s="3" t="s">
-        <v>1187</v>
+        <v>1184</v>
       </c>
       <c r="C606" s="3" t="s">
         <v>200</v>
@@ -16439,15 +16454,15 @@
         <v>237</v>
       </c>
       <c r="H606" s="3" t="s">
-        <v>1191</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="607" spans="1:8">
       <c r="A607" s="3" t="s">
-        <v>1188</v>
+        <v>1185</v>
       </c>
       <c r="B607" s="3" t="s">
-        <v>1189</v>
+        <v>1186</v>
       </c>
       <c r="C607" s="3" t="s">
         <v>199</v>
@@ -16465,15 +16480,15 @@
         <v>239</v>
       </c>
       <c r="H607" s="3" t="s">
-        <v>1192</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="608" spans="1:8">
       <c r="A608" s="3" t="s">
-        <v>1190</v>
+        <v>1187</v>
       </c>
       <c r="B608" s="3" t="s">
-        <v>1182</v>
+        <v>1179</v>
       </c>
       <c r="C608" s="3" t="s">
         <v>200</v>
@@ -16491,15 +16506,15 @@
         <v>239</v>
       </c>
       <c r="H608" s="3" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="609" spans="1:8">
       <c r="A609" s="3" t="s">
-        <v>1194</v>
+        <v>1191</v>
       </c>
       <c r="B609" s="3" t="s">
-        <v>1195</v>
+        <v>1192</v>
       </c>
       <c r="C609" s="3" t="s">
         <v>201</v>
@@ -16517,15 +16532,15 @@
         <v>239</v>
       </c>
       <c r="H609" s="3" t="s">
-        <v>1196</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="610" spans="1:8">
       <c r="A610" s="3" t="s">
-        <v>1197</v>
+        <v>1194</v>
       </c>
       <c r="B610" s="3" t="s">
-        <v>1198</v>
+        <v>1195</v>
       </c>
       <c r="C610" s="3" t="s">
         <v>200</v>
@@ -16543,15 +16558,15 @@
         <v>239</v>
       </c>
       <c r="H610" s="3" t="s">
-        <v>1199</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="611" spans="1:8">
       <c r="A611" s="3" t="s">
-        <v>1202</v>
+        <v>1199</v>
       </c>
       <c r="B611" s="3" t="s">
-        <v>1200</v>
+        <v>1197</v>
       </c>
       <c r="C611" s="3" t="s">
         <v>201</v>
@@ -16569,12 +16584,12 @@
         <v>237</v>
       </c>
       <c r="H611" s="3" t="s">
-        <v>1201</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="612" spans="1:8">
       <c r="A612" s="3" t="s">
-        <v>1203</v>
+        <v>1200</v>
       </c>
       <c r="C612" s="3" t="s">
         <v>199</v>
@@ -16588,7 +16603,7 @@
     </row>
     <row r="613" spans="1:8">
       <c r="A613" s="4" t="s">
-        <v>1206</v>
+        <v>1203</v>
       </c>
       <c r="B613" s="4" t="s">
         <v>144</v>
@@ -16609,15 +16624,15 @@
         <v>237</v>
       </c>
       <c r="H613" s="4" t="s">
-        <v>1207</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="614" spans="1:8">
       <c r="A614" s="3" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
       <c r="B614" s="3" t="s">
-        <v>1205</v>
+        <v>1202</v>
       </c>
       <c r="C614" s="3" t="s">
         <v>201</v>
@@ -16635,12 +16650,12 @@
         <v>237</v>
       </c>
       <c r="H614" s="3" t="s">
-        <v>1208</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="615" spans="1:8">
       <c r="A615" s="3" t="s">
-        <v>1209</v>
+        <v>1206</v>
       </c>
       <c r="B615" s="3" t="s">
         <v>748</v>
@@ -16661,15 +16676,15 @@
         <v>237</v>
       </c>
       <c r="H615" s="3" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="616" spans="1:8">
       <c r="A616" s="3" t="s">
-        <v>1211</v>
+        <v>1208</v>
       </c>
       <c r="B616" s="3" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="C616" s="3" t="s">
         <v>201</v>
@@ -16687,15 +16702,15 @@
         <v>237</v>
       </c>
       <c r="H616" s="3" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="617" spans="1:8">
       <c r="A617" s="3" t="s">
-        <v>1214</v>
+        <v>1211</v>
       </c>
       <c r="B617" s="3" t="s">
-        <v>1215</v>
+        <v>1212</v>
       </c>
       <c r="C617" s="3" t="s">
         <v>201</v>
@@ -16713,71 +16728,111 @@
         <v>237</v>
       </c>
       <c r="H617" s="3" t="s">
-        <v>1216</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="618" spans="1:8">
-      <c r="D618" s="6"/>
-      <c r="E618" s="6"/>
-      <c r="F618" s="6"/>
-      <c r="G618" s="6"/>
+      <c r="A618" s="3" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B618" s="3" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C618" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D618" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E618" s="6">
+        <v>1859</v>
+      </c>
+      <c r="F618" s="6">
+        <v>341</v>
+      </c>
+      <c r="G618" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H618" s="3" t="s">
+        <v>1219</v>
+      </c>
     </row>
     <row r="619" spans="1:8">
-      <c r="D619" s="6"/>
+      <c r="D619" s="6">
+        <v>2019</v>
+      </c>
       <c r="E619" s="6"/>
       <c r="F619" s="6"/>
       <c r="G619" s="6"/>
     </row>
     <row r="620" spans="1:8">
-      <c r="D620" s="6"/>
+      <c r="D620" s="6">
+        <v>2019</v>
+      </c>
       <c r="E620" s="6"/>
       <c r="F620" s="6"/>
       <c r="G620" s="6"/>
     </row>
     <row r="621" spans="1:8">
-      <c r="D621" s="6"/>
+      <c r="D621" s="6">
+        <v>2019</v>
+      </c>
       <c r="E621" s="6"/>
       <c r="F621" s="6"/>
       <c r="G621" s="6"/>
     </row>
     <row r="622" spans="1:8">
-      <c r="D622" s="6"/>
+      <c r="D622" s="6">
+        <v>2019</v>
+      </c>
       <c r="E622" s="6"/>
       <c r="F622" s="6"/>
       <c r="G622" s="6"/>
     </row>
     <row r="623" spans="1:8">
-      <c r="D623" s="6"/>
+      <c r="D623" s="6">
+        <v>2019</v>
+      </c>
       <c r="E623" s="6"/>
       <c r="F623" s="6"/>
       <c r="G623" s="6"/>
     </row>
     <row r="624" spans="1:8">
-      <c r="D624" s="6"/>
+      <c r="D624" s="6">
+        <v>2019</v>
+      </c>
       <c r="E624" s="6"/>
       <c r="F624" s="6"/>
       <c r="G624" s="6"/>
     </row>
     <row r="625" spans="4:7">
-      <c r="D625" s="6"/>
+      <c r="D625" s="6">
+        <v>2019</v>
+      </c>
       <c r="E625" s="6"/>
       <c r="F625" s="6"/>
       <c r="G625" s="6"/>
     </row>
     <row r="626" spans="4:7">
-      <c r="D626" s="6"/>
+      <c r="D626" s="6">
+        <v>2019</v>
+      </c>
       <c r="E626" s="6"/>
       <c r="F626" s="6"/>
       <c r="G626" s="6"/>
     </row>
     <row r="627" spans="4:7">
-      <c r="D627" s="6"/>
+      <c r="D627" s="6">
+        <v>2019</v>
+      </c>
       <c r="E627" s="6"/>
       <c r="F627" s="6"/>
       <c r="G627" s="6"/>
     </row>
     <row r="628" spans="4:7">
-      <c r="D628" s="6"/>
+      <c r="D628" s="6">
+        <v>2019</v>
+      </c>
       <c r="E628" s="6"/>
       <c r="F628" s="6"/>
       <c r="G628" s="6"/>

</xml_diff>

<commit_message>
How to Be Invisible and The Art of Invisibility
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A697AC-9274-054E-B33B-D58E0E9803DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" iterate="1" iterateCount="20"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="1220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="1226">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3685,13 +3679,31 @@
   </si>
   <si>
     <t>BC4: This was a struggle to get through but a beautiful story of love, resurrection, and sacrifice. The language is beautiful, the French Revolution is repulsive, and my difficulty with it points to the distraction of my mind and our age. We had a wonderful disucssion with Mrs. Russell, Ben and Johanna, Terry and Kate, Ashley, and Adam!</t>
+  </si>
+  <si>
+    <t>How to Be Invisible: Protect Your Home, Your Children, Your Assets, and Your Life</t>
+  </si>
+  <si>
+    <t>J. J. Luna</t>
+  </si>
+  <si>
+    <t>The Art of Invisibility: The World's Most Famous Hacker Teaches You How to Be Safe in the Age of Big Brother and Big Data</t>
+  </si>
+  <si>
+    <t>Kevin Mitnick</t>
+  </si>
+  <si>
+    <t>Apparently Tommy Thompson (the trasure hunting fugitive) was found with this book when he was arrested after evading authorities for many years. I found it to be scary, intriguing, and interesting. I don't plan to follow all of the recommendations but it has heightened my sensitivity to sharing information and I plan to be more careful moving forward.</t>
+  </si>
+  <si>
+    <t>This was a scary but informative overview of how to be better about keeping on top of your information, especially online.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4983,7 +4995,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -5035,7 +5047,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -5229,21 +5241,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A598" workbookViewId="0">
-      <selection activeCell="A619" sqref="A619"/>
+      <selection activeCell="E621" sqref="E621"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="98" style="3" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="3" customWidth="1"/>
@@ -16758,20 +16770,56 @@
       </c>
     </row>
     <row r="619" spans="1:8">
+      <c r="A619" s="3" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B619" s="3" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C619" s="3" t="s">
+        <v>200</v>
+      </c>
       <c r="D619" s="6">
         <v>2019</v>
       </c>
-      <c r="E619" s="6"/>
-      <c r="F619" s="6"/>
-      <c r="G619" s="6"/>
+      <c r="E619" s="6">
+        <v>2017</v>
+      </c>
+      <c r="F619" s="6">
+        <v>279</v>
+      </c>
+      <c r="G619" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H619" s="3" t="s">
+        <v>1225</v>
+      </c>
     </row>
     <row r="620" spans="1:8">
+      <c r="A620" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B620" s="3" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C620" s="3" t="s">
+        <v>201</v>
+      </c>
       <c r="D620" s="6">
         <v>2019</v>
       </c>
-      <c r="E620" s="6"/>
-      <c r="F620" s="6"/>
-      <c r="G620" s="6"/>
+      <c r="E620" s="6">
+        <v>2012</v>
+      </c>
+      <c r="F620" s="6">
+        <v>294</v>
+      </c>
+      <c r="G620" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H620" s="3" t="s">
+        <v>1224</v>
+      </c>
     </row>
     <row r="621" spans="1:8">
       <c r="D621" s="6">

</xml_diff>

<commit_message>
Men In Green Faces
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21628FD2-7AA7-6042-A7CD-30F512A6E45B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
+    <workbookView xWindow="8180" yWindow="1780" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="1226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2103" uniqueCount="1232">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3697,13 +3703,31 @@
   </si>
   <si>
     <t>This was a scary but informative overview of how to be better about keeping on top of your information, especially online.</t>
+  </si>
+  <si>
+    <t>The Woman Who Smashed Codes: A True Story of Love, Spies, and the Unlikely Heroine Who Outwitted America's Enemies</t>
+  </si>
+  <si>
+    <t>Jason Fagone</t>
+  </si>
+  <si>
+    <t>Austin got me this book for Christmas and it was super interesting, about the life of Elizabeth Friedman who ran the US Coast Guard's first code-breaking unit and who, with her husband, contributed greatly to the WWII effort and the establishment of the US intelligence community as we know it today.</t>
+  </si>
+  <si>
+    <t>Men in Green Faces: A Novel of U.S. Navy SEALs</t>
+  </si>
+  <si>
+    <t>Gene Wentz</t>
+  </si>
+  <si>
+    <t>Mark Owen referenced this in his book as inspiring him to become a Navy SEAL. This book is powerful, showing not just the horror of war in a gut-wrenching way, but also the love of a man for his family and comrades.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5241,21 +5265,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1173"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A598" workbookViewId="0">
-      <selection activeCell="E621" sqref="E621"/>
+      <selection activeCell="A623" sqref="A623"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="98" style="3" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="3" customWidth="1"/>
@@ -16771,10 +16795,10 @@
     </row>
     <row r="619" spans="1:8">
       <c r="A619" s="3" t="s">
-        <v>1222</v>
+        <v>1226</v>
       </c>
       <c r="B619" s="3" t="s">
-        <v>1223</v>
+        <v>1227</v>
       </c>
       <c r="C619" s="3" t="s">
         <v>200</v>
@@ -16786,56 +16810,92 @@
         <v>2017</v>
       </c>
       <c r="F619" s="6">
-        <v>279</v>
+        <v>345</v>
       </c>
       <c r="G619" s="6" t="s">
         <v>239</v>
       </c>
       <c r="H619" s="3" t="s">
-        <v>1225</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="620" spans="1:8">
       <c r="A620" s="3" t="s">
-        <v>1220</v>
+        <v>1222</v>
       </c>
       <c r="B620" s="3" t="s">
-        <v>1221</v>
+        <v>1223</v>
       </c>
       <c r="C620" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D620" s="6">
         <v>2019</v>
       </c>
       <c r="E620" s="6">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="F620" s="6">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="G620" s="6" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H620" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="621" spans="1:8">
+      <c r="A621" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B621" s="3" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C621" s="3" t="s">
+        <v>201</v>
+      </c>
       <c r="D621" s="6">
         <v>2019</v>
       </c>
-      <c r="E621" s="6"/>
-      <c r="F621" s="6"/>
-      <c r="G621" s="6"/>
+      <c r="E621" s="6">
+        <v>2012</v>
+      </c>
+      <c r="F621" s="6">
+        <v>294</v>
+      </c>
+      <c r="G621" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H621" s="3" t="s">
+        <v>1224</v>
+      </c>
     </row>
     <row r="622" spans="1:8">
+      <c r="A622" s="3" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B622" s="3" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C622" s="3" t="s">
+        <v>200</v>
+      </c>
       <c r="D622" s="6">
         <v>2019</v>
       </c>
-      <c r="E622" s="6"/>
-      <c r="F622" s="6"/>
-      <c r="G622" s="6"/>
+      <c r="E622" s="6">
+        <v>1992</v>
+      </c>
+      <c r="F622" s="6">
+        <v>304</v>
+      </c>
+      <c r="G622" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H622" s="3" t="s">
+        <v>1231</v>
+      </c>
     </row>
     <row r="623" spans="1:8">
       <c r="D623" s="6">
@@ -16886,13 +16946,17 @@
       <c r="G628" s="6"/>
     </row>
     <row r="629" spans="4:7">
-      <c r="D629" s="6"/>
+      <c r="D629" s="6">
+        <v>2019</v>
+      </c>
       <c r="E629" s="6"/>
       <c r="F629" s="6"/>
       <c r="G629" s="6"/>
     </row>
     <row r="630" spans="4:7">
-      <c r="D630" s="6"/>
+      <c r="D630" s="6">
+        <v>2019</v>
+      </c>
       <c r="E630" s="6"/>
       <c r="F630" s="6"/>
       <c r="G630" s="6"/>
@@ -20154,6 +20218,18 @@
       <c r="E1173" s="6"/>
       <c r="F1173" s="6"/>
       <c r="G1173" s="6"/>
+    </row>
+    <row r="1174" spans="4:7">
+      <c r="D1174" s="6"/>
+      <c r="E1174" s="6"/>
+      <c r="F1174" s="6"/>
+      <c r="G1174" s="6"/>
+    </row>
+    <row r="1175" spans="4:7">
+      <c r="D1175" s="6"/>
+      <c r="E1175" s="6"/>
+      <c r="F1175" s="6"/>
+      <c r="G1175" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Skunk Works and Fahrenheit 451
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21628FD2-7AA7-6042-A7CD-30F512A6E45B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8180" yWindow="1780" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2103" uniqueCount="1232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2112" uniqueCount="1235">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3721,13 +3715,22 @@
   </si>
   <si>
     <t>Mark Owen referenced this in his book as inspiring him to become a Navy SEAL. This book is powerful, showing not just the horror of war in a gut-wrenching way, but also the love of a man for his family and comrades.</t>
+  </si>
+  <si>
+    <t>Skunk Works: A Personal Memoir of My Years at Lockheed</t>
+  </si>
+  <si>
+    <t>Ben Rich</t>
+  </si>
+  <si>
+    <t>This was a fascenating exploration of Skunk Works (as a group and as a concept), portrait of Kelly Johnson, and history of US aviation development, filled with all kinds of interesting anectdotes and lessons for being lean in aerospace development.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5265,21 +5268,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A598" workbookViewId="0">
-      <selection activeCell="A623" sqref="A623"/>
+      <selection activeCell="A624" sqref="A624"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="98" style="3" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="3" customWidth="1"/>
@@ -16898,20 +16901,53 @@
       </c>
     </row>
     <row r="623" spans="1:8">
+      <c r="A623" s="3" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B623" s="3" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C623" s="3" t="s">
+        <v>200</v>
+      </c>
       <c r="D623" s="6">
         <v>2019</v>
       </c>
-      <c r="E623" s="6"/>
-      <c r="F623" s="6"/>
-      <c r="G623" s="6"/>
+      <c r="E623" s="6">
+        <v>1996</v>
+      </c>
+      <c r="F623" s="6">
+        <v>372</v>
+      </c>
+      <c r="G623" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H623" s="3" t="s">
+        <v>1234</v>
+      </c>
     </row>
     <row r="624" spans="1:8">
+      <c r="A624" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B624" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="C624" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D624" s="6">
         <v>2019</v>
       </c>
-      <c r="E624" s="6"/>
-      <c r="F624" s="6"/>
-      <c r="G624" s="6"/>
+      <c r="E624" s="6">
+        <v>1953</v>
+      </c>
+      <c r="F624" s="6">
+        <v>256</v>
+      </c>
+      <c r="G624" s="6" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="625" spans="4:7">
       <c r="D625" s="6">

</xml_diff>

<commit_message>
Catch Me If You Can
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2112" uniqueCount="1235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="1238">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3724,6 +3724,15 @@
   </si>
   <si>
     <t>This was a fascenating exploration of Skunk Works (as a group and as a concept), portrait of Kelly Johnson, and history of US aviation development, filled with all kinds of interesting anectdotes and lessons for being lean in aerospace development.</t>
+  </si>
+  <si>
+    <t>Catch Me If You Can: The True Story of a Real Fake</t>
+  </si>
+  <si>
+    <t>Frank Abagnale Jr.</t>
+  </si>
+  <si>
+    <t>I recently watched a talk Frank Abagnale gave at Google, and decided to check out his book. His story is fascenating and, admittedly, alluring. Two lessons to take from a con man, even for those who don't want to con but who just want to get their way with other people, are to (1) dress in a way that commands respect, and (2) act with confidence.</t>
   </si>
 </sst>
 </file>
@@ -5268,7 +5277,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5279,7 +5288,7 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A598" workbookViewId="0">
-      <selection activeCell="A624" sqref="A624"/>
+      <selection activeCell="E626" sqref="E626"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -16949,15 +16958,33 @@
         <v>239</v>
       </c>
     </row>
-    <row r="625" spans="4:7">
+    <row r="625" spans="1:8">
+      <c r="A625" s="3" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B625" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C625" s="3" t="s">
+        <v>200</v>
+      </c>
       <c r="D625" s="6">
         <v>2019</v>
       </c>
-      <c r="E625" s="6"/>
-      <c r="F625" s="6"/>
-      <c r="G625" s="6"/>
-    </row>
-    <row r="626" spans="4:7">
+      <c r="E625" s="6">
+        <v>1980</v>
+      </c>
+      <c r="F625" s="6">
+        <v>253</v>
+      </c>
+      <c r="G625" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H625" s="3" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="626" spans="1:8">
       <c r="D626" s="6">
         <v>2019</v>
       </c>
@@ -16965,7 +16992,7 @@
       <c r="F626" s="6"/>
       <c r="G626" s="6"/>
     </row>
-    <row r="627" spans="4:7">
+    <row r="627" spans="1:8">
       <c r="D627" s="6">
         <v>2019</v>
       </c>
@@ -16973,7 +17000,7 @@
       <c r="F627" s="6"/>
       <c r="G627" s="6"/>
     </row>
-    <row r="628" spans="4:7">
+    <row r="628" spans="1:8">
       <c r="D628" s="6">
         <v>2019</v>
       </c>
@@ -16981,7 +17008,7 @@
       <c r="F628" s="6"/>
       <c r="G628" s="6"/>
     </row>
-    <row r="629" spans="4:7">
+    <row r="629" spans="1:8">
       <c r="D629" s="6">
         <v>2019</v>
       </c>
@@ -16989,7 +17016,7 @@
       <c r="F629" s="6"/>
       <c r="G629" s="6"/>
     </row>
-    <row r="630" spans="4:7">
+    <row r="630" spans="1:8">
       <c r="D630" s="6">
         <v>2019</v>
       </c>
@@ -16997,61 +17024,61 @@
       <c r="F630" s="6"/>
       <c r="G630" s="6"/>
     </row>
-    <row r="631" spans="4:7">
+    <row r="631" spans="1:8">
       <c r="D631" s="6"/>
       <c r="E631" s="6"/>
       <c r="F631" s="6"/>
       <c r="G631" s="6"/>
     </row>
-    <row r="632" spans="4:7">
+    <row r="632" spans="1:8">
       <c r="D632" s="6"/>
       <c r="E632" s="6"/>
       <c r="F632" s="6"/>
       <c r="G632" s="6"/>
     </row>
-    <row r="633" spans="4:7">
+    <row r="633" spans="1:8">
       <c r="D633" s="6"/>
       <c r="E633" s="6"/>
       <c r="F633" s="6"/>
       <c r="G633" s="6"/>
     </row>
-    <row r="634" spans="4:7">
+    <row r="634" spans="1:8">
       <c r="D634" s="6"/>
       <c r="E634" s="6"/>
       <c r="F634" s="6"/>
       <c r="G634" s="6"/>
     </row>
-    <row r="635" spans="4:7">
+    <row r="635" spans="1:8">
       <c r="D635" s="6"/>
       <c r="E635" s="6"/>
       <c r="F635" s="6"/>
       <c r="G635" s="6"/>
     </row>
-    <row r="636" spans="4:7">
+    <row r="636" spans="1:8">
       <c r="D636" s="6"/>
       <c r="E636" s="6"/>
       <c r="F636" s="6"/>
       <c r="G636" s="6"/>
     </row>
-    <row r="637" spans="4:7">
+    <row r="637" spans="1:8">
       <c r="D637" s="6"/>
       <c r="E637" s="6"/>
       <c r="F637" s="6"/>
       <c r="G637" s="6"/>
     </row>
-    <row r="638" spans="4:7">
+    <row r="638" spans="1:8">
       <c r="D638" s="6"/>
       <c r="E638" s="6"/>
       <c r="F638" s="6"/>
       <c r="G638" s="6"/>
     </row>
-    <row r="639" spans="4:7">
+    <row r="639" spans="1:8">
       <c r="D639" s="6"/>
       <c r="E639" s="6"/>
       <c r="F639" s="6"/>
       <c r="G639" s="6"/>
     </row>
-    <row r="640" spans="4:7">
+    <row r="640" spans="1:8">
       <c r="D640" s="6"/>
       <c r="E640" s="6"/>
       <c r="F640" s="6"/>

</xml_diff>

<commit_message>
Quiet, Little Oratory, Red Bandanna
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8D839F-4B3E-4D45-A83D-98D954306FBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2123" uniqueCount="1241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2137" uniqueCount="1249">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3748,13 +3742,37 @@
   </si>
   <si>
     <t>BC5: This is a profound warning abou the dangers of not thinking, scarily prophetic, and a beautiful ode to good books and ideas. We had a wonderful conversation and it was a joy to read again.</t>
+  </si>
+  <si>
+    <t>Quiet: The Power of Introverts in a World That Can't Stop Talking</t>
+  </si>
+  <si>
+    <t>Susan Cain</t>
+  </si>
+  <si>
+    <t>The Little Oratory: A Beginner's Guide to Praying in the Home</t>
+  </si>
+  <si>
+    <t>David Clayton &amp; Leila Lawler</t>
+  </si>
+  <si>
+    <t>The takeaway from this book is that the modern Western ideal of extroversion is new and not always helpful, and that there are good reasons to value the contribution of introverts and specific strategies to help them (or yourself) work well in this extroverted world.</t>
+  </si>
+  <si>
+    <t>The Red Bandanna: A life. A choice. A Legacy.</t>
+  </si>
+  <si>
+    <t>Tom Rinaldi</t>
+  </si>
+  <si>
+    <t>A book about Welles Crowther, who sacrificed his life saving others in the South Tower on 9/11. A tragic but beautiful story and a challenge to live your life for others.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3813,7 +3831,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="577">
+  <cellStyleXfs count="579">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4300,6 +4318,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4411,7 +4431,7 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="577">
+  <cellStyles count="579">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4943,6 +4963,7 @@
     <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="574" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="578" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="489" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="491" builtinId="8" hidden="1"/>
@@ -4988,6 +5009,7 @@
     <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="573" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="575" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="577" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5292,21 +5314,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A598" workbookViewId="0">
-      <selection activeCell="A627" sqref="A627"/>
+    <sheetView tabSelected="1" topLeftCell="A621" workbookViewId="0">
+      <selection activeCell="A630" sqref="A630"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="98" style="3" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="3" customWidth="1"/>
@@ -17029,28 +17051,79 @@
       </c>
     </row>
     <row r="627" spans="1:8">
+      <c r="A627" s="3" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B627" s="3" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C627" s="3" t="s">
+        <v>200</v>
+      </c>
       <c r="D627" s="6">
         <v>2019</v>
       </c>
-      <c r="E627" s="6"/>
-      <c r="F627" s="6"/>
-      <c r="G627" s="6"/>
+      <c r="E627" s="6">
+        <v>2012</v>
+      </c>
+      <c r="F627" s="6">
+        <v>276</v>
+      </c>
+      <c r="G627" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H627" s="3" t="s">
+        <v>1245</v>
+      </c>
     </row>
     <row r="628" spans="1:8">
+      <c r="A628" s="3" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B628" s="3" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C628" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D628" s="6">
         <v>2019</v>
       </c>
-      <c r="E628" s="6"/>
-      <c r="F628" s="6"/>
-      <c r="G628" s="6"/>
+      <c r="E628" s="6">
+        <v>209</v>
+      </c>
+      <c r="F628" s="6">
+        <v>2014</v>
+      </c>
+      <c r="G628" s="6" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="629" spans="1:8">
+      <c r="A629" s="3" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B629" s="3" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C629" s="3" t="s">
+        <v>201</v>
+      </c>
       <c r="D629" s="6">
         <v>2019</v>
       </c>
-      <c r="E629" s="6"/>
-      <c r="F629" s="6"/>
-      <c r="G629" s="6"/>
+      <c r="E629" s="6">
+        <v>211</v>
+      </c>
+      <c r="F629" s="6">
+        <v>2016</v>
+      </c>
+      <c r="G629" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H629" s="3" t="s">
+        <v>1248</v>
+      </c>
     </row>
     <row r="630" spans="1:8">
       <c r="D630" s="6">
@@ -17061,55 +17134,73 @@
       <c r="G630" s="6"/>
     </row>
     <row r="631" spans="1:8">
-      <c r="D631" s="6"/>
+      <c r="D631" s="6">
+        <v>2019</v>
+      </c>
       <c r="E631" s="6"/>
       <c r="F631" s="6"/>
       <c r="G631" s="6"/>
     </row>
     <row r="632" spans="1:8">
-      <c r="D632" s="6"/>
+      <c r="D632" s="6">
+        <v>2019</v>
+      </c>
       <c r="E632" s="6"/>
       <c r="F632" s="6"/>
       <c r="G632" s="6"/>
     </row>
     <row r="633" spans="1:8">
-      <c r="D633" s="6"/>
+      <c r="D633" s="6">
+        <v>2019</v>
+      </c>
       <c r="E633" s="6"/>
       <c r="F633" s="6"/>
       <c r="G633" s="6"/>
     </row>
     <row r="634" spans="1:8">
-      <c r="D634" s="6"/>
+      <c r="D634" s="6">
+        <v>2019</v>
+      </c>
       <c r="E634" s="6"/>
       <c r="F634" s="6"/>
       <c r="G634" s="6"/>
     </row>
     <row r="635" spans="1:8">
-      <c r="D635" s="6"/>
+      <c r="D635" s="6">
+        <v>2019</v>
+      </c>
       <c r="E635" s="6"/>
       <c r="F635" s="6"/>
       <c r="G635" s="6"/>
     </row>
     <row r="636" spans="1:8">
-      <c r="D636" s="6"/>
+      <c r="D636" s="6">
+        <v>2019</v>
+      </c>
       <c r="E636" s="6"/>
       <c r="F636" s="6"/>
       <c r="G636" s="6"/>
     </row>
     <row r="637" spans="1:8">
-      <c r="D637" s="6"/>
+      <c r="D637" s="6">
+        <v>2019</v>
+      </c>
       <c r="E637" s="6"/>
       <c r="F637" s="6"/>
       <c r="G637" s="6"/>
     </row>
     <row r="638" spans="1:8">
-      <c r="D638" s="6"/>
+      <c r="D638" s="6">
+        <v>2019</v>
+      </c>
       <c r="E638" s="6"/>
       <c r="F638" s="6"/>
       <c r="G638" s="6"/>
     </row>
     <row r="639" spans="1:8">
-      <c r="D639" s="6"/>
+      <c r="D639" s="6">
+        <v>2019</v>
+      </c>
       <c r="E639" s="6"/>
       <c r="F639" s="6"/>
       <c r="G639" s="6"/>

</xml_diff>

<commit_message>
The Gift of Failure
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="1258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="1263">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3738,9 +3738,6 @@
     <t>Digital Minimalism: Choosing a Focused Life in a Noisy World</t>
   </si>
   <si>
-    <t>This book is profound, particularly the chapter on solitude (being away from the inputs of other minds) and while reading Cardinal Sarah's Silence. I have a lot to learn and implement from this. This caused me to take notes with pen and paper for library books and I need to do some more work to map out and understand my idea consumption processes.</t>
-  </si>
-  <si>
     <t>BC5: This is a profound warning abou the dangers of not thinking, scarily prophetic, and a beautiful ode to good books and ideas. We had a wonderful conversation and it was a joy to read again.</t>
   </si>
   <si>
@@ -3793,6 +3790,24 @@
   </si>
   <si>
     <t>A fascenating scientific history, and a warning about the many moral issues that surround genetics, particularly abortion, eugenics, and modifying the human genome.</t>
+  </si>
+  <si>
+    <t>This book is profound, particularly the chapters on leisure and solitude (being away from the inputs of other minds) and while reading Cardinal Sarah's Silence. I have a lot to learn and implement from this. This caused me to take notes with pen and paper for library books and I need to do some more work to map out and understand my idea consumption processes.</t>
+  </si>
+  <si>
+    <t>Notes from Underground</t>
+  </si>
+  <si>
+    <t>BC6: This novel was *weird*, but made some interesting points about the limits of science and reason, the importance of free will, and what would later be called behavioral economics.</t>
+  </si>
+  <si>
+    <t>The Gift of Failure: How the Best Parents Learn to Let Go So Their Children Can Succeed</t>
+  </si>
+  <si>
+    <t>Jessica Lahey</t>
+  </si>
+  <si>
+    <t>I had been meaning to read this for awhile and was inspired finally when Jordan read *There's No Such Thing as Bad Weather* (only bad clothes) by a Swedish mother. I think these two books made many of the same points, namely that every time you save your child from a failure now, you set them up to fail in the long term.</t>
   </si>
 </sst>
 </file>
@@ -5356,7 +5371,7 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A612" workbookViewId="0">
-      <selection activeCell="A633" sqref="A633"/>
+      <selection activeCell="A635" sqref="A635"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -17026,7 +17041,7 @@
         <v>239</v>
       </c>
       <c r="H624" s="3" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="625" spans="1:8">
@@ -17078,15 +17093,15 @@
         <v>237</v>
       </c>
       <c r="H626" s="3" t="s">
-        <v>1239</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="627" spans="1:8">
       <c r="A627" s="3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B627" s="3" t="s">
         <v>1241</v>
-      </c>
-      <c r="B627" s="3" t="s">
-        <v>1242</v>
       </c>
       <c r="C627" s="3" t="s">
         <v>200</v>
@@ -17104,15 +17119,15 @@
         <v>239</v>
       </c>
       <c r="H627" s="3" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="628" spans="1:8">
       <c r="A628" s="3" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B628" s="3" t="s">
         <v>1243</v>
-      </c>
-      <c r="B628" s="3" t="s">
-        <v>1244</v>
       </c>
       <c r="C628" s="3" t="s">
         <v>199</v>
@@ -17130,15 +17145,15 @@
         <v>237</v>
       </c>
       <c r="H628" s="3" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="629" spans="1:8">
       <c r="A629" s="3" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B629" s="3" t="s">
         <v>1246</v>
-      </c>
-      <c r="B629" s="3" t="s">
-        <v>1247</v>
       </c>
       <c r="C629" s="3" t="s">
         <v>201</v>
@@ -17156,15 +17171,15 @@
         <v>237</v>
       </c>
       <c r="H629" s="3" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="630" spans="1:8">
       <c r="A630" s="3" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B630" s="3" t="s">
         <v>1249</v>
-      </c>
-      <c r="B630" s="3" t="s">
-        <v>1250</v>
       </c>
       <c r="C630" s="3" t="s">
         <v>201</v>
@@ -17184,10 +17199,10 @@
     </row>
     <row r="631" spans="1:8">
       <c r="A631" s="3" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B631" s="3" t="s">
         <v>1252</v>
-      </c>
-      <c r="B631" s="3" t="s">
-        <v>1253</v>
       </c>
       <c r="C631" s="3" t="s">
         <v>949</v>
@@ -17205,15 +17220,15 @@
         <v>237</v>
       </c>
       <c r="H631" s="3" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="632" spans="1:8">
       <c r="A632" s="3" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B632" s="3" t="s">
         <v>1255</v>
-      </c>
-      <c r="B632" s="3" t="s">
-        <v>1256</v>
       </c>
       <c r="C632" s="3" t="s">
         <v>200</v>
@@ -17231,24 +17246,60 @@
         <v>237</v>
       </c>
       <c r="H632" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="633" spans="1:8">
+      <c r="A633" s="3" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B633" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="C633" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D633" s="6">
         <v>2019</v>
       </c>
-      <c r="E633" s="6"/>
-      <c r="F633" s="6"/>
-      <c r="G633" s="6"/>
+      <c r="E633" s="6">
+        <v>1864</v>
+      </c>
+      <c r="F633" s="6">
+        <v>123</v>
+      </c>
+      <c r="G633" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H633" s="3" t="s">
+        <v>1259</v>
+      </c>
     </row>
     <row r="634" spans="1:8">
+      <c r="A634" s="3" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B634" s="3" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C634" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D634" s="6">
         <v>2019</v>
       </c>
-      <c r="E634" s="6"/>
-      <c r="F634" s="6"/>
-      <c r="G634" s="6"/>
+      <c r="E634" s="6">
+        <v>2015</v>
+      </c>
+      <c r="F634" s="6">
+        <v>243</v>
+      </c>
+      <c r="G634" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H634" s="3" t="s">
+        <v>1262</v>
+      </c>
     </row>
     <row r="635" spans="1:8">
       <c r="D635" s="6">

</xml_diff>

<commit_message>
Jesus of Nazareth + Fix Forster spelling
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1CB81E-2B18-814F-A046-1D53DEDA0CCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2188" uniqueCount="1279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2193" uniqueCount="1281">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -2460,9 +2466,6 @@
     <t>Peter Fox-Penner</t>
   </si>
   <si>
-    <t>E.M. Forester</t>
-  </si>
-  <si>
     <t xml:space="preserve">David Halberstam </t>
   </si>
   <si>
@@ -3856,13 +3859,22 @@
   </si>
   <si>
     <t>BC7: A beautiful reflection on marriage, which we read aloud together.</t>
+  </si>
+  <si>
+    <t>Jesus of Nazareth: Holy Week: from the Entrance into Jerusalem to the Resurrection</t>
+  </si>
+  <si>
+    <t>Fr. Dailey recommended this, and I read it during Lent. This is a beautiful portrait of Jesus' life, and I was struck by the historicity of his description as well as how he draws out the scriptural connection between the old and new covenants.</t>
+  </si>
+  <si>
+    <t>E. M. Forster</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5432,21 +5444,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A612" workbookViewId="0">
-      <selection activeCell="A639" sqref="A639"/>
+    <sheetView tabSelected="1" topLeftCell="A608" workbookViewId="0">
+      <selection activeCell="A641" sqref="A641"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="98" style="3" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="3" customWidth="1"/>
@@ -5481,10 +5493,10 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>199</v>
@@ -5499,10 +5511,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>199</v>
@@ -5517,10 +5529,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>199</v>
@@ -5535,10 +5547,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>199</v>
@@ -5553,10 +5565,10 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>199</v>
@@ -5571,10 +5583,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>199</v>
@@ -5589,10 +5601,10 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>199</v>
@@ -5607,10 +5619,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>199</v>
@@ -5625,7 +5637,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>630</v>
@@ -5643,7 +5655,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>630</v>
@@ -5661,7 +5673,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>630</v>
@@ -5679,10 +5691,10 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>199</v>
@@ -5697,10 +5709,10 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>1009</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>1010</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>199</v>
@@ -5715,10 +5727,10 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>199</v>
@@ -5733,10 +5745,10 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>199</v>
@@ -5751,10 +5763,10 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>199</v>
@@ -5769,10 +5781,10 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>199</v>
@@ -5787,10 +5799,10 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>199</v>
@@ -5805,10 +5817,10 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>199</v>
@@ -5823,10 +5835,10 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>199</v>
@@ -5841,7 +5853,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>642</v>
@@ -5859,10 +5871,10 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>199</v>
@@ -5877,10 +5889,10 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>199</v>
@@ -5895,7 +5907,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>628</v>
@@ -5913,7 +5925,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>688</v>
@@ -5931,7 +5943,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>627</v>
@@ -5949,10 +5961,10 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>199</v>
@@ -5967,7 +5979,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>632</v>
@@ -5985,10 +5997,10 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>199</v>
@@ -6003,10 +6015,10 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>199</v>
@@ -6021,10 +6033,10 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>199</v>
@@ -6039,10 +6051,10 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>199</v>
@@ -6057,7 +6069,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>246</v>
@@ -6312,7 +6324,7 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="8" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>627</v>
@@ -8560,7 +8572,7 @@
         <v>406</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D191" s="6">
         <v>2013</v>
@@ -8759,7 +8771,7 @@
     </row>
     <row r="204" spans="1:6">
       <c r="A204" s="3" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="B204" s="3" t="s">
         <v>739</v>
@@ -9018,7 +9030,7 @@
         <v>188</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D220" s="6">
         <v>2013</v>
@@ -9079,7 +9091,7 @@
         <v>438</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C224" s="4" t="s">
         <v>199</v>
@@ -9098,7 +9110,7 @@
         <v>188</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D225" s="6">
         <v>2014</v>
@@ -9111,7 +9123,7 @@
         <v>440</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D226" s="6">
         <v>2014</v>
@@ -9124,7 +9136,7 @@
         <v>441</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D227" s="6">
         <v>2014</v>
@@ -9137,7 +9149,7 @@
         <v>442</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D228" s="6">
         <v>2014</v>
@@ -9153,7 +9165,7 @@
         <v>610</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D229" s="6">
         <v>2014</v>
@@ -9329,7 +9341,7 @@
         <v>759</v>
       </c>
       <c r="C240" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D240" s="6">
         <v>2014</v>
@@ -9921,7 +9933,7 @@
         <v>668</v>
       </c>
       <c r="C277" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D277" s="6">
         <v>2015</v>
@@ -9969,7 +9981,7 @@
         <v>788</v>
       </c>
       <c r="C280" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D280" s="6">
         <v>2015</v>
@@ -10321,7 +10333,7 @@
         <v>803</v>
       </c>
       <c r="C302" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D302" s="6">
         <v>2015</v>
@@ -10337,7 +10349,7 @@
         <v>804</v>
       </c>
       <c r="C303" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D303" s="6">
         <v>2015</v>
@@ -10369,7 +10381,7 @@
         <v>806</v>
       </c>
       <c r="C305" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D305" s="6">
         <v>2015</v>
@@ -10472,7 +10484,7 @@
     </row>
     <row r="312" spans="1:6">
       <c r="A312" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C312" s="3" t="s">
         <v>199</v>
@@ -10536,10 +10548,10 @@
         <v>526</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>813</v>
+        <v>1280</v>
       </c>
       <c r="C316" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D316" s="6">
         <v>2016</v>
@@ -10552,7 +10564,7 @@
         <v>527</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C317" s="3" t="s">
         <v>200</v>
@@ -10568,7 +10580,7 @@
         <v>528</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C318" s="3" t="s">
         <v>199</v>
@@ -10584,7 +10596,7 @@
         <v>529</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C319" s="3" t="s">
         <v>199</v>
@@ -10613,7 +10625,7 @@
         <v>531</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C321" s="3" t="s">
         <v>202</v>
@@ -10629,7 +10641,7 @@
         <v>532</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C322" s="3" t="s">
         <v>199</v>
@@ -10645,7 +10657,7 @@
         <v>533</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C323" s="3" t="s">
         <v>200</v>
@@ -10661,7 +10673,7 @@
         <v>534</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C324" s="3" t="s">
         <v>202</v>
@@ -10677,7 +10689,7 @@
         <v>535</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C325" s="3" t="s">
         <v>200</v>
@@ -10693,7 +10705,7 @@
         <v>536</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C326" s="3" t="s">
         <v>199</v>
@@ -10725,7 +10737,7 @@
         <v>538</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C328" s="3" t="s">
         <v>200</v>
@@ -10741,7 +10753,7 @@
         <v>539</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C329" s="3" t="s">
         <v>200</v>
@@ -10757,7 +10769,7 @@
         <v>540</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C330" s="3" t="s">
         <v>199</v>
@@ -10789,7 +10801,7 @@
         <v>542</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C332" s="3" t="s">
         <v>200</v>
@@ -10805,7 +10817,7 @@
         <v>543</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C333" s="3" t="s">
         <v>201</v>
@@ -10821,7 +10833,7 @@
         <v>544</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C334" s="3" t="s">
         <v>200</v>
@@ -10853,7 +10865,7 @@
         <v>188</v>
       </c>
       <c r="C336" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D336" s="6">
         <v>2016</v>
@@ -10866,7 +10878,7 @@
         <v>547</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C337" s="3" t="s">
         <v>200</v>
@@ -10879,10 +10891,10 @@
     </row>
     <row r="338" spans="1:6">
       <c r="A338" s="3" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C338" s="3" t="s">
         <v>202</v>
@@ -10898,7 +10910,7 @@
         <v>548</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C339" s="3" t="s">
         <v>200</v>
@@ -10930,7 +10942,7 @@
         <v>550</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C341" s="3" t="s">
         <v>200</v>
@@ -10959,7 +10971,7 @@
         <v>552</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C343" s="3" t="s">
         <v>200</v>
@@ -10975,7 +10987,7 @@
         <v>553</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C344" s="3" t="s">
         <v>200</v>
@@ -10991,7 +11003,7 @@
         <v>554</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C345" s="3" t="s">
         <v>200</v>
@@ -11023,7 +11035,7 @@
         <v>556</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C347" s="3" t="s">
         <v>200</v>
@@ -11039,7 +11051,7 @@
         <v>557</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C348" s="3" t="s">
         <v>200</v>
@@ -11055,7 +11067,7 @@
         <v>558</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C349" s="3" t="s">
         <v>199</v>
@@ -11071,7 +11083,7 @@
         <v>559</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C350" s="3" t="s">
         <v>199</v>
@@ -11087,7 +11099,7 @@
         <v>560</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C351" s="3" t="s">
         <v>200</v>
@@ -11103,7 +11115,7 @@
         <v>561</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C352" s="3" t="s">
         <v>199</v>
@@ -11135,7 +11147,7 @@
         <v>563</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C354" s="3" t="s">
         <v>200</v>
@@ -11151,7 +11163,7 @@
         <v>564</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C355" s="3" t="s">
         <v>200</v>
@@ -11167,7 +11179,7 @@
         <v>565</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C356" s="3" t="s">
         <v>199</v>
@@ -11183,7 +11195,7 @@
         <v>566</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C357" s="3" t="s">
         <v>199</v>
@@ -11199,7 +11211,7 @@
         <v>567</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C358" s="3" t="s">
         <v>200</v>
@@ -11215,10 +11227,10 @@
         <v>568</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C359" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D359" s="6">
         <v>2016</v>
@@ -11247,7 +11259,7 @@
         <v>570</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C361" s="3" t="s">
         <v>202</v>
@@ -11263,7 +11275,7 @@
         <v>571</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C362" s="3" t="s">
         <v>200</v>
@@ -11279,7 +11291,7 @@
         <v>572</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C363" s="3" t="s">
         <v>202</v>
@@ -11295,7 +11307,7 @@
         <v>573</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C364" s="3" t="s">
         <v>202</v>
@@ -11311,7 +11323,7 @@
         <v>574</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C365" s="3" t="s">
         <v>200</v>
@@ -11327,7 +11339,7 @@
         <v>575</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C366" s="3" t="s">
         <v>199</v>
@@ -11343,7 +11355,7 @@
         <v>576</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C367" s="3" t="s">
         <v>200</v>
@@ -11375,7 +11387,7 @@
         <v>578</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C369" s="3" t="s">
         <v>200</v>
@@ -11407,7 +11419,7 @@
         <v>580</v>
       </c>
       <c r="C371" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D371" s="6">
         <v>2016</v>
@@ -11420,7 +11432,7 @@
         <v>581</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C372" s="3" t="s">
         <v>200</v>
@@ -11436,7 +11448,7 @@
         <v>582</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C373" s="3" t="s">
         <v>199</v>
@@ -11452,7 +11464,7 @@
         <v>583</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C374" s="3" t="s">
         <v>199</v>
@@ -11468,7 +11480,7 @@
         <v>584</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C375" s="3" t="s">
         <v>199</v>
@@ -11484,7 +11496,7 @@
         <v>585</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C376" s="3" t="s">
         <v>200</v>
@@ -11500,7 +11512,7 @@
         <v>586</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C377" s="3" t="s">
         <v>200</v>
@@ -11516,7 +11528,7 @@
         <v>587</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C378" s="3" t="s">
         <v>201</v>
@@ -11548,7 +11560,7 @@
         <v>589</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C380" s="3" t="s">
         <v>199</v>
@@ -11564,7 +11576,7 @@
         <v>590</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C381" s="3" t="s">
         <v>201</v>
@@ -11580,7 +11592,7 @@
         <v>591</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C382" s="3" t="s">
         <v>200</v>
@@ -11596,7 +11608,7 @@
         <v>592</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C383" s="3" t="s">
         <v>200</v>
@@ -11644,10 +11656,10 @@
         <v>595</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C386" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D386" s="6">
         <v>2016</v>
@@ -11676,7 +11688,7 @@
         <v>597</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C388" s="3" t="s">
         <v>200</v>
@@ -11692,7 +11704,7 @@
         <v>598</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C389" s="3" t="s">
         <v>201</v>
@@ -11740,7 +11752,7 @@
         <v>601</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C392" s="3" t="s">
         <v>201</v>
@@ -11756,7 +11768,7 @@
         <v>602</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="C393" s="3" t="s">
         <v>200</v>
@@ -11772,7 +11784,7 @@
         <v>603</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C394" s="3" t="s">
         <v>200</v>
@@ -11804,7 +11816,7 @@
         <v>605</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="C396" s="3" t="s">
         <v>200</v>
@@ -11820,7 +11832,7 @@
         <v>606</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="C397" s="3" t="s">
         <v>199</v>
@@ -11836,7 +11848,7 @@
         <v>607</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="C398" s="3" t="s">
         <v>201</v>
@@ -11852,7 +11864,7 @@
         <v>608</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C399" s="3" t="s">
         <v>199</v>
@@ -11865,7 +11877,7 @@
     </row>
     <row r="400" spans="1:6">
       <c r="A400" s="3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C400" s="3" t="s">
         <v>199</v>
@@ -12317,7 +12329,7 @@
         <v>120</v>
       </c>
       <c r="C422" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D422" s="6">
         <v>2017</v>
@@ -12370,7 +12382,7 @@
       </c>
       <c r="G424" s="7"/>
       <c r="H424" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="425" spans="1:8">
@@ -12461,7 +12473,7 @@
         <v>127</v>
       </c>
       <c r="C429" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D429" s="6">
         <v>2017</v>
@@ -12981,7 +12993,7 @@
     </row>
     <row r="455" spans="1:6">
       <c r="A455" s="3" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B455" s="3" t="s">
         <v>153</v>
@@ -13973,7 +13985,7 @@
     </row>
     <row r="503" spans="1:8">
       <c r="A503" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="C503" s="3" t="s">
         <v>199</v>
@@ -14218,10 +14230,10 @@
     </row>
     <row r="513" spans="1:8">
       <c r="A513" s="3" t="s">
+        <v>876</v>
+      </c>
+      <c r="B513" s="3" t="s">
         <v>877</v>
-      </c>
-      <c r="B513" s="3" t="s">
-        <v>878</v>
       </c>
       <c r="C513" s="3" t="s">
         <v>200</v>
@@ -14239,15 +14251,15 @@
         <v>239</v>
       </c>
       <c r="H513" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="514" spans="1:8">
       <c r="A514" s="3" t="s">
+        <v>880</v>
+      </c>
+      <c r="B514" s="3" t="s">
         <v>881</v>
-      </c>
-      <c r="B514" s="3" t="s">
-        <v>882</v>
       </c>
       <c r="C514" s="3" t="s">
         <v>201</v>
@@ -14265,15 +14277,15 @@
         <v>237</v>
       </c>
       <c r="H514" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="515" spans="1:8">
       <c r="A515" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="B515" s="3" t="s">
         <v>884</v>
-      </c>
-      <c r="B515" s="3" t="s">
-        <v>885</v>
       </c>
       <c r="C515" s="3" t="s">
         <v>201</v>
@@ -14291,7 +14303,7 @@
         <v>237</v>
       </c>
       <c r="H515" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="516" spans="1:8">
@@ -14317,15 +14329,15 @@
         <v>237</v>
       </c>
       <c r="H516" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="517" spans="1:8">
       <c r="A517" s="3" t="s">
+        <v>886</v>
+      </c>
+      <c r="B517" s="3" t="s">
         <v>887</v>
-      </c>
-      <c r="B517" s="3" t="s">
-        <v>888</v>
       </c>
       <c r="C517" s="3" t="s">
         <v>199</v>
@@ -14343,15 +14355,15 @@
         <v>237</v>
       </c>
       <c r="H517" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="518" spans="1:8">
       <c r="A518" s="3" t="s">
+        <v>890</v>
+      </c>
+      <c r="B518" s="3" t="s">
         <v>891</v>
-      </c>
-      <c r="B518" s="3" t="s">
-        <v>892</v>
       </c>
       <c r="C518" s="3" t="s">
         <v>201</v>
@@ -14369,15 +14381,15 @@
         <v>237</v>
       </c>
       <c r="H518" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="519" spans="1:8">
       <c r="A519" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="B519" s="3" t="s">
         <v>894</v>
-      </c>
-      <c r="B519" s="3" t="s">
-        <v>895</v>
       </c>
       <c r="C519" s="3" t="s">
         <v>199</v>
@@ -14395,15 +14407,15 @@
         <v>237</v>
       </c>
       <c r="H519" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="520" spans="1:8">
       <c r="A520" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="B520" s="3" t="s">
         <v>897</v>
-      </c>
-      <c r="B520" s="3" t="s">
-        <v>898</v>
       </c>
       <c r="C520" s="3" t="s">
         <v>199</v>
@@ -14421,15 +14433,15 @@
         <v>239</v>
       </c>
       <c r="H520" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="521" spans="1:8">
       <c r="A521" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="B521" s="3" t="s">
         <v>900</v>
-      </c>
-      <c r="B521" s="3" t="s">
-        <v>901</v>
       </c>
       <c r="C521" s="3" t="s">
         <v>200</v>
@@ -14447,15 +14459,15 @@
         <v>237</v>
       </c>
       <c r="H521" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="522" spans="1:8">
       <c r="A522" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="B522" s="3" t="s">
         <v>902</v>
-      </c>
-      <c r="B522" s="3" t="s">
-        <v>903</v>
       </c>
       <c r="C522" s="3" t="s">
         <v>200</v>
@@ -14473,15 +14485,15 @@
         <v>237</v>
       </c>
       <c r="H522" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="523" spans="1:8">
       <c r="A523" s="3" t="s">
+        <v>903</v>
+      </c>
+      <c r="B523" s="3" t="s">
         <v>904</v>
-      </c>
-      <c r="B523" s="3" t="s">
-        <v>905</v>
       </c>
       <c r="C523" s="3" t="s">
         <v>200</v>
@@ -14499,15 +14511,15 @@
         <v>239</v>
       </c>
       <c r="H523" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="524" spans="1:8">
       <c r="A524" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B524" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C524" s="3" t="s">
         <v>199</v>
@@ -14525,15 +14537,15 @@
         <v>237</v>
       </c>
       <c r="H524" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="525" spans="1:8">
       <c r="A525" s="3" t="s">
+        <v>908</v>
+      </c>
+      <c r="B525" s="3" t="s">
         <v>909</v>
-      </c>
-      <c r="B525" s="3" t="s">
-        <v>910</v>
       </c>
       <c r="C525" s="3" t="s">
         <v>200</v>
@@ -14551,15 +14563,15 @@
         <v>239</v>
       </c>
       <c r="H525" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="526" spans="1:8">
       <c r="A526" s="3" t="s">
+        <v>912</v>
+      </c>
+      <c r="B526" s="3" t="s">
         <v>913</v>
-      </c>
-      <c r="B526" s="3" t="s">
-        <v>914</v>
       </c>
       <c r="C526" s="3" t="s">
         <v>200</v>
@@ -14577,15 +14589,15 @@
         <v>239</v>
       </c>
       <c r="H526" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="527" spans="1:8">
       <c r="A527" s="3" t="s">
+        <v>914</v>
+      </c>
+      <c r="B527" s="3" t="s">
         <v>915</v>
-      </c>
-      <c r="B527" s="3" t="s">
-        <v>916</v>
       </c>
       <c r="C527" s="3" t="s">
         <v>201</v>
@@ -14603,15 +14615,15 @@
         <v>239</v>
       </c>
       <c r="H527" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="528" spans="1:8">
       <c r="A528" s="3" t="s">
+        <v>917</v>
+      </c>
+      <c r="B528" s="3" t="s">
         <v>918</v>
-      </c>
-      <c r="B528" s="3" t="s">
-        <v>919</v>
       </c>
       <c r="C528" s="3" t="s">
         <v>200</v>
@@ -14629,15 +14641,15 @@
         <v>239</v>
       </c>
       <c r="H528" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="529" spans="1:8">
       <c r="A529" s="3" t="s">
+        <v>925</v>
+      </c>
+      <c r="B529" s="3" t="s">
         <v>926</v>
-      </c>
-      <c r="B529" s="3" t="s">
-        <v>927</v>
       </c>
       <c r="C529" s="3" t="s">
         <v>200</v>
@@ -14655,15 +14667,15 @@
         <v>237</v>
       </c>
       <c r="H529" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="530" spans="1:8">
       <c r="A530" s="3" t="s">
+        <v>923</v>
+      </c>
+      <c r="B530" s="3" t="s">
         <v>924</v>
-      </c>
-      <c r="B530" s="3" t="s">
-        <v>925</v>
       </c>
       <c r="C530" s="3" t="s">
         <v>200</v>
@@ -14681,15 +14693,15 @@
         <v>237</v>
       </c>
       <c r="H530" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="531" spans="1:8">
       <c r="A531" s="3" t="s">
+        <v>927</v>
+      </c>
+      <c r="B531" s="3" t="s">
         <v>928</v>
-      </c>
-      <c r="B531" s="3" t="s">
-        <v>929</v>
       </c>
       <c r="C531" s="3" t="s">
         <v>201</v>
@@ -14707,15 +14719,15 @@
         <v>237</v>
       </c>
       <c r="H531" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="532" spans="1:8">
       <c r="A532" s="3" t="s">
+        <v>932</v>
+      </c>
+      <c r="B532" s="3" t="s">
         <v>933</v>
-      </c>
-      <c r="B532" s="3" t="s">
-        <v>934</v>
       </c>
       <c r="C532" s="3" t="s">
         <v>201</v>
@@ -14733,18 +14745,18 @@
         <v>237</v>
       </c>
       <c r="H532" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="533" spans="1:8">
       <c r="A533" s="3" t="s">
+        <v>935</v>
+      </c>
+      <c r="B533" s="3" t="s">
         <v>936</v>
       </c>
-      <c r="B533" s="3" t="s">
-        <v>937</v>
-      </c>
       <c r="C533" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D533" s="6">
         <v>2018</v>
@@ -14759,15 +14771,15 @@
         <v>239</v>
       </c>
       <c r="H533" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="534" spans="1:8">
       <c r="A534" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B534" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="C534" s="3" t="s">
         <v>201</v>
@@ -14785,12 +14797,12 @@
         <v>237</v>
       </c>
       <c r="H534" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="535" spans="1:8">
       <c r="A535" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B535" s="3" t="s">
         <v>159</v>
@@ -14811,15 +14823,15 @@
         <v>237</v>
       </c>
       <c r="H535" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="536" spans="1:8">
       <c r="A536" s="3" t="s">
+        <v>941</v>
+      </c>
+      <c r="B536" s="3" t="s">
         <v>942</v>
-      </c>
-      <c r="B536" s="3" t="s">
-        <v>943</v>
       </c>
       <c r="C536" s="3" t="s">
         <v>200</v>
@@ -14837,12 +14849,12 @@
         <v>239</v>
       </c>
       <c r="H536" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="537" spans="1:8">
       <c r="A537" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B537" s="3" t="s">
         <v>167</v>
@@ -14863,18 +14875,18 @@
         <v>237</v>
       </c>
       <c r="H537" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="538" spans="1:8">
       <c r="A538" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B538" s="3" t="s">
         <v>188</v>
       </c>
       <c r="C538" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D538" s="6">
         <v>2018</v>
@@ -14889,15 +14901,15 @@
         <v>237</v>
       </c>
       <c r="H538" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="539" spans="1:8">
       <c r="A539" s="3" t="s">
+        <v>950</v>
+      </c>
+      <c r="B539" s="3" t="s">
         <v>951</v>
-      </c>
-      <c r="B539" s="3" t="s">
-        <v>952</v>
       </c>
       <c r="C539" s="3" t="s">
         <v>200</v>
@@ -14915,15 +14927,15 @@
         <v>239</v>
       </c>
       <c r="H539" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="540" spans="1:8">
       <c r="A540" s="3" t="s">
+        <v>954</v>
+      </c>
+      <c r="B540" s="3" t="s">
         <v>955</v>
-      </c>
-      <c r="B540" s="3" t="s">
-        <v>956</v>
       </c>
       <c r="C540" s="3" t="s">
         <v>200</v>
@@ -14941,15 +14953,15 @@
         <v>239</v>
       </c>
       <c r="H540" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="541" spans="1:8">
       <c r="A541" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B541" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="C541" s="3" t="s">
         <v>199</v>
@@ -14967,15 +14979,15 @@
         <v>239</v>
       </c>
       <c r="H541" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="542" spans="1:8">
       <c r="A542" s="3" t="s">
+        <v>960</v>
+      </c>
+      <c r="B542" s="3" t="s">
         <v>961</v>
-      </c>
-      <c r="B542" s="3" t="s">
-        <v>962</v>
       </c>
       <c r="C542" s="3" t="s">
         <v>202</v>
@@ -14993,15 +15005,15 @@
         <v>237</v>
       </c>
       <c r="H542" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="543" spans="1:8">
       <c r="A543" s="3" t="s">
+        <v>963</v>
+      </c>
+      <c r="B543" s="3" t="s">
         <v>964</v>
-      </c>
-      <c r="B543" s="3" t="s">
-        <v>965</v>
       </c>
       <c r="C543" s="3" t="s">
         <v>200</v>
@@ -15019,18 +15031,18 @@
         <v>239</v>
       </c>
       <c r="H543" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="544" spans="1:8">
       <c r="A544" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="B544" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="C544" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D544" s="6">
         <v>2018</v>
@@ -15045,15 +15057,15 @@
         <v>237</v>
       </c>
       <c r="H544" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="545" spans="1:8">
       <c r="A545" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="B545" s="3" t="s">
         <v>970</v>
-      </c>
-      <c r="B545" s="3" t="s">
-        <v>971</v>
       </c>
       <c r="C545" s="3" t="s">
         <v>199</v>
@@ -15071,12 +15083,12 @@
         <v>239</v>
       </c>
       <c r="H545" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="546" spans="1:8">
       <c r="A546" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="B546" s="3" t="s">
         <v>186</v>
@@ -15097,15 +15109,15 @@
         <v>239</v>
       </c>
       <c r="H546" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="547" spans="1:8">
       <c r="A547" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B547" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C547" s="3" t="s">
         <v>200</v>
@@ -15123,12 +15135,12 @@
         <v>239</v>
       </c>
       <c r="H547" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="548" spans="1:8">
       <c r="A548" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B548" s="3" t="s">
         <v>777</v>
@@ -15149,15 +15161,15 @@
         <v>239</v>
       </c>
       <c r="H548" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="549" spans="1:8">
       <c r="A549" s="3" t="s">
+        <v>975</v>
+      </c>
+      <c r="B549" s="3" t="s">
         <v>976</v>
-      </c>
-      <c r="B549" s="3" t="s">
-        <v>977</v>
       </c>
       <c r="C549" s="3" t="s">
         <v>201</v>
@@ -15175,12 +15187,12 @@
         <v>239</v>
       </c>
       <c r="H549" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="550" spans="1:8">
       <c r="A550" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B550" s="3" t="s">
         <v>248</v>
@@ -15201,15 +15213,15 @@
         <v>237</v>
       </c>
       <c r="H550" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="551" spans="1:8">
       <c r="A551" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="B551" s="3" t="s">
         <v>985</v>
-      </c>
-      <c r="B551" s="3" t="s">
-        <v>986</v>
       </c>
       <c r="C551" s="3" t="s">
         <v>200</v>
@@ -15227,15 +15239,15 @@
         <v>237</v>
       </c>
       <c r="H551" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="552" spans="1:8">
       <c r="A552" s="3" t="s">
+        <v>987</v>
+      </c>
+      <c r="B552" s="3" t="s">
         <v>988</v>
-      </c>
-      <c r="B552" s="3" t="s">
-        <v>989</v>
       </c>
       <c r="C552" s="3" t="s">
         <v>200</v>
@@ -15253,15 +15265,15 @@
         <v>237</v>
       </c>
       <c r="H552" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="553" spans="1:8">
       <c r="A553" s="3" t="s">
+        <v>990</v>
+      </c>
+      <c r="B553" s="3" t="s">
         <v>991</v>
-      </c>
-      <c r="B553" s="3" t="s">
-        <v>992</v>
       </c>
       <c r="C553" s="3" t="s">
         <v>200</v>
@@ -15279,15 +15291,15 @@
         <v>237</v>
       </c>
       <c r="H553" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="554" spans="1:8">
       <c r="A554" s="3" t="s">
+        <v>993</v>
+      </c>
+      <c r="B554" s="3" t="s">
         <v>994</v>
-      </c>
-      <c r="B554" s="3" t="s">
-        <v>995</v>
       </c>
       <c r="C554" s="3" t="s">
         <v>201</v>
@@ -15305,15 +15317,15 @@
         <v>237</v>
       </c>
       <c r="H554" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="555" spans="1:8">
       <c r="A555" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="B555" s="3" t="s">
         <v>997</v>
-      </c>
-      <c r="B555" s="3" t="s">
-        <v>998</v>
       </c>
       <c r="C555" s="3" t="s">
         <v>201</v>
@@ -15331,15 +15343,15 @@
         <v>239</v>
       </c>
       <c r="H555" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="556" spans="1:8">
       <c r="A556" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="B556" s="3" t="s">
         <v>1000</v>
-      </c>
-      <c r="B556" s="3" t="s">
-        <v>1001</v>
       </c>
       <c r="C556" s="3" t="s">
         <v>200</v>
@@ -15357,15 +15369,15 @@
         <v>239</v>
       </c>
       <c r="H556" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="557" spans="1:8">
       <c r="A557" s="3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B557" s="3" t="s">
         <v>1003</v>
-      </c>
-      <c r="B557" s="3" t="s">
-        <v>1004</v>
       </c>
       <c r="C557" s="3" t="s">
         <v>200</v>
@@ -15383,15 +15395,15 @@
         <v>239</v>
       </c>
       <c r="H557" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="558" spans="1:8">
       <c r="A558" s="3" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B558" s="3" t="s">
         <v>1006</v>
-      </c>
-      <c r="B558" s="3" t="s">
-        <v>1007</v>
       </c>
       <c r="C558" s="3" t="s">
         <v>199</v>
@@ -15409,15 +15421,15 @@
         <v>239</v>
       </c>
       <c r="H558" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="559" spans="1:8">
       <c r="A559" s="3" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B559" s="3" t="s">
         <v>1009</v>
-      </c>
-      <c r="B559" s="3" t="s">
-        <v>1010</v>
       </c>
       <c r="C559" s="3" t="s">
         <v>200</v>
@@ -15435,12 +15447,12 @@
         <v>239</v>
       </c>
       <c r="H559" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="560" spans="1:8">
       <c r="A560" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B560" s="3" t="s">
         <v>106</v>
@@ -15461,15 +15473,15 @@
         <v>239</v>
       </c>
       <c r="H560" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="561" spans="1:8">
       <c r="A561" s="3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B561" s="3" t="s">
         <v>1014</v>
-      </c>
-      <c r="B561" s="3" t="s">
-        <v>1015</v>
       </c>
       <c r="C561" s="3" t="s">
         <v>201</v>
@@ -15487,15 +15499,15 @@
         <v>239</v>
       </c>
       <c r="H561" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="562" spans="1:8">
       <c r="A562" s="3" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B562" s="3" t="s">
         <v>1017</v>
-      </c>
-      <c r="B562" s="3" t="s">
-        <v>1018</v>
       </c>
       <c r="C562" s="3" t="s">
         <v>200</v>
@@ -15513,15 +15525,15 @@
         <v>239</v>
       </c>
       <c r="H562" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="563" spans="1:8">
       <c r="A563" s="3" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B563" s="3" t="s">
         <v>1020</v>
-      </c>
-      <c r="B563" s="3" t="s">
-        <v>1021</v>
       </c>
       <c r="C563" s="3" t="s">
         <v>199</v>
@@ -15539,15 +15551,15 @@
         <v>237</v>
       </c>
       <c r="H563" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="564" spans="1:8">
       <c r="A564" s="3" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B564" s="3" t="s">
         <v>1022</v>
-      </c>
-      <c r="B564" s="3" t="s">
-        <v>1023</v>
       </c>
       <c r="C564" s="3" t="s">
         <v>200</v>
@@ -15565,15 +15577,15 @@
         <v>239</v>
       </c>
       <c r="H564" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="565" spans="1:8">
       <c r="A565" s="3" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B565" s="3" t="s">
         <v>1024</v>
-      </c>
-      <c r="B565" s="3" t="s">
-        <v>1025</v>
       </c>
       <c r="C565" s="3" t="s">
         <v>200</v>
@@ -15591,7 +15603,7 @@
         <v>239</v>
       </c>
       <c r="H565" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="566" spans="1:8">
@@ -15617,15 +15629,15 @@
         <v>237</v>
       </c>
       <c r="H566" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="567" spans="1:8">
       <c r="A567" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B567" s="3" t="s">
         <v>1030</v>
-      </c>
-      <c r="B567" s="3" t="s">
-        <v>1031</v>
       </c>
       <c r="C567" s="3" t="s">
         <v>199</v>
@@ -15643,15 +15655,15 @@
         <v>237</v>
       </c>
       <c r="H567" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="568" spans="1:8">
       <c r="A568" s="3" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B568" s="3" t="s">
         <v>1033</v>
-      </c>
-      <c r="B568" s="3" t="s">
-        <v>1034</v>
       </c>
       <c r="C568" s="3" t="s">
         <v>200</v>
@@ -15669,15 +15681,15 @@
         <v>237</v>
       </c>
       <c r="H568" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="569" spans="1:8">
       <c r="A569" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B569" s="3" t="s">
         <v>1036</v>
-      </c>
-      <c r="B569" s="3" t="s">
-        <v>1037</v>
       </c>
       <c r="C569" s="3" t="s">
         <v>199</v>
@@ -15695,15 +15707,15 @@
         <v>239</v>
       </c>
       <c r="H569" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="570" spans="1:8">
       <c r="A570" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B570" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C570" s="3" t="s">
         <v>200</v>
@@ -15721,15 +15733,15 @@
         <v>239</v>
       </c>
       <c r="H570" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="571" spans="1:8">
       <c r="A571" s="3" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B571" s="3" t="s">
         <v>1041</v>
-      </c>
-      <c r="B571" s="3" t="s">
-        <v>1042</v>
       </c>
       <c r="C571" s="3" t="s">
         <v>201</v>
@@ -15747,15 +15759,15 @@
         <v>239</v>
       </c>
       <c r="H571" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="572" spans="1:8">
       <c r="A572" s="3" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B572" s="3" t="s">
         <v>1044</v>
-      </c>
-      <c r="B572" s="3" t="s">
-        <v>1045</v>
       </c>
       <c r="C572" s="3" t="s">
         <v>199</v>
@@ -15773,15 +15785,15 @@
         <v>239</v>
       </c>
       <c r="H572" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="573" spans="1:8">
       <c r="A573" s="3" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B573" s="3" t="s">
         <v>1047</v>
-      </c>
-      <c r="B573" s="3" t="s">
-        <v>1048</v>
       </c>
       <c r="C573" s="3" t="s">
         <v>201</v>
@@ -15799,15 +15811,15 @@
         <v>237</v>
       </c>
       <c r="H573" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="574" spans="1:8">
       <c r="A574" s="3" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B574" s="3" t="s">
         <v>1050</v>
-      </c>
-      <c r="B574" s="3" t="s">
-        <v>1051</v>
       </c>
       <c r="C574" s="3" t="s">
         <v>200</v>
@@ -15825,15 +15837,15 @@
         <v>239</v>
       </c>
       <c r="H574" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="575" spans="1:8">
       <c r="A575" s="3" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B575" s="3" t="s">
         <v>1053</v>
-      </c>
-      <c r="B575" s="3" t="s">
-        <v>1054</v>
       </c>
       <c r="C575" s="3" t="s">
         <v>201</v>
@@ -15851,15 +15863,15 @@
         <v>237</v>
       </c>
       <c r="H575" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="576" spans="1:8">
       <c r="A576" s="3" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B576" s="3" t="s">
         <v>1108</v>
-      </c>
-      <c r="B576" s="3" t="s">
-        <v>1109</v>
       </c>
       <c r="C576" s="3" t="s">
         <v>200</v>
@@ -15877,12 +15889,12 @@
         <v>237</v>
       </c>
       <c r="H576" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="577" spans="1:8">
       <c r="A577" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B577" s="3" t="s">
         <v>172</v>
@@ -15903,12 +15915,12 @@
         <v>237</v>
       </c>
       <c r="H577" s="3" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="578" spans="1:8">
       <c r="A578" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B578" s="3" t="s">
         <v>627</v>
@@ -15929,15 +15941,15 @@
         <v>239</v>
       </c>
       <c r="H578" s="3" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="579" spans="1:8">
       <c r="A579" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B579" s="3" t="s">
         <v>1113</v>
-      </c>
-      <c r="B579" s="3" t="s">
-        <v>1114</v>
       </c>
       <c r="C579" s="3" t="s">
         <v>199</v>
@@ -15955,7 +15967,7 @@
         <v>239</v>
       </c>
       <c r="H579" s="3" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="580" spans="1:8">
@@ -15981,15 +15993,15 @@
         <v>237</v>
       </c>
       <c r="H580" s="3" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="581" spans="1:8">
       <c r="A581" s="3" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B581" s="3" t="s">
         <v>1116</v>
-      </c>
-      <c r="B581" s="3" t="s">
-        <v>1117</v>
       </c>
       <c r="C581" s="3" t="s">
         <v>200</v>
@@ -16007,7 +16019,7 @@
         <v>239</v>
       </c>
       <c r="H581" s="3" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="582" spans="1:8">
@@ -16033,15 +16045,15 @@
         <v>239</v>
       </c>
       <c r="H582" s="3" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="583" spans="1:8">
       <c r="A583" s="3" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B583" s="3" t="s">
         <v>1121</v>
-      </c>
-      <c r="B583" s="3" t="s">
-        <v>1122</v>
       </c>
       <c r="C583" s="3" t="s">
         <v>200</v>
@@ -16059,15 +16071,15 @@
         <v>239</v>
       </c>
       <c r="H583" s="3" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="584" spans="1:8">
       <c r="A584" s="3" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B584" s="3" t="s">
         <v>1124</v>
-      </c>
-      <c r="B584" s="3" t="s">
-        <v>1125</v>
       </c>
       <c r="C584" s="3" t="s">
         <v>199</v>
@@ -16085,15 +16097,15 @@
         <v>237</v>
       </c>
       <c r="H584" s="3" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="585" spans="1:8">
       <c r="A585" s="3" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B585" s="3" t="s">
         <v>1127</v>
-      </c>
-      <c r="B585" s="3" t="s">
-        <v>1128</v>
       </c>
       <c r="C585" s="3" t="s">
         <v>200</v>
@@ -16111,15 +16123,15 @@
         <v>239</v>
       </c>
       <c r="H585" s="3" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="586" spans="1:8">
       <c r="A586" s="3" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B586" s="3" t="s">
         <v>1129</v>
-      </c>
-      <c r="B586" s="3" t="s">
-        <v>1130</v>
       </c>
       <c r="C586" s="3" t="s">
         <v>199</v>
@@ -16137,15 +16149,15 @@
         <v>237</v>
       </c>
       <c r="H586" s="3" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="587" spans="1:8">
       <c r="A587" s="3" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B587" s="3" t="s">
         <v>1131</v>
-      </c>
-      <c r="B587" s="3" t="s">
-        <v>1132</v>
       </c>
       <c r="C587" s="3" t="s">
         <v>200</v>
@@ -16163,15 +16175,15 @@
         <v>239</v>
       </c>
       <c r="H587" s="3" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="588" spans="1:8">
       <c r="A588" s="3" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B588" s="3" t="s">
         <v>1136</v>
-      </c>
-      <c r="B588" s="3" t="s">
-        <v>1137</v>
       </c>
       <c r="C588" s="3" t="s">
         <v>199</v>
@@ -16189,15 +16201,15 @@
         <v>239</v>
       </c>
       <c r="H588" s="3" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="589" spans="1:8">
       <c r="A589" s="3" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B589" s="3" t="s">
         <v>1140</v>
-      </c>
-      <c r="B589" s="3" t="s">
-        <v>1141</v>
       </c>
       <c r="C589" s="3" t="s">
         <v>201</v>
@@ -16215,12 +16227,12 @@
         <v>237</v>
       </c>
       <c r="H589" s="3" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="590" spans="1:8">
       <c r="A590" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B590" s="3" t="s">
         <v>630</v>
@@ -16241,15 +16253,15 @@
         <v>239</v>
       </c>
       <c r="H590" s="3" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="591" spans="1:8">
       <c r="A591" s="3" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B591" s="3" t="s">
         <v>1143</v>
-      </c>
-      <c r="B591" s="3" t="s">
-        <v>1144</v>
       </c>
       <c r="C591" s="3" t="s">
         <v>200</v>
@@ -16267,15 +16279,15 @@
         <v>237</v>
       </c>
       <c r="H591" s="3" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="592" spans="1:8">
       <c r="A592" s="3" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B592" s="3" t="s">
         <v>1146</v>
-      </c>
-      <c r="B592" s="3" t="s">
-        <v>1147</v>
       </c>
       <c r="C592" s="3" t="s">
         <v>201</v>
@@ -16293,12 +16305,12 @@
         <v>237</v>
       </c>
       <c r="H592" s="3" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="593" spans="1:8">
       <c r="A593" s="3" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B593" s="3" t="s">
         <v>179</v>
@@ -16319,15 +16331,15 @@
         <v>237</v>
       </c>
       <c r="H593" s="3" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="594" spans="1:8">
       <c r="A594" s="3" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B594" s="3" t="s">
         <v>1151</v>
-      </c>
-      <c r="B594" s="3" t="s">
-        <v>1152</v>
       </c>
       <c r="C594" s="3" t="s">
         <v>200</v>
@@ -16345,15 +16357,15 @@
         <v>239</v>
       </c>
       <c r="H594" s="3" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="595" spans="1:8">
       <c r="A595" s="3" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B595" s="3" t="s">
         <v>1154</v>
-      </c>
-      <c r="B595" s="3" t="s">
-        <v>1155</v>
       </c>
       <c r="C595" s="3" t="s">
         <v>200</v>
@@ -16371,7 +16383,7 @@
         <v>237</v>
       </c>
       <c r="H595" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="596" spans="1:8">
@@ -16397,15 +16409,15 @@
         <v>239</v>
       </c>
       <c r="H596" s="3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="597" spans="1:8">
       <c r="A597" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B597" s="3" t="s">
         <v>1157</v>
-      </c>
-      <c r="B597" s="3" t="s">
-        <v>1158</v>
       </c>
       <c r="C597" s="3" t="s">
         <v>200</v>
@@ -16423,15 +16435,15 @@
         <v>239</v>
       </c>
       <c r="H597" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="598" spans="1:8">
       <c r="A598" s="3" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B598" s="3" t="s">
         <v>1161</v>
-      </c>
-      <c r="B598" s="3" t="s">
-        <v>1162</v>
       </c>
       <c r="C598" s="3" t="s">
         <v>201</v>
@@ -16449,15 +16461,15 @@
         <v>237</v>
       </c>
       <c r="H598" s="3" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="599" spans="1:8">
       <c r="A599" s="3" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B599" s="3" t="s">
         <v>1164</v>
-      </c>
-      <c r="B599" s="3" t="s">
-        <v>1165</v>
       </c>
       <c r="C599" s="3" t="s">
         <v>201</v>
@@ -16475,15 +16487,15 @@
         <v>237</v>
       </c>
       <c r="H599" s="3" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="600" spans="1:8">
       <c r="A600" s="3" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B600" s="3" t="s">
         <v>1167</v>
-      </c>
-      <c r="B600" s="3" t="s">
-        <v>1168</v>
       </c>
       <c r="C600" s="3" t="s">
         <v>200</v>
@@ -16501,15 +16513,15 @@
         <v>237</v>
       </c>
       <c r="H600" s="3" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="601" spans="1:8">
       <c r="A601" s="3" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B601" s="3" t="s">
         <v>1170</v>
-      </c>
-      <c r="B601" s="3" t="s">
-        <v>1171</v>
       </c>
       <c r="C601" s="3" t="s">
         <v>199</v>
@@ -16527,12 +16539,12 @@
         <v>239</v>
       </c>
       <c r="H601" s="3" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="602" spans="1:8">
       <c r="A602" s="3" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="B602" s="3" t="s">
         <v>739</v>
@@ -16553,15 +16565,15 @@
         <v>239</v>
       </c>
       <c r="H602" s="3" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="603" spans="1:8">
       <c r="A603" s="3" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B603" s="3" t="s">
         <v>1175</v>
-      </c>
-      <c r="B603" s="3" t="s">
-        <v>1176</v>
       </c>
       <c r="C603" s="3" t="s">
         <v>200</v>
@@ -16579,15 +16591,15 @@
         <v>239</v>
       </c>
       <c r="H603" s="3" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="604" spans="1:8">
       <c r="A604" s="3" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B604" s="3" t="s">
         <v>1178</v>
-      </c>
-      <c r="B604" s="3" t="s">
-        <v>1179</v>
       </c>
       <c r="C604" s="3" t="s">
         <v>200</v>
@@ -16605,15 +16617,15 @@
         <v>239</v>
       </c>
       <c r="H604" s="3" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="605" spans="1:8">
       <c r="A605" s="3" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="B605" s="3" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="C605" s="3" t="s">
         <v>201</v>
@@ -16631,15 +16643,15 @@
         <v>237</v>
       </c>
       <c r="H605" s="3" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="606" spans="1:8">
       <c r="A606" s="3" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B606" s="3" t="s">
         <v>1183</v>
-      </c>
-      <c r="B606" s="3" t="s">
-        <v>1184</v>
       </c>
       <c r="C606" s="3" t="s">
         <v>200</v>
@@ -16657,15 +16669,15 @@
         <v>237</v>
       </c>
       <c r="H606" s="3" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="607" spans="1:8">
       <c r="A607" s="3" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B607" s="3" t="s">
         <v>1185</v>
-      </c>
-      <c r="B607" s="3" t="s">
-        <v>1186</v>
       </c>
       <c r="C607" s="3" t="s">
         <v>199</v>
@@ -16683,15 +16695,15 @@
         <v>239</v>
       </c>
       <c r="H607" s="3" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="608" spans="1:8">
       <c r="A608" s="3" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="B608" s="3" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C608" s="3" t="s">
         <v>200</v>
@@ -16709,15 +16721,15 @@
         <v>239</v>
       </c>
       <c r="H608" s="3" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="609" spans="1:8">
       <c r="A609" s="3" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B609" s="3" t="s">
         <v>1191</v>
-      </c>
-      <c r="B609" s="3" t="s">
-        <v>1192</v>
       </c>
       <c r="C609" s="3" t="s">
         <v>201</v>
@@ -16735,15 +16747,15 @@
         <v>239</v>
       </c>
       <c r="H609" s="3" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="610" spans="1:8">
       <c r="A610" s="3" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B610" s="3" t="s">
         <v>1194</v>
-      </c>
-      <c r="B610" s="3" t="s">
-        <v>1195</v>
       </c>
       <c r="C610" s="3" t="s">
         <v>200</v>
@@ -16761,15 +16773,15 @@
         <v>239</v>
       </c>
       <c r="H610" s="3" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="611" spans="1:8">
       <c r="A611" s="3" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B611" s="3" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="C611" s="3" t="s">
         <v>201</v>
@@ -16787,12 +16799,12 @@
         <v>237</v>
       </c>
       <c r="H611" s="3" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="612" spans="1:8">
       <c r="A612" s="3" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="C612" s="3" t="s">
         <v>199</v>
@@ -16806,7 +16818,7 @@
     </row>
     <row r="613" spans="1:8">
       <c r="A613" s="4" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B613" s="4" t="s">
         <v>144</v>
@@ -16827,15 +16839,15 @@
         <v>237</v>
       </c>
       <c r="H613" s="4" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="614" spans="1:8">
       <c r="A614" s="3" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B614" s="3" t="s">
         <v>1201</v>
-      </c>
-      <c r="B614" s="3" t="s">
-        <v>1202</v>
       </c>
       <c r="C614" s="3" t="s">
         <v>201</v>
@@ -16853,12 +16865,12 @@
         <v>237</v>
       </c>
       <c r="H614" s="3" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="615" spans="1:8">
       <c r="A615" s="3" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B615" s="3" t="s">
         <v>748</v>
@@ -16879,15 +16891,15 @@
         <v>237</v>
       </c>
       <c r="H615" s="3" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="616" spans="1:8">
       <c r="A616" s="3" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B616" s="3" t="s">
         <v>1208</v>
-      </c>
-      <c r="B616" s="3" t="s">
-        <v>1209</v>
       </c>
       <c r="C616" s="3" t="s">
         <v>201</v>
@@ -16905,15 +16917,15 @@
         <v>237</v>
       </c>
       <c r="H616" s="3" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="617" spans="1:8">
       <c r="A617" s="3" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B617" s="3" t="s">
         <v>1211</v>
-      </c>
-      <c r="B617" s="3" t="s">
-        <v>1212</v>
       </c>
       <c r="C617" s="3" t="s">
         <v>201</v>
@@ -16931,15 +16943,15 @@
         <v>237</v>
       </c>
       <c r="H617" s="3" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="618" spans="1:8">
       <c r="A618" s="3" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B618" s="3" t="s">
         <v>1214</v>
-      </c>
-      <c r="B618" s="3" t="s">
-        <v>1215</v>
       </c>
       <c r="C618" s="3" t="s">
         <v>199</v>
@@ -16957,15 +16969,15 @@
         <v>239</v>
       </c>
       <c r="H618" s="3" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="619" spans="1:8">
       <c r="A619" s="3" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B619" s="3" t="s">
         <v>1226</v>
-      </c>
-      <c r="B619" s="3" t="s">
-        <v>1227</v>
       </c>
       <c r="C619" s="3" t="s">
         <v>200</v>
@@ -16983,15 +16995,15 @@
         <v>239</v>
       </c>
       <c r="H619" s="3" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="620" spans="1:8">
       <c r="A620" s="3" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B620" s="3" t="s">
         <v>1222</v>
-      </c>
-      <c r="B620" s="3" t="s">
-        <v>1223</v>
       </c>
       <c r="C620" s="3" t="s">
         <v>200</v>
@@ -17009,15 +17021,15 @@
         <v>239</v>
       </c>
       <c r="H620" s="3" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="621" spans="1:8">
       <c r="A621" s="3" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B621" s="3" t="s">
         <v>1220</v>
-      </c>
-      <c r="B621" s="3" t="s">
-        <v>1221</v>
       </c>
       <c r="C621" s="3" t="s">
         <v>201</v>
@@ -17035,15 +17047,15 @@
         <v>237</v>
       </c>
       <c r="H621" s="3" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="622" spans="1:8">
       <c r="A622" s="3" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B622" s="3" t="s">
         <v>1229</v>
-      </c>
-      <c r="B622" s="3" t="s">
-        <v>1230</v>
       </c>
       <c r="C622" s="3" t="s">
         <v>200</v>
@@ -17061,15 +17073,15 @@
         <v>239</v>
       </c>
       <c r="H622" s="3" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="623" spans="1:8">
       <c r="A623" s="3" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B623" s="3" t="s">
         <v>1232</v>
-      </c>
-      <c r="B623" s="3" t="s">
-        <v>1233</v>
       </c>
       <c r="C623" s="3" t="s">
         <v>200</v>
@@ -17087,7 +17099,7 @@
         <v>237</v>
       </c>
       <c r="H623" s="3" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="624" spans="1:8">
@@ -17113,15 +17125,15 @@
         <v>239</v>
       </c>
       <c r="H624" s="3" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="625" spans="1:8">
       <c r="A625" s="3" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B625" s="3" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="C625" s="3" t="s">
         <v>200</v>
@@ -17139,12 +17151,12 @@
         <v>239</v>
       </c>
       <c r="H625" s="3" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="626" spans="1:8">
       <c r="A626" s="3" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="B626" s="3" t="s">
         <v>99</v>
@@ -17165,15 +17177,15 @@
         <v>237</v>
       </c>
       <c r="H626" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="627" spans="1:8">
       <c r="A627" s="3" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B627" s="3" t="s">
         <v>1240</v>
-      </c>
-      <c r="B627" s="3" t="s">
-        <v>1241</v>
       </c>
       <c r="C627" s="3" t="s">
         <v>200</v>
@@ -17191,15 +17203,15 @@
         <v>239</v>
       </c>
       <c r="H627" s="3" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="628" spans="1:8">
       <c r="A628" s="3" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B628" s="3" t="s">
         <v>1242</v>
-      </c>
-      <c r="B628" s="3" t="s">
-        <v>1243</v>
       </c>
       <c r="C628" s="3" t="s">
         <v>199</v>
@@ -17217,15 +17229,15 @@
         <v>237</v>
       </c>
       <c r="H628" s="3" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="629" spans="1:8">
       <c r="A629" s="3" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B629" s="3" t="s">
         <v>1245</v>
-      </c>
-      <c r="B629" s="3" t="s">
-        <v>1246</v>
       </c>
       <c r="C629" s="3" t="s">
         <v>201</v>
@@ -17243,15 +17255,15 @@
         <v>237</v>
       </c>
       <c r="H629" s="3" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="630" spans="1:8">
       <c r="A630" s="3" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B630" s="3" t="s">
         <v>1248</v>
-      </c>
-      <c r="B630" s="3" t="s">
-        <v>1249</v>
       </c>
       <c r="C630" s="3" t="s">
         <v>201</v>
@@ -17269,18 +17281,18 @@
         <v>237</v>
       </c>
       <c r="H630" s="3" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="631" spans="1:8">
       <c r="A631" s="3" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B631" s="3" t="s">
         <v>1251</v>
       </c>
-      <c r="B631" s="3" t="s">
-        <v>1252</v>
-      </c>
       <c r="C631" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D631" s="6">
         <v>2019</v>
@@ -17295,15 +17307,15 @@
         <v>237</v>
       </c>
       <c r="H631" s="3" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="632" spans="1:8">
       <c r="A632" s="3" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B632" s="3" t="s">
         <v>1254</v>
-      </c>
-      <c r="B632" s="3" t="s">
-        <v>1255</v>
       </c>
       <c r="C632" s="3" t="s">
         <v>200</v>
@@ -17321,12 +17333,12 @@
         <v>237</v>
       </c>
       <c r="H632" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="633" spans="1:8">
       <c r="A633" s="3" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B633" s="3" t="s">
         <v>800</v>
@@ -17347,15 +17359,15 @@
         <v>239</v>
       </c>
       <c r="H633" s="3" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="634" spans="1:8">
       <c r="A634" s="3" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B634" s="3" t="s">
         <v>1260</v>
-      </c>
-      <c r="B634" s="3" t="s">
-        <v>1261</v>
       </c>
       <c r="C634" s="3" t="s">
         <v>199</v>
@@ -17373,15 +17385,15 @@
         <v>237</v>
       </c>
       <c r="H634" s="3" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="635" spans="1:8">
       <c r="A635" s="3" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="B635" s="3" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="C635" s="3" t="s">
         <v>201</v>
@@ -17399,15 +17411,15 @@
         <v>237</v>
       </c>
       <c r="H635" s="3" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="636" spans="1:8">
       <c r="A636" s="3" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B636" s="3" t="s">
         <v>1267</v>
-      </c>
-      <c r="B636" s="3" t="s">
-        <v>1268</v>
       </c>
       <c r="C636" s="3" t="s">
         <v>199</v>
@@ -17425,15 +17437,15 @@
         <v>237</v>
       </c>
       <c r="H636" s="3" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="637" spans="1:8">
       <c r="A637" s="3" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B637" s="3" t="s">
         <v>1270</v>
-      </c>
-      <c r="B637" s="3" t="s">
-        <v>1271</v>
       </c>
       <c r="C637" s="3" t="s">
         <v>201</v>
@@ -17451,15 +17463,15 @@
         <v>237</v>
       </c>
       <c r="H637" s="3" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="638" spans="1:8">
       <c r="A638" s="3" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B638" s="3" t="s">
         <v>1272</v>
-      </c>
-      <c r="B638" s="3" t="s">
-        <v>1273</v>
       </c>
       <c r="C638" s="3" t="s">
         <v>199</v>
@@ -17477,15 +17489,15 @@
         <v>239</v>
       </c>
       <c r="H638" s="3" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="639" spans="1:8">
       <c r="A639" s="3" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B639" s="3" t="s">
         <v>1276</v>
-      </c>
-      <c r="B639" s="3" t="s">
-        <v>1277</v>
       </c>
       <c r="C639" s="3" t="s">
         <v>201</v>
@@ -17503,16 +17515,34 @@
         <v>239</v>
       </c>
       <c r="H639" s="3" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="640" spans="1:8">
+      <c r="A640" s="3" t="s">
         <v>1278</v>
       </c>
-    </row>
-    <row r="640" spans="1:8">
+      <c r="B640" s="3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C640" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D640" s="6">
         <v>2019</v>
       </c>
-      <c r="E640" s="6"/>
-      <c r="F640" s="6"/>
-      <c r="G640" s="6"/>
+      <c r="E640" s="6">
+        <v>2011</v>
+      </c>
+      <c r="F640" s="6">
+        <v>293</v>
+      </c>
+      <c r="G640" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H640" s="3" t="s">
+        <v>1279</v>
+      </c>
     </row>
     <row r="641" spans="4:7">
       <c r="D641" s="6">

</xml_diff>

<commit_message>
Man of the House
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF63C74-9596-D947-8A07-CCE23F6DB245}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE92137-AD51-8347-990C-516EE4674B2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2203" uniqueCount="1284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2208" uniqueCount="1287">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3877,6 +3877,15 @@
   </si>
   <si>
     <t>A year later, I read the second installment of Manchester's biography of Churchill. These books are wonderful and you get lost in them in a good way. While reading this I started reading and listening to The Rise and Fall of the Third Reich by Shirer, and was amazed to see that this volume is dedicated to him, and references him frequently. It is appalling how the leadership of Britain and France gave Hitler everything he wanted and more to avoid war, and it becomes apparent how WWII is really just the continuation of unsolved problems (esp. Versailles) from WWI. Churchill's firmness during a decade of ridicule and his consistency in speaking the truth about Hitler is nothing short of a lesson in holding firm to values. It was tragedy that brought him to power, and a vindication in spite of that tragedy. And even knowing how everything ends, Manchester makes the suspense real.</t>
+  </si>
+  <si>
+    <t>Man of the House: A Handbook for Building a Shelter That Will Last in a World That Is Falling Apart</t>
+  </si>
+  <si>
+    <t>C. R. Wiley</t>
+  </si>
+  <si>
+    <t>I came across C.R. Wiley in an excellent article in First Things, and this book was an inspiring call to arms for fathers as the head of the house. I want to build a family along the lines he describes: cultivating virtue, managing productive property, and taking responsibility.</t>
   </si>
 </sst>
 </file>
@@ -5464,7 +5473,7 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A625" workbookViewId="0">
-      <selection activeCell="A642" sqref="A642"/>
+      <selection activeCell="A643" sqref="A643"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -17606,12 +17615,30 @@
       </c>
     </row>
     <row r="643" spans="1:8">
+      <c r="A643" s="3" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B643" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C643" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D643" s="6">
         <v>2019</v>
       </c>
-      <c r="E643" s="6"/>
-      <c r="F643" s="6"/>
-      <c r="G643" s="6"/>
+      <c r="E643" s="6">
+        <v>2017</v>
+      </c>
+      <c r="F643" s="6">
+        <v>139</v>
+      </c>
+      <c r="G643" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H643" s="3" t="s">
+        <v>1286</v>
+      </c>
     </row>
     <row r="644" spans="1:8">
       <c r="D644" s="6">

</xml_diff>

<commit_message>
You Are Not a Gadget
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE92137-AD51-8347-990C-516EE4674B2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D189F49B-5DD2-0D4F-B95F-BB6006737D85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2208" uniqueCount="1287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2213" uniqueCount="1290">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3886,6 +3886,15 @@
   </si>
   <si>
     <t>I came across C.R. Wiley in an excellent article in First Things, and this book was an inspiring call to arms for fathers as the head of the house. I want to build a family along the lines he describes: cultivating virtue, managing productive property, and taking responsibility.</t>
+  </si>
+  <si>
+    <t>You Are Not a Gadget: A Manifesto</t>
+  </si>
+  <si>
+    <t>Jaron Lanier</t>
+  </si>
+  <si>
+    <t>I bought this in early 2017 on a recommendation from Cal Newport and finally got around to reading it. I do not agree with his worldview entirely (c.f. his comments on abortion), but he provides an interesting and helpful vision for technology development: - Main thesis: technology needs to consider the human person: "people have often respected bits too much, resulting in a creeping degradation of their own qualities as human beings" (119) --&gt; "If you hope for technology to be designed to serve people, you must have at least a rough idea of what a person is and is not." (154) - Technology reflects the philosophy of the person who created it. It is important to understand this both as a creator of technology (know your philosophy and have it be right) and as a consumer of technology (know what philosophy is enshrined in what you are using). - Technology is not reality, but a digital abstraction of reality), so keep these properly ordered.</t>
   </si>
 </sst>
 </file>
@@ -5473,7 +5482,7 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A625" workbookViewId="0">
-      <selection activeCell="A643" sqref="A643"/>
+      <selection activeCell="A645" sqref="A645"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -17641,12 +17650,30 @@
       </c>
     </row>
     <row r="644" spans="1:8">
+      <c r="A644" s="3" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B644" s="3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C644" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D644" s="6">
         <v>2019</v>
       </c>
-      <c r="E644" s="6"/>
-      <c r="F644" s="6"/>
-      <c r="G644" s="6"/>
+      <c r="E644" s="6">
+        <v>2010</v>
+      </c>
+      <c r="F644" s="6">
+        <v>192</v>
+      </c>
+      <c r="G644" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H644" s="3" t="s">
+        <v>1289</v>
+      </c>
     </row>
     <row r="645" spans="1:8">
       <c r="D645" s="6">

</xml_diff>

<commit_message>
The Rise and Fall of the Third Reich
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2218" uniqueCount="1293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2223" uniqueCount="1296">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3898,6 +3898,15 @@
   </si>
   <si>
     <t>Lauren Norelli recommended it and it is a page-turner for sure, as well as a terrifying look at what WWIII might look like. I espeically appreciated the role of the USS Zumwalt and its rail gun.</t>
+  </si>
+  <si>
+    <t>The Rise and Fall of the Third Reich: A History of Nazi Germany</t>
+  </si>
+  <si>
+    <t>William L. Shirer</t>
+  </si>
+  <si>
+    <t>I listened to this staring on Easter and it took me the whole season (plus a few days) to finish, but it was well worth the time to be immersed in the lessons coming from WWII. This was especially while finishing the second volume of *The Last Lion*. A sad fact is that there were so many opportunities to stop Hitler's rise. And yet the people of Germany were either unaware of easily distracted, and the Western democracies (led by Chamberlain) were so horrified by WWI that they went to absurd lengths to give Hitler whatever he wanted in the hope he wouldn't bring war. Likewise, once the Third Reich was at the peak of its power, there were many times it could have crushed Western civilization, but Hitler hesitated or made the wrong military decisions and thus the downfall was brought about. Shirer lets the facts speak for themselves, but he clearly disdains Hitler and the evil he brought about. More importantly for us though is his illustration of how people who could have easily stopped him allowed him to come to power, particularly the German people, the Appeasers in the West (Chamberlain), and his subordinates who never carried out a coup.</t>
   </si>
 </sst>
 </file>
@@ -5474,7 +5483,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5484,8 +5493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A625" workbookViewId="0">
-      <selection activeCell="A646" sqref="A646"/>
+    <sheetView tabSelected="1" topLeftCell="A637" workbookViewId="0">
+      <selection activeCell="A647" sqref="A647"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -17705,12 +17714,30 @@
       </c>
     </row>
     <row r="646" spans="1:8">
+      <c r="A646" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B646" s="3" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C646" s="3" t="s">
+        <v>200</v>
+      </c>
       <c r="D646" s="6">
         <v>2019</v>
       </c>
-      <c r="E646" s="6"/>
-      <c r="F646" s="6"/>
-      <c r="G646" s="6"/>
+      <c r="E646" s="6">
+        <v>1960</v>
+      </c>
+      <c r="F646" s="6">
+        <v>1143</v>
+      </c>
+      <c r="G646" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H646" s="3" t="s">
+        <v>1295</v>
+      </c>
     </row>
     <row r="647" spans="1:8">
       <c r="D647" s="6">

</xml_diff>

<commit_message>
The House At Pooh Corner
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2223" uniqueCount="1296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2228" uniqueCount="1298">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3907,6 +3907,12 @@
   </si>
   <si>
     <t>I listened to this staring on Easter and it took me the whole season (plus a few days) to finish, but it was well worth the time to be immersed in the lessons coming from WWII. This was especially while finishing the second volume of *The Last Lion*. A sad fact is that there were so many opportunities to stop Hitler's rise. And yet the people of Germany were either unaware of easily distracted, and the Western democracies (led by Chamberlain) were so horrified by WWI that they went to absurd lengths to give Hitler whatever he wanted in the hope he wouldn't bring war. Likewise, once the Third Reich was at the peak of its power, there were many times it could have crushed Western civilization, but Hitler hesitated or made the wrong military decisions and thus the downfall was brought about. Shirer lets the facts speak for themselves, but he clearly disdains Hitler and the evil he brought about. More importantly for us though is his illustration of how people who could have easily stopped him allowed him to come to power, particularly the German people, the Appeasers in the West (Chamberlain), and his subordinates who never carried out a coup.</t>
+  </si>
+  <si>
+    <t>The House At Pooh Corner</t>
+  </si>
+  <si>
+    <t>I started reading this with Henry last year, but he has become progressively impatient with and destructive toward books with paper pages. So I finished the last two myself and it was appropriate that  I did so on a Thursday that was particularly blustery!</t>
   </si>
 </sst>
 </file>
@@ -5483,7 +5489,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5493,8 +5499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A637" workbookViewId="0">
-      <selection activeCell="A647" sqref="A647"/>
+    <sheetView tabSelected="1" topLeftCell="A616" workbookViewId="0">
+      <selection activeCell="A648" sqref="A648"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -17740,12 +17746,30 @@
       </c>
     </row>
     <row r="647" spans="1:8">
+      <c r="A647" s="3" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B647" s="3" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C647" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D647" s="6">
         <v>2019</v>
       </c>
-      <c r="E647" s="6"/>
-      <c r="F647" s="6"/>
-      <c r="G647" s="6"/>
+      <c r="E647" s="6">
+        <v>1928</v>
+      </c>
+      <c r="F647" s="6">
+        <v>180</v>
+      </c>
+      <c r="G647" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H647" s="3" t="s">
+        <v>1297</v>
+      </c>
     </row>
     <row r="648" spans="1:8">
       <c r="D648" s="6">

</xml_diff>

<commit_message>
The Abolition of Man
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF405163-A3C9-6F4C-906C-8F4E37664DAE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="1302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2243" uniqueCount="1304">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -3925,13 +3931,19 @@
   </si>
   <si>
     <t>edited by Cassian A. Miles, O.F.M.</t>
+  </si>
+  <si>
+    <t>The Abolition of Man</t>
+  </si>
+  <si>
+    <t>This is the most visionary of Lewis' works I have read in his warnings against moral relativism and "men without chests", those ruled—in the end—only by their whims. It is scary how the picture he paints so closely resembles popular thought today. Natural law is, in fact, a thing, and forgetting this has some pretty unfortunate consequenses if allowed to play out to its end.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5505,21 +5517,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A631" workbookViewId="0">
-      <selection activeCell="A650" sqref="A650"/>
+      <selection activeCell="A651" sqref="A651"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="98" style="3" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="3" customWidth="1"/>
@@ -17840,12 +17852,30 @@
       </c>
     </row>
     <row r="650" spans="1:8">
+      <c r="A650" s="3" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B650" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C650" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D650" s="6">
         <v>2019</v>
       </c>
-      <c r="E650" s="6"/>
-      <c r="F650" s="6"/>
-      <c r="G650" s="6"/>
+      <c r="E650" s="6">
+        <v>1943</v>
+      </c>
+      <c r="F650" s="6">
+        <v>128</v>
+      </c>
+      <c r="G650" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H650" s="3" t="s">
+        <v>1303</v>
+      </c>
     </row>
     <row r="651" spans="1:8">
       <c r="D651" s="6">

</xml_diff>

<commit_message>
Into the Rising Sun
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E09E61-A77B-4541-A701-7BF021EDD51A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA6B35D-9346-744D-9709-B621AAF55991}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2283" uniqueCount="1324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2288" uniqueCount="1327">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4003,6 +4003,15 @@
   </si>
   <si>
     <t>Peter Kreeft recommended this to me in his response to my letter asking about Aquinas' view of capitalism. It took me a little while to finish despite being a short book, but it has a simple thesis: capitalism is inherently unstable and will eventually devolve into a) communism, b) distributism, or c) the servile state. He agrues that because of difficulties transitioning to a) and b) the natural end state is the servile state. The servile state consists of compulsory labor legally enforcible upon those who do not own the means of production for the advantage of those who do. Interesting is his foresight into later developments in the 20th century toward a more servile working class, and his example of liability laws (workers compensation for example) that while they may seem to be good, actually codify the class differences he describes.</t>
+  </si>
+  <si>
+    <t>Into the Rising Sun: World War II's Pacific Veterans Reveal the Heart of Combat</t>
+  </si>
+  <si>
+    <t>Patrick K. O'Donnell</t>
+  </si>
+  <si>
+    <t>Dad sent a clip from this book about a soldier who just kept going despite two broken arms, maggots eating his flesh, several days without food, and found it within himself to get back and survive. I know less about the war in the Pacific as compared with that in Europe, and the stories here show how it was hell in its own way. This is important to remember and helpful to put our struggles in perspective.</t>
   </si>
 </sst>
 </file>
@@ -5603,7 +5612,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A634" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A659" sqref="A659"/>
+      <selection pane="bottomLeft" activeCell="A660" sqref="A660"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18166,12 +18175,30 @@
       </c>
     </row>
     <row r="659" spans="1:8">
+      <c r="A659" s="3" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B659" s="3" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C659" s="3" t="s">
+        <v>200</v>
+      </c>
       <c r="D659" s="6">
         <v>2019</v>
       </c>
-      <c r="E659" s="6"/>
-      <c r="F659" s="6"/>
-      <c r="G659" s="6"/>
+      <c r="E659" s="6">
+        <v>2002</v>
+      </c>
+      <c r="F659" s="6">
+        <v>320</v>
+      </c>
+      <c r="G659" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H659" s="3" t="s">
+        <v>1326</v>
+      </c>
     </row>
     <row r="660" spans="1:8">
       <c r="D660" s="6">

</xml_diff>

<commit_message>
A Plan of Life
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABF3BA7-1100-A74D-A666-7A2BF27EB44E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC8CF8C-4238-744C-8CF3-53B15D8C29CF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2298" uniqueCount="1330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2303" uniqueCount="1333">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4021,6 +4021,15 @@
   </si>
   <si>
     <t>Great to listen to while moving, and really interesting to view from the point of view of an animal.</t>
+  </si>
+  <si>
+    <t>Joseph M. Muntadas</t>
+  </si>
+  <si>
+    <t>A Plan of Life</t>
+  </si>
+  <si>
+    <t>In looking for *Reading* by Joseph B. Stenson, I came across all the free booklets online published by Scepter publishers, and decided to read this one first. Very short but very practical advice from St. Josemaría Escrivá about living a Christian life well.</t>
   </si>
 </sst>
 </file>
@@ -5620,8 +5629,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A648" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A662" sqref="A662"/>
+      <pane ySplit="1" topLeftCell="A645" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A663" sqref="A663"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18262,12 +18271,30 @@
       </c>
     </row>
     <row r="662" spans="1:8">
+      <c r="A662" s="3" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B662" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C662" s="3" t="s">
+        <v>947</v>
+      </c>
       <c r="D662" s="6">
         <v>2019</v>
       </c>
-      <c r="E662" s="6"/>
-      <c r="F662" s="6"/>
-      <c r="G662" s="6"/>
+      <c r="E662" s="6">
+        <v>1977</v>
+      </c>
+      <c r="F662" s="6">
+        <v>23</v>
+      </c>
+      <c r="G662" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H662" s="3" t="s">
+        <v>1332</v>
+      </c>
     </row>
     <row r="663" spans="1:8">
       <c r="D663" s="6">
@@ -18278,49 +18305,65 @@
       <c r="G663" s="6"/>
     </row>
     <row r="664" spans="1:8">
-      <c r="D664" s="6"/>
+      <c r="D664" s="6">
+        <v>2019</v>
+      </c>
       <c r="E664" s="6"/>
       <c r="F664" s="6"/>
       <c r="G664" s="6"/>
     </row>
     <row r="665" spans="1:8">
-      <c r="D665" s="6"/>
+      <c r="D665" s="6">
+        <v>2019</v>
+      </c>
       <c r="E665" s="6"/>
       <c r="F665" s="6"/>
       <c r="G665" s="6"/>
     </row>
     <row r="666" spans="1:8">
-      <c r="D666" s="6"/>
+      <c r="D666" s="6">
+        <v>2019</v>
+      </c>
       <c r="E666" s="6"/>
       <c r="F666" s="6"/>
       <c r="G666" s="6"/>
     </row>
     <row r="667" spans="1:8">
-      <c r="D667" s="6"/>
+      <c r="D667" s="6">
+        <v>2019</v>
+      </c>
       <c r="E667" s="6"/>
       <c r="F667" s="6"/>
       <c r="G667" s="6"/>
     </row>
     <row r="668" spans="1:8">
-      <c r="D668" s="6"/>
+      <c r="D668" s="6">
+        <v>2019</v>
+      </c>
       <c r="E668" s="6"/>
       <c r="F668" s="6"/>
       <c r="G668" s="6"/>
     </row>
     <row r="669" spans="1:8">
-      <c r="D669" s="6"/>
+      <c r="D669" s="6">
+        <v>2019</v>
+      </c>
       <c r="E669" s="6"/>
       <c r="F669" s="6"/>
       <c r="G669" s="6"/>
     </row>
     <row r="670" spans="1:8">
-      <c r="D670" s="6"/>
+      <c r="D670" s="6">
+        <v>2019</v>
+      </c>
       <c r="E670" s="6"/>
       <c r="F670" s="6"/>
       <c r="G670" s="6"/>
     </row>
     <row r="671" spans="1:8">
-      <c r="D671" s="6"/>
+      <c r="D671" s="6">
+        <v>2019</v>
+      </c>
       <c r="E671" s="6"/>
       <c r="F671" s="6"/>
       <c r="G671" s="6"/>

</xml_diff>

<commit_message>
Think and Grow Rich
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC8CF8C-4238-744C-8CF3-53B15D8C29CF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2D595A-C64E-CA47-9D0F-13EF85BC4DB1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2303" uniqueCount="1333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2308" uniqueCount="1336">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4030,6 +4030,15 @@
   </si>
   <si>
     <t>In looking for *Reading* by Joseph B. Stenson, I came across all the free booklets online published by Scepter publishers, and decided to read this one first. Very short but very practical advice from St. Josemaría Escrivá about living a Christian life well.</t>
+  </si>
+  <si>
+    <t>Think and Grow Rich</t>
+  </si>
+  <si>
+    <t>Napoleon Hill</t>
+  </si>
+  <si>
+    <t>Despite seeing this highly recommended a few places, I cannot do the same. Half of this book is common sense for which a book is not required, and the other half is either unhelpful, unscientific, heretical, or lacking in the proper ordering of the pursuit of money in life. Self-help money books that give the advice that you "need to make money your first and only priority in life" kind of miss the point. And this book is openly anti-Christian in a way that feels very early-20th century.</t>
   </si>
 </sst>
 </file>
@@ -5630,7 +5639,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A645" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A663" sqref="A663"/>
+      <selection pane="bottomLeft" activeCell="A664" sqref="A664"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18297,12 +18306,30 @@
       </c>
     </row>
     <row r="663" spans="1:8">
+      <c r="A663" s="3" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B663" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C663" s="3" t="s">
+        <v>200</v>
+      </c>
       <c r="D663" s="6">
         <v>2019</v>
       </c>
-      <c r="E663" s="6"/>
-      <c r="F663" s="6"/>
-      <c r="G663" s="6"/>
+      <c r="E663" s="6">
+        <v>1937</v>
+      </c>
+      <c r="F663" s="6">
+        <v>273</v>
+      </c>
+      <c r="G663" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H663" s="3" t="s">
+        <v>1335</v>
+      </c>
     </row>
     <row r="664" spans="1:8">
       <c r="D664" s="6">

</xml_diff>

<commit_message>
Heaven in Stone and Glass
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6794EC5C-1CF7-DD48-B5E7-EE538F426A01}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE5E192-0E72-F34C-B462-CB8B9B07DFF9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="1345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2328" uniqueCount="1347">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4066,6 +4066,12 @@
   </si>
   <si>
     <t>A beautiful reflection on how "there is no pit so deep that God's love is not deeper still." Nazi Germany was horrible and yet it created so many beautiful saints.</t>
+  </si>
+  <si>
+    <t>Heaven in Stone and Glass: Experiencing the Spirituality of the Great Cathedrals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You know a book is good (and points to something more) when your pulse is elevated when reading it and you feel at peace and like you have so much to do at the same time. This is a beautiful reflection on the spirituality of gothic cathedrals. It brought me back to Chartres and Notre Dame de Paris (and want to return in person). </t>
   </si>
 </sst>
 </file>
@@ -5666,7 +5672,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A645" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A667" sqref="A667"/>
+      <selection pane="bottomLeft" activeCell="A668" sqref="A668"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18437,12 +18443,30 @@
       </c>
     </row>
     <row r="667" spans="1:8">
+      <c r="A667" s="3" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B667" s="3" t="s">
+        <v>797</v>
+      </c>
+      <c r="C667" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D667" s="6">
         <v>2019</v>
       </c>
-      <c r="E667" s="6"/>
-      <c r="F667" s="6"/>
-      <c r="G667" s="6"/>
+      <c r="E667" s="6">
+        <v>2000</v>
+      </c>
+      <c r="F667" s="6">
+        <v>128</v>
+      </c>
+      <c r="G667" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H667" s="3" t="s">
+        <v>1346</v>
+      </c>
     </row>
     <row r="668" spans="1:8">
       <c r="D668" s="6">

</xml_diff>

<commit_message>
Edith Stein: Essential Writings
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069274DB-B21B-8B4D-A837-B269FB35E66C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0906635-DE0A-6D41-844A-DB7D70CDCF00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="1350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2338" uniqueCount="1353">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4081,6 +4081,15 @@
   </si>
   <si>
     <t>This was a scary read revealing the science behind behavioral addition tied to mobile technology and social networks. Another reminder to guard our attention and that of our kids.</t>
+  </si>
+  <si>
+    <t>Edith Stein: Essential Writings</t>
+  </si>
+  <si>
+    <t>Edith Stein (selected by John Sullivan, OCD)</t>
+  </si>
+  <si>
+    <t>Somehow reading Edith Stein feels like I'm reading someone much *older* than her, perhaps St. Theresa of Ávila who she looked up to so much. She is a beautiful saint.</t>
   </si>
 </sst>
 </file>
@@ -5681,7 +5690,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A645" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A669" sqref="A669"/>
+      <selection pane="bottomLeft" activeCell="A670" sqref="A670"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18504,12 +18513,30 @@
       </c>
     </row>
     <row r="669" spans="1:8">
+      <c r="A669" s="3" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B669" s="3" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C669" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D669" s="6">
         <v>2019</v>
       </c>
-      <c r="E669" s="6"/>
-      <c r="F669" s="6"/>
-      <c r="G669" s="6"/>
+      <c r="E669" s="6">
+        <v>2002</v>
+      </c>
+      <c r="F669" s="6">
+        <v>158</v>
+      </c>
+      <c r="G669" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H669" s="3" t="s">
+        <v>1352</v>
+      </c>
     </row>
     <row r="670" spans="1:8">
       <c r="D670" s="6">

</xml_diff>

<commit_message>
How to Make a Good Confession
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0906635-DE0A-6D41-844A-DB7D70CDCF00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA5307C-92DA-534B-9E0B-26C7A2EE6AA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2338" uniqueCount="1353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="1356">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4090,6 +4090,15 @@
   </si>
   <si>
     <t>Somehow reading Edith Stein feels like I'm reading someone much *older* than her, perhaps St. Theresa of Ávila who she looked up to so much. She is a beautiful saint.</t>
+  </si>
+  <si>
+    <t>How to Make a Good Confession: A Pocket Guide to Reconciliation with God</t>
+  </si>
+  <si>
+    <t>John A. Kane</t>
+  </si>
+  <si>
+    <t>I saw someone reading this at St. Pats and am glad I read it also. Fr. Kane discusses how to cultivate true contrition, found your repantence on Christ’s tender mercy, let sorrow for sin help you overcome your sins, combat your pride though sacramental confession, make reparation for your sins, resolve to change. Especially important to me is the need to be perpetually penitent.</t>
   </si>
 </sst>
 </file>
@@ -5690,7 +5699,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A645" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A670" sqref="A670"/>
+      <selection pane="bottomLeft" activeCell="A671" sqref="A671"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18539,12 +18548,30 @@
       </c>
     </row>
     <row r="670" spans="1:8">
+      <c r="A670" s="3" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B670" s="3" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C670" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D670" s="6">
         <v>2019</v>
       </c>
-      <c r="E670" s="6"/>
-      <c r="F670" s="6"/>
-      <c r="G670" s="6"/>
+      <c r="E670" s="6">
+        <v>1943</v>
+      </c>
+      <c r="F670" s="6">
+        <v>130</v>
+      </c>
+      <c r="G670" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H670" s="3" t="s">
+        <v>1355</v>
+      </c>
     </row>
     <row r="671" spans="1:8">
       <c r="D671" s="6">

</xml_diff>

<commit_message>
The Rule of St. Benedict
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA5307C-92DA-534B-9E0B-26C7A2EE6AA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95731771-F175-3E48-9D63-9B14E2C1AC34}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="1356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2348" uniqueCount="1359">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4099,6 +4099,15 @@
   </si>
   <si>
     <t>I saw someone reading this at St. Pats and am glad I read it also. Fr. Kane discusses how to cultivate true contrition, found your repantence on Christ’s tender mercy, let sorrow for sin help you overcome your sins, combat your pride though sacramental confession, make reparation for your sins, resolve to change. Especially important to me is the need to be perpetually penitent.</t>
+  </si>
+  <si>
+    <t>The Rule of St. Benedict in English</t>
+  </si>
+  <si>
+    <t>St. Benedict (edited by Timothy Fry, O.S.B.)</t>
+  </si>
+  <si>
+    <t>This has been referenced repeatedly in my other reading, most recently by Edith Stein. His rule is simple for a simple way of life.</t>
   </si>
 </sst>
 </file>
@@ -5698,8 +5707,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A645" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A671" sqref="A671"/>
+      <pane ySplit="1" topLeftCell="A650" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A672" sqref="A672"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18574,12 +18583,30 @@
       </c>
     </row>
     <row r="671" spans="1:8">
+      <c r="A671" s="3" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B671" s="3" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C671" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D671" s="6">
         <v>2019</v>
       </c>
-      <c r="E671" s="6"/>
-      <c r="F671" s="6"/>
-      <c r="G671" s="6"/>
+      <c r="E671" s="6">
+        <v>516</v>
+      </c>
+      <c r="F671" s="6">
+        <v>96</v>
+      </c>
+      <c r="G671" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H671" s="3" t="s">
+        <v>1358</v>
+      </c>
     </row>
     <row r="672" spans="1:8">
       <c r="D672" s="6"/>

</xml_diff>

<commit_message>
The Hard Thing About Hard Things
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C6ACAC-DAFC-EB47-9442-6CBC17F3FF71}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FD53DF-7AD4-6C49-9792-4C0E87FEA14D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="1361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2358" uniqueCount="1364">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4114,6 +4114,15 @@
   </si>
   <si>
     <t>St. Augustine (introduction and commentary by Tarsicius J. Van Bavel, OSA)</t>
+  </si>
+  <si>
+    <t>The Hard Thing About Hard Things: Building a Business When There Are No Easy Answers</t>
+  </si>
+  <si>
+    <t>Ben Horowitz</t>
+  </si>
+  <si>
+    <t>Cory gave this to me before leaving Milestone and it was a fascenating read. Unlike a lot of "management" book, this guy actually has experience making tough calls and has some great advice, some of which is for a level I don't want to be at, but some of which (like good product manager, bad product manager and the concept of management debt) are very helpful.</t>
   </si>
 </sst>
 </file>
@@ -5714,7 +5723,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A648" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A673" sqref="A673"/>
+      <selection pane="bottomLeft" activeCell="A674" sqref="A674"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18640,15 +18649,33 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="673" spans="4:7">
+    <row r="673" spans="1:8">
+      <c r="A673" s="3" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B673" s="3" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C673" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="D673" s="6">
         <v>2019</v>
       </c>
-      <c r="E673" s="6"/>
-      <c r="F673" s="6"/>
-      <c r="G673" s="6"/>
-    </row>
-    <row r="674" spans="4:7">
+      <c r="E673" s="6">
+        <v>2014</v>
+      </c>
+      <c r="F673" s="6">
+        <v>286</v>
+      </c>
+      <c r="G673" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H673" s="3" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="674" spans="1:8">
       <c r="D674" s="6">
         <v>2019</v>
       </c>
@@ -18656,7 +18683,7 @@
       <c r="F674" s="6"/>
       <c r="G674" s="6"/>
     </row>
-    <row r="675" spans="4:7">
+    <row r="675" spans="1:8">
       <c r="D675" s="6">
         <v>2019</v>
       </c>
@@ -18664,7 +18691,7 @@
       <c r="F675" s="6"/>
       <c r="G675" s="6"/>
     </row>
-    <row r="676" spans="4:7">
+    <row r="676" spans="1:8">
       <c r="D676" s="6">
         <v>2019</v>
       </c>
@@ -18672,7 +18699,7 @@
       <c r="F676" s="6"/>
       <c r="G676" s="6"/>
     </row>
-    <row r="677" spans="4:7">
+    <row r="677" spans="1:8">
       <c r="D677" s="6">
         <v>2019</v>
       </c>
@@ -18680,7 +18707,7 @@
       <c r="F677" s="6"/>
       <c r="G677" s="6"/>
     </row>
-    <row r="678" spans="4:7">
+    <row r="678" spans="1:8">
       <c r="D678" s="6">
         <v>2019</v>
       </c>
@@ -18688,7 +18715,7 @@
       <c r="F678" s="6"/>
       <c r="G678" s="6"/>
     </row>
-    <row r="679" spans="4:7">
+    <row r="679" spans="1:8">
       <c r="D679" s="6">
         <v>2019</v>
       </c>
@@ -18696,7 +18723,7 @@
       <c r="F679" s="6"/>
       <c r="G679" s="6"/>
     </row>
-    <row r="680" spans="4:7">
+    <row r="680" spans="1:8">
       <c r="D680" s="6">
         <v>2019</v>
       </c>
@@ -18704,7 +18731,7 @@
       <c r="F680" s="6"/>
       <c r="G680" s="6"/>
     </row>
-    <row r="681" spans="4:7">
+    <row r="681" spans="1:8">
       <c r="D681" s="6">
         <v>2019</v>
       </c>
@@ -18712,7 +18739,7 @@
       <c r="F681" s="6"/>
       <c r="G681" s="6"/>
     </row>
-    <row r="682" spans="4:7">
+    <row r="682" spans="1:8">
       <c r="D682" s="6">
         <v>2019</v>
       </c>
@@ -18720,7 +18747,7 @@
       <c r="F682" s="6"/>
       <c r="G682" s="6"/>
     </row>
-    <row r="683" spans="4:7">
+    <row r="683" spans="1:8">
       <c r="D683" s="6">
         <v>2019</v>
       </c>
@@ -18728,7 +18755,7 @@
       <c r="F683" s="6"/>
       <c r="G683" s="6"/>
     </row>
-    <row r="684" spans="4:7">
+    <row r="684" spans="1:8">
       <c r="D684" s="6">
         <v>2019</v>
       </c>
@@ -18736,7 +18763,7 @@
       <c r="F684" s="6"/>
       <c r="G684" s="6"/>
     </row>
-    <row r="685" spans="4:7">
+    <row r="685" spans="1:8">
       <c r="D685" s="6">
         <v>2019</v>
       </c>
@@ -18744,7 +18771,7 @@
       <c r="F685" s="6"/>
       <c r="G685" s="6"/>
     </row>
-    <row r="686" spans="4:7">
+    <row r="686" spans="1:8">
       <c r="D686" s="6">
         <v>2019</v>
       </c>
@@ -18752,7 +18779,7 @@
       <c r="F686" s="6"/>
       <c r="G686" s="6"/>
     </row>
-    <row r="687" spans="4:7">
+    <row r="687" spans="1:8">
       <c r="D687" s="6">
         <v>2019</v>
       </c>
@@ -18760,7 +18787,7 @@
       <c r="F687" s="6"/>
       <c r="G687" s="6"/>
     </row>
-    <row r="688" spans="4:7">
+    <row r="688" spans="1:8">
       <c r="D688" s="6">
         <v>2019</v>
       </c>

</xml_diff>

<commit_message>
Edgar Allan Poe short stories
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FD53DF-7AD4-6C49-9792-4C0E87FEA14D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91805DBA-2A3F-5549-B3C6-D97C35B998BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="16720" windowWidth="28800" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2358" uniqueCount="1364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="1367">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4123,6 +4123,15 @@
   </si>
   <si>
     <t>Cory gave this to me before leaving Milestone and it was a fascenating read. Unlike a lot of "management" book, this guy actually has experience making tough calls and has some great advice, some of which is for a level I don't want to be at, but some of which (like good product manager, bad product manager and the concept of management debt) are very helpful.</t>
+  </si>
+  <si>
+    <t>Edgar Allan Poe</t>
+  </si>
+  <si>
+    <t>"The Pit and the Pendulum", "The Tell-Tale Heart", and "The Cask of Amontillado"</t>
+  </si>
+  <si>
+    <t>BC11: Ben suggested we read some Poe for our next read-aloud book club, and we had fun reading and discussing "The Pit and the Pendulum". I decided to read a couple others of his that others recommended.</t>
   </si>
 </sst>
 </file>
@@ -5722,8 +5731,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A648" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A674" sqref="A674"/>
+      <pane ySplit="1" topLeftCell="A666" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F675" sqref="F675"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18676,12 +18685,30 @@
       </c>
     </row>
     <row r="674" spans="1:8">
+      <c r="A674" s="3" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B674" s="3" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C674" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="D674" s="6">
         <v>2019</v>
       </c>
-      <c r="E674" s="6"/>
-      <c r="F674" s="6"/>
-      <c r="G674" s="6"/>
+      <c r="E674" s="6">
+        <v>1842</v>
+      </c>
+      <c r="F674" s="6">
+        <v>50</v>
+      </c>
+      <c r="G674" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H674" s="3" t="s">
+        <v>1366</v>
+      </c>
     </row>
     <row r="675" spans="1:8">
       <c r="D675" s="6">

</xml_diff>

<commit_message>
The Way of a Pilgrim
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91805DBA-2A3F-5549-B3C6-D97C35B998BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CDAF0C-25F6-E642-81F1-9CB67D632852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="16720" windowWidth="28800" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="1367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2368" uniqueCount="1370">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4132,6 +4132,15 @@
   </si>
   <si>
     <t>BC11: Ben suggested we read some Poe for our next read-aloud book club, and we had fun reading and discussing "The Pit and the Pendulum". I decided to read a couple others of his that others recommended.</t>
+  </si>
+  <si>
+    <t>The Way of a Pilgrim</t>
+  </si>
+  <si>
+    <t>edited by G. P. Fedotov</t>
+  </si>
+  <si>
+    <t>Apparently this was one of Pops' favorite books, and for good reason being a beautiful reflection on interior prayer. "Lord Jesus Chris, have mercy on me."</t>
   </si>
 </sst>
 </file>
@@ -5732,7 +5741,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A666" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F675" sqref="F675"/>
+      <selection pane="bottomLeft" activeCell="A676" sqref="A676"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18701,7 +18710,7 @@
         <v>1842</v>
       </c>
       <c r="F674" s="6">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G674" s="6" t="s">
         <v>238</v>
@@ -18711,12 +18720,30 @@
       </c>
     </row>
     <row r="675" spans="1:8">
+      <c r="A675" s="3" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B675" s="3" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C675" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="D675" s="6">
         <v>2019</v>
       </c>
-      <c r="E675" s="6"/>
-      <c r="F675" s="6"/>
-      <c r="G675" s="6"/>
+      <c r="E675" s="6">
+        <v>1884</v>
+      </c>
+      <c r="F675" s="6">
+        <v>65</v>
+      </c>
+      <c r="G675" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H675" s="3" t="s">
+        <v>1369</v>
+      </c>
     </row>
     <row r="676" spans="1:8">
       <c r="D676" s="6">

</xml_diff>

<commit_message>
The Jesus Storybook Bible
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CDAF0C-25F6-E642-81F1-9CB67D632852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCED449-AE7B-0548-BF9B-AC5B3596498F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2368" uniqueCount="1370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2373" uniqueCount="1373">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4141,6 +4141,15 @@
   </si>
   <si>
     <t>Apparently this was one of Pops' favorite books, and for good reason being a beautiful reflection on interior prayer. "Lord Jesus Chris, have mercy on me."</t>
+  </si>
+  <si>
+    <t>The Jesus Storybook Bible: Every Story Whispers His Name</t>
+  </si>
+  <si>
+    <t>Sally Lloyd-Jones</t>
+  </si>
+  <si>
+    <t>This is a great bible for kids, and maybe even a better bible for grownups. The stories are necessarily shortened, but in doing so Sally is always hinting at Christ and weaving the narrative of the story of salvation, or God's "rescue plan." I read this to Henry over the course of many months, at a much slower pace recently now that he has no attention span. But it's a perfect size for him to hold and he loves gently flipping through the pictures.</t>
   </si>
 </sst>
 </file>
@@ -5741,7 +5750,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A666" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A676" sqref="A676"/>
+      <selection pane="bottomLeft" activeCell="A677" sqref="A677"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18746,12 +18755,30 @@
       </c>
     </row>
     <row r="676" spans="1:8">
+      <c r="A676" s="3" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B676" s="3" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C676" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="D676" s="6">
         <v>2019</v>
       </c>
-      <c r="E676" s="6"/>
-      <c r="F676" s="6"/>
-      <c r="G676" s="6"/>
+      <c r="E676" s="6">
+        <v>2007</v>
+      </c>
+      <c r="F676" s="6">
+        <v>352</v>
+      </c>
+      <c r="G676" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H676" s="3" t="s">
+        <v>1372</v>
+      </c>
     </row>
     <row r="677" spans="1:8">
       <c r="D677" s="6">

</xml_diff>

<commit_message>
Structures: Or Why Things Don't Fall Down
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCED449-AE7B-0548-BF9B-AC5B3596498F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EFF60A-5661-194F-8E34-3D1AF3D80523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2373" uniqueCount="1373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2378" uniqueCount="1374">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -2349,9 +2349,6 @@
     <t>Fr. Godfrey Poage, C.P.</t>
   </si>
   <si>
-    <t>J.E. Gordon</t>
-  </si>
-  <si>
     <t xml:space="preserve">Maura Poston Zagrans </t>
   </si>
   <si>
@@ -4150,6 +4147,12 @@
   </si>
   <si>
     <t>This is a great bible for kids, and maybe even a better bible for grownups. The stories are necessarily shortened, but in doing so Sally is always hinting at Christ and weaving the narrative of the story of salvation, or God's "rescue plan." I read this to Henry over the course of many months, at a much slower pace recently now that he has no attention span. But it's a perfect size for him to hold and he loves gently flipping through the pictures.</t>
+  </si>
+  <si>
+    <t>J. E. Gordon</t>
+  </si>
+  <si>
+    <t>I first read this at Cape Cod the summer before starting as an engineer at SpaceX. I think it really can be considered a classic in that it demonstrates mastery of its subject in an accessible way while relating that to all other knowledge. A thoroughly enjoyable and interesting book, as well as one that challenges you to think about the philosphy of design in the last two chapters.</t>
   </si>
 </sst>
 </file>
@@ -5749,8 +5752,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A666" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A677" sqref="A677"/>
+      <pane ySplit="1" topLeftCell="A632" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A678" sqref="A678"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5788,10 +5791,10 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>198</v>
@@ -5806,10 +5809,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>198</v>
@@ -5824,10 +5827,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>198</v>
@@ -5842,10 +5845,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>198</v>
@@ -5860,10 +5863,10 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>198</v>
@@ -5878,10 +5881,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>198</v>
@@ -5896,10 +5899,10 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>198</v>
@@ -5914,10 +5917,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>198</v>
@@ -5932,7 +5935,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>628</v>
@@ -5950,7 +5953,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>628</v>
@@ -5968,7 +5971,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>628</v>
@@ -5986,10 +5989,10 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>198</v>
@@ -6004,10 +6007,10 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>1006</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>1007</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>198</v>
@@ -6022,10 +6025,10 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>198</v>
@@ -6040,10 +6043,10 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>198</v>
@@ -6058,10 +6061,10 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>198</v>
@@ -6076,10 +6079,10 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>198</v>
@@ -6094,10 +6097,10 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>198</v>
@@ -6112,10 +6115,10 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>198</v>
@@ -6130,10 +6133,10 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>198</v>
@@ -6148,7 +6151,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>640</v>
@@ -6166,10 +6169,10 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>198</v>
@@ -6184,10 +6187,10 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>198</v>
@@ -6202,7 +6205,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>626</v>
@@ -6220,7 +6223,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>686</v>
@@ -6238,7 +6241,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>625</v>
@@ -6256,10 +6259,10 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>198</v>
@@ -6274,7 +6277,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>630</v>
@@ -6292,10 +6295,10 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>198</v>
@@ -6310,10 +6313,10 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>198</v>
@@ -6328,10 +6331,10 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>198</v>
@@ -6346,10 +6349,10 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>198</v>
@@ -6364,7 +6367,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>245</v>
@@ -6619,7 +6622,7 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="8" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>625</v>
@@ -8083,7 +8086,7 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" s="3" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>690</v>
@@ -8867,7 +8870,7 @@
         <v>404</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D191" s="6">
         <v>2013</v>
@@ -9066,7 +9069,7 @@
     </row>
     <row r="204" spans="1:6">
       <c r="A204" s="3" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="B204" s="3" t="s">
         <v>737</v>
@@ -9325,7 +9328,7 @@
         <v>187</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D220" s="6">
         <v>2013</v>
@@ -9386,7 +9389,7 @@
         <v>436</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="C224" s="4" t="s">
         <v>198</v>
@@ -9405,7 +9408,7 @@
         <v>187</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D225" s="6">
         <v>2014</v>
@@ -9418,7 +9421,7 @@
         <v>438</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D226" s="6">
         <v>2014</v>
@@ -9431,7 +9434,7 @@
         <v>439</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D227" s="6">
         <v>2014</v>
@@ -9444,7 +9447,7 @@
         <v>440</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D228" s="6">
         <v>2014</v>
@@ -9460,7 +9463,7 @@
         <v>608</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D229" s="6">
         <v>2014</v>
@@ -9636,7 +9639,7 @@
         <v>757</v>
       </c>
       <c r="C240" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D240" s="6">
         <v>2014</v>
@@ -9889,7 +9892,7 @@
         <v>467</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>772</v>
+        <v>1372</v>
       </c>
       <c r="C256" s="3" t="s">
         <v>200</v>
@@ -9921,7 +9924,7 @@
         <v>469</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C258" s="3" t="s">
         <v>199</v>
@@ -9937,7 +9940,7 @@
         <v>470</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C259" s="3" t="s">
         <v>198</v>
@@ -9953,7 +9956,7 @@
         <v>471</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C260" s="3" t="s">
         <v>199</v>
@@ -9969,7 +9972,7 @@
         <v>472</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C261" s="3" t="s">
         <v>198</v>
@@ -10001,7 +10004,7 @@
         <v>474</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C263" s="3" t="s">
         <v>198</v>
@@ -10033,7 +10036,7 @@
         <v>476</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C265" s="3" t="s">
         <v>199</v>
@@ -10049,7 +10052,7 @@
         <v>477</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C266" s="3" t="s">
         <v>198</v>
@@ -10065,7 +10068,7 @@
         <v>478</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C267" s="3" t="s">
         <v>200</v>
@@ -10097,7 +10100,7 @@
         <v>480</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C269" s="3" t="s">
         <v>198</v>
@@ -10145,7 +10148,7 @@
         <v>483</v>
       </c>
       <c r="B272" s="4" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C272" s="4" t="s">
         <v>198</v>
@@ -10161,7 +10164,7 @@
         <v>304</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C273" s="3" t="s">
         <v>198</v>
@@ -10177,7 +10180,7 @@
         <v>484</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C274" s="3" t="s">
         <v>198</v>
@@ -10228,7 +10231,7 @@
         <v>666</v>
       </c>
       <c r="C277" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D277" s="6">
         <v>2015</v>
@@ -10241,7 +10244,7 @@
         <v>488</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C278" s="3" t="s">
         <v>198</v>
@@ -10257,7 +10260,7 @@
         <v>489</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C279" s="3" t="s">
         <v>198</v>
@@ -10273,10 +10276,10 @@
         <v>490</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C280" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D280" s="6">
         <v>2015</v>
@@ -10289,7 +10292,7 @@
         <v>491</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C281" s="3" t="s">
         <v>198</v>
@@ -10337,7 +10340,7 @@
         <v>494</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C284" s="3" t="s">
         <v>198</v>
@@ -10369,7 +10372,7 @@
         <v>496</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C286" s="3" t="s">
         <v>199</v>
@@ -10385,7 +10388,7 @@
         <v>497</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C287" s="3" t="s">
         <v>199</v>
@@ -10401,7 +10404,7 @@
         <v>498</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C288" s="3" t="s">
         <v>198</v>
@@ -10449,7 +10452,7 @@
         <v>501</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C291" s="3" t="s">
         <v>199</v>
@@ -10465,7 +10468,7 @@
         <v>502</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C292" s="3" t="s">
         <v>200</v>
@@ -10481,7 +10484,7 @@
         <v>503</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C293" s="3" t="s">
         <v>199</v>
@@ -10497,7 +10500,7 @@
         <v>504</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C294" s="3" t="s">
         <v>199</v>
@@ -10513,7 +10516,7 @@
         <v>505</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C295" s="3" t="s">
         <v>198</v>
@@ -10529,7 +10532,7 @@
         <v>506</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C296" s="3" t="s">
         <v>198</v>
@@ -10545,7 +10548,7 @@
         <v>507</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C297" s="3" t="s">
         <v>198</v>
@@ -10577,7 +10580,7 @@
         <v>509</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C299" s="3" t="s">
         <v>199</v>
@@ -10593,7 +10596,7 @@
         <v>510</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C300" s="3" t="s">
         <v>198</v>
@@ -10609,7 +10612,7 @@
         <v>511</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C301" s="3" t="s">
         <v>198</v>
@@ -10625,10 +10628,10 @@
         <v>512</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C302" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D302" s="6">
         <v>2015</v>
@@ -10641,10 +10644,10 @@
         <v>513</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C303" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D303" s="6">
         <v>2015</v>
@@ -10657,7 +10660,7 @@
         <v>514</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C304" s="3" t="s">
         <v>198</v>
@@ -10673,10 +10676,10 @@
         <v>515</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C305" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D305" s="6">
         <v>2015</v>
@@ -10689,7 +10692,7 @@
         <v>516</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C306" s="3" t="s">
         <v>199</v>
@@ -10721,7 +10724,7 @@
         <v>518</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C308" s="3" t="s">
         <v>198</v>
@@ -10753,7 +10756,7 @@
         <v>519</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C310" s="3" t="s">
         <v>198</v>
@@ -10779,7 +10782,7 @@
     </row>
     <row r="312" spans="1:6">
       <c r="A312" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="C312" s="3" t="s">
         <v>198</v>
@@ -10795,7 +10798,7 @@
         <v>521</v>
       </c>
       <c r="B313" s="4" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C313" s="4" t="s">
         <v>201</v>
@@ -10811,7 +10814,7 @@
         <v>522</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C314" s="3" t="s">
         <v>198</v>
@@ -10827,7 +10830,7 @@
         <v>523</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C315" s="3" t="s">
         <v>198</v>
@@ -10843,10 +10846,10 @@
         <v>524</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="C316" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D316" s="6">
         <v>2016</v>
@@ -10859,7 +10862,7 @@
         <v>525</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C317" s="3" t="s">
         <v>199</v>
@@ -10875,7 +10878,7 @@
         <v>526</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C318" s="3" t="s">
         <v>198</v>
@@ -10891,7 +10894,7 @@
         <v>527</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C319" s="3" t="s">
         <v>198</v>
@@ -10920,7 +10923,7 @@
         <v>529</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C321" s="3" t="s">
         <v>201</v>
@@ -10936,7 +10939,7 @@
         <v>530</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C322" s="3" t="s">
         <v>198</v>
@@ -10952,7 +10955,7 @@
         <v>531</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C323" s="3" t="s">
         <v>199</v>
@@ -10968,7 +10971,7 @@
         <v>532</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C324" s="3" t="s">
         <v>201</v>
@@ -10984,7 +10987,7 @@
         <v>533</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C325" s="3" t="s">
         <v>199</v>
@@ -11000,7 +11003,7 @@
         <v>534</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C326" s="3" t="s">
         <v>198</v>
@@ -11032,7 +11035,7 @@
         <v>536</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C328" s="3" t="s">
         <v>199</v>
@@ -11048,7 +11051,7 @@
         <v>537</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C329" s="3" t="s">
         <v>199</v>
@@ -11064,7 +11067,7 @@
         <v>538</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C330" s="3" t="s">
         <v>198</v>
@@ -11096,7 +11099,7 @@
         <v>540</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C332" s="3" t="s">
         <v>199</v>
@@ -11112,7 +11115,7 @@
         <v>541</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C333" s="3" t="s">
         <v>200</v>
@@ -11128,7 +11131,7 @@
         <v>542</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C334" s="3" t="s">
         <v>199</v>
@@ -11160,7 +11163,7 @@
         <v>187</v>
       </c>
       <c r="C336" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D336" s="6">
         <v>2016</v>
@@ -11173,7 +11176,7 @@
         <v>545</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C337" s="3" t="s">
         <v>199</v>
@@ -11186,10 +11189,10 @@
     </row>
     <row r="338" spans="1:6">
       <c r="A338" s="3" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C338" s="3" t="s">
         <v>201</v>
@@ -11205,7 +11208,7 @@
         <v>546</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C339" s="3" t="s">
         <v>199</v>
@@ -11237,7 +11240,7 @@
         <v>548</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C341" s="3" t="s">
         <v>199</v>
@@ -11266,7 +11269,7 @@
         <v>550</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C343" s="3" t="s">
         <v>199</v>
@@ -11282,7 +11285,7 @@
         <v>551</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C344" s="3" t="s">
         <v>199</v>
@@ -11298,7 +11301,7 @@
         <v>552</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C345" s="3" t="s">
         <v>199</v>
@@ -11330,7 +11333,7 @@
         <v>554</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C347" s="3" t="s">
         <v>199</v>
@@ -11346,7 +11349,7 @@
         <v>555</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C348" s="3" t="s">
         <v>199</v>
@@ -11362,7 +11365,7 @@
         <v>556</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C349" s="3" t="s">
         <v>198</v>
@@ -11378,7 +11381,7 @@
         <v>557</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C350" s="3" t="s">
         <v>198</v>
@@ -11394,7 +11397,7 @@
         <v>558</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C351" s="3" t="s">
         <v>199</v>
@@ -11410,7 +11413,7 @@
         <v>559</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C352" s="3" t="s">
         <v>198</v>
@@ -11442,7 +11445,7 @@
         <v>561</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C354" s="3" t="s">
         <v>199</v>
@@ -11458,7 +11461,7 @@
         <v>562</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C355" s="3" t="s">
         <v>199</v>
@@ -11474,7 +11477,7 @@
         <v>563</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C356" s="3" t="s">
         <v>198</v>
@@ -11490,7 +11493,7 @@
         <v>564</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C357" s="3" t="s">
         <v>198</v>
@@ -11506,7 +11509,7 @@
         <v>565</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C358" s="3" t="s">
         <v>199</v>
@@ -11522,10 +11525,10 @@
         <v>566</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C359" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D359" s="6">
         <v>2016</v>
@@ -11554,7 +11557,7 @@
         <v>568</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C361" s="3" t="s">
         <v>201</v>
@@ -11570,7 +11573,7 @@
         <v>569</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C362" s="3" t="s">
         <v>199</v>
@@ -11586,7 +11589,7 @@
         <v>570</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C363" s="3" t="s">
         <v>201</v>
@@ -11602,7 +11605,7 @@
         <v>571</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C364" s="3" t="s">
         <v>201</v>
@@ -11618,7 +11621,7 @@
         <v>572</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C365" s="3" t="s">
         <v>199</v>
@@ -11634,7 +11637,7 @@
         <v>573</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C366" s="3" t="s">
         <v>198</v>
@@ -11650,7 +11653,7 @@
         <v>574</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C367" s="3" t="s">
         <v>199</v>
@@ -11682,7 +11685,7 @@
         <v>576</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C369" s="3" t="s">
         <v>199</v>
@@ -11714,7 +11717,7 @@
         <v>578</v>
       </c>
       <c r="C371" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D371" s="6">
         <v>2016</v>
@@ -11727,7 +11730,7 @@
         <v>579</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C372" s="3" t="s">
         <v>199</v>
@@ -11743,7 +11746,7 @@
         <v>580</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C373" s="3" t="s">
         <v>198</v>
@@ -11759,7 +11762,7 @@
         <v>581</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C374" s="3" t="s">
         <v>198</v>
@@ -11775,7 +11778,7 @@
         <v>582</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C375" s="3" t="s">
         <v>198</v>
@@ -11791,7 +11794,7 @@
         <v>583</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C376" s="3" t="s">
         <v>199</v>
@@ -11807,7 +11810,7 @@
         <v>584</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C377" s="3" t="s">
         <v>199</v>
@@ -11823,7 +11826,7 @@
         <v>585</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C378" s="3" t="s">
         <v>200</v>
@@ -11839,7 +11842,7 @@
         <v>586</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C379" s="3" t="s">
         <v>199</v>
@@ -11855,7 +11858,7 @@
         <v>587</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C380" s="3" t="s">
         <v>198</v>
@@ -11871,7 +11874,7 @@
         <v>588</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C381" s="3" t="s">
         <v>200</v>
@@ -11887,7 +11890,7 @@
         <v>589</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C382" s="3" t="s">
         <v>199</v>
@@ -11903,7 +11906,7 @@
         <v>590</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C383" s="3" t="s">
         <v>199</v>
@@ -11951,10 +11954,10 @@
         <v>593</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C386" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D386" s="6">
         <v>2016</v>
@@ -11983,7 +11986,7 @@
         <v>595</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C388" s="3" t="s">
         <v>199</v>
@@ -11999,7 +12002,7 @@
         <v>596</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C389" s="3" t="s">
         <v>200</v>
@@ -12047,7 +12050,7 @@
         <v>599</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C392" s="3" t="s">
         <v>200</v>
@@ -12063,7 +12066,7 @@
         <v>600</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C393" s="3" t="s">
         <v>199</v>
@@ -12079,7 +12082,7 @@
         <v>601</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C394" s="3" t="s">
         <v>199</v>
@@ -12111,7 +12114,7 @@
         <v>603</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C396" s="3" t="s">
         <v>199</v>
@@ -12127,7 +12130,7 @@
         <v>604</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="C397" s="3" t="s">
         <v>198</v>
@@ -12143,7 +12146,7 @@
         <v>605</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C398" s="3" t="s">
         <v>200</v>
@@ -12159,7 +12162,7 @@
         <v>606</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="C399" s="3" t="s">
         <v>198</v>
@@ -12172,7 +12175,7 @@
     </row>
     <row r="400" spans="1:6">
       <c r="A400" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="C400" s="3" t="s">
         <v>198</v>
@@ -12624,7 +12627,7 @@
         <v>119</v>
       </c>
       <c r="C422" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D422" s="6">
         <v>2017</v>
@@ -12677,7 +12680,7 @@
       </c>
       <c r="G424" s="7"/>
       <c r="H424" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="425" spans="1:8">
@@ -12768,7 +12771,7 @@
         <v>126</v>
       </c>
       <c r="C429" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D429" s="6">
         <v>2017</v>
@@ -13288,7 +13291,7 @@
     </row>
     <row r="455" spans="1:6">
       <c r="A455" s="3" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="B455" s="3" t="s">
         <v>152</v>
@@ -14280,7 +14283,7 @@
     </row>
     <row r="503" spans="1:8">
       <c r="A503" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C503" s="3" t="s">
         <v>198</v>
@@ -14528,10 +14531,10 @@
     </row>
     <row r="513" spans="1:8">
       <c r="A513" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="B513" s="3" t="s">
         <v>874</v>
-      </c>
-      <c r="B513" s="3" t="s">
-        <v>875</v>
       </c>
       <c r="C513" s="3" t="s">
         <v>199</v>
@@ -14549,15 +14552,15 @@
         <v>238</v>
       </c>
       <c r="H513" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="514" spans="1:8">
       <c r="A514" s="3" t="s">
+        <v>877</v>
+      </c>
+      <c r="B514" s="3" t="s">
         <v>878</v>
-      </c>
-      <c r="B514" s="3" t="s">
-        <v>879</v>
       </c>
       <c r="C514" s="3" t="s">
         <v>200</v>
@@ -14575,15 +14578,15 @@
         <v>236</v>
       </c>
       <c r="H514" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="515" spans="1:8">
       <c r="A515" s="3" t="s">
+        <v>880</v>
+      </c>
+      <c r="B515" s="3" t="s">
         <v>881</v>
-      </c>
-      <c r="B515" s="3" t="s">
-        <v>882</v>
       </c>
       <c r="C515" s="3" t="s">
         <v>200</v>
@@ -14601,7 +14604,7 @@
         <v>236</v>
       </c>
       <c r="H515" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="516" spans="1:8">
@@ -14609,7 +14612,7 @@
         <v>502</v>
       </c>
       <c r="B516" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C516" s="3" t="s">
         <v>199</v>
@@ -14627,15 +14630,15 @@
         <v>236</v>
       </c>
       <c r="H516" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="517" spans="1:8">
       <c r="A517" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="B517" s="3" t="s">
         <v>884</v>
-      </c>
-      <c r="B517" s="3" t="s">
-        <v>885</v>
       </c>
       <c r="C517" s="3" t="s">
         <v>198</v>
@@ -14653,15 +14656,15 @@
         <v>236</v>
       </c>
       <c r="H517" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="518" spans="1:8">
       <c r="A518" s="3" t="s">
+        <v>887</v>
+      </c>
+      <c r="B518" s="3" t="s">
         <v>888</v>
-      </c>
-      <c r="B518" s="3" t="s">
-        <v>889</v>
       </c>
       <c r="C518" s="3" t="s">
         <v>200</v>
@@ -14679,15 +14682,15 @@
         <v>236</v>
       </c>
       <c r="H518" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="519" spans="1:8">
       <c r="A519" s="3" t="s">
+        <v>890</v>
+      </c>
+      <c r="B519" s="3" t="s">
         <v>891</v>
-      </c>
-      <c r="B519" s="3" t="s">
-        <v>892</v>
       </c>
       <c r="C519" s="3" t="s">
         <v>198</v>
@@ -14705,15 +14708,15 @@
         <v>236</v>
       </c>
       <c r="H519" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="520" spans="1:8">
       <c r="A520" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="B520" s="3" t="s">
         <v>894</v>
-      </c>
-      <c r="B520" s="3" t="s">
-        <v>895</v>
       </c>
       <c r="C520" s="3" t="s">
         <v>198</v>
@@ -14731,15 +14734,15 @@
         <v>238</v>
       </c>
       <c r="H520" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="521" spans="1:8">
       <c r="A521" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="B521" s="3" t="s">
         <v>897</v>
-      </c>
-      <c r="B521" s="3" t="s">
-        <v>898</v>
       </c>
       <c r="C521" s="3" t="s">
         <v>199</v>
@@ -14757,15 +14760,15 @@
         <v>236</v>
       </c>
       <c r="H521" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="522" spans="1:8">
       <c r="A522" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="B522" s="3" t="s">
         <v>899</v>
-      </c>
-      <c r="B522" s="3" t="s">
-        <v>900</v>
       </c>
       <c r="C522" s="3" t="s">
         <v>199</v>
@@ -14783,15 +14786,15 @@
         <v>236</v>
       </c>
       <c r="H522" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="523" spans="1:8">
       <c r="A523" s="3" t="s">
+        <v>900</v>
+      </c>
+      <c r="B523" s="3" t="s">
         <v>901</v>
-      </c>
-      <c r="B523" s="3" t="s">
-        <v>902</v>
       </c>
       <c r="C523" s="3" t="s">
         <v>199</v>
@@ -14809,15 +14812,15 @@
         <v>238</v>
       </c>
       <c r="H523" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="524" spans="1:8">
       <c r="A524" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="B524" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C524" s="3" t="s">
         <v>198</v>
@@ -14835,15 +14838,15 @@
         <v>236</v>
       </c>
       <c r="H524" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="525" spans="1:8">
       <c r="A525" s="3" t="s">
+        <v>905</v>
+      </c>
+      <c r="B525" s="3" t="s">
         <v>906</v>
-      </c>
-      <c r="B525" s="3" t="s">
-        <v>907</v>
       </c>
       <c r="C525" s="3" t="s">
         <v>199</v>
@@ -14861,15 +14864,15 @@
         <v>238</v>
       </c>
       <c r="H525" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="526" spans="1:8">
       <c r="A526" s="3" t="s">
+        <v>909</v>
+      </c>
+      <c r="B526" s="3" t="s">
         <v>910</v>
-      </c>
-      <c r="B526" s="3" t="s">
-        <v>911</v>
       </c>
       <c r="C526" s="3" t="s">
         <v>199</v>
@@ -14887,15 +14890,15 @@
         <v>238</v>
       </c>
       <c r="H526" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="527" spans="1:8">
       <c r="A527" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="B527" s="3" t="s">
         <v>912</v>
-      </c>
-      <c r="B527" s="3" t="s">
-        <v>913</v>
       </c>
       <c r="C527" s="3" t="s">
         <v>200</v>
@@ -14913,15 +14916,15 @@
         <v>238</v>
       </c>
       <c r="H527" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="528" spans="1:8">
       <c r="A528" s="3" t="s">
+        <v>914</v>
+      </c>
+      <c r="B528" s="3" t="s">
         <v>915</v>
-      </c>
-      <c r="B528" s="3" t="s">
-        <v>916</v>
       </c>
       <c r="C528" s="3" t="s">
         <v>199</v>
@@ -14939,15 +14942,15 @@
         <v>238</v>
       </c>
       <c r="H528" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="529" spans="1:8">
       <c r="A529" s="3" t="s">
+        <v>922</v>
+      </c>
+      <c r="B529" s="3" t="s">
         <v>923</v>
-      </c>
-      <c r="B529" s="3" t="s">
-        <v>924</v>
       </c>
       <c r="C529" s="3" t="s">
         <v>199</v>
@@ -14965,15 +14968,15 @@
         <v>236</v>
       </c>
       <c r="H529" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="530" spans="1:8">
       <c r="A530" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="B530" s="3" t="s">
         <v>921</v>
-      </c>
-      <c r="B530" s="3" t="s">
-        <v>922</v>
       </c>
       <c r="C530" s="3" t="s">
         <v>199</v>
@@ -14991,15 +14994,15 @@
         <v>236</v>
       </c>
       <c r="H530" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="531" spans="1:8">
       <c r="A531" s="3" t="s">
+        <v>924</v>
+      </c>
+      <c r="B531" s="3" t="s">
         <v>925</v>
-      </c>
-      <c r="B531" s="3" t="s">
-        <v>926</v>
       </c>
       <c r="C531" s="3" t="s">
         <v>200</v>
@@ -15017,15 +15020,15 @@
         <v>236</v>
       </c>
       <c r="H531" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="532" spans="1:8">
       <c r="A532" s="3" t="s">
+        <v>929</v>
+      </c>
+      <c r="B532" s="3" t="s">
         <v>930</v>
-      </c>
-      <c r="B532" s="3" t="s">
-        <v>931</v>
       </c>
       <c r="C532" s="3" t="s">
         <v>200</v>
@@ -15043,18 +15046,18 @@
         <v>236</v>
       </c>
       <c r="H532" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="533" spans="1:8">
       <c r="A533" s="3" t="s">
+        <v>932</v>
+      </c>
+      <c r="B533" s="3" t="s">
         <v>933</v>
       </c>
-      <c r="B533" s="3" t="s">
-        <v>934</v>
-      </c>
       <c r="C533" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D533" s="6">
         <v>2018</v>
@@ -15069,15 +15072,15 @@
         <v>238</v>
       </c>
       <c r="H533" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="534" spans="1:8">
       <c r="A534" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B534" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C534" s="3" t="s">
         <v>200</v>
@@ -15095,12 +15098,12 @@
         <v>236</v>
       </c>
       <c r="H534" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="535" spans="1:8">
       <c r="A535" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B535" s="3" t="s">
         <v>158</v>
@@ -15121,15 +15124,15 @@
         <v>236</v>
       </c>
       <c r="H535" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="536" spans="1:8">
       <c r="A536" s="3" t="s">
+        <v>938</v>
+      </c>
+      <c r="B536" s="3" t="s">
         <v>939</v>
-      </c>
-      <c r="B536" s="3" t="s">
-        <v>940</v>
       </c>
       <c r="C536" s="3" t="s">
         <v>199</v>
@@ -15147,12 +15150,12 @@
         <v>238</v>
       </c>
       <c r="H536" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="537" spans="1:8">
       <c r="A537" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B537" s="3" t="s">
         <v>166</v>
@@ -15173,18 +15176,18 @@
         <v>236</v>
       </c>
       <c r="H537" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="538" spans="1:8">
       <c r="A538" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B538" s="3" t="s">
         <v>187</v>
       </c>
       <c r="C538" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D538" s="6">
         <v>2018</v>
@@ -15199,15 +15202,15 @@
         <v>236</v>
       </c>
       <c r="H538" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="539" spans="1:8">
       <c r="A539" s="3" t="s">
+        <v>947</v>
+      </c>
+      <c r="B539" s="3" t="s">
         <v>948</v>
-      </c>
-      <c r="B539" s="3" t="s">
-        <v>949</v>
       </c>
       <c r="C539" s="3" t="s">
         <v>199</v>
@@ -15225,15 +15228,15 @@
         <v>238</v>
       </c>
       <c r="H539" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="540" spans="1:8">
       <c r="A540" s="3" t="s">
+        <v>951</v>
+      </c>
+      <c r="B540" s="3" t="s">
         <v>952</v>
-      </c>
-      <c r="B540" s="3" t="s">
-        <v>953</v>
       </c>
       <c r="C540" s="3" t="s">
         <v>199</v>
@@ -15251,15 +15254,15 @@
         <v>238</v>
       </c>
       <c r="H540" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="541" spans="1:8">
       <c r="A541" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B541" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C541" s="3" t="s">
         <v>198</v>
@@ -15277,15 +15280,15 @@
         <v>238</v>
       </c>
       <c r="H541" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="542" spans="1:8">
       <c r="A542" s="3" t="s">
+        <v>957</v>
+      </c>
+      <c r="B542" s="3" t="s">
         <v>958</v>
-      </c>
-      <c r="B542" s="3" t="s">
-        <v>959</v>
       </c>
       <c r="C542" s="3" t="s">
         <v>201</v>
@@ -15303,15 +15306,15 @@
         <v>236</v>
       </c>
       <c r="H542" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="543" spans="1:8">
       <c r="A543" s="3" t="s">
+        <v>960</v>
+      </c>
+      <c r="B543" s="3" t="s">
         <v>961</v>
-      </c>
-      <c r="B543" s="3" t="s">
-        <v>962</v>
       </c>
       <c r="C543" s="3" t="s">
         <v>199</v>
@@ -15329,18 +15332,18 @@
         <v>238</v>
       </c>
       <c r="H543" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="544" spans="1:8">
       <c r="A544" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B544" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C544" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D544" s="6">
         <v>2018</v>
@@ -15355,15 +15358,15 @@
         <v>236</v>
       </c>
       <c r="H544" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="545" spans="1:8">
       <c r="A545" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="B545" s="3" t="s">
         <v>967</v>
-      </c>
-      <c r="B545" s="3" t="s">
-        <v>968</v>
       </c>
       <c r="C545" s="3" t="s">
         <v>198</v>
@@ -15381,12 +15384,12 @@
         <v>238</v>
       </c>
       <c r="H545" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="546" spans="1:8">
       <c r="A546" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B546" s="3" t="s">
         <v>185</v>
@@ -15407,15 +15410,15 @@
         <v>238</v>
       </c>
       <c r="H546" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="547" spans="1:8">
       <c r="A547" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B547" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C547" s="3" t="s">
         <v>199</v>
@@ -15433,15 +15436,15 @@
         <v>238</v>
       </c>
       <c r="H547" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="548" spans="1:8">
       <c r="A548" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B548" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C548" s="3" t="s">
         <v>199</v>
@@ -15459,15 +15462,15 @@
         <v>238</v>
       </c>
       <c r="H548" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="549" spans="1:8">
       <c r="A549" s="3" t="s">
+        <v>972</v>
+      </c>
+      <c r="B549" s="3" t="s">
         <v>973</v>
-      </c>
-      <c r="B549" s="3" t="s">
-        <v>974</v>
       </c>
       <c r="C549" s="3" t="s">
         <v>200</v>
@@ -15485,12 +15488,12 @@
         <v>238</v>
       </c>
       <c r="H549" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="550" spans="1:8">
       <c r="A550" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B550" s="3" t="s">
         <v>247</v>
@@ -15511,15 +15514,15 @@
         <v>236</v>
       </c>
       <c r="H550" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="551" spans="1:8">
       <c r="A551" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B551" s="3" t="s">
         <v>982</v>
-      </c>
-      <c r="B551" s="3" t="s">
-        <v>983</v>
       </c>
       <c r="C551" s="3" t="s">
         <v>199</v>
@@ -15537,15 +15540,15 @@
         <v>236</v>
       </c>
       <c r="H551" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="552" spans="1:8">
       <c r="A552" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="B552" s="3" t="s">
         <v>985</v>
-      </c>
-      <c r="B552" s="3" t="s">
-        <v>986</v>
       </c>
       <c r="C552" s="3" t="s">
         <v>199</v>
@@ -15563,15 +15566,15 @@
         <v>236</v>
       </c>
       <c r="H552" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="553" spans="1:8">
       <c r="A553" s="3" t="s">
+        <v>987</v>
+      </c>
+      <c r="B553" s="3" t="s">
         <v>988</v>
-      </c>
-      <c r="B553" s="3" t="s">
-        <v>989</v>
       </c>
       <c r="C553" s="3" t="s">
         <v>199</v>
@@ -15589,15 +15592,15 @@
         <v>236</v>
       </c>
       <c r="H553" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="554" spans="1:8">
       <c r="A554" s="3" t="s">
+        <v>990</v>
+      </c>
+      <c r="B554" s="3" t="s">
         <v>991</v>
-      </c>
-      <c r="B554" s="3" t="s">
-        <v>992</v>
       </c>
       <c r="C554" s="3" t="s">
         <v>200</v>
@@ -15615,15 +15618,15 @@
         <v>236</v>
       </c>
       <c r="H554" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="555" spans="1:8">
       <c r="A555" s="3" t="s">
+        <v>993</v>
+      </c>
+      <c r="B555" s="3" t="s">
         <v>994</v>
-      </c>
-      <c r="B555" s="3" t="s">
-        <v>995</v>
       </c>
       <c r="C555" s="3" t="s">
         <v>200</v>
@@ -15641,15 +15644,15 @@
         <v>238</v>
       </c>
       <c r="H555" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="556" spans="1:8">
       <c r="A556" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="B556" s="3" t="s">
         <v>997</v>
-      </c>
-      <c r="B556" s="3" t="s">
-        <v>998</v>
       </c>
       <c r="C556" s="3" t="s">
         <v>199</v>
@@ -15667,15 +15670,15 @@
         <v>238</v>
       </c>
       <c r="H556" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="557" spans="1:8">
       <c r="A557" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="B557" s="3" t="s">
         <v>1000</v>
-      </c>
-      <c r="B557" s="3" t="s">
-        <v>1001</v>
       </c>
       <c r="C557" s="3" t="s">
         <v>199</v>
@@ -15693,15 +15696,15 @@
         <v>238</v>
       </c>
       <c r="H557" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="558" spans="1:8">
       <c r="A558" s="3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B558" s="3" t="s">
         <v>1003</v>
-      </c>
-      <c r="B558" s="3" t="s">
-        <v>1004</v>
       </c>
       <c r="C558" s="3" t="s">
         <v>198</v>
@@ -15719,15 +15722,15 @@
         <v>238</v>
       </c>
       <c r="H558" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="559" spans="1:8">
       <c r="A559" s="3" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B559" s="3" t="s">
         <v>1006</v>
-      </c>
-      <c r="B559" s="3" t="s">
-        <v>1007</v>
       </c>
       <c r="C559" s="3" t="s">
         <v>199</v>
@@ -15745,12 +15748,12 @@
         <v>238</v>
       </c>
       <c r="H559" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="560" spans="1:8">
       <c r="A560" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B560" s="3" t="s">
         <v>106</v>
@@ -15771,15 +15774,15 @@
         <v>238</v>
       </c>
       <c r="H560" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="561" spans="1:8">
       <c r="A561" s="3" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B561" s="3" t="s">
         <v>1011</v>
-      </c>
-      <c r="B561" s="3" t="s">
-        <v>1012</v>
       </c>
       <c r="C561" s="3" t="s">
         <v>200</v>
@@ -15797,15 +15800,15 @@
         <v>238</v>
       </c>
       <c r="H561" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="562" spans="1:8">
       <c r="A562" s="3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B562" s="3" t="s">
         <v>1014</v>
-      </c>
-      <c r="B562" s="3" t="s">
-        <v>1015</v>
       </c>
       <c r="C562" s="3" t="s">
         <v>199</v>
@@ -15823,15 +15826,15 @@
         <v>238</v>
       </c>
       <c r="H562" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="563" spans="1:8">
       <c r="A563" s="3" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B563" s="3" t="s">
         <v>1017</v>
-      </c>
-      <c r="B563" s="3" t="s">
-        <v>1018</v>
       </c>
       <c r="C563" s="3" t="s">
         <v>198</v>
@@ -15849,15 +15852,15 @@
         <v>236</v>
       </c>
       <c r="H563" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="564" spans="1:8">
       <c r="A564" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B564" s="3" t="s">
         <v>1019</v>
-      </c>
-      <c r="B564" s="3" t="s">
-        <v>1020</v>
       </c>
       <c r="C564" s="3" t="s">
         <v>199</v>
@@ -15875,15 +15878,15 @@
         <v>238</v>
       </c>
       <c r="H564" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="565" spans="1:8">
       <c r="A565" s="3" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B565" s="3" t="s">
         <v>1021</v>
-      </c>
-      <c r="B565" s="3" t="s">
-        <v>1022</v>
       </c>
       <c r="C565" s="3" t="s">
         <v>199</v>
@@ -15901,7 +15904,7 @@
         <v>238</v>
       </c>
       <c r="H565" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="566" spans="1:8">
@@ -15927,15 +15930,15 @@
         <v>236</v>
       </c>
       <c r="H566" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="567" spans="1:8">
       <c r="A567" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B567" s="3" t="s">
         <v>1027</v>
-      </c>
-      <c r="B567" s="3" t="s">
-        <v>1028</v>
       </c>
       <c r="C567" s="3" t="s">
         <v>198</v>
@@ -15953,15 +15956,15 @@
         <v>236</v>
       </c>
       <c r="H567" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="568" spans="1:8">
       <c r="A568" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B568" s="3" t="s">
         <v>1030</v>
-      </c>
-      <c r="B568" s="3" t="s">
-        <v>1031</v>
       </c>
       <c r="C568" s="3" t="s">
         <v>199</v>
@@ -15979,15 +15982,15 @@
         <v>236</v>
       </c>
       <c r="H568" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="569" spans="1:8">
       <c r="A569" s="3" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B569" s="3" t="s">
         <v>1033</v>
-      </c>
-      <c r="B569" s="3" t="s">
-        <v>1034</v>
       </c>
       <c r="C569" s="3" t="s">
         <v>198</v>
@@ -16005,15 +16008,15 @@
         <v>238</v>
       </c>
       <c r="H569" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="570" spans="1:8">
       <c r="A570" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B570" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="C570" s="3" t="s">
         <v>199</v>
@@ -16031,15 +16034,15 @@
         <v>238</v>
       </c>
       <c r="H570" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="571" spans="1:8">
       <c r="A571" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B571" s="3" t="s">
         <v>1038</v>
-      </c>
-      <c r="B571" s="3" t="s">
-        <v>1039</v>
       </c>
       <c r="C571" s="3" t="s">
         <v>200</v>
@@ -16057,15 +16060,15 @@
         <v>238</v>
       </c>
       <c r="H571" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="572" spans="1:8">
       <c r="A572" s="3" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B572" s="3" t="s">
         <v>1041</v>
-      </c>
-      <c r="B572" s="3" t="s">
-        <v>1042</v>
       </c>
       <c r="C572" s="3" t="s">
         <v>198</v>
@@ -16083,15 +16086,15 @@
         <v>238</v>
       </c>
       <c r="H572" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="573" spans="1:8">
       <c r="A573" s="3" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B573" s="3" t="s">
         <v>1044</v>
-      </c>
-      <c r="B573" s="3" t="s">
-        <v>1045</v>
       </c>
       <c r="C573" s="3" t="s">
         <v>200</v>
@@ -16109,15 +16112,15 @@
         <v>236</v>
       </c>
       <c r="H573" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="574" spans="1:8">
       <c r="A574" s="3" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B574" s="3" t="s">
         <v>1047</v>
-      </c>
-      <c r="B574" s="3" t="s">
-        <v>1048</v>
       </c>
       <c r="C574" s="3" t="s">
         <v>199</v>
@@ -16135,15 +16138,15 @@
         <v>238</v>
       </c>
       <c r="H574" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="575" spans="1:8">
       <c r="A575" s="3" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B575" s="3" t="s">
         <v>1050</v>
-      </c>
-      <c r="B575" s="3" t="s">
-        <v>1051</v>
       </c>
       <c r="C575" s="3" t="s">
         <v>200</v>
@@ -16161,15 +16164,15 @@
         <v>236</v>
       </c>
       <c r="H575" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="576" spans="1:8">
       <c r="A576" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B576" s="3" t="s">
         <v>1105</v>
-      </c>
-      <c r="B576" s="3" t="s">
-        <v>1106</v>
       </c>
       <c r="C576" s="3" t="s">
         <v>199</v>
@@ -16187,12 +16190,12 @@
         <v>236</v>
       </c>
       <c r="H576" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="577" spans="1:8">
       <c r="A577" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="B577" s="3" t="s">
         <v>171</v>
@@ -16213,12 +16216,12 @@
         <v>236</v>
       </c>
       <c r="H577" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="578" spans="1:8">
       <c r="A578" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B578" s="3" t="s">
         <v>625</v>
@@ -16239,15 +16242,15 @@
         <v>238</v>
       </c>
       <c r="H578" s="3" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="579" spans="1:8">
       <c r="A579" s="3" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B579" s="3" t="s">
         <v>1110</v>
-      </c>
-      <c r="B579" s="3" t="s">
-        <v>1111</v>
       </c>
       <c r="C579" s="3" t="s">
         <v>198</v>
@@ -16265,7 +16268,7 @@
         <v>238</v>
       </c>
       <c r="H579" s="3" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="580" spans="1:8">
@@ -16291,15 +16294,15 @@
         <v>236</v>
       </c>
       <c r="H580" s="3" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="581" spans="1:8">
       <c r="A581" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B581" s="3" t="s">
         <v>1113</v>
-      </c>
-      <c r="B581" s="3" t="s">
-        <v>1114</v>
       </c>
       <c r="C581" s="3" t="s">
         <v>199</v>
@@ -16317,7 +16320,7 @@
         <v>238</v>
       </c>
       <c r="H581" s="3" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="582" spans="1:8">
@@ -16343,15 +16346,15 @@
         <v>238</v>
       </c>
       <c r="H582" s="3" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="583" spans="1:8">
       <c r="A583" s="3" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B583" s="3" t="s">
         <v>1118</v>
-      </c>
-      <c r="B583" s="3" t="s">
-        <v>1119</v>
       </c>
       <c r="C583" s="3" t="s">
         <v>199</v>
@@ -16369,15 +16372,15 @@
         <v>238</v>
       </c>
       <c r="H583" s="3" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="584" spans="1:8">
       <c r="A584" s="3" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B584" s="3" t="s">
         <v>1121</v>
-      </c>
-      <c r="B584" s="3" t="s">
-        <v>1122</v>
       </c>
       <c r="C584" s="3" t="s">
         <v>198</v>
@@ -16395,15 +16398,15 @@
         <v>236</v>
       </c>
       <c r="H584" s="3" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="585" spans="1:8">
       <c r="A585" s="3" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B585" s="3" t="s">
         <v>1124</v>
-      </c>
-      <c r="B585" s="3" t="s">
-        <v>1125</v>
       </c>
       <c r="C585" s="3" t="s">
         <v>199</v>
@@ -16421,15 +16424,15 @@
         <v>238</v>
       </c>
       <c r="H585" s="3" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="586" spans="1:8">
       <c r="A586" s="3" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B586" s="3" t="s">
         <v>1126</v>
-      </c>
-      <c r="B586" s="3" t="s">
-        <v>1127</v>
       </c>
       <c r="C586" s="3" t="s">
         <v>198</v>
@@ -16447,15 +16450,15 @@
         <v>236</v>
       </c>
       <c r="H586" s="3" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="587" spans="1:8">
       <c r="A587" s="3" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B587" s="3" t="s">
         <v>1128</v>
-      </c>
-      <c r="B587" s="3" t="s">
-        <v>1129</v>
       </c>
       <c r="C587" s="3" t="s">
         <v>199</v>
@@ -16473,15 +16476,15 @@
         <v>238</v>
       </c>
       <c r="H587" s="3" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="588" spans="1:8">
       <c r="A588" s="3" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B588" s="3" t="s">
         <v>1133</v>
-      </c>
-      <c r="B588" s="3" t="s">
-        <v>1134</v>
       </c>
       <c r="C588" s="3" t="s">
         <v>198</v>
@@ -16499,15 +16502,15 @@
         <v>238</v>
       </c>
       <c r="H588" s="3" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="589" spans="1:8">
       <c r="A589" s="3" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B589" s="3" t="s">
         <v>1137</v>
-      </c>
-      <c r="B589" s="3" t="s">
-        <v>1138</v>
       </c>
       <c r="C589" s="3" t="s">
         <v>200</v>
@@ -16525,12 +16528,12 @@
         <v>236</v>
       </c>
       <c r="H589" s="3" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="590" spans="1:8">
       <c r="A590" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B590" s="3" t="s">
         <v>628</v>
@@ -16551,15 +16554,15 @@
         <v>238</v>
       </c>
       <c r="H590" s="3" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="591" spans="1:8">
       <c r="A591" s="3" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B591" s="3" t="s">
         <v>1140</v>
-      </c>
-      <c r="B591" s="3" t="s">
-        <v>1141</v>
       </c>
       <c r="C591" s="3" t="s">
         <v>199</v>
@@ -16577,15 +16580,15 @@
         <v>236</v>
       </c>
       <c r="H591" s="3" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="592" spans="1:8">
       <c r="A592" s="3" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B592" s="3" t="s">
         <v>1143</v>
-      </c>
-      <c r="B592" s="3" t="s">
-        <v>1144</v>
       </c>
       <c r="C592" s="3" t="s">
         <v>200</v>
@@ -16603,12 +16606,12 @@
         <v>236</v>
       </c>
       <c r="H592" s="3" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="593" spans="1:8">
       <c r="A593" s="3" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="B593" s="3" t="s">
         <v>178</v>
@@ -16629,15 +16632,15 @@
         <v>236</v>
       </c>
       <c r="H593" s="3" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="594" spans="1:8">
       <c r="A594" s="3" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B594" s="3" t="s">
         <v>1148</v>
-      </c>
-      <c r="B594" s="3" t="s">
-        <v>1149</v>
       </c>
       <c r="C594" s="3" t="s">
         <v>199</v>
@@ -16655,15 +16658,15 @@
         <v>238</v>
       </c>
       <c r="H594" s="3" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="595" spans="1:8">
       <c r="A595" s="3" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B595" s="3" t="s">
         <v>1151</v>
-      </c>
-      <c r="B595" s="3" t="s">
-        <v>1152</v>
       </c>
       <c r="C595" s="3" t="s">
         <v>199</v>
@@ -16681,7 +16684,7 @@
         <v>236</v>
       </c>
       <c r="H595" s="3" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="596" spans="1:8">
@@ -16707,15 +16710,15 @@
         <v>238</v>
       </c>
       <c r="H596" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="597" spans="1:8">
       <c r="A597" s="3" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B597" s="3" t="s">
         <v>1154</v>
-      </c>
-      <c r="B597" s="3" t="s">
-        <v>1155</v>
       </c>
       <c r="C597" s="3" t="s">
         <v>199</v>
@@ -16733,15 +16736,15 @@
         <v>238</v>
       </c>
       <c r="H597" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="598" spans="1:8">
       <c r="A598" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B598" s="3" t="s">
         <v>1158</v>
-      </c>
-      <c r="B598" s="3" t="s">
-        <v>1159</v>
       </c>
       <c r="C598" s="3" t="s">
         <v>200</v>
@@ -16759,15 +16762,15 @@
         <v>236</v>
       </c>
       <c r="H598" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="599" spans="1:8">
       <c r="A599" s="3" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B599" s="3" t="s">
         <v>1161</v>
-      </c>
-      <c r="B599" s="3" t="s">
-        <v>1162</v>
       </c>
       <c r="C599" s="3" t="s">
         <v>200</v>
@@ -16785,15 +16788,15 @@
         <v>236</v>
       </c>
       <c r="H599" s="3" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="600" spans="1:8">
       <c r="A600" s="3" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B600" s="3" t="s">
         <v>1164</v>
-      </c>
-      <c r="B600" s="3" t="s">
-        <v>1165</v>
       </c>
       <c r="C600" s="3" t="s">
         <v>199</v>
@@ -16811,15 +16814,15 @@
         <v>236</v>
       </c>
       <c r="H600" s="3" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="601" spans="1:8">
       <c r="A601" s="3" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B601" s="3" t="s">
         <v>1167</v>
-      </c>
-      <c r="B601" s="3" t="s">
-        <v>1168</v>
       </c>
       <c r="C601" s="3" t="s">
         <v>198</v>
@@ -16837,12 +16840,12 @@
         <v>238</v>
       </c>
       <c r="H601" s="3" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="602" spans="1:8">
       <c r="A602" s="3" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="B602" s="3" t="s">
         <v>737</v>
@@ -16863,15 +16866,15 @@
         <v>238</v>
       </c>
       <c r="H602" s="3" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="603" spans="1:8">
       <c r="A603" s="3" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B603" s="3" t="s">
         <v>1172</v>
-      </c>
-      <c r="B603" s="3" t="s">
-        <v>1173</v>
       </c>
       <c r="C603" s="3" t="s">
         <v>199</v>
@@ -16889,15 +16892,15 @@
         <v>238</v>
       </c>
       <c r="H603" s="3" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="604" spans="1:8">
       <c r="A604" s="3" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B604" s="3" t="s">
         <v>1175</v>
-      </c>
-      <c r="B604" s="3" t="s">
-        <v>1176</v>
       </c>
       <c r="C604" s="3" t="s">
         <v>199</v>
@@ -16915,15 +16918,15 @@
         <v>238</v>
       </c>
       <c r="H604" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="605" spans="1:8">
       <c r="A605" s="3" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="B605" s="3" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="C605" s="3" t="s">
         <v>200</v>
@@ -16941,15 +16944,15 @@
         <v>236</v>
       </c>
       <c r="H605" s="3" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="606" spans="1:8">
       <c r="A606" s="3" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B606" s="3" t="s">
         <v>1180</v>
-      </c>
-      <c r="B606" s="3" t="s">
-        <v>1181</v>
       </c>
       <c r="C606" s="3" t="s">
         <v>199</v>
@@ -16967,15 +16970,15 @@
         <v>236</v>
       </c>
       <c r="H606" s="3" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="607" spans="1:8">
       <c r="A607" s="3" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B607" s="3" t="s">
         <v>1182</v>
-      </c>
-      <c r="B607" s="3" t="s">
-        <v>1183</v>
       </c>
       <c r="C607" s="3" t="s">
         <v>198</v>
@@ -16993,15 +16996,15 @@
         <v>238</v>
       </c>
       <c r="H607" s="3" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="608" spans="1:8">
       <c r="A608" s="3" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="B608" s="3" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="C608" s="3" t="s">
         <v>199</v>
@@ -17019,15 +17022,15 @@
         <v>238</v>
       </c>
       <c r="H608" s="3" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="609" spans="1:8">
       <c r="A609" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B609" s="3" t="s">
         <v>1188</v>
-      </c>
-      <c r="B609" s="3" t="s">
-        <v>1189</v>
       </c>
       <c r="C609" s="3" t="s">
         <v>200</v>
@@ -17045,15 +17048,15 @@
         <v>238</v>
       </c>
       <c r="H609" s="3" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="610" spans="1:8">
       <c r="A610" s="3" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B610" s="3" t="s">
         <v>1191</v>
-      </c>
-      <c r="B610" s="3" t="s">
-        <v>1192</v>
       </c>
       <c r="C610" s="3" t="s">
         <v>199</v>
@@ -17071,15 +17074,15 @@
         <v>238</v>
       </c>
       <c r="H610" s="3" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="611" spans="1:8">
       <c r="A611" s="3" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B611" s="3" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="C611" s="3" t="s">
         <v>200</v>
@@ -17097,12 +17100,12 @@
         <v>236</v>
       </c>
       <c r="H611" s="3" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="612" spans="1:8">
       <c r="A612" s="3" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="C612" s="3" t="s">
         <v>198</v>
@@ -17118,7 +17121,7 @@
     </row>
     <row r="613" spans="1:8">
       <c r="A613" s="4" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B613" s="4" t="s">
         <v>143</v>
@@ -17139,15 +17142,15 @@
         <v>236</v>
       </c>
       <c r="H613" s="4" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="614" spans="1:8">
       <c r="A614" s="3" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B614" s="3" t="s">
         <v>1198</v>
-      </c>
-      <c r="B614" s="3" t="s">
-        <v>1199</v>
       </c>
       <c r="C614" s="3" t="s">
         <v>200</v>
@@ -17165,12 +17168,12 @@
         <v>236</v>
       </c>
       <c r="H614" s="3" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="615" spans="1:8">
       <c r="A615" s="3" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B615" s="3" t="s">
         <v>746</v>
@@ -17191,15 +17194,15 @@
         <v>236</v>
       </c>
       <c r="H615" s="3" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="616" spans="1:8">
       <c r="A616" s="3" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B616" s="3" t="s">
         <v>1205</v>
-      </c>
-      <c r="B616" s="3" t="s">
-        <v>1206</v>
       </c>
       <c r="C616" s="3" t="s">
         <v>200</v>
@@ -17217,15 +17220,15 @@
         <v>236</v>
       </c>
       <c r="H616" s="3" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="617" spans="1:8">
       <c r="A617" s="3" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B617" s="3" t="s">
         <v>1208</v>
-      </c>
-      <c r="B617" s="3" t="s">
-        <v>1209</v>
       </c>
       <c r="C617" s="3" t="s">
         <v>200</v>
@@ -17243,15 +17246,15 @@
         <v>236</v>
       </c>
       <c r="H617" s="3" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="618" spans="1:8">
       <c r="A618" s="3" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B618" s="3" t="s">
         <v>1211</v>
-      </c>
-      <c r="B618" s="3" t="s">
-        <v>1212</v>
       </c>
       <c r="C618" s="3" t="s">
         <v>198</v>
@@ -17269,15 +17272,15 @@
         <v>238</v>
       </c>
       <c r="H618" s="3" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="619" spans="1:8">
       <c r="A619" s="3" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B619" s="3" t="s">
         <v>1223</v>
-      </c>
-      <c r="B619" s="3" t="s">
-        <v>1224</v>
       </c>
       <c r="C619" s="3" t="s">
         <v>199</v>
@@ -17295,15 +17298,15 @@
         <v>238</v>
       </c>
       <c r="H619" s="3" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="620" spans="1:8">
       <c r="A620" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B620" s="3" t="s">
         <v>1219</v>
-      </c>
-      <c r="B620" s="3" t="s">
-        <v>1220</v>
       </c>
       <c r="C620" s="3" t="s">
         <v>199</v>
@@ -17321,15 +17324,15 @@
         <v>238</v>
       </c>
       <c r="H620" s="3" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="621" spans="1:8">
       <c r="A621" s="3" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B621" s="3" t="s">
         <v>1217</v>
-      </c>
-      <c r="B621" s="3" t="s">
-        <v>1218</v>
       </c>
       <c r="C621" s="3" t="s">
         <v>200</v>
@@ -17347,15 +17350,15 @@
         <v>236</v>
       </c>
       <c r="H621" s="3" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="622" spans="1:8">
       <c r="A622" s="3" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B622" s="3" t="s">
         <v>1226</v>
-      </c>
-      <c r="B622" s="3" t="s">
-        <v>1227</v>
       </c>
       <c r="C622" s="3" t="s">
         <v>199</v>
@@ -17373,15 +17376,15 @@
         <v>238</v>
       </c>
       <c r="H622" s="3" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="623" spans="1:8">
       <c r="A623" s="3" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B623" s="3" t="s">
         <v>1229</v>
-      </c>
-      <c r="B623" s="3" t="s">
-        <v>1230</v>
       </c>
       <c r="C623" s="3" t="s">
         <v>199</v>
@@ -17399,7 +17402,7 @@
         <v>236</v>
       </c>
       <c r="H623" s="3" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="624" spans="1:8">
@@ -17425,15 +17428,15 @@
         <v>238</v>
       </c>
       <c r="H624" s="3" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="625" spans="1:8">
       <c r="A625" s="3" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B625" s="3" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C625" s="3" t="s">
         <v>199</v>
@@ -17451,12 +17454,12 @@
         <v>238</v>
       </c>
       <c r="H625" s="3" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="626" spans="1:8">
       <c r="A626" s="3" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B626" s="3" t="s">
         <v>99</v>
@@ -17477,15 +17480,15 @@
         <v>236</v>
       </c>
       <c r="H626" s="3" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="627" spans="1:8">
       <c r="A627" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B627" s="3" t="s">
         <v>1237</v>
-      </c>
-      <c r="B627" s="3" t="s">
-        <v>1238</v>
       </c>
       <c r="C627" s="3" t="s">
         <v>199</v>
@@ -17503,15 +17506,15 @@
         <v>238</v>
       </c>
       <c r="H627" s="3" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="628" spans="1:8">
       <c r="A628" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B628" s="3" t="s">
         <v>1239</v>
-      </c>
-      <c r="B628" s="3" t="s">
-        <v>1240</v>
       </c>
       <c r="C628" s="3" t="s">
         <v>198</v>
@@ -17529,15 +17532,15 @@
         <v>236</v>
       </c>
       <c r="H628" s="3" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="629" spans="1:8">
       <c r="A629" s="3" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B629" s="3" t="s">
         <v>1242</v>
-      </c>
-      <c r="B629" s="3" t="s">
-        <v>1243</v>
       </c>
       <c r="C629" s="3" t="s">
         <v>200</v>
@@ -17555,15 +17558,15 @@
         <v>236</v>
       </c>
       <c r="H629" s="3" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="630" spans="1:8">
       <c r="A630" s="3" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B630" s="3" t="s">
         <v>1245</v>
-      </c>
-      <c r="B630" s="3" t="s">
-        <v>1246</v>
       </c>
       <c r="C630" s="3" t="s">
         <v>200</v>
@@ -17581,18 +17584,18 @@
         <v>236</v>
       </c>
       <c r="H630" s="3" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="631" spans="1:8">
       <c r="A631" s="3" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B631" s="3" t="s">
         <v>1248</v>
       </c>
-      <c r="B631" s="3" t="s">
-        <v>1249</v>
-      </c>
       <c r="C631" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D631" s="6">
         <v>2019</v>
@@ -17607,15 +17610,15 @@
         <v>236</v>
       </c>
       <c r="H631" s="3" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="632" spans="1:8">
       <c r="A632" s="3" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B632" s="3" t="s">
         <v>1251</v>
-      </c>
-      <c r="B632" s="3" t="s">
-        <v>1252</v>
       </c>
       <c r="C632" s="3" t="s">
         <v>199</v>
@@ -17633,15 +17636,15 @@
         <v>236</v>
       </c>
       <c r="H632" s="3" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="633" spans="1:8">
       <c r="A633" s="3" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B633" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C633" s="3" t="s">
         <v>198</v>
@@ -17659,15 +17662,15 @@
         <v>238</v>
       </c>
       <c r="H633" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="634" spans="1:8">
       <c r="A634" s="3" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B634" s="3" t="s">
         <v>1257</v>
-      </c>
-      <c r="B634" s="3" t="s">
-        <v>1258</v>
       </c>
       <c r="C634" s="3" t="s">
         <v>198</v>
@@ -17685,15 +17688,15 @@
         <v>236</v>
       </c>
       <c r="H634" s="3" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="635" spans="1:8">
       <c r="A635" s="3" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="B635" s="3" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="C635" s="3" t="s">
         <v>200</v>
@@ -17711,15 +17714,15 @@
         <v>236</v>
       </c>
       <c r="H635" s="3" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="636" spans="1:8">
       <c r="A636" s="3" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B636" s="3" t="s">
         <v>1264</v>
-      </c>
-      <c r="B636" s="3" t="s">
-        <v>1265</v>
       </c>
       <c r="C636" s="3" t="s">
         <v>198</v>
@@ -17737,15 +17740,15 @@
         <v>236</v>
       </c>
       <c r="H636" s="3" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="637" spans="1:8">
       <c r="A637" s="3" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B637" s="3" t="s">
         <v>1267</v>
-      </c>
-      <c r="B637" s="3" t="s">
-        <v>1268</v>
       </c>
       <c r="C637" s="3" t="s">
         <v>200</v>
@@ -17763,15 +17766,15 @@
         <v>236</v>
       </c>
       <c r="H637" s="3" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="638" spans="1:8">
       <c r="A638" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B638" s="3" t="s">
         <v>1269</v>
-      </c>
-      <c r="B638" s="3" t="s">
-        <v>1270</v>
       </c>
       <c r="C638" s="3" t="s">
         <v>198</v>
@@ -17789,15 +17792,15 @@
         <v>238</v>
       </c>
       <c r="H638" s="3" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="639" spans="1:8">
       <c r="A639" s="3" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B639" s="3" t="s">
         <v>1273</v>
-      </c>
-      <c r="B639" s="3" t="s">
-        <v>1274</v>
       </c>
       <c r="C639" s="3" t="s">
         <v>200</v>
@@ -17815,15 +17818,15 @@
         <v>238</v>
       </c>
       <c r="H639" s="3" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="640" spans="1:8">
       <c r="A640" s="3" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="B640" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C640" s="3" t="s">
         <v>198</v>
@@ -17841,7 +17844,7 @@
         <v>238</v>
       </c>
       <c r="H640" s="3" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="641" spans="1:8">
@@ -17867,15 +17870,15 @@
         <v>238</v>
       </c>
       <c r="H641" s="3" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="642" spans="1:8">
       <c r="A642" s="3" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="B642" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C642" s="3" t="s">
         <v>198</v>
@@ -17893,15 +17896,15 @@
         <v>236</v>
       </c>
       <c r="H642" s="3" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="643" spans="1:8">
       <c r="A643" s="3" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B643" s="3" t="s">
         <v>1282</v>
-      </c>
-      <c r="B643" s="3" t="s">
-        <v>1283</v>
       </c>
       <c r="C643" s="3" t="s">
         <v>198</v>
@@ -17919,15 +17922,15 @@
         <v>236</v>
       </c>
       <c r="H643" s="3" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="644" spans="1:8">
       <c r="A644" s="3" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B644" s="3" t="s">
         <v>1285</v>
-      </c>
-      <c r="B644" s="3" t="s">
-        <v>1286</v>
       </c>
       <c r="C644" s="3" t="s">
         <v>198</v>
@@ -17945,15 +17948,15 @@
         <v>236</v>
       </c>
       <c r="H644" s="3" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="645" spans="1:8">
       <c r="A645" s="3" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B645" s="3" t="s">
         <v>1288</v>
-      </c>
-      <c r="B645" s="3" t="s">
-        <v>1289</v>
       </c>
       <c r="C645" s="3" t="s">
         <v>200</v>
@@ -17971,15 +17974,15 @@
         <v>238</v>
       </c>
       <c r="H645" s="3" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="646" spans="1:8">
       <c r="A646" s="3" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B646" s="3" t="s">
         <v>1291</v>
-      </c>
-      <c r="B646" s="3" t="s">
-        <v>1292</v>
       </c>
       <c r="C646" s="3" t="s">
         <v>199</v>
@@ -17997,15 +18000,15 @@
         <v>236</v>
       </c>
       <c r="H646" s="3" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="647" spans="1:8">
       <c r="A647" s="3" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="B647" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="C647" s="3" t="s">
         <v>198</v>
@@ -18023,7 +18026,7 @@
         <v>238</v>
       </c>
       <c r="H647" s="3" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="648" spans="1:8">
@@ -18049,15 +18052,15 @@
         <v>236</v>
       </c>
       <c r="H648" s="3" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="649" spans="1:8">
       <c r="A649" s="3" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="B649" s="3" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="C649" s="3" t="s">
         <v>198</v>
@@ -18075,12 +18078,12 @@
         <v>238</v>
       </c>
       <c r="H649" s="3" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="650" spans="1:8">
       <c r="A650" s="3" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="B650" s="3" t="s">
         <v>170</v>
@@ -18101,7 +18104,7 @@
         <v>238</v>
       </c>
       <c r="H650" s="3" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="651" spans="1:8">
@@ -18127,15 +18130,15 @@
         <v>238</v>
       </c>
       <c r="H651" s="3" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="652" spans="1:8">
       <c r="A652" s="3" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B652" s="3" t="s">
         <v>1302</v>
-      </c>
-      <c r="B652" s="3" t="s">
-        <v>1303</v>
       </c>
       <c r="C652" s="3" t="s">
         <v>199</v>
@@ -18153,15 +18156,15 @@
         <v>238</v>
       </c>
       <c r="H652" s="3" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="653" spans="1:8">
       <c r="A653" s="3" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B653" s="3" t="s">
         <v>1305</v>
-      </c>
-      <c r="B653" s="3" t="s">
-        <v>1306</v>
       </c>
       <c r="C653" s="3" t="s">
         <v>199</v>
@@ -18179,15 +18182,15 @@
         <v>238</v>
       </c>
       <c r="H653" s="3" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="654" spans="1:8">
       <c r="A654" s="3" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B654" s="3" t="s">
         <v>1309</v>
-      </c>
-      <c r="B654" s="3" t="s">
-        <v>1310</v>
       </c>
       <c r="C654" s="3" t="s">
         <v>199</v>
@@ -18205,15 +18208,15 @@
         <v>238</v>
       </c>
       <c r="H654" s="3" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="655" spans="1:8">
       <c r="A655" s="3" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B655" s="3" t="s">
         <v>1312</v>
-      </c>
-      <c r="B655" s="3" t="s">
-        <v>1313</v>
       </c>
       <c r="C655" s="3" t="s">
         <v>198</v>
@@ -18231,7 +18234,7 @@
         <v>238</v>
       </c>
       <c r="H655" s="3" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="656" spans="1:8">
@@ -18257,15 +18260,15 @@
         <v>238</v>
       </c>
       <c r="H656" s="3" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="657" spans="1:8">
       <c r="A657" s="3" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B657" s="3" t="s">
         <v>1316</v>
-      </c>
-      <c r="B657" s="3" t="s">
-        <v>1317</v>
       </c>
       <c r="C657" s="3" t="s">
         <v>198</v>
@@ -18283,15 +18286,15 @@
         <v>236</v>
       </c>
       <c r="H657" s="3" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="658" spans="1:8">
       <c r="A658" s="3" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B658" s="3" t="s">
         <v>1319</v>
-      </c>
-      <c r="B658" s="3" t="s">
-        <v>1320</v>
       </c>
       <c r="C658" s="3" t="s">
         <v>198</v>
@@ -18309,15 +18312,15 @@
         <v>236</v>
       </c>
       <c r="H658" s="3" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="659" spans="1:8">
       <c r="A659" s="3" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B659" s="3" t="s">
         <v>1322</v>
-      </c>
-      <c r="B659" s="3" t="s">
-        <v>1323</v>
       </c>
       <c r="C659" s="3" t="s">
         <v>199</v>
@@ -18335,12 +18338,12 @@
         <v>238</v>
       </c>
       <c r="H659" s="3" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="660" spans="1:8">
       <c r="A660" s="3" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="B660" s="3" t="s">
         <v>690</v>
@@ -18361,12 +18364,12 @@
         <v>238</v>
       </c>
       <c r="H660" s="3" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="661" spans="1:8">
       <c r="A661" s="3" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="B661" s="3" t="s">
         <v>690</v>
@@ -18387,18 +18390,18 @@
         <v>238</v>
       </c>
       <c r="H661" s="3" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="662" spans="1:8">
       <c r="A662" s="3" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="B662" s="3" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="C662" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D662" s="6">
         <v>2019</v>
@@ -18413,15 +18416,15 @@
         <v>236</v>
       </c>
       <c r="H662" s="3" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="663" spans="1:8">
       <c r="A663" s="3" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B663" s="3" t="s">
         <v>1332</v>
-      </c>
-      <c r="B663" s="3" t="s">
-        <v>1333</v>
       </c>
       <c r="C663" s="3" t="s">
         <v>199</v>
@@ -18439,15 +18442,15 @@
         <v>238</v>
       </c>
       <c r="H663" s="3" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="664" spans="1:8">
       <c r="A664" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="B664" s="3" t="s">
         <v>1335</v>
-      </c>
-      <c r="B664" s="3" t="s">
-        <v>1336</v>
       </c>
       <c r="C664" s="3" t="s">
         <v>198</v>
@@ -18465,15 +18468,15 @@
         <v>238</v>
       </c>
       <c r="H664" s="3" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="665" spans="1:8">
       <c r="A665" s="3" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="B665" s="3" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="C665" s="3" t="s">
         <v>199</v>
@@ -18491,15 +18494,15 @@
         <v>238</v>
       </c>
       <c r="H665" s="3" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="666" spans="1:8">
       <c r="A666" s="3" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B666" s="3" t="s">
         <v>1341</v>
-      </c>
-      <c r="B666" s="3" t="s">
-        <v>1342</v>
       </c>
       <c r="C666" s="3" t="s">
         <v>198</v>
@@ -18517,15 +18520,15 @@
         <v>238</v>
       </c>
       <c r="H666" s="3" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="667" spans="1:8">
       <c r="A667" s="3" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="B667" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C667" s="3" t="s">
         <v>198</v>
@@ -18543,15 +18546,15 @@
         <v>238</v>
       </c>
       <c r="H667" s="3" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="668" spans="1:8">
       <c r="A668" s="3" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B668" s="3" t="s">
         <v>1346</v>
-      </c>
-      <c r="B668" s="3" t="s">
-        <v>1347</v>
       </c>
       <c r="C668" s="3" t="s">
         <v>198</v>
@@ -18569,15 +18572,15 @@
         <v>238</v>
       </c>
       <c r="H668" s="3" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="669" spans="1:8">
       <c r="A669" s="3" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B669" s="3" t="s">
         <v>1349</v>
-      </c>
-      <c r="B669" s="3" t="s">
-        <v>1350</v>
       </c>
       <c r="C669" s="3" t="s">
         <v>198</v>
@@ -18595,15 +18598,15 @@
         <v>236</v>
       </c>
       <c r="H669" s="3" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="670" spans="1:8">
       <c r="A670" s="3" t="s">
+        <v>1351</v>
+      </c>
+      <c r="B670" s="3" t="s">
         <v>1352</v>
-      </c>
-      <c r="B670" s="3" t="s">
-        <v>1353</v>
       </c>
       <c r="C670" s="3" t="s">
         <v>198</v>
@@ -18621,15 +18624,15 @@
         <v>238</v>
       </c>
       <c r="H670" s="3" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="671" spans="1:8">
       <c r="A671" s="3" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B671" s="3" t="s">
         <v>1355</v>
-      </c>
-      <c r="B671" s="3" t="s">
-        <v>1356</v>
       </c>
       <c r="C671" s="3" t="s">
         <v>198</v>
@@ -18647,15 +18650,15 @@
         <v>238</v>
       </c>
       <c r="H671" s="3" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="672" spans="1:8">
       <c r="A672" s="3" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="B672" s="3" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="C672" s="3" t="s">
         <v>198</v>
@@ -18673,15 +18676,15 @@
         <v>238</v>
       </c>
       <c r="H672" s="3" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="673" spans="1:8">
       <c r="A673" s="3" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B673" s="3" t="s">
         <v>1361</v>
-      </c>
-      <c r="B673" s="3" t="s">
-        <v>1362</v>
       </c>
       <c r="C673" s="3" t="s">
         <v>198</v>
@@ -18699,15 +18702,15 @@
         <v>238</v>
       </c>
       <c r="H673" s="3" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="674" spans="1:8">
       <c r="A674" s="3" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="B674" s="3" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="C674" s="3" t="s">
         <v>198</v>
@@ -18725,15 +18728,15 @@
         <v>238</v>
       </c>
       <c r="H674" s="3" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="675" spans="1:8">
       <c r="A675" s="3" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B675" s="3" t="s">
         <v>1367</v>
-      </c>
-      <c r="B675" s="3" t="s">
-        <v>1368</v>
       </c>
       <c r="C675" s="3" t="s">
         <v>198</v>
@@ -18751,15 +18754,15 @@
         <v>238</v>
       </c>
       <c r="H675" s="3" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="676" spans="1:8">
       <c r="A676" s="3" t="s">
+        <v>1369</v>
+      </c>
+      <c r="B676" s="3" t="s">
         <v>1370</v>
-      </c>
-      <c r="B676" s="3" t="s">
-        <v>1371</v>
       </c>
       <c r="C676" s="3" t="s">
         <v>198</v>
@@ -18777,16 +18780,34 @@
         <v>238</v>
       </c>
       <c r="H676" s="3" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="677" spans="1:8">
+      <c r="A677" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="B677" s="3" t="s">
         <v>1372</v>
       </c>
-    </row>
-    <row r="677" spans="1:8">
+      <c r="C677" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="D677" s="6">
         <v>2019</v>
       </c>
-      <c r="E677" s="6"/>
-      <c r="F677" s="6"/>
-      <c r="G677" s="6"/>
+      <c r="E677" s="6">
+        <v>1978</v>
+      </c>
+      <c r="F677" s="6">
+        <v>390</v>
+      </c>
+      <c r="G677" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H677" s="3" t="s">
+        <v>1373</v>
+      </c>
     </row>
     <row r="678" spans="1:8">
       <c r="D678" s="6">

</xml_diff>

<commit_message>
Machine Learning & The Giver
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FE35B1-A43B-564D-BD5A-C6E3A6D6EA93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF8B4BB-86EF-3E4D-B7D9-F1175361C8B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2383" uniqueCount="1376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2393" uniqueCount="1380">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4158,7 +4158,19 @@
     <t>Joan of Arc</t>
   </si>
   <si>
-    <t>Most interesting about this book is the unlikely devotion a man such as Twain had toward a girl such as Joan. Her simplicity and sincerity clearly won him over across hundreds of years of history, and his telling of her story allows her to win us over as well.</t>
+    <t>Machine Learning: The High-Interest Credit Card of Technical Debt</t>
+  </si>
+  <si>
+    <t>D. Sculley et al.</t>
+  </si>
+  <si>
+    <t>William suggested this and Joe emphasized its relevance for Root. I think I have come across this before but have much more understanding of it now, and it has some great suggestions for handling the technical debt specific to machine learing.</t>
+  </si>
+  <si>
+    <t>A horrible but beautiful story. I read this many years ago in school and decided to listen to it after Jordan read it recently. The future it describes is sterile and flat, but love prevails.</t>
+  </si>
+  <si>
+    <t>Most interesting about this book is the unlikely devotion a man such as Twain had toward a girl such as Joan. Her simplicity and sincerity clearly won him over across hundreds of years of history, and his telling of her story allows her to win us over as well. Shortly after finishing this I stumbled across Winston Churchill singing her praises in his History of the English Speaking Peoples: "Joan...find no equal in a thousand years...She embodied the natural goodness and valour of the human race in unexampled perfection." (vol 1, 422).</t>
   </si>
 </sst>
 </file>
@@ -4826,7 +4838,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4846,6 +4858,9 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="595">
@@ -5758,8 +5773,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A654" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A679" sqref="A679"/>
+      <pane ySplit="1" topLeftCell="A639" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A681" sqref="A681"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18838,24 +18853,60 @@
         <v>238</v>
       </c>
       <c r="H678" s="3" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="679" spans="1:8" ht="17">
+      <c r="A679" s="10" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="679" spans="1:8">
+      <c r="B679" s="3" t="s">
+        <v>1376</v>
+      </c>
+      <c r="C679" s="3" t="s">
+        <v>945</v>
+      </c>
       <c r="D679" s="6">
         <v>2019</v>
       </c>
-      <c r="E679" s="6"/>
-      <c r="F679" s="6"/>
-      <c r="G679" s="6"/>
+      <c r="E679" s="6">
+        <v>2014</v>
+      </c>
+      <c r="F679" s="6">
+        <v>9</v>
+      </c>
+      <c r="G679" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H679" s="3" t="s">
+        <v>1377</v>
+      </c>
     </row>
     <row r="680" spans="1:8">
+      <c r="A680" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B680" s="3" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C680" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D680" s="6">
         <v>2019</v>
       </c>
-      <c r="E680" s="6"/>
-      <c r="F680" s="6"/>
-      <c r="G680" s="6"/>
+      <c r="E680" s="6">
+        <v>1993</v>
+      </c>
+      <c r="F680" s="6">
+        <v>240</v>
+      </c>
+      <c r="G680" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H680" s="3" t="s">
+        <v>1378</v>
+      </c>
     </row>
     <row r="681" spans="1:8">
       <c r="D681" s="6">

</xml_diff>

<commit_message>
Gathering Blue & Hunted Priest
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF8B4BB-86EF-3E4D-B7D9-F1175361C8B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CDD080-CA74-AE46-8513-23132F169EC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2393" uniqueCount="1380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2403" uniqueCount="1385">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4171,6 +4171,21 @@
   </si>
   <si>
     <t>Most interesting about this book is the unlikely devotion a man such as Twain had toward a girl such as Joan. Her simplicity and sincerity clearly won him over across hundreds of years of history, and his telling of her story allows her to win us over as well. Shortly after finishing this I stumbled across Winston Churchill singing her praises in his History of the English Speaking Peoples: "Joan...find no equal in a thousand years...She embodied the natural goodness and valour of the human race in unexampled perfection." (vol 1, 422).</t>
+  </si>
+  <si>
+    <t>The Autobiography of a Hunted Priest</t>
+  </si>
+  <si>
+    <t>John Gerard, S.J.</t>
+  </si>
+  <si>
+    <t>Gathering Blue</t>
+  </si>
+  <si>
+    <t>Part 2 of the Giver Quartet.</t>
+  </si>
+  <si>
+    <t>This is the memoir of a courageous and humble priest persecuted by English Protestants. His stories demonstrate all that we have to be grateful for with free exercise of religion, and what may be demanded of us if that ever fades.</t>
   </si>
 </sst>
 </file>
@@ -5774,7 +5789,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A639" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A681" sqref="A681"/>
+      <selection pane="bottomLeft" activeCell="A683" sqref="A683"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18909,20 +18924,56 @@
       </c>
     </row>
     <row r="681" spans="1:8">
+      <c r="A681" s="3" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B681" s="3" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C681" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D681" s="6">
         <v>2019</v>
       </c>
-      <c r="E681" s="6"/>
-      <c r="F681" s="6"/>
-      <c r="G681" s="6"/>
+      <c r="E681" s="6">
+        <v>2000</v>
+      </c>
+      <c r="F681" s="6">
+        <v>256</v>
+      </c>
+      <c r="G681" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H681" s="3" t="s">
+        <v>1383</v>
+      </c>
     </row>
     <row r="682" spans="1:8">
+      <c r="A682" s="3" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B682" s="3" t="s">
+        <v>1381</v>
+      </c>
+      <c r="C682" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="D682" s="6">
         <v>2019</v>
       </c>
-      <c r="E682" s="6"/>
-      <c r="F682" s="6"/>
-      <c r="G682" s="6"/>
+      <c r="E682" s="6">
+        <v>1637</v>
+      </c>
+      <c r="F682" s="6">
+        <v>264</v>
+      </c>
+      <c r="G682" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="H682" s="3" t="s">
+        <v>1384</v>
+      </c>
     </row>
     <row r="683" spans="1:8">
       <c r="D683" s="6">

</xml_diff>

<commit_message>
John Paul the Great
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870DF312-7990-3A46-9A97-8BE5F6572959}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E85FE29-4F01-8C46-86AD-5F487CA8DEEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2408" uniqueCount="1387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2413" uniqueCount="1390">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4192,6 +4192,15 @@
   </si>
   <si>
     <t>Part 3 of the Giver Quartet.</t>
+  </si>
+  <si>
+    <t>John Paul the Great: Remembering a Spiritual Father</t>
+  </si>
+  <si>
+    <t>Peggy Noonan</t>
+  </si>
+  <si>
+    <t>The more I read about John Paul II the more I fall in love which Christ. This book is her spiritual memoir in parts, but the best parts are just about John Paul.</t>
   </si>
 </sst>
 </file>
@@ -5794,8 +5803,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A639" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A684" sqref="A684"/>
+      <pane ySplit="1" topLeftCell="A653" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A685" sqref="A685"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19008,12 +19017,30 @@
       </c>
     </row>
     <row r="684" spans="1:8">
+      <c r="A684" s="3" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B684" s="3" t="s">
+        <v>1388</v>
+      </c>
+      <c r="C684" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="D684" s="6">
         <v>2019</v>
       </c>
-      <c r="E684" s="6"/>
-      <c r="F684" s="6"/>
-      <c r="G684" s="6"/>
+      <c r="E684" s="6">
+        <v>2005</v>
+      </c>
+      <c r="F684" s="6">
+        <v>235</v>
+      </c>
+      <c r="G684" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H684" s="3" t="s">
+        <v>1389</v>
+      </c>
     </row>
     <row r="685" spans="1:8">
       <c r="D685" s="6">

</xml_diff>

<commit_message>
Property & Casualty Insurance Primer
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C644935A-FAE6-B342-9623-C71C3342CF4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9090DF7-1E30-E849-A813-056B7B6CE6A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2423" uniqueCount="1394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2428" uniqueCount="1397">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4213,6 +4213,15 @@
   </si>
   <si>
     <t xml:space="preserve">I listened to most of this on the way back from Scott's wedding in Nashville. Flannery is dark and weird but uses those things to point to something beautiful. I would love to hear Bishop Barron explain this book. </t>
+  </si>
+  <si>
+    <t>Property &amp; Casualty Insurance Primer</t>
+  </si>
+  <si>
+    <t>Cliff Gallant et al. (KBW)</t>
+  </si>
+  <si>
+    <t>This was a helpful industry overview.</t>
   </si>
 </sst>
 </file>
@@ -19107,12 +19116,30 @@
       </c>
     </row>
     <row r="687" spans="1:8">
+      <c r="A687" s="3" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B687" s="3" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C687" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="D687" s="6">
         <v>2019</v>
       </c>
-      <c r="E687" s="6"/>
-      <c r="F687" s="6"/>
-      <c r="G687" s="6"/>
+      <c r="E687" s="6">
+        <v>2010</v>
+      </c>
+      <c r="F687" s="6">
+        <v>119</v>
+      </c>
+      <c r="G687" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H687" s="3" t="s">
+        <v>1396</v>
+      </c>
     </row>
     <row r="688" spans="1:8">
       <c r="D688" s="6">

</xml_diff>

<commit_message>
The Death of Ivan Ilyich
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9090DF7-1E30-E849-A813-056B7B6CE6A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED338BF-0585-354E-8FCE-F2A24404B267}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="191029" iterate="1" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2428" uniqueCount="1397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2433" uniqueCount="1398">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4222,6 +4222,9 @@
   </si>
   <si>
     <t>This was a helpful industry overview.</t>
+  </si>
+  <si>
+    <t>BC 12: I first read this in my MBA ethics class, and again for book club. It is a good time for me to read with some changes at work, and a reminder to live the right kind of life, as well as the importance of living and dying well.</t>
   </si>
 </sst>
 </file>
@@ -5825,7 +5828,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A653" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A687" sqref="A687"/>
+      <selection pane="bottomLeft" activeCell="A689" sqref="A689"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19142,39 +19145,67 @@
       </c>
     </row>
     <row r="688" spans="1:8">
+      <c r="A688" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B688" s="3" t="s">
+        <v>710</v>
+      </c>
+      <c r="C688" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="D688" s="6">
         <v>2019</v>
       </c>
-      <c r="E688" s="6"/>
-      <c r="F688" s="6"/>
-      <c r="G688" s="6"/>
+      <c r="E688" s="6">
+        <v>1886</v>
+      </c>
+      <c r="F688" s="6">
+        <v>113</v>
+      </c>
+      <c r="G688" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H688" s="3" t="s">
+        <v>1397</v>
+      </c>
     </row>
     <row r="689" spans="4:7">
-      <c r="D689" s="6"/>
+      <c r="D689" s="6">
+        <v>2019</v>
+      </c>
       <c r="E689" s="6"/>
       <c r="F689" s="6"/>
       <c r="G689" s="6"/>
     </row>
     <row r="690" spans="4:7">
-      <c r="D690" s="6"/>
+      <c r="D690" s="6">
+        <v>2019</v>
+      </c>
       <c r="E690" s="6"/>
       <c r="F690" s="6"/>
       <c r="G690" s="6"/>
     </row>
     <row r="691" spans="4:7">
-      <c r="D691" s="6"/>
+      <c r="D691" s="6">
+        <v>2019</v>
+      </c>
       <c r="E691" s="6"/>
       <c r="F691" s="6"/>
       <c r="G691" s="6"/>
     </row>
     <row r="692" spans="4:7">
-      <c r="D692" s="6"/>
+      <c r="D692" s="6">
+        <v>2019</v>
+      </c>
       <c r="E692" s="6"/>
       <c r="F692" s="6"/>
       <c r="G692" s="6"/>
     </row>
     <row r="693" spans="4:7">
-      <c r="D693" s="6"/>
+      <c r="D693" s="6">
+        <v>2019</v>
+      </c>
       <c r="E693" s="6"/>
       <c r="F693" s="6"/>
       <c r="G693" s="6"/>

</xml_diff>

<commit_message>
The Love That Keeps Us Sane
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED338BF-0585-354E-8FCE-F2A24404B267}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205A5E85-D9EF-5449-8D59-C270E319324E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2433" uniqueCount="1398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="1401">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4225,6 +4225,15 @@
   </si>
   <si>
     <t>BC 12: I first read this in my MBA ethics class, and again for book club. It is a good time for me to read with some changes at work, and a reminder to live the right kind of life, as well as the importance of living and dying well.</t>
+  </si>
+  <si>
+    <t>The Love That Keeps Us Sane: Living the Little Way of St. Thérèse of Lisieux</t>
+  </si>
+  <si>
+    <t>Marc Foley, O.C.D.</t>
+  </si>
+  <si>
+    <t>Jordan gave me this after she read it, and it is a short and beautiful reflection on St. Therese's way of loving simply and in the midst of the real world. It has some particularly good practical advice for loving in our relationships while keeping appropriate boundaries and distance.</t>
   </si>
 </sst>
 </file>
@@ -5828,7 +5837,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A653" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A689" sqref="A689"/>
+      <selection pane="bottomLeft" activeCell="B690" sqref="B690"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19170,15 +19179,33 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="689" spans="4:7">
+    <row r="689" spans="1:8">
+      <c r="A689" s="3" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B689" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C689" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="D689" s="6">
         <v>2019</v>
       </c>
-      <c r="E689" s="6"/>
-      <c r="F689" s="6"/>
-      <c r="G689" s="6"/>
-    </row>
-    <row r="690" spans="4:7">
+      <c r="E689" s="6">
+        <v>2000</v>
+      </c>
+      <c r="F689" s="6">
+        <v>82</v>
+      </c>
+      <c r="G689" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H689" s="3" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="690" spans="1:8">
       <c r="D690" s="6">
         <v>2019</v>
       </c>
@@ -19186,7 +19213,7 @@
       <c r="F690" s="6"/>
       <c r="G690" s="6"/>
     </row>
-    <row r="691" spans="4:7">
+    <row r="691" spans="1:8">
       <c r="D691" s="6">
         <v>2019</v>
       </c>
@@ -19194,7 +19221,7 @@
       <c r="F691" s="6"/>
       <c r="G691" s="6"/>
     </row>
-    <row r="692" spans="4:7">
+    <row r="692" spans="1:8">
       <c r="D692" s="6">
         <v>2019</v>
       </c>
@@ -19202,7 +19229,7 @@
       <c r="F692" s="6"/>
       <c r="G692" s="6"/>
     </row>
-    <row r="693" spans="4:7">
+    <row r="693" spans="1:8">
       <c r="D693" s="6">
         <v>2019</v>
       </c>
@@ -19210,67 +19237,67 @@
       <c r="F693" s="6"/>
       <c r="G693" s="6"/>
     </row>
-    <row r="694" spans="4:7">
+    <row r="694" spans="1:8">
       <c r="D694" s="6"/>
       <c r="E694" s="6"/>
       <c r="F694" s="6"/>
       <c r="G694" s="6"/>
     </row>
-    <row r="695" spans="4:7">
+    <row r="695" spans="1:8">
       <c r="D695" s="6"/>
       <c r="E695" s="6"/>
       <c r="F695" s="6"/>
       <c r="G695" s="6"/>
     </row>
-    <row r="696" spans="4:7">
+    <row r="696" spans="1:8">
       <c r="D696" s="6"/>
       <c r="E696" s="6"/>
       <c r="F696" s="6"/>
       <c r="G696" s="6"/>
     </row>
-    <row r="697" spans="4:7">
+    <row r="697" spans="1:8">
       <c r="D697" s="6"/>
       <c r="E697" s="6"/>
       <c r="F697" s="6"/>
       <c r="G697" s="6"/>
     </row>
-    <row r="698" spans="4:7">
+    <row r="698" spans="1:8">
       <c r="D698" s="6"/>
       <c r="E698" s="6"/>
       <c r="F698" s="6"/>
       <c r="G698" s="6"/>
     </row>
-    <row r="699" spans="4:7">
+    <row r="699" spans="1:8">
       <c r="D699" s="6"/>
       <c r="E699" s="6"/>
       <c r="F699" s="6"/>
       <c r="G699" s="6"/>
     </row>
-    <row r="700" spans="4:7">
+    <row r="700" spans="1:8">
       <c r="D700" s="6"/>
       <c r="E700" s="6"/>
       <c r="F700" s="6"/>
       <c r="G700" s="6"/>
     </row>
-    <row r="701" spans="4:7">
+    <row r="701" spans="1:8">
       <c r="D701" s="6"/>
       <c r="E701" s="6"/>
       <c r="F701" s="6"/>
       <c r="G701" s="6"/>
     </row>
-    <row r="702" spans="4:7">
+    <row r="702" spans="1:8">
       <c r="D702" s="6"/>
       <c r="E702" s="6"/>
       <c r="F702" s="6"/>
       <c r="G702" s="6"/>
     </row>
-    <row r="703" spans="4:7">
+    <row r="703" spans="1:8">
       <c r="D703" s="6"/>
       <c r="E703" s="6"/>
       <c r="F703" s="6"/>
       <c r="G703" s="6"/>
     </row>
-    <row r="704" spans="4:7">
+    <row r="704" spans="1:8">
       <c r="D704" s="6"/>
       <c r="E704" s="6"/>
       <c r="F704" s="6"/>

</xml_diff>

<commit_message>
The Sun Does Shine
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205A5E85-D9EF-5449-8D59-C270E319324E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F3F3D4-01CA-8047-8061-A1DCDA34744E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" calcOnSave="0"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="1401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2443" uniqueCount="1404">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4234,6 +4234,15 @@
   </si>
   <si>
     <t>Jordan gave me this after she read it, and it is a short and beautiful reflection on St. Therese's way of loving simply and in the midst of the real world. It has some particularly good practical advice for loving in our relationships while keeping appropriate boundaries and distance.</t>
+  </si>
+  <si>
+    <t>The Sun Does Shine: How I Found Life and Freedom on Death Row</t>
+  </si>
+  <si>
+    <t>Anthony Ray Hinton</t>
+  </si>
+  <si>
+    <t>Another recommendation from Jordan, and a heartbreaking but beautiful story of death row and redemption.</t>
   </si>
 </sst>
 </file>
@@ -5837,7 +5846,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A653" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B690" sqref="B690"/>
+      <selection pane="bottomLeft" activeCell="A691" sqref="A691"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19206,12 +19215,30 @@
       </c>
     </row>
     <row r="690" spans="1:8">
+      <c r="A690" s="3" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B690" s="3" t="s">
+        <v>1402</v>
+      </c>
+      <c r="C690" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D690" s="6">
         <v>2019</v>
       </c>
-      <c r="E690" s="6"/>
-      <c r="F690" s="6"/>
-      <c r="G690" s="6"/>
+      <c r="E690" s="6">
+        <v>2018</v>
+      </c>
+      <c r="F690" s="6">
+        <v>288</v>
+      </c>
+      <c r="G690" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H690" s="3" t="s">
+        <v>1403</v>
+      </c>
     </row>
     <row r="691" spans="1:8">
       <c r="D691" s="6">

</xml_diff>

<commit_message>
A Theology of the Body
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED76D0DE-53CD-5149-8434-5F48DD99E10E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6461D3F2-8E27-F346-A24E-624AD2264DE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2448" uniqueCount="1407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2453" uniqueCount="1409">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4252,6 +4252,12 @@
   </si>
   <si>
     <t>Fr. Dailey recommended that I read a general biography of Padre Pio to get to know him, and this was perfect. It was written by a priest who knew him firsthand, and gives the facts of his life from a perspetive of faith. He lived a beautiful life.</t>
+  </si>
+  <si>
+    <t>Man and Woman He Created Them: A Theology of the Body</t>
+  </si>
+  <si>
+    <t>Jordan and I read this together over the course of 2019 (finishing a bit early because it was challenging to keep going with small progress). To be honest it was a challenge. JPII's thought can be dense, but there definitely shone through some nuggets that are very relatable and helpful. Of particular note is his lengthy meditation on Matthew 5:28 (commit adultery on your heart), the Song of Songs and Tobit, and the last section on Humanae Vitae.</t>
   </si>
 </sst>
 </file>
@@ -5855,7 +5861,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A653" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A692" sqref="A692"/>
+      <selection pane="bottomLeft" activeCell="A693" sqref="A693"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19276,12 +19282,30 @@
       </c>
     </row>
     <row r="692" spans="1:8">
+      <c r="A692" s="3" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B692" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="C692" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="D692" s="6">
         <v>2019</v>
       </c>
-      <c r="E692" s="6"/>
-      <c r="F692" s="6"/>
-      <c r="G692" s="6"/>
+      <c r="E692" s="6">
+        <v>1986</v>
+      </c>
+      <c r="F692" s="6">
+        <v>663</v>
+      </c>
+      <c r="G692" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H692" s="3" t="s">
+        <v>1408</v>
+      </c>
     </row>
     <row r="693" spans="1:8">
       <c r="D693" s="6">

</xml_diff>

<commit_message>
American Caesar: Douglas MacArthur
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C59EC57-C70F-8E41-8885-99EC8249E2CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759CF107-0524-6B4E-8CDF-410B298F47F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2458" uniqueCount="1412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2463" uniqueCount="1414">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4267,6 +4267,12 @@
   </si>
   <si>
     <t>After learning about his life, Don Bosco is one of my favorite saints. His simplicity, practical holiness, and devotion to Mary are beautiful examples.</t>
+  </si>
+  <si>
+    <t>American Caesar: Douglas MacArthur 1880 - 1964</t>
+  </si>
+  <si>
+    <t>What a fascinating life and what a majestic storyteller. Jacket describes him as "Inspiring, outrageous... A thundering paradox of a man." His deep sense of duty, arrogance, courage, and the depths to which he fell and the heights to which he towered. As always with Manchester (and any good biography), I learned much about the world he lived in.</t>
   </si>
 </sst>
 </file>
@@ -5870,7 +5876,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A653" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F694" sqref="F694"/>
+      <selection pane="bottomLeft" activeCell="H695" sqref="H695"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19343,12 +19349,30 @@
       </c>
     </row>
     <row r="694" spans="1:8">
+      <c r="A694" s="3" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B694" s="3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C694" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="D694" s="6">
         <v>2019</v>
       </c>
-      <c r="E694" s="6"/>
-      <c r="F694" s="6"/>
-      <c r="G694" s="6"/>
+      <c r="E694" s="6">
+        <v>1978</v>
+      </c>
+      <c r="F694" s="6">
+        <v>816</v>
+      </c>
+      <c r="G694" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="H694" s="3" t="s">
+        <v>1413</v>
+      </c>
     </row>
     <row r="695" spans="1:8">
       <c r="D695" s="6">

</xml_diff>

<commit_message>
The Imitation of Christ
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956316C6-0336-7E40-B180-E375F3333212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A635AD53-9C62-8747-915B-4C777E23C1FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2473" uniqueCount="1420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2478" uniqueCount="1423">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4291,6 +4291,15 @@
   </si>
   <si>
     <t xml:space="preserve">Becca got this for my birthday, and it is hilarious! </t>
+  </si>
+  <si>
+    <t>The Imitation of Christ</t>
+  </si>
+  <si>
+    <t>Thomas à Kempis</t>
+  </si>
+  <si>
+    <t>This is definitely on my short list of the top 7 books to re-read over a lifetime. My first reading took place over the course of more than a year, during which time it was on my nightstand. I went long stretches without reading from it at all, but it is always a joy to come back to. Such a beautiful devotional book.</t>
   </si>
 </sst>
 </file>
@@ -5893,8 +5902,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A653" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A697" sqref="A697"/>
+      <pane ySplit="1" topLeftCell="A668" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A698" sqref="A698"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19445,12 +19454,30 @@
       </c>
     </row>
     <row r="697" spans="1:8">
+      <c r="A697" s="3" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B697" s="3" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C697" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="D697" s="6">
         <v>2019</v>
       </c>
-      <c r="E697" s="6"/>
-      <c r="F697" s="6"/>
-      <c r="G697" s="6"/>
+      <c r="E697" s="6">
+        <v>1418</v>
+      </c>
+      <c r="F697" s="6">
+        <v>249</v>
+      </c>
+      <c r="G697" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H697" s="3" t="s">
+        <v>1422</v>
+      </c>
     </row>
     <row r="698" spans="1:8">
       <c r="D698" s="6">

</xml_diff>

<commit_message>
The Complete Book of Woodworking
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF5BCDF-A883-5747-B4AD-7B2952390425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E91DB5-6466-5B4E-B3F4-82FF1CD82017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2483" uniqueCount="1424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2488" uniqueCount="1427">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4303,6 +4303,15 @@
   </si>
   <si>
     <t>A beautiful reflection on the incarnation, especially during Advent.</t>
+  </si>
+  <si>
+    <t>The Complete Book of Woodworking</t>
+  </si>
+  <si>
+    <t>This was a great birthday present from Jordan! I really appreciated all the detailed instructions and information in the first half of the book, some of which I have gotten scattered from videos but this goes through everything systematically and will be a good future reference as well. The whole second half of the book has projects.</t>
+  </si>
+  <si>
+    <t>Tom Carpenter &amp; Mark Johanson</t>
   </si>
 </sst>
 </file>
@@ -5905,8 +5914,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A667" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A699" sqref="A699"/>
+      <pane ySplit="1" topLeftCell="A660" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A700" sqref="A700"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19509,12 +19518,30 @@
       </c>
     </row>
     <row r="699" spans="1:8">
+      <c r="A699" s="3" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B699" s="3" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C699" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="D699" s="6">
         <v>2019</v>
       </c>
-      <c r="E699" s="6"/>
-      <c r="F699" s="6"/>
-      <c r="G699" s="6"/>
+      <c r="E699" s="6">
+        <v>2001</v>
+      </c>
+      <c r="F699" s="6">
+        <v>155</v>
+      </c>
+      <c r="G699" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H699" s="3" t="s">
+        <v>1425</v>
+      </c>
     </row>
     <row r="700" spans="1:8">
       <c r="D700" s="6">

</xml_diff>

<commit_message>
Sapiens: A Brief History of Humankind
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E91DB5-6466-5B4E-B3F4-82FF1CD82017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259BD241-532B-3345-9C2A-FE32E780044A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2488" uniqueCount="1427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2493" uniqueCount="1430">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4312,6 +4312,15 @@
   </si>
   <si>
     <t>Tom Carpenter &amp; Mark Johanson</t>
+  </si>
+  <si>
+    <t>Sapiens: A Brief History of Humankind</t>
+  </si>
+  <si>
+    <t>Yuval Noah Harari</t>
+  </si>
+  <si>
+    <t>A very interesting read but very scary if his materialism and atheism is taken to *forward* in history. I would love to read "A Brief History of Humankind" by someone as intelligent and good at writing as Harari, but who also believes in God.</t>
   </si>
 </sst>
 </file>
@@ -5914,8 +5923,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A660" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A700" sqref="A700"/>
+      <pane ySplit="1" topLeftCell="A673" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A701" sqref="A701"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19544,12 +19553,30 @@
       </c>
     </row>
     <row r="700" spans="1:8">
+      <c r="A700" s="3" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B700" s="3" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C700" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D700" s="6">
         <v>2019</v>
       </c>
-      <c r="E700" s="6"/>
-      <c r="F700" s="6"/>
-      <c r="G700" s="6"/>
+      <c r="E700" s="6">
+        <v>2015</v>
+      </c>
+      <c r="F700" s="6">
+        <v>464</v>
+      </c>
+      <c r="G700" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H700" s="3" t="s">
+        <v>1429</v>
+      </c>
     </row>
     <row r="701" spans="1:8">
       <c r="D701" s="6">

</xml_diff>

<commit_message>
How to Raise Good Catholic Children
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6BBB67-E088-484F-8B44-DC40E1AE3D30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05374186-DDC2-9548-8EDA-1394836D02BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2498" uniqueCount="1431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2503" uniqueCount="1434">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4324,16 +4324,22 @@
   </si>
   <si>
     <t>I started reading this for a men's group which led to a wonderful discussion, and I enjoyed reading the rest of the letter on my own. John Paul especially calls the laity to use the instruments of property, markets, and government to support the common good and build the Kingdom of God.</t>
+  </si>
+  <si>
+    <t>How to Raise Good Catholic Children</t>
+  </si>
+  <si>
+    <t>Mary Reed Newland</t>
+  </si>
+  <si>
+    <t>This was a very practical and helpful guide to raising Catholic children. I particularly like her dialogue and suggested ways of talking to kids.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-  </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4373,12 +4379,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri (Body)"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -5000,7 +5000,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5024,7 +5024,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="595">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -5936,8 +5935,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A657" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A702" sqref="A702"/>
+      <pane ySplit="1" topLeftCell="A656" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A703" sqref="A703"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19592,7 +19591,7 @@
       </c>
     </row>
     <row r="701" spans="1:8">
-      <c r="A701" s="11" t="s">
+      <c r="A701" s="3" t="s">
         <v>1429</v>
       </c>
       <c r="B701" s="3" t="s">
@@ -19618,12 +19617,30 @@
       </c>
     </row>
     <row r="702" spans="1:8">
+      <c r="A702" s="3" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B702" s="3" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C702" s="3" t="s">
+        <v>200</v>
+      </c>
       <c r="D702" s="6">
         <v>2019</v>
       </c>
-      <c r="E702" s="6"/>
-      <c r="F702" s="6"/>
-      <c r="G702" s="6"/>
+      <c r="E702" s="6">
+        <v>1954</v>
+      </c>
+      <c r="F702" s="6">
+        <v>336</v>
+      </c>
+      <c r="G702" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H702" s="3" t="s">
+        <v>1433</v>
+      </c>
     </row>
     <row r="703" spans="1:8">
       <c r="D703" s="6">

</xml_diff>

<commit_message>
Walking: One Step At a Time
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C7EA21-A0D2-B64A-8441-7B3E4C4A82F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D425B1F1-8435-494E-A51C-956D6D3143E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="760" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2508" uniqueCount="1436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2513" uniqueCount="1438">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4339,6 +4339,12 @@
   </si>
   <si>
     <t>I have of course heard of Scrooge but never read this classic. It is appropriate to read adjacent to The Death of Ivan Ilyich.</t>
+  </si>
+  <si>
+    <t>Walking: One Step At a Time</t>
+  </si>
+  <si>
+    <t>This book has a lot of great thoughts and I took some notes on them. I appreciate the message about walking to improve health, thinking, and general wellbeing by being close to nature and building in time for solitude. The "adventure" explorer side of his philosophy does not resonate as much with me, and I find it challenging to take advice from someone when their home life is not in order: first things must be first.</t>
   </si>
 </sst>
 </file>
@@ -5941,8 +5947,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A661" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A704" sqref="A704"/>
+      <pane ySplit="1" topLeftCell="A666" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E705" sqref="E705"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -17992,7 +17998,7 @@
         <v>1272</v>
       </c>
       <c r="C639" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D639" s="6">
         <v>2019</v>
@@ -19675,13 +19681,35 @@
       </c>
     </row>
     <row r="704" spans="1:8">
-      <c r="D704" s="6"/>
-      <c r="E704" s="6"/>
-      <c r="F704" s="6"/>
-      <c r="G704" s="6"/>
+      <c r="A704" s="3" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B704" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="C704" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D704" s="6">
+        <v>2019</v>
+      </c>
+      <c r="E704" s="6">
+        <v>2019</v>
+      </c>
+      <c r="F704" s="6">
+        <v>192</v>
+      </c>
+      <c r="G704" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H704" s="3" t="s">
+        <v>1437</v>
+      </c>
     </row>
     <row r="705" spans="4:7">
-      <c r="D705" s="6"/>
+      <c r="D705" s="6">
+        <v>2019</v>
+      </c>
       <c r="E705" s="6"/>
       <c r="F705" s="6"/>
       <c r="G705" s="6"/>

</xml_diff>

<commit_message>
Manual for Eucharistic Adoration
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,37 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E3070C-76F1-194E-9F61-CC5CADC57710}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="760" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2515" uniqueCount="1439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2520" uniqueCount="1442">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4348,13 +4342,22 @@
   </si>
   <si>
     <t>Bible: Second Catholic Edition RSV (Mark, Luke, Matthew, John, Acts, Song of Songs, Daniel)</t>
+  </si>
+  <si>
+    <t>Manual for Eucharistic Adoration</t>
+  </si>
+  <si>
+    <t>The Poor Clares of Perpetual Adoration &amp; Paul Thigpen</t>
+  </si>
+  <si>
+    <t>This has been a helpful guide and companion during my time before the Blessed Sacrament. I am again drawn to the quote from Tolkien: "I put before you the one grat thing to love on earth: the Blessed Sacrament….There you will find romance, glory, honor, fidelity, and the true way of all your loves upon earth."</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5693,7 +5696,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -5745,7 +5748,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -5939,22 +5942,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A678" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A706" sqref="A706"/>
+      <selection pane="bottomLeft" activeCell="A707" sqref="A707"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="98" style="3" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="3" customWidth="1"/>
@@ -19033,7 +19036,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="679" spans="1:8" ht="17">
+    <row r="679" spans="1:8">
       <c r="A679" s="10" t="s">
         <v>1374</v>
       </c>
@@ -19728,16 +19731,30 @@
       <c r="G705" s="6"/>
     </row>
     <row r="706" spans="1:8">
-      <c r="A706" s="4"/>
-      <c r="B706" s="4"/>
-      <c r="C706" s="4"/>
+      <c r="A706" s="4" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B706" s="4" t="s">
+        <v>1440</v>
+      </c>
+      <c r="C706" s="4" t="s">
+        <v>197</v>
+      </c>
       <c r="D706" s="5">
         <v>2020</v>
       </c>
-      <c r="E706" s="5"/>
-      <c r="F706" s="5"/>
-      <c r="G706" s="5"/>
-      <c r="H706" s="4"/>
+      <c r="E706" s="5">
+        <v>2016</v>
+      </c>
+      <c r="F706" s="5">
+        <v>130</v>
+      </c>
+      <c r="G706" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="H706" s="4" t="s">
+        <v>1441</v>
+      </c>
     </row>
     <row r="707" spans="1:8">
       <c r="D707" s="6"/>

</xml_diff>

<commit_message>
A Hobbit, a Wardrobe, and a Great War
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C4688B-E86E-664E-B158-837098B2AA80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2520" uniqueCount="1442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2525" uniqueCount="1445">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4351,13 +4357,22 @@
   </si>
   <si>
     <t>This has been a helpful guide and companion during my time before the Blessed Sacrament. I am again drawn to the quote from Tolkien: "I put before you the one grat thing to love on earth: the Blessed Sacrament….There you will find romance, glory, honor, fidelity, and the true way of all your loves upon earth."</t>
+  </si>
+  <si>
+    <t>A Hobbit, a Wardrobe, and a Great War: How J.R.R. Tolkien and C.S. Lewis Rediscovered Faith, Friendship, and Heroism in the Cataclysm of 1914-1918</t>
+  </si>
+  <si>
+    <t>Joseph Loconte</t>
+  </si>
+  <si>
+    <t>Whenever I read a book about Tolkien and Lewis I feel inspired. They are so real and so honest and so noble. This book does a great job of putting their lives and friendship and works into the context of their struggle in WWI. It's surprising how forgotten WWI seems to be, and yet how monumental it was in the havoc it wrought and then beauty that sprang forth from its fires.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5942,22 +5957,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A678" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A707" sqref="A707"/>
+      <pane ySplit="1" topLeftCell="A690" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H708" sqref="H708"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="98" style="3" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="3" customWidth="1"/>
@@ -19036,7 +19051,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="679" spans="1:8">
+    <row r="679" spans="1:8" ht="17">
       <c r="A679" s="10" t="s">
         <v>1374</v>
       </c>
@@ -19757,91 +19772,139 @@
       </c>
     </row>
     <row r="707" spans="1:8">
-      <c r="D707" s="6"/>
-      <c r="E707" s="6"/>
-      <c r="F707" s="6"/>
-      <c r="G707" s="6"/>
+      <c r="A707" s="3" t="s">
+        <v>1442</v>
+      </c>
+      <c r="B707" s="3" t="s">
+        <v>1443</v>
+      </c>
+      <c r="C707" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D707" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E707" s="6">
+        <v>2015</v>
+      </c>
+      <c r="F707" s="6">
+        <v>196</v>
+      </c>
+      <c r="G707" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H707" s="3" t="s">
+        <v>1444</v>
+      </c>
     </row>
     <row r="708" spans="1:8">
-      <c r="D708" s="6"/>
+      <c r="D708" s="6">
+        <v>2020</v>
+      </c>
       <c r="E708" s="6"/>
       <c r="F708" s="6"/>
       <c r="G708" s="6"/>
     </row>
     <row r="709" spans="1:8">
-      <c r="D709" s="6"/>
+      <c r="D709" s="6">
+        <v>2020</v>
+      </c>
       <c r="E709" s="6"/>
       <c r="F709" s="6"/>
       <c r="G709" s="6"/>
     </row>
     <row r="710" spans="1:8">
-      <c r="D710" s="6"/>
+      <c r="D710" s="6">
+        <v>2020</v>
+      </c>
       <c r="E710" s="6"/>
       <c r="F710" s="6"/>
       <c r="G710" s="6"/>
     </row>
     <row r="711" spans="1:8">
-      <c r="D711" s="6"/>
+      <c r="D711" s="6">
+        <v>2020</v>
+      </c>
       <c r="E711" s="6"/>
       <c r="F711" s="6"/>
       <c r="G711" s="6"/>
     </row>
     <row r="712" spans="1:8">
-      <c r="D712" s="6"/>
+      <c r="D712" s="6">
+        <v>2020</v>
+      </c>
       <c r="E712" s="6"/>
       <c r="F712" s="6"/>
       <c r="G712" s="6"/>
     </row>
     <row r="713" spans="1:8">
-      <c r="D713" s="6"/>
+      <c r="D713" s="6">
+        <v>2020</v>
+      </c>
       <c r="E713" s="6"/>
       <c r="F713" s="6"/>
       <c r="G713" s="6"/>
     </row>
     <row r="714" spans="1:8">
-      <c r="D714" s="6"/>
+      <c r="D714" s="6">
+        <v>2020</v>
+      </c>
       <c r="E714" s="6"/>
       <c r="F714" s="6"/>
       <c r="G714" s="6"/>
     </row>
     <row r="715" spans="1:8">
-      <c r="D715" s="6"/>
+      <c r="D715" s="6">
+        <v>2020</v>
+      </c>
       <c r="E715" s="6"/>
       <c r="F715" s="6"/>
       <c r="G715" s="6"/>
     </row>
     <row r="716" spans="1:8">
-      <c r="D716" s="6"/>
+      <c r="D716" s="6">
+        <v>2020</v>
+      </c>
       <c r="E716" s="6"/>
       <c r="F716" s="6"/>
       <c r="G716" s="6"/>
     </row>
     <row r="717" spans="1:8">
-      <c r="D717" s="6"/>
+      <c r="D717" s="6">
+        <v>2020</v>
+      </c>
       <c r="E717" s="6"/>
       <c r="F717" s="6"/>
       <c r="G717" s="6"/>
     </row>
     <row r="718" spans="1:8">
-      <c r="D718" s="6"/>
+      <c r="D718" s="6">
+        <v>2020</v>
+      </c>
       <c r="E718" s="6"/>
       <c r="F718" s="6"/>
       <c r="G718" s="6"/>
     </row>
     <row r="719" spans="1:8">
-      <c r="D719" s="6"/>
+      <c r="D719" s="6">
+        <v>2020</v>
+      </c>
       <c r="E719" s="6"/>
       <c r="F719" s="6"/>
       <c r="G719" s="6"/>
     </row>
     <row r="720" spans="1:8">
-      <c r="D720" s="6"/>
+      <c r="D720" s="6">
+        <v>2020</v>
+      </c>
       <c r="E720" s="6"/>
       <c r="F720" s="6"/>
       <c r="G720" s="6"/>
     </row>
     <row r="721" spans="4:7">
-      <c r="D721" s="6"/>
+      <c r="D721" s="6">
+        <v>2020</v>
+      </c>
       <c r="E721" s="6"/>
       <c r="F721" s="6"/>
       <c r="G721" s="6"/>

</xml_diff>

<commit_message>
The Family & the New Totalitarianism
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C4688B-E86E-664E-B158-837098B2AA80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3F47EA-636F-3941-97D8-88678ECECE4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2525" uniqueCount="1445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2530" uniqueCount="1447">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4366,6 +4366,12 @@
   </si>
   <si>
     <t>Whenever I read a book about Tolkien and Lewis I feel inspired. They are so real and so honest and so noble. This book does a great job of putting their lives and friendship and works into the context of their struggle in WWI. It's surprising how forgotten WWI seems to be, and yet how monumental it was in the havoc it wrought and then beauty that sprang forth from its fires.</t>
+  </si>
+  <si>
+    <t>The Family &amp; the New Totalitarianism</t>
+  </si>
+  <si>
+    <t>This book created mixed feelings: fear and anguish over the state of the State in relation to the family; hope and gratitude for the beauty of the Truth as given in the Church. A couple essays in the middle were overly "political", but overall was a good reminder to draw close to the Church to build up our families.</t>
   </si>
 </sst>
 </file>
@@ -5711,7 +5717,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -5763,7 +5769,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -5969,7 +5975,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A690" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H708" sqref="H708"/>
+      <selection pane="bottomLeft" activeCell="A709" sqref="A709"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19798,12 +19804,30 @@
       </c>
     </row>
     <row r="708" spans="1:8">
+      <c r="A708" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="B708" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="C708" s="3" t="s">
+        <v>197</v>
+      </c>
       <c r="D708" s="6">
         <v>2020</v>
       </c>
-      <c r="E708" s="6"/>
-      <c r="F708" s="6"/>
-      <c r="G708" s="6"/>
+      <c r="E708" s="6">
+        <v>2019</v>
+      </c>
+      <c r="F708" s="6">
+        <v>248</v>
+      </c>
+      <c r="G708" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H708" s="3" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="709" spans="1:8">
       <c r="D709" s="6">

</xml_diff>

<commit_message>
Death Comes for the Archbishop
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3F47EA-636F-3941-97D8-88678ECECE4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43BEAC9-6802-B24A-9517-CF194D803CE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2530" uniqueCount="1447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2535" uniqueCount="1450">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4372,6 +4374,15 @@
   </si>
   <si>
     <t>This book created mixed feelings: fear and anguish over the state of the State in relation to the family; hope and gratitude for the beauty of the Truth as given in the Church. A couple essays in the middle were overly "political", but overall was a good reminder to draw close to the Church to build up our families.</t>
+  </si>
+  <si>
+    <t>Death Comes for the Archbishop</t>
+  </si>
+  <si>
+    <t>Willa Cather</t>
+  </si>
+  <si>
+    <t>A beautiful book, especially the life-long friendship between Fr. Latour and Fr. Vaillant, their love for the poorest of the poor, and the working of God's grace in all places.</t>
   </si>
 </sst>
 </file>
@@ -5975,7 +5986,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A690" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A709" sqref="A709"/>
+      <selection pane="bottomLeft" activeCell="A710" sqref="A710"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19830,12 +19841,30 @@
       </c>
     </row>
     <row r="709" spans="1:8">
+      <c r="A709" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="B709" s="3" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C709" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D709" s="6">
         <v>2020</v>
       </c>
-      <c r="E709" s="6"/>
-      <c r="F709" s="6"/>
-      <c r="G709" s="6"/>
+      <c r="E709" s="6">
+        <v>1927</v>
+      </c>
+      <c r="F709" s="6">
+        <v>297</v>
+      </c>
+      <c r="G709" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H709" s="3" t="s">
+        <v>1449</v>
+      </c>
     </row>
     <row r="710" spans="1:8">
       <c r="D710" s="6">

</xml_diff>

<commit_message>
The 35 Doctors of the Church
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2473765-3F94-F24D-B2F4-1EE5973EFEC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A750310-83C5-D946-BCB5-ED751411CEF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2545" uniqueCount="1454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2550" uniqueCount="1457">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4395,6 +4395,15 @@
   </si>
   <si>
     <t>Not only an epic adventure and enthralling read, but full of acute observations about psychology, duty, and honor.</t>
+  </si>
+  <si>
+    <t>The 35 Doctors of the Church</t>
+  </si>
+  <si>
+    <t>Fr. Christopher Rengers O.F.M.Cap. and Matthew E Bunson</t>
+  </si>
+  <si>
+    <t>I got this book at Generations last year when looking for a book about St. Anthony, and I am so grateful for the time I have spent with it getting to know these great saints. My favorite is whichever one I read about most recently. They are all amazing and beautiful and I want more.</t>
   </si>
 </sst>
 </file>
@@ -5997,8 +6006,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A709" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A712" sqref="A712"/>
+      <pane ySplit="1" topLeftCell="A701" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A713" sqref="A713"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19931,12 +19940,30 @@
       </c>
     </row>
     <row r="712" spans="1:8">
+      <c r="A712" s="3" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B712" s="3" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C712" s="3" t="s">
+        <v>197</v>
+      </c>
       <c r="D712" s="6">
         <v>2020</v>
       </c>
-      <c r="E712" s="6"/>
-      <c r="F712" s="6"/>
-      <c r="G712" s="6"/>
+      <c r="E712" s="6">
+        <v>2000</v>
+      </c>
+      <c r="F712" s="6">
+        <v>723</v>
+      </c>
+      <c r="G712" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H712" s="3" t="s">
+        <v>1456</v>
+      </c>
     </row>
     <row r="713" spans="1:8">
       <c r="D713" s="6">

</xml_diff>

<commit_message>
The Man Who Made Things Out of Trees
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F423D8B-2C79-3F4C-AB40-967AFCB4331B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C2BF51-6002-DD49-9105-96A155CD2C1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2570" uniqueCount="1469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2575" uniqueCount="1472">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4440,6 +4440,15 @@
   </si>
   <si>
     <t>Scott Parker at Root recommended this. Making decisions in life is the same as making bets, and we can incorporate some poker-inspired thinking to be more confident in the bets we place.</t>
+  </si>
+  <si>
+    <t>The Man Who Made Things Out of Trees: The Ash in Human Culture and History</t>
+  </si>
+  <si>
+    <t>Robert Penn</t>
+  </si>
+  <si>
+    <t>This came from Good Clean Fun, and is a great book. He chops down an ash tree and this chronicles the whole process of making things out of it. A great book that makes you want to be in a forest and work with wood.</t>
   </si>
 </sst>
 </file>
@@ -6043,7 +6052,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A701" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A717" sqref="A717"/>
+      <selection pane="bottomLeft" activeCell="A718" sqref="A718"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20106,12 +20115,30 @@
       </c>
     </row>
     <row r="717" spans="1:8">
+      <c r="A717" s="3" t="s">
+        <v>1469</v>
+      </c>
+      <c r="B717" s="3" t="s">
+        <v>1470</v>
+      </c>
+      <c r="C717" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D717" s="6">
         <v>2020</v>
       </c>
-      <c r="E717" s="6"/>
-      <c r="F717" s="6"/>
-      <c r="G717" s="6"/>
+      <c r="E717" s="6">
+        <v>2015</v>
+      </c>
+      <c r="F717" s="6">
+        <v>245</v>
+      </c>
+      <c r="G717" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H717" s="3" t="s">
+        <v>1471</v>
+      </c>
     </row>
     <row r="718" spans="1:8">
       <c r="D718" s="6">

</xml_diff>

<commit_message>
Common Trees of Ohio
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C2BF51-6002-DD49-9105-96A155CD2C1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E733D835-89A0-8848-ADE3-DC81F361EDC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2575" uniqueCount="1472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2580" uniqueCount="1475">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4449,6 +4449,15 @@
   </si>
   <si>
     <t>This came from Good Clean Fun, and is a great book. He chops down an ash tree and this chronicles the whole process of making things out of it. A great book that makes you want to be in a forest and work with wood.</t>
+  </si>
+  <si>
+    <t>Common Trees of Ohio</t>
+  </si>
+  <si>
+    <t>Joseph Illick</t>
+  </si>
+  <si>
+    <t>This book is part tree identification manual and part poetic praise of the place of the tree in our lives. The audience is schoolchildren of early 20th century Ohio and it has a certain nostalgic aire to it.</t>
   </si>
 </sst>
 </file>
@@ -20141,12 +20150,30 @@
       </c>
     </row>
     <row r="718" spans="1:8">
+      <c r="A718" s="3" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B718" s="3" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C718" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D718" s="6">
         <v>2020</v>
       </c>
-      <c r="E718" s="6"/>
-      <c r="F718" s="6"/>
-      <c r="G718" s="6"/>
+      <c r="E718" s="6">
+        <v>1927</v>
+      </c>
+      <c r="F718" s="6">
+        <v>108</v>
+      </c>
+      <c r="G718" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H718" s="3" t="s">
+        <v>1474</v>
+      </c>
     </row>
     <row r="719" spans="1:8">
       <c r="D719" s="6">

</xml_diff>

<commit_message>
The Divine Favors Granted to St. Joseph
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6FA613-0528-524F-9FA2-9ED61A27175C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA69DD7A-BBCB-E14E-BE2D-E1F57ADFA6A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2585" uniqueCount="1478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2590" uniqueCount="1481">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4467,6 +4467,15 @@
   </si>
   <si>
     <t>This was another recommendation from Good Clean Fun and a great book. I love his philosophy of using mostly hand tools: no dust, no noise, accurate enough, and perfect if you don't need to produce many of the same thing. This book makes me want to get a low angle jack plane.</t>
+  </si>
+  <si>
+    <t>The Divine Favors Granted to St. Joseph</t>
+  </si>
+  <si>
+    <t>Pere Binet</t>
+  </si>
+  <si>
+    <t>A lovely short little book on St. Joseph. I love the description of St. Joseph's silence on 144 in which he let's Mary do all his speaking, and we should also.</t>
   </si>
 </sst>
 </file>
@@ -6070,7 +6079,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A701" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A720" sqref="A720"/>
+      <selection pane="bottomLeft" activeCell="G721" sqref="G721"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20211,12 +20220,30 @@
       </c>
     </row>
     <row r="720" spans="1:8">
+      <c r="A720" s="3" t="s">
+        <v>1478</v>
+      </c>
+      <c r="B720" s="3" t="s">
+        <v>1479</v>
+      </c>
+      <c r="C720" s="3" t="s">
+        <v>197</v>
+      </c>
       <c r="D720" s="6">
         <v>2020</v>
       </c>
-      <c r="E720" s="6"/>
-      <c r="F720" s="6"/>
-      <c r="G720" s="6"/>
+      <c r="E720" s="6">
+        <v>1973</v>
+      </c>
+      <c r="F720" s="6">
+        <v>176</v>
+      </c>
+      <c r="G720" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H720" s="3" t="s">
+        <v>1480</v>
+      </c>
     </row>
     <row r="721" spans="4:7">
       <c r="D721" s="6">

</xml_diff>

<commit_message>
Forty Dreams of St. John Bosco
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA69DD7A-BBCB-E14E-BE2D-E1F57ADFA6A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8749C1-0CA5-4C41-AAAD-211B61111929}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34680" yWindow="4500" windowWidth="25600" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2590" uniqueCount="1481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2595" uniqueCount="1484">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4476,6 +4476,15 @@
   </si>
   <si>
     <t>A lovely short little book on St. Joseph. I love the description of St. Joseph's silence on 144 in which he let's Mary do all his speaking, and we should also.</t>
+  </si>
+  <si>
+    <t>Forty Dreams of St. John Bosco: The Apostle of Youth</t>
+  </si>
+  <si>
+    <t>St. John Bosco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don Bosco's advice is good for all of us: frequent confession and communion and visits to the Blessed Sacrament, keeping busy to avoid tempataion, and avoiding impurity and gluttony. </t>
   </si>
 </sst>
 </file>
@@ -6079,7 +6088,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A701" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G721" sqref="G721"/>
+      <selection pane="bottomLeft" activeCell="A722" sqref="A722"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20245,99 +20254,117 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="721" spans="4:7">
+    <row r="721" spans="1:8">
+      <c r="A721" s="3" t="s">
+        <v>1481</v>
+      </c>
+      <c r="B721" s="3" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C721" s="3" t="s">
+        <v>197</v>
+      </c>
       <c r="D721" s="6">
         <v>2020</v>
       </c>
-      <c r="E721" s="6"/>
-      <c r="F721" s="6"/>
-      <c r="G721" s="6"/>
-    </row>
-    <row r="722" spans="4:7">
+      <c r="E721" s="6">
+        <v>1898</v>
+      </c>
+      <c r="F721" s="6">
+        <v>225</v>
+      </c>
+      <c r="G721" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H721" s="3" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="722" spans="1:8">
       <c r="D722" s="6"/>
       <c r="E722" s="6"/>
       <c r="F722" s="6"/>
       <c r="G722" s="6"/>
     </row>
-    <row r="723" spans="4:7">
+    <row r="723" spans="1:8">
       <c r="D723" s="6"/>
       <c r="E723" s="6"/>
       <c r="F723" s="6"/>
       <c r="G723" s="6"/>
     </row>
-    <row r="724" spans="4:7">
+    <row r="724" spans="1:8">
       <c r="D724" s="6"/>
       <c r="E724" s="6"/>
       <c r="F724" s="6"/>
       <c r="G724" s="6"/>
     </row>
-    <row r="725" spans="4:7">
+    <row r="725" spans="1:8">
       <c r="D725" s="6"/>
       <c r="E725" s="6"/>
       <c r="F725" s="6"/>
       <c r="G725" s="6"/>
     </row>
-    <row r="726" spans="4:7">
+    <row r="726" spans="1:8">
       <c r="D726" s="6"/>
       <c r="E726" s="6"/>
       <c r="F726" s="6"/>
       <c r="G726" s="6"/>
     </row>
-    <row r="727" spans="4:7">
+    <row r="727" spans="1:8">
       <c r="D727" s="6"/>
       <c r="E727" s="6"/>
       <c r="F727" s="6"/>
       <c r="G727" s="6"/>
     </row>
-    <row r="728" spans="4:7">
+    <row r="728" spans="1:8">
       <c r="D728" s="6"/>
       <c r="E728" s="6"/>
       <c r="F728" s="6"/>
       <c r="G728" s="6"/>
     </row>
-    <row r="729" spans="4:7">
+    <row r="729" spans="1:8">
       <c r="D729" s="6"/>
       <c r="E729" s="6"/>
       <c r="F729" s="6"/>
       <c r="G729" s="6"/>
     </row>
-    <row r="730" spans="4:7">
+    <row r="730" spans="1:8">
       <c r="D730" s="6"/>
       <c r="E730" s="6"/>
       <c r="F730" s="6"/>
       <c r="G730" s="6"/>
     </row>
-    <row r="731" spans="4:7">
+    <row r="731" spans="1:8">
       <c r="D731" s="6"/>
       <c r="E731" s="6"/>
       <c r="F731" s="6"/>
       <c r="G731" s="6"/>
     </row>
-    <row r="732" spans="4:7">
+    <row r="732" spans="1:8">
       <c r="D732" s="6"/>
       <c r="E732" s="6"/>
       <c r="F732" s="6"/>
       <c r="G732" s="6"/>
     </row>
-    <row r="733" spans="4:7">
+    <row r="733" spans="1:8">
       <c r="D733" s="6"/>
       <c r="E733" s="6"/>
       <c r="F733" s="6"/>
       <c r="G733" s="6"/>
     </row>
-    <row r="734" spans="4:7">
+    <row r="734" spans="1:8">
       <c r="D734" s="6"/>
       <c r="E734" s="6"/>
       <c r="F734" s="6"/>
       <c r="G734" s="6"/>
     </row>
-    <row r="735" spans="4:7">
+    <row r="735" spans="1:8">
       <c r="D735" s="6"/>
       <c r="E735" s="6"/>
       <c r="F735" s="6"/>
       <c r="G735" s="6"/>
     </row>
-    <row r="736" spans="4:7">
+    <row r="736" spans="1:8">
       <c r="D736" s="6"/>
       <c r="E736" s="6"/>
       <c r="F736" s="6"/>

</xml_diff>

<commit_message>
Skin in the Game
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABC434E-8D17-AB4A-8088-374B7F0DD2FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D333C0E6-13DE-D74F-AF6C-B44C82021824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2605" uniqueCount="1489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2610" uniqueCount="1492">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4500,6 +4500,15 @@
   </si>
   <si>
     <t>This ranks up there with *A Visual Dictionary of Architecture* on the list of books that are just wonderful to look at the detailed drawings in. This claims to be the "complete" reference, and it is the most complete I have seen. A great source of ideas and information and perusal pleasure.</t>
+  </si>
+  <si>
+    <t>Skin in the Game: Hidden Asymmetries in Daily Life</t>
+  </si>
+  <si>
+    <t>Nassim Nicholas Taleb</t>
+  </si>
+  <si>
+    <t>On Cory's recommendation I started reading Taleb. I'm physically reading The Black Swan and listened to Skin in the Game because it was available and to get more of his thought. I will re-read it once I finish the rest of the Incerto, but this is just phenomenal if for nothing other than how direct and unabashed it is. I need to more fully study the Incerto (including criticisms), but nevertheless these ideas are important and likely some of the most influential reading I will do this year.</t>
   </si>
 </sst>
 </file>
@@ -6103,7 +6112,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A701" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A724" sqref="A724"/>
+      <selection pane="bottomLeft" activeCell="A725" sqref="A725"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20348,10 +20357,30 @@
       </c>
     </row>
     <row r="724" spans="1:8">
-      <c r="D724" s="6"/>
-      <c r="E724" s="6"/>
-      <c r="F724" s="6"/>
-      <c r="G724" s="6"/>
+      <c r="A724" s="3" t="s">
+        <v>1489</v>
+      </c>
+      <c r="B724" s="3" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C724" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D724" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E724" s="6">
+        <v>2018</v>
+      </c>
+      <c r="F724" s="6">
+        <v>304</v>
+      </c>
+      <c r="G724" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H724" s="3" t="s">
+        <v>1491</v>
+      </c>
     </row>
     <row r="725" spans="1:8">
       <c r="D725" s="6"/>

</xml_diff>

<commit_message>
So Long as I Can Read
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D333C0E6-13DE-D74F-AF6C-B44C82021824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E61085B-007E-3048-87C8-B4B45E0E5298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52800" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2610" uniqueCount="1492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2615" uniqueCount="1495">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4509,6 +4509,15 @@
   </si>
   <si>
     <t>On Cory's recommendation I started reading Taleb. I'm physically reading The Black Swan and listened to Skin in the Game because it was available and to get more of his thought. I will re-read it once I finish the rest of the Incerto, but this is just phenomenal if for nothing other than how direct and unabashed it is. I need to more fully study the Incerto (including criticisms), but nevertheless these ideas are important and likely some of the most influential reading I will do this year.</t>
+  </si>
+  <si>
+    <t>"So Long as I Can Read": Farm Women's Reading Experiences in Depression-Era South Dakota</t>
+  </si>
+  <si>
+    <t>Lisa Lindell</t>
+  </si>
+  <si>
+    <t>I came across this gem in a brief article and traced back to this hunting down a great quote about reading. I decided to read the whole thing, which is relevant now with the current economic crisis and beautiful to see how people in very dire straits found such comfort and hope in reading.</t>
   </si>
 </sst>
 </file>
@@ -6112,7 +6121,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A701" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A725" sqref="A725"/>
+      <selection pane="bottomLeft" activeCell="A726" sqref="A726"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20382,11 +20391,31 @@
         <v>1491</v>
       </c>
     </row>
-    <row r="725" spans="1:8">
-      <c r="D725" s="6"/>
-      <c r="E725" s="6"/>
-      <c r="F725" s="6"/>
-      <c r="G725" s="6"/>
+    <row r="725" spans="1:8" ht="17">
+      <c r="A725" s="10" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B725" s="3" t="s">
+        <v>1493</v>
+      </c>
+      <c r="C725" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="D725" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E725" s="6">
+        <v>2009</v>
+      </c>
+      <c r="F725" s="6">
+        <v>24</v>
+      </c>
+      <c r="G725" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H725" s="3" t="s">
+        <v>1494</v>
+      </c>
     </row>
     <row r="726" spans="1:8">
       <c r="D726" s="6"/>

</xml_diff>

<commit_message>
Shorting Home Equity Mezzanine Tranches
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0852FC3D-5ADA-6342-BC88-5EDE22FDF6A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6B2994-4643-FB47-9B4E-CF5845AB0F60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2635" uniqueCount="1504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2640" uniqueCount="1507">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4545,6 +4545,15 @@
   </si>
   <si>
     <t>I read this four years ago and watched the movie when it came out but I have learned enough since then about finance that it made a much bigger impression on me this time around. How we got there is just a ridiculous story, and the description in the epilogue about how everyone who created the catastrphe got rich and bailed out by the government is just sickening hearing it again. Chapter 5 about the Cornwall Capital guys and their early experimentation with underpriced options was especially compelling coming out of a lot of reading of Taleb since this is his whole strategy. This is a book I will keep coming back to.</t>
+  </si>
+  <si>
+    <t>Greg Lippmann</t>
+  </si>
+  <si>
+    <t>Shorting Home Equity Mezzanine Tranches</t>
+  </si>
+  <si>
+    <t>I found this online after it was mentioned in The Big Short. What a fascenating time capsule into just before the subprime mortgage crisis blew, and an interesting view of a deck now that I have been involved in or read a good number for work.</t>
   </si>
 </sst>
 </file>
@@ -6148,7 +6157,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A684" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A730" sqref="A730"/>
+      <selection pane="bottomLeft" activeCell="A731" sqref="A731"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20549,10 +20558,30 @@
       </c>
     </row>
     <row r="730" spans="1:8">
-      <c r="D730" s="6"/>
-      <c r="E730" s="6"/>
-      <c r="F730" s="6"/>
-      <c r="G730" s="6"/>
+      <c r="A730" s="3" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B730" s="3" t="s">
+        <v>1504</v>
+      </c>
+      <c r="C730" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="D730" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E730" s="6">
+        <v>2007</v>
+      </c>
+      <c r="F730" s="6">
+        <v>73</v>
+      </c>
+      <c r="G730" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H730" s="3" t="s">
+        <v>1506</v>
+      </c>
     </row>
     <row r="731" spans="1:8">
       <c r="D731" s="6"/>

</xml_diff>

<commit_message>
The Bed of Procrustes
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A16C19-D124-6F4D-B536-E68473118819}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED23FD8-C9C2-5D4F-9B2C-FE717505DAF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2645" uniqueCount="1509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2650" uniqueCount="1511">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4560,6 +4560,12 @@
   </si>
   <si>
     <t>Taleb keeps getting better. Many of the concepts here are similar to the Black Swan but this is the first book so some more background information. As always with him, an entertaining read.</t>
+  </si>
+  <si>
+    <t>The Bed of Procrustes: Philosophical and Practical Aphorisms</t>
+  </si>
+  <si>
+    <t>I read these slowly while reading his other works. Some are misses, a lot speak truth, and some are just magnificient.</t>
   </si>
 </sst>
 </file>
@@ -6162,8 +6168,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A684" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A732" sqref="A732"/>
+      <pane ySplit="1" topLeftCell="A701" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A733" sqref="A733"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20616,10 +20622,30 @@
       </c>
     </row>
     <row r="732" spans="1:8">
-      <c r="D732" s="6"/>
-      <c r="E732" s="6"/>
-      <c r="F732" s="6"/>
-      <c r="G732" s="6"/>
+      <c r="A732" s="3" t="s">
+        <v>1509</v>
+      </c>
+      <c r="B732" s="3" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C732" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D732" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E732" s="6">
+        <v>2010</v>
+      </c>
+      <c r="F732" s="6">
+        <v>156</v>
+      </c>
+      <c r="G732" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H732" s="3" t="s">
+        <v>1510</v>
+      </c>
     </row>
     <row r="733" spans="1:8">
       <c r="D733" s="6"/>

</xml_diff>

<commit_message>
Seacoast Fortifications of the United States
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39511AED-BB60-F846-83E4-A58A0F1A87BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1B316D-7BBF-E44A-9AEB-A6847BF5636F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2660" uniqueCount="1515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2665" uniqueCount="1518">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4578,6 +4578,15 @@
   </si>
   <si>
     <t>Again I'm digging more into DHH and this is appropriate given our current state of remote work for so many including myself. My first exposure to the benefits of remote work was the 4 hour work week, and this is a more thoughtful and realistic approach.</t>
+  </si>
+  <si>
+    <t>Seacoast Fortifications of the United States: An Introductory History</t>
+  </si>
+  <si>
+    <t>Emanuel Raymond Lewis</t>
+  </si>
+  <si>
+    <t>This was an interesting book I found at home and enjoyed for an evening. The history behing US reliance on seacoast fortification is intriguing: they were favored by those who disliked standing armies because they are efficiently maintained by few men in times of peace, and by those who disliked aggression because they are defensive only in nature.</t>
   </si>
 </sst>
 </file>
@@ -6181,7 +6190,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A701" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A735" sqref="A735"/>
+      <selection pane="bottomLeft" activeCell="A736" sqref="A736"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20712,10 +20721,30 @@
       </c>
     </row>
     <row r="735" spans="1:8">
-      <c r="D735" s="6"/>
-      <c r="E735" s="6"/>
-      <c r="F735" s="6"/>
-      <c r="G735" s="6"/>
+      <c r="A735" s="3" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B735" s="3" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C735" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D735" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E735" s="6">
+        <v>1970</v>
+      </c>
+      <c r="F735" s="6">
+        <v>144</v>
+      </c>
+      <c r="G735" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H735" s="3" t="s">
+        <v>1517</v>
+      </c>
     </row>
     <row r="736" spans="1:8">
       <c r="D736" s="6"/>

</xml_diff>

<commit_message>
Chop Wood Carry Water
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512133F7-51C5-084B-A418-AA0FDCCC9BE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B897EAE-8B2B-C543-833C-F1A10C257895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2675" uniqueCount="1524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2680" uniqueCount="1527">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4605,6 +4605,15 @@
   </si>
   <si>
     <t xml:space="preserve">This was a challenging book to both confront racism in the way DiAngelo suggests and to think about what changes as a result of reading this. I am tempted at times when reading about racism to dismiss it as progressive extremism along similar lines as abortion for example, and it takes careful thought to separate out truthful arguments and observations about racism from ideological observations. </t>
+  </si>
+  <si>
+    <t>Chop Wood Carry Water: How to Fall in Love with the Process of Becoming Great</t>
+  </si>
+  <si>
+    <t>Joshua Medcalf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I forget where I heard about this but it was a nice little parable about the importance of the process rather than the goal.</t>
   </si>
 </sst>
 </file>
@@ -6208,7 +6217,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A701" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A738" sqref="A738"/>
+      <selection pane="bottomLeft" activeCell="A739" sqref="A739"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20817,10 +20826,30 @@
       </c>
     </row>
     <row r="738" spans="1:8">
-      <c r="D738" s="6"/>
-      <c r="E738" s="6"/>
-      <c r="F738" s="6"/>
-      <c r="G738" s="6"/>
+      <c r="A738" s="3" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B738" s="3" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C738" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D738" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E738" s="6">
+        <v>2015</v>
+      </c>
+      <c r="F738" s="6">
+        <v>125</v>
+      </c>
+      <c r="G738" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H738" s="3" t="s">
+        <v>1526</v>
+      </c>
     </row>
     <row r="739" spans="1:8">
       <c r="D739" s="6"/>

</xml_diff>

<commit_message>
The Last Full Measure
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA083207-2764-1542-A0D6-19CB59C6D9E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CD5450-C7CE-A84C-A300-0E357C55D8F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2695" uniqueCount="1536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2700" uniqueCount="1539">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4641,6 +4641,15 @@
   </si>
   <si>
     <t>This books is both fascenating and envy-inducing. I plan to make a nice wood wall tool holder and I put in a retractable extension cord after looking through this.</t>
+  </si>
+  <si>
+    <t>The Last Full Measure: How Soldiers Die in Battle</t>
+  </si>
+  <si>
+    <t>Michael Stephenson</t>
+  </si>
+  <si>
+    <t>I heard about this from AOM around memorial day and got it from the library. This is a sobering book and he acknowledges the need to honor the fallen without glorifying violence, a line he walks well mostly by drawing from contemporary accounts. I read the chapters in reverse chronological order on medical history, modern warfare, WWII, WWI, and the middle ages. It would be good to revisit the others especially the American Civil War. This is really learned only from experience I am sure, but I am grateful to be more aware of the sacrifices made for my freedom.</t>
   </si>
 </sst>
 </file>
@@ -6244,7 +6253,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A701" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A742" sqref="A742"/>
+      <selection pane="bottomLeft" activeCell="A743" sqref="A743"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20957,10 +20966,30 @@
       </c>
     </row>
     <row r="742" spans="1:8">
-      <c r="D742" s="6"/>
-      <c r="E742" s="6"/>
-      <c r="F742" s="6"/>
-      <c r="G742" s="6"/>
+      <c r="A742" s="3" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B742" s="3" t="s">
+        <v>1537</v>
+      </c>
+      <c r="C742" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D742" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E742" s="6">
+        <v>2012</v>
+      </c>
+      <c r="F742" s="6">
+        <v>407</v>
+      </c>
+      <c r="G742" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H742" s="3" t="s">
+        <v>1538</v>
+      </c>
     </row>
     <row r="743" spans="1:8">
       <c r="D743" s="6"/>

</xml_diff>

<commit_message>
A Canticle for Leibowitz
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CD5450-C7CE-A84C-A300-0E357C55D8F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B440F57B-2F1A-1E44-9CF5-A68E16FB86E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36000" yWindow="760" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2700" uniqueCount="1539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2705" uniqueCount="1541">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4650,6 +4650,12 @@
   </si>
   <si>
     <t>I heard about this from AOM around memorial day and got it from the library. This is a sobering book and he acknowledges the need to honor the fallen without glorifying violence, a line he walks well mostly by drawing from contemporary accounts. I read the chapters in reverse chronological order on medical history, modern warfare, WWII, WWI, and the middle ages. It would be good to revisit the others especially the American Civil War. This is really learned only from experience I am sure, but I am grateful to be more aware of the sacrifices made for my freedom.</t>
+  </si>
+  <si>
+    <t>A Canticle for Leibowitz</t>
+  </si>
+  <si>
+    <t>I read this at ND and it was a pleasure to revisit, especially now in this time of crisis and thinking about the Church's defense of life in an increasingly hostile world.</t>
   </si>
 </sst>
 </file>
@@ -6252,8 +6258,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A701" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A743" sqref="A743"/>
+      <pane ySplit="1" topLeftCell="A697" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C744" sqref="C744"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20992,10 +20998,30 @@
       </c>
     </row>
     <row r="743" spans="1:8">
-      <c r="D743" s="6"/>
-      <c r="E743" s="6"/>
-      <c r="F743" s="6"/>
-      <c r="G743" s="6"/>
+      <c r="A743" s="3" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B743" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="C743" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D743" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E743" s="6">
+        <v>1959</v>
+      </c>
+      <c r="F743" s="6">
+        <v>320</v>
+      </c>
+      <c r="G743" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H743" s="3" t="s">
+        <v>1540</v>
+      </c>
     </row>
     <row r="744" spans="1:8">
       <c r="D744" s="6"/>

</xml_diff>

<commit_message>
Listen To The Silence
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259C96D1-8443-C644-8CB9-318D6ECC3AD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8D9920-5AE9-174B-8494-5752216BF99D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2736" uniqueCount="1558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2741" uniqueCount="1561">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4707,6 +4707,15 @@
   </si>
   <si>
     <t>True work builds character, and boys need this to become men rather than stay boys.</t>
+  </si>
+  <si>
+    <t>Listen To The Silence: A Retreat With Père Jacques</t>
+  </si>
+  <si>
+    <t>Pére Jacques, translated by Francis J. Murphy</t>
+  </si>
+  <si>
+    <t>Fr. Dailey gave me this book after a conversation about reading John of the Cross' *Dark Night*, and this is a retreat Pere Jacques gave in 1943 to the Carmelite nuns. It is a beautiful portrait of his spirituality and I felt especially moved by this conference on Silence.</t>
   </si>
 </sst>
 </file>
@@ -6309,8 +6318,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A703" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H750" sqref="H750"/>
+      <pane ySplit="1" topLeftCell="A711" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A750" sqref="A750"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21234,10 +21243,30 @@
       </c>
     </row>
     <row r="750" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D750" s="6"/>
-      <c r="E750" s="6"/>
-      <c r="F750" s="6"/>
-      <c r="G750" s="6"/>
+      <c r="A750" s="3" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B750" s="3" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C750" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D750" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E750" s="6">
+        <v>1943</v>
+      </c>
+      <c r="F750" s="6">
+        <v>113</v>
+      </c>
+      <c r="G750" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H750" s="3" t="s">
+        <v>1560</v>
+      </c>
     </row>
     <row r="751" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D751" s="6"/>

</xml_diff>

<commit_message>
Oh Crap! Potty Training
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8D9920-5AE9-174B-8494-5752216BF99D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509E6C9B-A699-5849-97BF-3104BB42A08D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2741" uniqueCount="1561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2746" uniqueCount="1564">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4716,6 +4716,15 @@
   </si>
   <si>
     <t>Fr. Dailey gave me this book after a conversation about reading John of the Cross' *Dark Night*, and this is a retreat Pere Jacques gave in 1943 to the Carmelite nuns. It is a beautiful portrait of his spirituality and I felt especially moved by this conference on Silence.</t>
+  </si>
+  <si>
+    <t>Oh Crap! Potty Training: Everything Modern Parents Need to Know</t>
+  </si>
+  <si>
+    <t>Jamie Glowacki</t>
+  </si>
+  <si>
+    <t>Jordan had me listen to the first 5 chapters of this before potty training Henry and it was a helpful overview and presentation of the methodology. I like her no BS style.</t>
   </si>
 </sst>
 </file>
@@ -6319,7 +6328,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A711" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A750" sqref="A750"/>
+      <selection pane="bottomLeft" activeCell="A752" sqref="A752"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21269,10 +21278,30 @@
       </c>
     </row>
     <row r="751" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D751" s="6"/>
-      <c r="E751" s="6"/>
-      <c r="F751" s="6"/>
-      <c r="G751" s="6"/>
+      <c r="A751" s="3" t="s">
+        <v>1561</v>
+      </c>
+      <c r="B751" s="3" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C751" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D751" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E751" s="6">
+        <v>2015</v>
+      </c>
+      <c r="F751" s="6">
+        <v>94</v>
+      </c>
+      <c r="G751" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H751" s="3" t="s">
+        <v>1563</v>
+      </c>
     </row>
     <row r="752" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D752" s="6"/>

</xml_diff>

<commit_message>
The Aquinas Prayer Book
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7182F791-ADF3-D942-ACC0-D75943501376}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2E578F-9398-A44B-9079-33218734F290}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2751" uniqueCount="1567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2756" uniqueCount="1570">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4734,6 +4734,15 @@
   </si>
   <si>
     <t>Fr. Raymund raved about this and I got my Full Focus Planner and have started implementing these principles in my life.</t>
+  </si>
+  <si>
+    <t>The Aquinas Prayer Book: The Prayers and Hymns of St. Thomas Aquinas</t>
+  </si>
+  <si>
+    <t>St. Thomas Aquinas, edited by Robert Anderson &amp; Johannes Moser</t>
+  </si>
+  <si>
+    <t>Jordan found this for me when I was looking for Latin prayers, and this is a wonderful side-by-side Latin-English presentation of his prayers and hymns. I especially like his prayer before/after communion and before work/study "disperse from my soul the twofold darkness into which I was born: sin and ignorance".</t>
   </si>
 </sst>
 </file>
@@ -6337,7 +6346,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A711" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A752" sqref="A752"/>
+      <selection pane="bottomLeft" activeCell="A753" sqref="A753"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21338,97 +21347,117 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="753" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D753" s="6"/>
-      <c r="E753" s="6"/>
-      <c r="F753" s="6"/>
-      <c r="G753" s="6"/>
-    </row>
-    <row r="754" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="753" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A753" s="3" t="s">
+        <v>1567</v>
+      </c>
+      <c r="B753" s="3" t="s">
+        <v>1568</v>
+      </c>
+      <c r="C753" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D753" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E753" s="6">
+        <v>1264</v>
+      </c>
+      <c r="F753" s="6">
+        <v>113</v>
+      </c>
+      <c r="G753" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H753" s="3" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="754" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D754" s="6"/>
       <c r="E754" s="6"/>
       <c r="F754" s="6"/>
       <c r="G754" s="6"/>
     </row>
-    <row r="755" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="755" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D755" s="6"/>
       <c r="E755" s="6"/>
       <c r="F755" s="6"/>
       <c r="G755" s="6"/>
     </row>
-    <row r="756" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="756" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D756" s="6"/>
       <c r="E756" s="6"/>
       <c r="F756" s="6"/>
       <c r="G756" s="6"/>
     </row>
-    <row r="757" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="757" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D757" s="6"/>
       <c r="E757" s="6"/>
       <c r="F757" s="6"/>
       <c r="G757" s="6"/>
     </row>
-    <row r="758" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="758" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D758" s="6"/>
       <c r="E758" s="6"/>
       <c r="F758" s="6"/>
       <c r="G758" s="6"/>
     </row>
-    <row r="759" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="759" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D759" s="6"/>
       <c r="E759" s="6"/>
       <c r="F759" s="6"/>
       <c r="G759" s="6"/>
     </row>
-    <row r="760" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="760" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D760" s="6"/>
       <c r="E760" s="6"/>
       <c r="F760" s="6"/>
       <c r="G760" s="6"/>
     </row>
-    <row r="761" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="761" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D761" s="6"/>
       <c r="E761" s="6"/>
       <c r="F761" s="6"/>
       <c r="G761" s="6"/>
     </row>
-    <row r="762" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="762" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D762" s="6"/>
       <c r="E762" s="6"/>
       <c r="F762" s="6"/>
       <c r="G762" s="6"/>
     </row>
-    <row r="763" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="763" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D763" s="6"/>
       <c r="E763" s="6"/>
       <c r="F763" s="6"/>
       <c r="G763" s="6"/>
     </row>
-    <row r="764" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="764" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D764" s="6"/>
       <c r="E764" s="6"/>
       <c r="F764" s="6"/>
       <c r="G764" s="6"/>
     </row>
-    <row r="765" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="765" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D765" s="6"/>
       <c r="E765" s="6"/>
       <c r="F765" s="6"/>
       <c r="G765" s="6"/>
     </row>
-    <row r="766" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="766" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D766" s="6"/>
       <c r="E766" s="6"/>
       <c r="F766" s="6"/>
       <c r="G766" s="6"/>
     </row>
-    <row r="767" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="767" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D767" s="6"/>
       <c r="E767" s="6"/>
       <c r="F767" s="6"/>
       <c r="G767" s="6"/>
     </row>
-    <row r="768" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="768" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D768" s="6"/>
       <c r="E768" s="6"/>
       <c r="F768" s="6"/>

</xml_diff>

<commit_message>
An Exorcist Explains the Demonic
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2E578F-9398-A44B-9079-33218734F290}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2E8D33-5C15-6849-9E89-94D4647C76DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2756" uniqueCount="1570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2761" uniqueCount="1573">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4743,6 +4743,15 @@
   </si>
   <si>
     <t>Jordan found this for me when I was looking for Latin prayers, and this is a wonderful side-by-side Latin-English presentation of his prayers and hymns. I especially like his prayer before/after communion and before work/study "disperse from my soul the twofold darkness into which I was born: sin and ignorance".</t>
+  </si>
+  <si>
+    <t>An Exorcist Explains the Demonic: The Antics of Satan and His Army of Fallen Angels</t>
+  </si>
+  <si>
+    <t>Fr. Gabriele Amorth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This was an honest and insightful look at demonic activity, keeping a steady course between those who would sensationalize it or deny Satan's existence. The first chapter in particular—grounding the reader in the life, death, and resurrection of Jesus—was beautiful and caused me to really ponder eternity. </t>
   </si>
 </sst>
 </file>
@@ -6344,9 +6353,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A711" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A753" sqref="A753"/>
+      <selection pane="bottomLeft" activeCell="H755" sqref="H755"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21374,10 +21383,30 @@
       </c>
     </row>
     <row r="754" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D754" s="6"/>
-      <c r="E754" s="6"/>
-      <c r="F754" s="6"/>
-      <c r="G754" s="6"/>
+      <c r="A754" s="3" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B754" s="3" t="s">
+        <v>1571</v>
+      </c>
+      <c r="C754" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D754" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E754" s="6">
+        <v>2016</v>
+      </c>
+      <c r="F754" s="6">
+        <v>145</v>
+      </c>
+      <c r="G754" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H754" s="3" t="s">
+        <v>1572</v>
+      </c>
     </row>
     <row r="755" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D755" s="6"/>

</xml_diff>

<commit_message>
Defender of the Realm
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2E8D33-5C15-6849-9E89-94D4647C76DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED7F149-EEA1-9D45-B4B4-5AFF52DD7798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2761" uniqueCount="1573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2766" uniqueCount="1576">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4752,6 +4752,15 @@
   </si>
   <si>
     <t xml:space="preserve">This was an honest and insightful look at demonic activity, keeping a steady course between those who would sensationalize it or deny Satan's existence. The first chapter in particular—grounding the reader in the life, death, and resurrection of Jesus—was beautiful and caused me to really ponder eternity. </t>
+  </si>
+  <si>
+    <t>The Last Lion: Winston Spencer Churchill: Defender of the Realm, 1940-1965</t>
+  </si>
+  <si>
+    <t>William Manchester and Paul Reid</t>
+  </si>
+  <si>
+    <t>So ends an epic journey started when I received these volumes for Christmas in 2017 and read one each year in 2018, 2019, and 2020. Winston Churchill was a giant of a man, by no means perfect but so fascenating to get to know. Remember Winston Churchill.</t>
   </si>
 </sst>
 </file>
@@ -6353,9 +6362,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A711" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H755" sqref="H755"/>
+      <selection pane="bottomLeft" activeCell="A755" sqref="A755"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21409,10 +21418,30 @@
       </c>
     </row>
     <row r="755" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D755" s="6"/>
-      <c r="E755" s="6"/>
-      <c r="F755" s="6"/>
-      <c r="G755" s="6"/>
+      <c r="A755" s="3" t="s">
+        <v>1573</v>
+      </c>
+      <c r="B755" s="3" t="s">
+        <v>1574</v>
+      </c>
+      <c r="C755" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D755" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E755" s="6">
+        <v>2012</v>
+      </c>
+      <c r="F755" s="6">
+        <v>1053</v>
+      </c>
+      <c r="G755" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H755" s="3" t="s">
+        <v>1575</v>
+      </c>
     </row>
     <row r="756" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D756" s="6"/>

</xml_diff>

<commit_message>
Born to Run; Scalia
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED7F149-EEA1-9D45-B4B4-5AFF52DD7798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7222D7E-16F3-A945-8789-65DB6EF1FAA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2766" uniqueCount="1576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2776" uniqueCount="1582">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4761,6 +4761,24 @@
   </si>
   <si>
     <t>So ends an epic journey started when I received these volumes for Christmas in 2017 and read one each year in 2018, 2019, and 2020. Winston Churchill was a giant of a man, by no means perfect but so fascenating to get to know. Remember Winston Churchill.</t>
+  </si>
+  <si>
+    <t>Born to Run: A Hidden Tribe, Superathletes, and the Greatest Race the World Has Never Seen</t>
+  </si>
+  <si>
+    <t>Christopher McDougall</t>
+  </si>
+  <si>
+    <t>On Faith: Lessons from an American Believer</t>
+  </si>
+  <si>
+    <t>Antonin Scalia, edited by Christopher J. Scalia &amp; Edward Whelan</t>
+  </si>
+  <si>
+    <t>My interest in Scalia was sparked again by the recent death of RBG: the two of them were close friends despite vastly different jurisprudence and worldview. This book is worth having just for Fr. Scalia's homily at his father's funeral at the end, but has so much beyond that. He talks about retreats, capital punishment, and again and again the importance of religion to the moral foundation of our democracy.</t>
+  </si>
+  <si>
+    <t>Austin and Jordan read this and I found it to be fascenating as well. He tells the story of the Tarahumara Indians of Mexico's Copper Canyons and how running is a way of life for them and was for our anscesors. The most fascenating part of this book was his description of the evolutionary biology of humans related to our running as a form of hunting. Fascenating.</t>
   </si>
 </sst>
 </file>
@@ -6364,7 +6382,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A711" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A755" sqref="A755"/>
+      <selection pane="bottomLeft" activeCell="A757" sqref="A757"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21444,16 +21462,56 @@
       </c>
     </row>
     <row r="756" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D756" s="6"/>
-      <c r="E756" s="6"/>
-      <c r="F756" s="6"/>
-      <c r="G756" s="6"/>
+      <c r="A756" s="3" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B756" s="3" t="s">
+        <v>1577</v>
+      </c>
+      <c r="C756" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D756" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E756" s="6">
+        <v>2009</v>
+      </c>
+      <c r="F756" s="6">
+        <v>304</v>
+      </c>
+      <c r="G756" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H756" s="3" t="s">
+        <v>1581</v>
+      </c>
     </row>
     <row r="757" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D757" s="6"/>
-      <c r="E757" s="6"/>
-      <c r="F757" s="6"/>
-      <c r="G757" s="6"/>
+      <c r="A757" s="3" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B757" s="3" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C757" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D757" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E757" s="6">
+        <v>2019</v>
+      </c>
+      <c r="F757" s="6">
+        <v>224</v>
+      </c>
+      <c r="G757" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H757" s="3" t="s">
+        <v>1580</v>
+      </c>
     </row>
     <row r="758" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D758" s="6"/>

</xml_diff>

<commit_message>
Strangers in a Strange Land
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7222D7E-16F3-A945-8789-65DB6EF1FAA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6B5BC6-1DB0-E748-B654-BE57123FF58D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2776" uniqueCount="1582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2781" uniqueCount="1583">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4779,6 +4779,9 @@
   </si>
   <si>
     <t>Austin and Jordan read this and I found it to be fascenating as well. He tells the story of the Tarahumara Indians of Mexico's Copper Canyons and how running is a way of life for them and was for our anscesors. The most fascenating part of this book was his description of the evolutionary biology of humans related to our running as a form of hunting. Fascenating.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I listened to this again since Jordan was and my big take-away this time was that it got me to start re-reading *After Virtue* which I have been meaning to do for awhile. </t>
   </si>
 </sst>
 </file>
@@ -6381,8 +6384,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A711" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A757" sqref="A757"/>
+      <pane ySplit="1" topLeftCell="A715" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A759" sqref="A759"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21514,25 +21517,51 @@
       </c>
     </row>
     <row r="758" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D758" s="6"/>
-      <c r="E758" s="6"/>
-      <c r="F758" s="6"/>
-      <c r="G758" s="6"/>
+      <c r="A758" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B758" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C758" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D758" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E758" s="6">
+        <v>2017</v>
+      </c>
+      <c r="F758" s="6">
+        <v>288</v>
+      </c>
+      <c r="G758" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H758" s="3" t="s">
+        <v>1582</v>
+      </c>
     </row>
     <row r="759" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D759" s="6"/>
+      <c r="D759" s="6">
+        <v>2020</v>
+      </c>
       <c r="E759" s="6"/>
       <c r="F759" s="6"/>
       <c r="G759" s="6"/>
     </row>
     <row r="760" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D760" s="6"/>
+      <c r="D760" s="6">
+        <v>2020</v>
+      </c>
       <c r="E760" s="6"/>
       <c r="F760" s="6"/>
       <c r="G760" s="6"/>
     </row>
     <row r="761" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D761" s="6"/>
+      <c r="D761" s="6">
+        <v>2020</v>
+      </c>
       <c r="E761" s="6"/>
       <c r="F761" s="6"/>
       <c r="G761" s="6"/>

</xml_diff>

<commit_message>
Consecration to St. Joseph
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6B5BC6-1DB0-E748-B654-BE57123FF58D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3735381E-B45D-8846-9DAD-38D424DF1409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2781" uniqueCount="1583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2786" uniqueCount="1586">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4782,6 +4782,15 @@
   </si>
   <si>
     <t xml:space="preserve">I listened to this again since Jordan was and my big take-away this time was that it got me to start re-reading *After Virtue* which I have been meaning to do for awhile. </t>
+  </si>
+  <si>
+    <t>Consecration to St. Joseph: The Wonders of Our Spiritual Father</t>
+  </si>
+  <si>
+    <t>Fr Donald Calloway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr. Dailey told me about this and I borrowed the book from Mrs. Russell. I made the consecration over 33 days to end on All Saints day. These are beautiful reflections on Joseph and included a lot of things I did not know about him and the Holy Family. </t>
   </si>
 </sst>
 </file>
@@ -6385,7 +6394,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A715" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A759" sqref="A759"/>
+      <selection pane="bottomLeft" activeCell="A760" sqref="A760"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21543,12 +21552,30 @@
       </c>
     </row>
     <row r="759" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A759" s="3" t="s">
+        <v>1583</v>
+      </c>
+      <c r="B759" s="3" t="s">
+        <v>1584</v>
+      </c>
+      <c r="C759" s="3" t="s">
+        <v>197</v>
+      </c>
       <c r="D759" s="6">
         <v>2020</v>
       </c>
-      <c r="E759" s="6"/>
-      <c r="F759" s="6"/>
-      <c r="G759" s="6"/>
+      <c r="E759" s="6">
+        <v>2020</v>
+      </c>
+      <c r="F759" s="6">
+        <v>320</v>
+      </c>
+      <c r="G759" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H759" s="3" t="s">
+        <v>1585</v>
+      </c>
     </row>
     <row r="760" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D760" s="6">

</xml_diff>

<commit_message>
The History of the Catholic Church
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3735381E-B45D-8846-9DAD-38D424DF1409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BCA638-2055-F246-9230-813DB4A98A10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2786" uniqueCount="1586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2791" uniqueCount="1589">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4791,6 +4791,15 @@
   </si>
   <si>
     <t xml:space="preserve">Fr. Dailey told me about this and I borrowed the book from Mrs. Russell. I made the consecration over 33 days to end on All Saints day. These are beautiful reflections on Joseph and included a lot of things I did not know about him and the Holy Family. </t>
+  </si>
+  <si>
+    <t>The History of the Catholic Church: From the Apostolic Age to the Third Millennium</t>
+  </si>
+  <si>
+    <t>James Hitchcock</t>
+  </si>
+  <si>
+    <t>I was grateful to inherit this book when Fr. Romano passed away, and Fr. Dailey sung its praises and encouraged me to read it when he was over for dinner. The history of the Church is also in large part the history of Western civilization in terms of religion, culture, politics, art, and other domains of life. Hitchcock undertakes the impossible task of presenting 2000 years of history in a way that seeks the truth from the eyes of faith. He is fair in his treatment of the great sin and failings of the Church over its history but also places this—and history itself—in the context of eternity. Indeed, as he concludes: "for Christians, there can be no final understanding of history in this life."</t>
   </si>
 </sst>
 </file>
@@ -21578,12 +21587,30 @@
       </c>
     </row>
     <row r="760" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A760" s="3" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B760" s="3" t="s">
+        <v>1587</v>
+      </c>
+      <c r="C760" s="3" t="s">
+        <v>200</v>
+      </c>
       <c r="D760" s="6">
         <v>2020</v>
       </c>
-      <c r="E760" s="6"/>
-      <c r="F760" s="6"/>
-      <c r="G760" s="6"/>
+      <c r="E760" s="6">
+        <v>2012</v>
+      </c>
+      <c r="F760" s="6">
+        <v>530</v>
+      </c>
+      <c r="G760" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H760" s="3" t="s">
+        <v>1588</v>
+      </c>
     </row>
     <row r="761" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D761" s="6">

</xml_diff>

<commit_message>
The Word on Fire Bible: Volume I
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D58EB0-8B1C-BA41-900A-7C440B38016C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F225E70-9E85-4B4C-8E12-985A0F3FD32D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2806" uniqueCount="1595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2810" uniqueCount="1597">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4818,6 +4818,12 @@
   </si>
   <si>
     <t>I first read *After Virtue* in a Morality &amp; Modernity course taught by David Solomon at Notre Dame in the spring of 2012 to fulfill my second philosophy requirement. I enjoyed and [undeservedly] did well in the course without my mind in any way ready to really absorb MacIntyre's thought. I'm embarassed to admit that after the course I sold the texts for the class, including *After Virtue*. I only bought a replacement copy a couple of years ago after other authors helped me see the full importance of what was wasted on me in my youth. Or perhaps not wasted, but simply a seed planted that has taken some time to germinate. I dug back in after reading Archibishop Chaput and am grateful for this reintroduction. \n It's important to note that *After Virtue* is a first statement of the problem and a sketch of a possible solution but not the complete argument. MacIntyre says as much in the postscript to the Second Edition and prologue to the Third Edition, and the argument is further developed in his subsequent books which I plan to dive into eventually. \n *After Virtue* starts by observing the problem that modern moral arguments are irreconcilable in nature and shrill in tone. MacIntyre argues that this is the result of the failure of the enlighenment project of justifying morality by removing the teleological end man moves toward. This leaves us with an *emotivist* approach to questions of morality where the answer is all a matter of preference. People and traditions clearly have different preferences, so this leaves us deadlocked. MacIntyre argues that the path forward is a rearticulation of the classical Aristotelian and Thomistic Virtues. He concludes with a haunting comparison between our society and the Roman society at the Dark Ages and suggests that our hope rests in the emergence of a "new St. Benedict" and the formation of local communities where the virtues can be practiced in spite of the barbarians who now rule us.</t>
+  </si>
+  <si>
+    <t>The Word on Fire Bible: Volume I - The Gospels</t>
+  </si>
+  <si>
+    <t>St. Thérèse of Lisieux said "As for me, with the exception of the Gospels, I no longer find anything in books. The Gospels are enough." Starting a few years ago I have made a point of re-reading the Gospels at least once a year, at a pace of maybe one chapter or so a day. This Word on Fire edition is wonderful for the brilliant reflections on the text by Bishop Barron and other figures in the Church (ancient through modern) as well as the beautiful artwork that accompanies the text. And it is a physical book worthy of the material it contains, being by far the most beautiful book we own.</t>
   </si>
 </sst>
 </file>
@@ -6421,7 +6427,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A718" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A763" sqref="A763"/>
+      <selection pane="bottomLeft" activeCell="A764" sqref="A764"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21709,10 +21715,27 @@
       </c>
     </row>
     <row r="764" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D764" s="6"/>
-      <c r="E764" s="6"/>
-      <c r="F764" s="6"/>
-      <c r="G764" s="6"/>
+      <c r="A764" s="3" t="s">
+        <v>1595</v>
+      </c>
+      <c r="C764" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D764" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E764" s="6">
+        <v>2020</v>
+      </c>
+      <c r="F764" s="6">
+        <v>592</v>
+      </c>
+      <c r="G764" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H764" s="3" t="s">
+        <v>1596</v>
+      </c>
     </row>
     <row r="765" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D765" s="6"/>

</xml_diff>

<commit_message>
Lord of the World
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F225E70-9E85-4B4C-8E12-985A0F3FD32D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4CF1D9-8C2F-9D40-BBD3-BA86D28241E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2810" uniqueCount="1597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2815" uniqueCount="1600">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4824,6 +4824,15 @@
   </si>
   <si>
     <t>St. Thérèse of Lisieux said "As for me, with the exception of the Gospels, I no longer find anything in books. The Gospels are enough." Starting a few years ago I have made a point of re-reading the Gospels at least once a year, at a pace of maybe one chapter or so a day. This Word on Fire edition is wonderful for the brilliant reflections on the text by Bishop Barron and other figures in the Church (ancient through modern) as well as the beautiful artwork that accompanies the text. And it is a physical book worthy of the material it contains, being by far the most beautiful book we own.</t>
+  </si>
+  <si>
+    <t>Lord of the World: A Novel</t>
+  </si>
+  <si>
+    <t>Robert Hugh Benson</t>
+  </si>
+  <si>
+    <t>I thought it was appropriate in 2020 to read some apocalyptic literature: *Father Elijah*, *A Canticle for Leibowitz*, and now *Lord of the World*. I started reading the kindle version of this a few years ago and didn't get very far—in a way I'm grateful since I know I appreciated it more now than I would have then. It was frightening seeing some of the parallels between Benson's view of the future and that future as it developed in the twentieth century and into today. His novel is a challenge to prepare our hearts for when the Church will see whatever form persecution takes next, and as Christians for the final judgment at the end of time.</t>
   </si>
 </sst>
 </file>
@@ -6426,8 +6435,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A718" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A764" sqref="A764"/>
+      <pane ySplit="1" topLeftCell="A734" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A766" sqref="A766"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21738,10 +21747,30 @@
       </c>
     </row>
     <row r="765" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D765" s="6"/>
-      <c r="E765" s="6"/>
-      <c r="F765" s="6"/>
-      <c r="G765" s="6"/>
+      <c r="A765" s="3" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B765" s="3" t="s">
+        <v>1598</v>
+      </c>
+      <c r="C765" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D765" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E765" s="6">
+        <v>1907</v>
+      </c>
+      <c r="F765" s="6">
+        <v>318</v>
+      </c>
+      <c r="G765" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H765" s="3" t="s">
+        <v>1599</v>
+      </c>
     </row>
     <row r="766" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D766" s="6"/>

</xml_diff>

<commit_message>
Abandonment to Divine Providence
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF97E802-FBF8-ED4F-9191-FF8C3D6EBA08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E0CBE1-360E-C64A-8C9B-2608296FFDD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2830" uniqueCount="1605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2835" uniqueCount="1608">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4848,6 +4848,15 @@
   </si>
   <si>
     <t>What a read—with this I read the whole *Incerto* in 2020. His summary is apt: "Everything gains or loses from volatility. Fragility is what loses from volatility and uncertainty." Antifragile feels like a synthesis and extension of everything in his prior books, and already leading to his ethics of "skin in the game". I will certainly be re-reading this book and digesting it for a long time to come.</t>
+  </si>
+  <si>
+    <t>Abandonment to Divine Providence</t>
+  </si>
+  <si>
+    <t>Jean Pierre de Caussade</t>
+  </si>
+  <si>
+    <t>Fr. Raymund mentioned this the first time we had him over and then again and the guy's night I went to, and I have enjoyed reading it slowly and allowing it to be a point of prayer in my day. This reminds me a lot of *The Practice of the Presence of God*, and is a wonderful daily devotional also like *The Imitation of Christ*. Abandonment is such a simple concept, and so full of meaning to unpack.</t>
   </si>
 </sst>
 </file>
@@ -6451,7 +6460,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A735" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A768" sqref="A768"/>
+      <selection pane="bottomLeft" activeCell="A769" sqref="A769"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21865,97 +21874,117 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="769" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D769" s="6"/>
-      <c r="E769" s="6"/>
-      <c r="F769" s="6"/>
-      <c r="G769" s="6"/>
-    </row>
-    <row r="770" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="769" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A769" s="3" t="s">
+        <v>1605</v>
+      </c>
+      <c r="B769" s="3" t="s">
+        <v>1606</v>
+      </c>
+      <c r="C769" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D769" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E769" s="6">
+        <v>1750</v>
+      </c>
+      <c r="F769" s="6">
+        <v>119</v>
+      </c>
+      <c r="G769" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H769" s="3" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="770" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D770" s="6"/>
       <c r="E770" s="6"/>
       <c r="F770" s="6"/>
       <c r="G770" s="6"/>
     </row>
-    <row r="771" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="771" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D771" s="6"/>
       <c r="E771" s="6"/>
       <c r="F771" s="6"/>
       <c r="G771" s="6"/>
     </row>
-    <row r="772" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="772" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D772" s="6"/>
       <c r="E772" s="6"/>
       <c r="F772" s="6"/>
       <c r="G772" s="6"/>
     </row>
-    <row r="773" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="773" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D773" s="6"/>
       <c r="E773" s="6"/>
       <c r="F773" s="6"/>
       <c r="G773" s="6"/>
     </row>
-    <row r="774" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="774" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D774" s="6"/>
       <c r="E774" s="6"/>
       <c r="F774" s="6"/>
       <c r="G774" s="6"/>
     </row>
-    <row r="775" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="775" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D775" s="6"/>
       <c r="E775" s="6"/>
       <c r="F775" s="6"/>
       <c r="G775" s="6"/>
     </row>
-    <row r="776" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="776" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D776" s="6"/>
       <c r="E776" s="6"/>
       <c r="F776" s="6"/>
       <c r="G776" s="6"/>
     </row>
-    <row r="777" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="777" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D777" s="6"/>
       <c r="E777" s="6"/>
       <c r="F777" s="6"/>
       <c r="G777" s="6"/>
     </row>
-    <row r="778" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="778" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D778" s="6"/>
       <c r="E778" s="6"/>
       <c r="F778" s="6"/>
       <c r="G778" s="6"/>
     </row>
-    <row r="779" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="779" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D779" s="6"/>
       <c r="E779" s="6"/>
       <c r="F779" s="6"/>
       <c r="G779" s="6"/>
     </row>
-    <row r="780" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="780" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D780" s="6"/>
       <c r="E780" s="6"/>
       <c r="F780" s="6"/>
       <c r="G780" s="6"/>
     </row>
-    <row r="781" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="781" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D781" s="6"/>
       <c r="E781" s="6"/>
       <c r="F781" s="6"/>
       <c r="G781" s="6"/>
     </row>
-    <row r="782" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="782" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D782" s="6"/>
       <c r="E782" s="6"/>
       <c r="F782" s="6"/>
       <c r="G782" s="6"/>
     </row>
-    <row r="783" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="783" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D783" s="6"/>
       <c r="E783" s="6"/>
       <c r="F783" s="6"/>
       <c r="G783" s="6"/>
     </row>
-    <row r="784" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="784" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D784" s="6"/>
       <c r="E784" s="6"/>
       <c r="F784" s="6"/>

</xml_diff>

<commit_message>
Living Forward + 2021
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E0CBE1-360E-C64A-8C9B-2608296FFDD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5012F43-9815-5343-90EC-1727FBCF4BE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2835" uniqueCount="1608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2840" uniqueCount="1611">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4857,6 +4857,15 @@
   </si>
   <si>
     <t>Fr. Raymund mentioned this the first time we had him over and then again and the guy's night I went to, and I have enjoyed reading it slowly and allowing it to be a point of prayer in my day. This reminds me a lot of *The Practice of the Presence of God*, and is a wonderful daily devotional also like *The Imitation of Christ*. Abandonment is such a simple concept, and so full of meaning to unpack.</t>
+  </si>
+  <si>
+    <t>Living Forward: A Proven Plan to Stop Drifting and Get the Life You Want</t>
+  </si>
+  <si>
+    <t>Michael Hyatt &amp; Daniel Harkavy</t>
+  </si>
+  <si>
+    <t>Dad recommended this to me and it was really a kick in the pants. I have started my Life Plan (need to keep working on it) and this has helped provide some framework for my goal of working out regularly. I want to continue to digest and implement Michael Hyatt's systems in my life.</t>
   </si>
 </sst>
 </file>
@@ -6460,7 +6469,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A735" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A769" sqref="A769"/>
+      <selection pane="bottomLeft" activeCell="A771" sqref="A771"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21901,31 +21910,59 @@
       </c>
     </row>
     <row r="770" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D770" s="6"/>
-      <c r="E770" s="6"/>
-      <c r="F770" s="6"/>
-      <c r="G770" s="6"/>
+      <c r="A770" s="3" t="s">
+        <v>1608</v>
+      </c>
+      <c r="B770" s="3" t="s">
+        <v>1609</v>
+      </c>
+      <c r="C770" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D770" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E770" s="6">
+        <v>2016</v>
+      </c>
+      <c r="F770" s="6">
+        <v>203</v>
+      </c>
+      <c r="G770" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H770" s="3" t="s">
+        <v>1610</v>
+      </c>
     </row>
     <row r="771" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D771" s="6"/>
+      <c r="D771" s="6">
+        <v>2021</v>
+      </c>
       <c r="E771" s="6"/>
       <c r="F771" s="6"/>
       <c r="G771" s="6"/>
     </row>
     <row r="772" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D772" s="6"/>
+      <c r="D772" s="6">
+        <v>2021</v>
+      </c>
       <c r="E772" s="6"/>
       <c r="F772" s="6"/>
       <c r="G772" s="6"/>
     </row>
     <row r="773" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D773" s="6"/>
+      <c r="D773" s="6">
+        <v>2021</v>
+      </c>
       <c r="E773" s="6"/>
       <c r="F773" s="6"/>
       <c r="G773" s="6"/>
     </row>
     <row r="774" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D774" s="6"/>
+      <c r="D774" s="6">
+        <v>2021</v>
+      </c>
       <c r="E774" s="6"/>
       <c r="F774" s="6"/>
       <c r="G774" s="6"/>

</xml_diff>

<commit_message>
Your Best Year Ever
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5012F43-9815-5343-90EC-1727FBCF4BE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374529FC-DF5D-2547-8918-EAB781874091}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2840" uniqueCount="1611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2845" uniqueCount="1613">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4866,6 +4866,12 @@
   </si>
   <si>
     <t>Dad recommended this to me and it was really a kick in the pants. I have started my Life Plan (need to keep working on it) and this has helped provide some framework for my goal of working out regularly. I want to continue to digest and implement Michael Hyatt's systems in my life.</t>
+  </si>
+  <si>
+    <t>Your Best Year Ever: A 5-Step Plan for Achieving Your Most Important Goals</t>
+  </si>
+  <si>
+    <t>I'm continuing my Michael Hyatt trifecta with his book on goals which I listened to most of while in CA. My challenge now is to try to condense the concepts from *Free to Focus*, *Living Forward*, and *Your Best Year Ever* into a cohesive process and start executing on it beyond just using the Full Focus Planner like I have been for the last quarter. My 2020 reflection and setting goals for 2021 is the place to start.</t>
   </si>
 </sst>
 </file>
@@ -6469,7 +6475,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A735" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A771" sqref="A771"/>
+      <selection pane="bottomLeft" activeCell="A772" sqref="A772"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21936,12 +21942,30 @@
       </c>
     </row>
     <row r="771" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A771" s="3" t="s">
+        <v>1611</v>
+      </c>
+      <c r="B771" s="3" t="s">
+        <v>1563</v>
+      </c>
+      <c r="C771" s="3" t="s">
+        <v>197</v>
+      </c>
       <c r="D771" s="6">
         <v>2021</v>
       </c>
-      <c r="E771" s="6"/>
-      <c r="F771" s="6"/>
-      <c r="G771" s="6"/>
+      <c r="E771" s="6">
+        <v>2018</v>
+      </c>
+      <c r="F771" s="6">
+        <v>255</v>
+      </c>
+      <c r="G771" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H771" s="3" t="s">
+        <v>1612</v>
+      </c>
     </row>
     <row r="772" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D772" s="6">

</xml_diff>

<commit_message>
What Can I Do
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B213CA0F-DEAD-E847-88D8-59FFC6BD6085}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F96ED21-8C95-CE43-9197-B0CA7D389FCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2850" uniqueCount="1616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2855" uniqueCount="1619">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4881,6 +4881,15 @@
   </si>
   <si>
     <t xml:space="preserve">Cory and Mom both recommended this and I listened to the first half midway thorugh 2020 and then finished it up once I got the CD from the library. It is, of course, an epic coming of age story. I especially like the fictional epigraphs scattered throughout from the writings of Princess Irulan. The audiobook production is excellent. </t>
+  </si>
+  <si>
+    <t>What Can I Do?: My Path from Climate Despair to Action</t>
+  </si>
+  <si>
+    <t>Jane Fonda</t>
+  </si>
+  <si>
+    <t>Dad mentioned this when I was home as in interesting look at the Green New Deal. Unfortunately, it was also a much more detailed look at Jane Fonda's activism than I was interested in, with rather little tangible or coherent summary of the Green New Deal itself.</t>
   </si>
 </sst>
 </file>
@@ -6484,7 +6493,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A735" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A773" sqref="A773"/>
+      <selection pane="bottomLeft" activeCell="A774" sqref="A774"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22003,12 +22012,30 @@
       </c>
     </row>
     <row r="773" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A773" s="3" t="s">
+        <v>1616</v>
+      </c>
+      <c r="B773" s="3" t="s">
+        <v>1617</v>
+      </c>
+      <c r="C773" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="D773" s="6">
         <v>2021</v>
       </c>
-      <c r="E773" s="6"/>
-      <c r="F773" s="6"/>
-      <c r="G773" s="6"/>
+      <c r="E773" s="6">
+        <v>2020</v>
+      </c>
+      <c r="F773" s="6">
+        <v>352</v>
+      </c>
+      <c r="G773" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H773" s="3" t="s">
+        <v>1618</v>
+      </c>
     </row>
     <row r="774" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D774" s="6">

</xml_diff>

<commit_message>
Get Your House Right
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F96ED21-8C95-CE43-9197-B0CA7D389FCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD88130E-0078-6F44-8699-D22F2539BD35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2855" uniqueCount="1619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2860" uniqueCount="1622">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4890,6 +4890,15 @@
   </si>
   <si>
     <t>Dad mentioned this when I was home as in interesting look at the Green New Deal. Unfortunately, it was also a much more detailed look at Jane Fonda's activism than I was interested in, with rather little tangible or coherent summary of the Green New Deal itself.</t>
+  </si>
+  <si>
+    <t>Get Your House Right: Architectural Elements to Use &amp; Avoid</t>
+  </si>
+  <si>
+    <t>Marianne Cusato &amp; Ben Pentreath</t>
+  </si>
+  <si>
+    <t>This came from an article I read about designing your own home, which I have no plans to do but would be neat one day. The essay at the beginning on the reasons why traditional or classical architecture are preferable is helpful in its own right, as is the thesis that architecture is a language with both a vocabulary (building elements) and grammar (rules for putting those elements together). This book is full of helpful rules of thumb with illustrations of how to think about this language. Perhaps the most insightful diagram for me is the "Tectonics of the Orders" on page 41 which illustrates the actual structural elements of the classical orders where the cyma is the gutter, the corona is the end of the roof rafters, the bedmold is the plate that supports the rafters, the frieze is the end of the ceiling joists, the archtrave is the bean that spans the columns, and the columns support everything. The logic of the orders flows naturally from the traditional materials and construction techniques used—they are anything but arbitrary.</t>
   </si>
 </sst>
 </file>
@@ -5557,7 +5566,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5581,6 +5590,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="595">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -6493,7 +6503,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A735" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A774" sqref="A774"/>
+      <selection pane="bottomLeft" activeCell="A775" sqref="A775"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22038,12 +22048,30 @@
       </c>
     </row>
     <row r="774" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A774" s="11" t="s">
+        <v>1619</v>
+      </c>
+      <c r="B774" s="3" t="s">
+        <v>1620</v>
+      </c>
+      <c r="C774" s="3" t="s">
+        <v>197</v>
+      </c>
       <c r="D774" s="6">
         <v>2021</v>
       </c>
-      <c r="E774" s="6"/>
-      <c r="F774" s="6"/>
-      <c r="G774" s="6"/>
+      <c r="E774" s="6">
+        <v>2007</v>
+      </c>
+      <c r="F774" s="6">
+        <v>252</v>
+      </c>
+      <c r="G774" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H774" s="3" t="s">
+        <v>1621</v>
+      </c>
     </row>
     <row r="775" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D775" s="6"/>

</xml_diff>

<commit_message>
A Voice in the Wind
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD88130E-0078-6F44-8699-D22F2539BD35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFFC54D-2E20-CD4D-AF6A-152C9D8C0334}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2860" uniqueCount="1622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2865" uniqueCount="1625">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4899,6 +4899,15 @@
   </si>
   <si>
     <t>This came from an article I read about designing your own home, which I have no plans to do but would be neat one day. The essay at the beginning on the reasons why traditional or classical architecture are preferable is helpful in its own right, as is the thesis that architecture is a language with both a vocabulary (building elements) and grammar (rules for putting those elements together). This book is full of helpful rules of thumb with illustrations of how to think about this language. Perhaps the most insightful diagram for me is the "Tectonics of the Orders" on page 41 which illustrates the actual structural elements of the classical orders where the cyma is the gutter, the corona is the end of the roof rafters, the bedmold is the plate that supports the rafters, the frieze is the end of the ceiling joists, the archtrave is the bean that spans the columns, and the columns support everything. The logic of the orders flows naturally from the traditional materials and construction techniques used—they are anything but arbitrary.</t>
+  </si>
+  <si>
+    <t>A Voice in the Wind</t>
+  </si>
+  <si>
+    <t>Francine Rivers</t>
+  </si>
+  <si>
+    <t>Wow, Laura G. recommended this to Jordan and what a story. Powerful and deeply sad at the same time. I love how Rivers weaves scripture into the whole tale as the immediate reccolection of Christ as it began. And I had chills when she introduced John.</t>
   </si>
 </sst>
 </file>
@@ -6503,7 +6512,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A735" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A775" sqref="A775"/>
+      <selection pane="bottomLeft" activeCell="A776" sqref="A776"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22074,10 +22083,30 @@
       </c>
     </row>
     <row r="775" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D775" s="6"/>
-      <c r="E775" s="6"/>
-      <c r="F775" s="6"/>
-      <c r="G775" s="6"/>
+      <c r="A775" s="11" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B775" s="3" t="s">
+        <v>1623</v>
+      </c>
+      <c r="C775" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D775" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E775" s="6">
+        <v>1993</v>
+      </c>
+      <c r="F775" s="6">
+        <v>520</v>
+      </c>
+      <c r="G775" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H775" s="3" t="s">
+        <v>1624</v>
+      </c>
     </row>
     <row r="776" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D776" s="6"/>

</xml_diff>

<commit_message>
The Spirit of the Liturgy
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFFC54D-2E20-CD4D-AF6A-152C9D8C0334}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF80825-1EE5-B74D-AE2E-DF6B40BBEA43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2865" uniqueCount="1625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2875" uniqueCount="1628">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4908,6 +4908,15 @@
   </si>
   <si>
     <t>Wow, Laura G. recommended this to Jordan and what a story. Powerful and deeply sad at the same time. I love how Rivers weaves scripture into the whole tale as the immediate reccolection of Christ as it began. And I had chills when she introduced John.</t>
+  </si>
+  <si>
+    <t>Fr. Dailey recommended this to me and I was reintroduced to it when finishing the *History of the Catholic Church*. Reading Ratzinger is always a special experience—he blends together all of scripture and salvation history into a beautiful narrative, and every word drips with a lifetime of thought behind it. This is a book to think about (before mass certainly) and come back to.</t>
+  </si>
+  <si>
+    <t>The Spirit of the Liturgy</t>
+  </si>
+  <si>
+    <t>I'm glad they included the original that Ratzinger's more recent book was based off in this commemorative edition from Ignatius press. I was on the fence about whether to read it but am glad I did. The weight and beauty of tradition just pours forth from this little volume and makes you see the liturgy in a new light.</t>
   </si>
 </sst>
 </file>
@@ -6511,8 +6520,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A735" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A776" sqref="A776"/>
+      <pane ySplit="1" topLeftCell="A731" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A778" sqref="A778"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22109,16 +22118,56 @@
       </c>
     </row>
     <row r="776" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D776" s="6"/>
-      <c r="E776" s="6"/>
-      <c r="F776" s="6"/>
-      <c r="G776" s="6"/>
+      <c r="A776" s="11" t="s">
+        <v>1626</v>
+      </c>
+      <c r="B776" s="3" t="s">
+        <v>748</v>
+      </c>
+      <c r="C776" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D776" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E776" s="6">
+        <v>2000</v>
+      </c>
+      <c r="F776" s="6">
+        <v>271</v>
+      </c>
+      <c r="G776" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H776" s="11" t="s">
+        <v>1625</v>
+      </c>
     </row>
     <row r="777" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D777" s="6"/>
-      <c r="E777" s="6"/>
-      <c r="F777" s="6"/>
-      <c r="G777" s="6"/>
+      <c r="A777" s="11" t="s">
+        <v>1626</v>
+      </c>
+      <c r="B777" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="C777" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D777" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E777" s="6">
+        <v>1918</v>
+      </c>
+      <c r="F777" s="6">
+        <v>98</v>
+      </c>
+      <c r="G777" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H777" s="11" t="s">
+        <v>1627</v>
+      </c>
     </row>
     <row r="778" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D778" s="6"/>

</xml_diff>

<commit_message>
Mortise & Tenon Magazine
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BF8E67-C66F-E749-93BC-95697218FBDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10957393-4631-3F48-BBE5-BD1F0070F6B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35300" yWindow="580" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2885" uniqueCount="1633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2890" uniqueCount="1636">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4932,6 +4932,15 @@
   </si>
   <si>
     <t>This is a short little book but—as with most of Kreeft's writing—so deep and thought provoking. It served as good travel reading on our month-long trip to California and morning reading since then. Having read Brother Lawrence a couple of years ago this made me remember how great his thoughts are and want to revisit them as well.</t>
+  </si>
+  <si>
+    <t>Mortise &amp; Tenon Magazine (09)</t>
+  </si>
+  <si>
+    <t>edited by Joshua klein</t>
+  </si>
+  <si>
+    <t>Wes suggested I subscribe to this and I started with one issue. It's technically a magazine, but looks and feels like—and is as expensive as—a book. But wow is it a beautiful testament to hand craftsmanship in everything from icons to chairs to *Shopclass as Soul Craft*. I want to be more like the craftsman in these pages.</t>
   </si>
 </sst>
 </file>
@@ -6535,8 +6544,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A735" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A779" sqref="A779"/>
+      <pane ySplit="1" topLeftCell="A746" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A781" sqref="A781"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22237,10 +22246,30 @@
       </c>
     </row>
     <row r="780" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D780" s="6"/>
-      <c r="E780" s="6"/>
-      <c r="F780" s="6"/>
-      <c r="G780" s="6"/>
+      <c r="A780" s="11" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B780" s="3" t="s">
+        <v>1634</v>
+      </c>
+      <c r="C780" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D780" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E780" s="6">
+        <v>2020</v>
+      </c>
+      <c r="F780" s="6">
+        <v>137</v>
+      </c>
+      <c r="G780" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H780" s="11" t="s">
+        <v>1635</v>
+      </c>
     </row>
     <row r="781" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D781" s="6"/>

</xml_diff>

<commit_message>
An Echo in the Darkness
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC80DE30-A626-8345-909A-0BA0F07EFB58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EFE0D1-D5D7-BE40-BD52-D5125A5DB55C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35300" yWindow="580" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="manual" iterate="1" calcOnSave="0"/>
+  <calcPr calcId="191029" calcMode="manual" iterate="1" calcOnSave="0" concurrentManualCount="12"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2895" uniqueCount="1639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2900" uniqueCount="1641">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4950,6 +4950,12 @@
   </si>
   <si>
     <t xml:space="preserve">I learned more about influenza (and therefore COVID-19) from listening to this than from any of the news articles or shorter form material I have read recently. This book shines in three particular ways: 1) in the discussion of the history of medical research in the US that set the stage for where we were at the start of the 1918 pandemic, 2) the discussion of the fascinating interplay between America's mobilization for WWI and the influenza pandemic, and 3) the discussion of the political response to the pandemic (again against the backdrop of WWI) in the form of free speech restrictions and public health measures. Naturally it was fascinating to hear all of this with the recent COVID-19 experience from the last year. Unfortunately I found the tone of this book to be overly dramatic—not helped by the audiobook narration—and prone to lots of "scientist" and anti-Christian implications. Nevertheless, the research and storytelling is newly relevant for our time and deeply informative. </t>
+  </si>
+  <si>
+    <t>An Echo in the Darkness</t>
+  </si>
+  <si>
+    <t>A beautiful and challenging follow-up to *A Voice in the Wind*.</t>
   </si>
 </sst>
 </file>
@@ -6554,7 +6560,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A746" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A781" sqref="A781"/>
+      <selection pane="bottomLeft" activeCell="A783" sqref="A783"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22307,10 +22313,30 @@
       </c>
     </row>
     <row r="782" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D782" s="6"/>
-      <c r="E782" s="6"/>
-      <c r="F782" s="6"/>
-      <c r="G782" s="6"/>
+      <c r="A782" s="11" t="s">
+        <v>1639</v>
+      </c>
+      <c r="B782" s="3" t="s">
+        <v>1623</v>
+      </c>
+      <c r="C782" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D782" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E782" s="6">
+        <v>1994</v>
+      </c>
+      <c r="F782" s="6">
+        <v>461</v>
+      </c>
+      <c r="G782" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H782" s="11" t="s">
+        <v>1640</v>
+      </c>
     </row>
     <row r="783" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D783" s="6"/>

</xml_diff>

<commit_message>
The Boy, the Mole, the Fox and the Horse
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EFE0D1-D5D7-BE40-BD52-D5125A5DB55C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E94D337-102D-3443-9341-F63247C2B714}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="manual" iterate="1" calcOnSave="0" concurrentManualCount="12"/>
+  <calcPr calcId="191029" calcMode="manual" iterate="1" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2900" uniqueCount="1641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2905" uniqueCount="1644">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4956,6 +4956,15 @@
   </si>
   <si>
     <t>A beautiful and challenging follow-up to *A Voice in the Wind*.</t>
+  </si>
+  <si>
+    <t>The Boy, the Mole, the Fox and the Horse</t>
+  </si>
+  <si>
+    <t>Charlie Mackesy</t>
+  </si>
+  <si>
+    <t>I read this to Henry in one sitting, and it is short and uplifting story with great illustrations.</t>
   </si>
 </sst>
 </file>
@@ -22339,10 +22348,30 @@
       </c>
     </row>
     <row r="783" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D783" s="6"/>
-      <c r="E783" s="6"/>
-      <c r="F783" s="6"/>
-      <c r="G783" s="6"/>
+      <c r="A783" s="11" t="s">
+        <v>1641</v>
+      </c>
+      <c r="B783" s="3" t="s">
+        <v>1642</v>
+      </c>
+      <c r="C783" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D783" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E783" s="6">
+        <v>2019</v>
+      </c>
+      <c r="F783" s="6">
+        <v>128</v>
+      </c>
+      <c r="G783" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H783" s="11" t="s">
+        <v>1643</v>
+      </c>
     </row>
     <row r="784" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D784" s="6"/>

</xml_diff>

<commit_message>
Lord of the Rings
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D52E52-F058-5943-AFD3-0F81D9389C9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD41351-9C1C-D94F-B577-40A6BEF3B14F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="manual" iterate="1" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2920" uniqueCount="1652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2940" uniqueCount="1656">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -4989,6 +4989,18 @@
   </si>
   <si>
     <t>Stephanie Kelton</t>
+  </si>
+  <si>
+    <t>The Lord of the Rings: A Reader's Companion</t>
+  </si>
+  <si>
+    <t>Wayne G. Hammond &amp; Christina Scull</t>
+  </si>
+  <si>
+    <t>This was my second time reading The Lord of the Rings, which I undertook as a lenten reading plan. I loved this story more a second time and loved walking the journey with them during Lent.</t>
+  </si>
+  <si>
+    <t>Ashley recommended this and it provided helpful and interesting commentary while reading the LOTR. I skimmed and skipped parts of it but on the whole really enjoyed flipping through and reading the interesting bits after I finished a chapter. I know I'll be coming back to this for future readings of the LOTR.</t>
   </si>
 </sst>
 </file>
@@ -6592,8 +6604,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A755" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A787" sqref="A787"/>
+      <pane ySplit="1" topLeftCell="A754" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E791" sqref="E791"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22476,28 +22488,108 @@
       </c>
     </row>
     <row r="787" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D787" s="6"/>
-      <c r="E787" s="6"/>
-      <c r="F787" s="6"/>
-      <c r="G787" s="6"/>
+      <c r="A787" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B787" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="C787" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D787" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E787" s="6">
+        <v>1954</v>
+      </c>
+      <c r="F787" s="6">
+        <v>458</v>
+      </c>
+      <c r="G787" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H787" s="11" t="s">
+        <v>1654</v>
+      </c>
     </row>
     <row r="788" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D788" s="6"/>
-      <c r="E788" s="6"/>
-      <c r="F788" s="6"/>
-      <c r="G788" s="6"/>
+      <c r="A788" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B788" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="C788" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D788" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E788" s="6">
+        <v>1954</v>
+      </c>
+      <c r="F788" s="6">
+        <v>398</v>
+      </c>
+      <c r="G788" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H788" s="11" t="s">
+        <v>1654</v>
+      </c>
     </row>
     <row r="789" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D789" s="6"/>
-      <c r="E789" s="6"/>
-      <c r="F789" s="6"/>
-      <c r="G789" s="6"/>
+      <c r="A789" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="B789" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="C789" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D789" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E789" s="6">
+        <v>1955</v>
+      </c>
+      <c r="F789" s="6">
+        <v>340</v>
+      </c>
+      <c r="G789" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H789" s="11" t="s">
+        <v>1654</v>
+      </c>
     </row>
     <row r="790" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D790" s="6"/>
-      <c r="E790" s="6"/>
-      <c r="F790" s="6"/>
-      <c r="G790" s="6"/>
+      <c r="A790" s="3" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B790" t="s">
+        <v>1653</v>
+      </c>
+      <c r="C790" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D790" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E790" s="6">
+        <v>2005</v>
+      </c>
+      <c r="F790" s="6">
+        <v>678</v>
+      </c>
+      <c r="G790" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H790" s="11" t="s">
+        <v>1655</v>
+      </c>
     </row>
     <row r="791" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D791" s="6"/>

</xml_diff>

<commit_message>
A Tree Grows in Brooklyn
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DA713F-2BB7-C64D-A0A6-2248DE888135}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646F618B-6830-284D-B128-5B97EA23B370}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2950" uniqueCount="1662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2955" uniqueCount="1665">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5019,6 +5019,15 @@
   </si>
   <si>
     <t>Matt recommended this to me and it's one of the most insightful operational books I've read. He introduces whole concepts that are revolutionary: output and leverage, task-relevant maturity and feedback, applying production principles to management, training and motivating and primary management activities. This system of thought feels like a new management operating system that got installed and I will reference these notes frequently. Also stagger charts are the key to forecasting.</t>
+  </si>
+  <si>
+    <t>A Tree Grows in Brooklyn</t>
+  </si>
+  <si>
+    <t>Betty Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I got this at the library (kids) book sale, and listened to it after Becca confirmed it's value. It is a beautiful coming of age story of Francie Nolan. Life is hard and messy and cruel, but faith in God and support of family and a sense of wonder and possibility can get you through anything. </t>
   </si>
 </sst>
 </file>
@@ -6623,7 +6632,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A754" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A793" sqref="A793"/>
+      <selection pane="bottomLeft" activeCell="A794" sqref="A794"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22662,10 +22671,30 @@
       </c>
     </row>
     <row r="793" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D793" s="6"/>
-      <c r="E793" s="6"/>
-      <c r="F793" s="6"/>
-      <c r="G793" s="6"/>
+      <c r="A793" s="3" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B793" s="3" t="s">
+        <v>1663</v>
+      </c>
+      <c r="C793" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D793" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E793" s="6">
+        <v>1943</v>
+      </c>
+      <c r="F793" s="6">
+        <v>493</v>
+      </c>
+      <c r="G793" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H793" s="11" t="s">
+        <v>1664</v>
+      </c>
     </row>
     <row r="794" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D794" s="6"/>

</xml_diff>

<commit_message>
How to Talk About Books You Haven't Read
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6C5A89-EFD5-DA44-926F-DACE38D6A5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C2700C-DD8C-944C-8E75-87AB11E44A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="manual" iterate="1" iterateCount="500"/>
+  <calcPr calcId="191029" calcMode="manual" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2965" uniqueCount="1670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2970" uniqueCount="1673">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5043,6 +5043,15 @@
   </si>
   <si>
     <t>This book was an important part of my journey in 2021: I started reading it while I was interviewing with Hagerty, and while I didn't take that role I finished it in the midst of my Bitcoin reading. The emphasis on *sovereignty* here is really the theme of much of my reading and thinking lately, from *The Bitcoin Standard* to *The Sovereign Individual* to this. This is the third book by Crawford I have read, and I am always just amazed at the integrated force he brings to a topic (and all the adjacent topics). This isn't really a book you can summarize, apart to say that it's about just about everything important in our political and cultural and economic world.</t>
+  </si>
+  <si>
+    <t>How to Talk About Books You Haven't Read</t>
+  </si>
+  <si>
+    <t>Pierre Bayard</t>
+  </si>
+  <si>
+    <t>I tend to be rather methodical in my reading of books, and I treat it as a discrete activity: a book is either read or not read, and I need to actually read (or listen to) a book to check it off and put it on the [list](https://matthewkudija.com/reading). This book challenges that notion and rightly observes that we relate to most books through some level of *non*-reading. &lt;br&gt; Books are just containers for ideas, and it is the ideas that matter much more than the containers we pass them around in. Reading this has challenged me to change my mental model for "reading" from a linear march of completion to a cyclical process that is perpetually active for every book I have ever heard of.&lt;br&gt;I can't let the goal of "reading" get in the way of spending some time with a book to get to know it and place it alongside other books in the collective library. My notes will transform into more "evergreen" notes for books that are started as early in the process as possible and record thoughts throughout the journey. I don't have use for cheeky premise of this book to handle delicate social situations surrounding books, but it has certainly transformed my relationship to books and reading.</t>
   </si>
 </sst>
 </file>
@@ -6647,7 +6656,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A754" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A796" sqref="A796"/>
+      <selection pane="bottomLeft" activeCell="A797" sqref="A797"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22764,10 +22773,30 @@
       </c>
     </row>
     <row r="796" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D796" s="6"/>
-      <c r="E796" s="6"/>
-      <c r="F796" s="6"/>
-      <c r="G796" s="6"/>
+      <c r="A796" s="3" t="s">
+        <v>1670</v>
+      </c>
+      <c r="B796" s="3" t="s">
+        <v>1671</v>
+      </c>
+      <c r="C796" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D796" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E796" s="6">
+        <v>2007</v>
+      </c>
+      <c r="F796" s="6">
+        <v>185</v>
+      </c>
+      <c r="G796" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H796" s="11" t="s">
+        <v>1672</v>
+      </c>
     </row>
     <row r="797" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D797" s="6"/>

</xml_diff>

<commit_message>
Brother Hugo and the Bear
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19848B9F-BDBA-6C4E-99D1-116DBB6A4EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E3A24F-E72E-694B-B0E4-53E4EFBFFCF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2975" uniqueCount="1676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2980" uniqueCount="1679">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5061,6 +5061,15 @@
   </si>
   <si>
     <t xml:space="preserve">This was a great find in the Grandview Library kid's section. Kid's books a great for learning the basics of something, and this book had awesome illustrations and text about the highlights of world history. I had fun re-reading about Lepanto and the Dardanelles during WWI in the Churchill volumes, and it was neat to see Damien of Molokai featured, which makes sense given it is a Dutch author. </t>
+  </si>
+  <si>
+    <t>Brother Hugo and the Bear</t>
+  </si>
+  <si>
+    <t>Katy Beebe</t>
+  </si>
+  <si>
+    <t>This was a lucky find at the library and such a wonderful kid's book about a monk copying a book in a monestary. It is beautiful in both language and decoration, historically accurate, and so delightful.</t>
   </si>
 </sst>
 </file>
@@ -6665,7 +6674,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A754" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A798" sqref="A798"/>
+      <selection pane="bottomLeft" activeCell="A799" sqref="A799"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22834,10 +22843,30 @@
       </c>
     </row>
     <row r="798" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D798" s="6"/>
-      <c r="E798" s="6"/>
-      <c r="F798" s="6"/>
-      <c r="G798" s="6"/>
+      <c r="A798" s="3" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B798" s="3" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C798" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D798" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E798" s="6">
+        <v>2014</v>
+      </c>
+      <c r="F798" s="6">
+        <v>34</v>
+      </c>
+      <c r="G798" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H798" s="11" t="s">
+        <v>1678</v>
+      </c>
     </row>
     <row r="799" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D799" s="6"/>

</xml_diff>

<commit_message>
Faith and the Future
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FC73C3-98A8-EF41-8256-3653577F361B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4577DDC9-6268-CA4E-88BD-7FEFE2656E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2985" uniqueCount="1681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2990" uniqueCount="1683">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5076,6 +5076,12 @@
   </si>
   <si>
     <t>As has become my tradition when a Kudija baby is born, I read the next Hornblower after Ruthie's arrival. Epic as always, fascinating seamanship, and a joy to revel in.</t>
+  </si>
+  <si>
+    <t>Faith and the Future</t>
+  </si>
+  <si>
+    <t>I vaguely recalled a quote by Ratzinger about a poorer and smaller church, and a search led me to this as the source. This is a beautiful refleciton on faith, and the last section espeically a beautiful reflection on the Church and the perspective—historical and eternal—that will give us peace.</t>
   </si>
 </sst>
 </file>
@@ -6680,7 +6686,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A775" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A800" sqref="A800"/>
+      <selection pane="bottomLeft" activeCell="A801" sqref="A801"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22901,10 +22907,30 @@
       </c>
     </row>
     <row r="800" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D800" s="6"/>
-      <c r="E800" s="6"/>
-      <c r="F800" s="6"/>
-      <c r="G800" s="6"/>
+      <c r="A800" s="3" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B800" s="3" t="s">
+        <v>748</v>
+      </c>
+      <c r="C800" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D800" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E800" s="6">
+        <v>1970</v>
+      </c>
+      <c r="F800" s="6">
+        <v>118</v>
+      </c>
+      <c r="G800" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H800" s="11" t="s">
+        <v>1682</v>
+      </c>
     </row>
     <row r="801" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D801" s="6"/>

</xml_diff>

<commit_message>
"Live Not by Lies"
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40339582-5095-9E4C-B752-0EE98826A3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970A38E4-4153-1E4A-8B90-A07DAE4B7162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3000" uniqueCount="1688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3005" uniqueCount="1691">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5097,6 +5097,15 @@
   </si>
   <si>
     <t>I loved Kurson's other books about Pirate Treasure and Apollo 8, and this one did not dissapoint. This is an epic story of the discovery and identification of a German WWI U-boat off the coast of New Jersey through the eyes of deep wreck divers Chatterton and Kohler. But not only is it an epic story, it has some epic life lessons: raising kids, testing yourself in life, the tug between family and accomplishment, decision making and risk management.</t>
+  </si>
+  <si>
+    <t>"Live Not by Lies"</t>
+  </si>
+  <si>
+    <t>Aleksandr Solzhenitsyn</t>
+  </si>
+  <si>
+    <t>I came across this originally in Rod Dreher's book by the same name, and then again in Winston Marshall's essay on why he's leaving Mumford &amp; Sons. Let us indeed live by the Truth rather than by lies.</t>
   </si>
 </sst>
 </file>
@@ -6701,7 +6710,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A775" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A803" sqref="A803"/>
+      <selection pane="bottomLeft" activeCell="A804" sqref="A804"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23000,10 +23009,30 @@
       </c>
     </row>
     <row r="803" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D803" s="6"/>
-      <c r="E803" s="6"/>
-      <c r="F803" s="6"/>
-      <c r="G803" s="6"/>
+      <c r="A803" s="3" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B803" s="3" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C803" s="3" t="s">
+        <v>942</v>
+      </c>
+      <c r="D803" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E803" s="6">
+        <v>1972</v>
+      </c>
+      <c r="F803" s="6">
+        <v>4</v>
+      </c>
+      <c r="G803" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H803" s="11" t="s">
+        <v>1690</v>
+      </c>
     </row>
     <row r="804" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D804" s="6"/>

</xml_diff>

<commit_message>
The Road + notes
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970A38E4-4153-1E4A-8B90-A07DAE4B7162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381A65B8-71BC-BE43-ABC0-6D048E8C5A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3005" uniqueCount="1691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3010" uniqueCount="1692">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5106,6 +5106,9 @@
   </si>
   <si>
     <t>I came across this originally in Rod Dreher's book by the same name, and then again in Winston Marshall's essay on why he's leaving Mumford &amp; Sons. Let us indeed live by the Truth rather than by lies.</t>
+  </si>
+  <si>
+    <t>I read this in high school, and decided to revisit it now after the post-apocalyptic novels and experience of 2020. This story hits you differently once you have kids, and is a reminder of the great blessings we enjoy.</t>
   </si>
 </sst>
 </file>
@@ -6709,7 +6712,7 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A775" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A760" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A804" sqref="A804"/>
     </sheetView>
   </sheetViews>
@@ -23035,10 +23038,30 @@
       </c>
     </row>
     <row r="804" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D804" s="6"/>
-      <c r="E804" s="6"/>
-      <c r="F804" s="6"/>
-      <c r="G804" s="6"/>
+      <c r="A804" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B804" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="C804" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D804" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E804" s="6">
+        <v>2006</v>
+      </c>
+      <c r="F804" s="6">
+        <v>287</v>
+      </c>
+      <c r="G804" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H804" s="11" t="s">
+        <v>1691</v>
+      </c>
     </row>
     <row r="805" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D805" s="6"/>

</xml_diff>

<commit_message>
My Sisters the Saints
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381A65B8-71BC-BE43-ABC0-6D048E8C5A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE05A0B8-E713-5F4A-8AD2-D611958EC505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3010" uniqueCount="1692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3015" uniqueCount="1695">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5109,6 +5109,15 @@
   </si>
   <si>
     <t>I read this in high school, and decided to revisit it now after the post-apocalyptic novels and experience of 2020. This story hits you differently once you have kids, and is a reminder of the great blessings we enjoy.</t>
+  </si>
+  <si>
+    <t>My Sisters the Saints: A Spiritual Memoir</t>
+  </si>
+  <si>
+    <t>Colleen Carroll Campbell</t>
+  </si>
+  <si>
+    <t>Jordan read this a few years ago and I absolutely loved it as a beautiful memoir of the saints, particularly the Carmelites: Theresa of Ávila, Thérèse of Lisieux, Edith Stein, and John of the Cross.</t>
   </si>
 </sst>
 </file>
@@ -6713,7 +6722,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A760" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A804" sqref="A804"/>
+      <selection pane="bottomLeft" activeCell="A805" sqref="A805"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23064,10 +23073,30 @@
       </c>
     </row>
     <row r="805" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D805" s="6"/>
-      <c r="E805" s="6"/>
-      <c r="F805" s="6"/>
-      <c r="G805" s="6"/>
+      <c r="A805" s="3" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B805" s="3" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C805" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D805" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E805" s="6">
+        <v>2012</v>
+      </c>
+      <c r="F805" s="6">
+        <v>214</v>
+      </c>
+      <c r="G805" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H805" s="11" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="806" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D806" s="6"/>

</xml_diff>

<commit_message>
Witness to Hope, Let us Dream
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701A9A10-2229-AF45-8953-ADFE714F0185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FEB72C-CA3E-E147-AFF0-A02B31780D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3035" uniqueCount="1706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3045" uniqueCount="1710">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5151,6 +5151,18 @@
   </si>
   <si>
     <t>I first heard about this after reading [[2021-07-14 Article-Mumford and Sons’ Winston Marshall Visits the Blessed Sacrament|an article]] ([*link*](https://www.ncregister.com/blog/mumford-and-sons-william-marshall)) about how [[Winston Marshall]] from Mumford &amp; Sons left the band because he read the book and commented about it on Twitter. He was attacked by the mob and ended up leaving the band to protect them from further criticism (his essay [[2021-08-15 Article-Why I’m Leaving Mumford &amp; Sons|here]]: [*Why I’m Leaving Mumford &amp; Sons*](https://mrwinstonmarshall.medium.com/why-im-leaving-mumford-sons-e6e731bbc255)). It fascinates me that a high-profile individual would take a stand like this, and even more so that he quoted [[Aleksandr Solzhenitsyn]]'s [[2021-07-15-"Live Not by Lies"|"Live Not by Lies"]] in doing so. I was most interested by three things from *Unmasked*. First, despite the significant controversy surrounding Andy Ngo and taking an initially-skeptical view of anyone commenting on such contentious issues, his first-hand accounts of Antifa are startling. Second, he presents a history of Antifa (chapter 6) and the alignment between Antifa and BLM (chapter 7); especially interesting is his claim about their shared underlying Marxism. Finally, and again taking a skeptical view of anyone actively commenting on these issues, I appreciate Ngo's reference to Antifa and adjacent literature which speaks for itself.</t>
+  </si>
+  <si>
+    <t>Let Us Dream: The Path to a Better Future</t>
+  </si>
+  <si>
+    <t>Fr. Missimi gave me this book, which is Pope Francis' reflection and response to the Covid pandemic. I remember watching the election of Pope Francis while on spring break in Panama City Beach in 2013 and his address before the US Congress from my desk at SpaceX in 2015, and I'm still trying to figure him out...</t>
+  </si>
+  <si>
+    <t>Witness to Hope: The Biography of Pope John Paul II</t>
+  </si>
+  <si>
+    <t>I bought this off Amazon for $4 back in June of 2015 when I was living in LA. I forget why I bought it then but it was perhaps after listening to *John Paul II: A Personal Portrait of the Pope and the Man* by Ray Flynn. Its great bulk sat on my shelf through three moves while I continued to read some other titles by John Paul II...</t>
   </si>
 </sst>
 </file>
@@ -6755,7 +6767,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A790" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A810" sqref="A810"/>
+      <selection pane="bottomLeft" activeCell="A812" sqref="A812"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23236,16 +23248,56 @@
       </c>
     </row>
     <row r="810" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D810" s="6"/>
-      <c r="E810" s="6"/>
-      <c r="F810" s="6"/>
-      <c r="G810" s="6"/>
+      <c r="A810" s="3" t="s">
+        <v>1706</v>
+      </c>
+      <c r="B810" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C810" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D810" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E810" s="6">
+        <v>2020</v>
+      </c>
+      <c r="F810" s="6">
+        <v>144</v>
+      </c>
+      <c r="G810" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H810" s="11" t="s">
+        <v>1707</v>
+      </c>
     </row>
     <row r="811" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D811" s="6"/>
-      <c r="E811" s="6"/>
-      <c r="F811" s="6"/>
-      <c r="G811" s="6"/>
+      <c r="A811" s="3" t="s">
+        <v>1708</v>
+      </c>
+      <c r="B811" s="3" t="s">
+        <v>761</v>
+      </c>
+      <c r="C811" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D811" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E811" s="6">
+        <v>1999</v>
+      </c>
+      <c r="F811" s="6">
+        <v>960</v>
+      </c>
+      <c r="G811" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H811" s="11" t="s">
+        <v>1709</v>
+      </c>
     </row>
     <row r="812" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D812" s="6"/>

</xml_diff>

<commit_message>
Last Thing He Told Me
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AA3E62-DCC2-D94F-BDF6-CC5CAE4C4F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0ABC56F-9BCA-B746-9BF4-1BB92E36F33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3549" uniqueCount="1713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3559" uniqueCount="1719">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5172,6 +5172,24 @@
   </si>
   <si>
     <t>https://matthewkudija.com/reading-notes/2020-11-18-After-Virtue.html</t>
+  </si>
+  <si>
+    <t>Cathedral: The Story of Its Construction</t>
+  </si>
+  <si>
+    <t>David Macaulay</t>
+  </si>
+  <si>
+    <t>I love Macaulay's books, and Henry wanted me to read this to him one Sunday—he was enthralled and then wanted to go build a Cathedral ("Chartres Cathedral") out of his legos and I took him down to the St. Joseph Cathedral for mass the next day and he was wide-eyed the whole time taking it all in. I've read a fair bit about cathedrals and learned plenty of new things from this straightforward and excellently illustrated book.</t>
+  </si>
+  <si>
+    <t>The Last Thing He Told Me: A Novel</t>
+  </si>
+  <si>
+    <t>Laura Dave</t>
+  </si>
+  <si>
+    <t>Jordan was listening to this as recommended by a friend and it was a thrilling story, centering around a woman who's husband disappears after a scandal at his tech company and she has to take care of his daughter while finding out about his past life.</t>
   </si>
 </sst>
 </file>
@@ -6792,8 +6810,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A761" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A763" sqref="A763"/>
+      <pane ySplit="1" topLeftCell="A768" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A814" sqref="A814"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24798,14 +24816,56 @@
       </c>
     </row>
     <row r="812" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D812" s="6"/>
-      <c r="E812" s="6"/>
-      <c r="F812" s="6"/>
+      <c r="A812" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B812" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C812" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D812" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E812" s="6">
+        <v>1973</v>
+      </c>
+      <c r="F812" s="6">
+        <v>80</v>
+      </c>
+      <c r="G812" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="H812" s="11" t="s">
+        <v>1715</v>
+      </c>
     </row>
     <row r="813" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D813" s="6"/>
-      <c r="E813" s="6"/>
-      <c r="F813" s="6"/>
+      <c r="A813" s="3" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B813" s="3" t="s">
+        <v>1717</v>
+      </c>
+      <c r="C813" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D813" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E813" s="6">
+        <v>2021</v>
+      </c>
+      <c r="F813" s="6">
+        <v>320</v>
+      </c>
+      <c r="G813" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="H813" s="11" t="s">
+        <v>1718</v>
+      </c>
     </row>
     <row r="814" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D814" s="6"/>

</xml_diff>

<commit_message>
I Alone Can Fix it
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745381D6-993A-C844-BED9-2A9BEE3B6C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3524F9D3-3F0B-7B40-9146-40F55629FC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3584" uniqueCount="1733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3589" uniqueCount="1736">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5232,6 +5232,15 @@
   </si>
   <si>
     <t>Scott Young gives a tour of ultralearning projects (including his own) to outline nine principles of how to best pursue self-directed and intense ultralearing projects</t>
+  </si>
+  <si>
+    <t>I Alone Can Fix It: Donald J. Trump's Catastrophic Final Year</t>
+  </si>
+  <si>
+    <t>Carol Leonnig &amp; Philip Rucker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This was one of a few books that Fr. John recommended to me at Peter's rehearsal dinner. Along with *The Promonition*, this is my preferred way to read about current events: recent but a few steps removed from the news cycle. Some items of note include the advise not to pull out of Afghanistan (interesting to see in retrospect), Pence's calm command during the Capitol riot and courage to stand up to Trump to cerify the vote, the trifecta of Milley, Pompeo, and Meadows trying to maintain control at the tail end of his presidency, and Doris Kearns Goodwin's dismay at Trump as president. I also liked Milley's quote preparing for Biden's inauguration: "The pain of preparation is much less than the pain of regret." </t>
   </si>
 </sst>
 </file>
@@ -6853,7 +6862,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A781" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A818" sqref="A818"/>
+      <selection pane="bottomLeft" activeCell="A819" sqref="A819"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25040,9 +25049,30 @@
       </c>
     </row>
     <row r="819" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D819" s="6"/>
-      <c r="E819" s="6"/>
-      <c r="F819" s="6"/>
+      <c r="A819" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="B819" s="3" t="s">
+        <v>1734</v>
+      </c>
+      <c r="C819" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D819" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E819" s="6">
+        <v>2021</v>
+      </c>
+      <c r="F819" s="6">
+        <v>591</v>
+      </c>
+      <c r="G819" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="H819" s="3" t="s">
+        <v>1735</v>
+      </c>
     </row>
     <row r="820" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D820" s="6"/>

</xml_diff>

<commit_message>
new notes, Live not by Lies, and updates
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F964CC41-1599-CC4E-8CEE-C7AC0640B75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C471B9-65DD-0D4D-B50E-E0DEC50A8E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3599" uniqueCount="1742">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3604" uniqueCount="1746">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5259,6 +5259,18 @@
   </si>
   <si>
     <t>This was my spiritual reading for my (very sporadic) mental prayer befor work in 2021. It is filled with great instruction and reflection on contemplation.</t>
+  </si>
+  <si>
+    <t>Live Not by Lies</t>
+  </si>
+  <si>
+    <t>Rod Dreher</t>
+  </si>
+  <si>
+    <t>https://matthewkudija.com/reading-notes/2021-10-30-Live-Not-By-Lies.html</t>
+  </si>
+  <si>
+    <t>Ben Harting told me about this and I really thought hard out this first while listening to the audiobook and then while listening to it again while reading the hard copy. The soft totalitarianism he speaks of is quite apparent and our responsibility—especially with our kids—to prepare is at the forefront of my mnd.</t>
   </si>
 </sst>
 </file>
@@ -6885,7 +6897,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A781" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A822" sqref="A822"/>
+      <selection pane="bottomLeft" activeCell="A823" sqref="A823"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25150,9 +25162,30 @@
       </c>
     </row>
     <row r="822" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D822" s="6"/>
-      <c r="E822" s="6"/>
-      <c r="F822" s="6"/>
+      <c r="A822" s="3" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B822" s="3" t="s">
+        <v>1743</v>
+      </c>
+      <c r="C822" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D822" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E822" s="6">
+        <v>2021</v>
+      </c>
+      <c r="F822" s="6">
+        <v>256</v>
+      </c>
+      <c r="G822" s="14" t="s">
+        <v>1744</v>
+      </c>
+      <c r="H822" s="3" t="s">
+        <v>1745</v>
+      </c>
     </row>
     <row r="823" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D823" s="6"/>
@@ -26930,6 +26963,7 @@
     <hyperlink ref="G763" r:id="rId2" xr:uid="{95A42AE5-2FF0-C449-AB16-444DCE23323B}"/>
     <hyperlink ref="G818" r:id="rId3" xr:uid="{ECD28476-958B-FE45-B614-823AA98C1276}"/>
     <hyperlink ref="G820" r:id="rId4" xr:uid="{429BDA50-7A44-794E-A131-7BB11C8FB7B3}"/>
+    <hyperlink ref="G822" r:id="rId5" xr:uid="{76A67651-1048-5140-9636-7754CDE7CD45}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
No Rules Rules, other
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C471B9-65DD-0D4D-B50E-E0DEC50A8E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1259DA9C-4414-F74C-8D8B-09183C5F3FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3604" uniqueCount="1746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3609" uniqueCount="1749">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5271,6 +5271,15 @@
   </si>
   <si>
     <t>Ben Harting told me about this and I really thought hard out this first while listening to the audiobook and then while listening to it again while reading the hard copy. The soft totalitarianism he speaks of is quite apparent and our responsibility—especially with our kids—to prepare is at the forefront of my mnd.</t>
+  </si>
+  <si>
+    <t>No Rules Rules: Netflix and the Culture of Reinvention</t>
+  </si>
+  <si>
+    <t>Reed Hastings &amp; Erin Meyer</t>
+  </si>
+  <si>
+    <t>This is a radically different vision of building a high-performing and innovative company. Netflix has build a compelling argument—backed by their performance—for building of team of top playersa and giving complete freedom and responsibility.</t>
   </si>
 </sst>
 </file>
@@ -6897,7 +6906,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A781" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A823" sqref="A823"/>
+      <selection pane="bottomLeft" activeCell="A824" sqref="A824"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25188,9 +25197,30 @@
       </c>
     </row>
     <row r="823" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D823" s="6"/>
-      <c r="E823" s="6"/>
-      <c r="F823" s="6"/>
+      <c r="A823" s="3" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B823" s="3" t="s">
+        <v>1747</v>
+      </c>
+      <c r="C823" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D823" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E823" s="6">
+        <v>2020</v>
+      </c>
+      <c r="F823" s="6">
+        <v>320</v>
+      </c>
+      <c r="G823" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="H823" s="3" t="s">
+        <v>1748</v>
+      </c>
     </row>
     <row r="824" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D824" s="6"/>

</xml_diff>

<commit_message>
The Price of Tomorrow
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996E23BA-57EB-1948-80D9-7DDE3B0D9291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58273CEE-AB62-1148-8254-1FBCE86DE507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="manual" iterate="1"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3639" uniqueCount="1766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3644" uniqueCount="1769">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5331,6 +5331,15 @@
   </si>
   <si>
     <t>I listened to this and finally actually *deleted* by Facebook and Twitter accounts which have been inactive for going on three years. I was especially intrigued with his tenth argument about how BUMMER is a new secular religion.</t>
+  </si>
+  <si>
+    <t>The Price of Tomorrow: Why Deflation is the Key to an Abundant Future</t>
+  </si>
+  <si>
+    <t>Jeff Booth</t>
+  </si>
+  <si>
+    <t>Booth's thesis is that technology is deflationary and accelerating exponentially, but our economy is propped up with debt and our governments have turned capitalism into crony capitalism by becoming lenders of last resort. I agree with many of his observation and found his summaries of quantitative easing, creative destruction, cognitive biases, energy, and AI to be interesting even if a bit full of cliché. He does not present a compelling solution, however, apart from a vague plea to embrace deflation and adopt [[Bitcoin]].</t>
   </si>
 </sst>
 </file>
@@ -6002,7 +6011,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6035,9 +6044,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="595" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6965,8 +6971,8 @@
   <dimension ref="A1:H1175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A783" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A830" sqref="A830"/>
+      <pane ySplit="1" topLeftCell="A796" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A831" sqref="A831"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25431,7 +25437,7 @@
       <c r="F829" s="6">
         <v>146</v>
       </c>
-      <c r="G829" s="16" t="s">
+      <c r="G829" s="15" t="s">
         <v>235</v>
       </c>
       <c r="H829" s="3" t="s">
@@ -25439,40 +25445,60 @@
       </c>
     </row>
     <row r="830" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D830" s="6"/>
-      <c r="E830" s="6"/>
-      <c r="F830" s="15"/>
-      <c r="G830" s="16"/>
+      <c r="A830" s="3" t="s">
+        <v>1766</v>
+      </c>
+      <c r="B830" s="3" t="s">
+        <v>1767</v>
+      </c>
+      <c r="C830" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D830" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E830" s="6">
+        <v>2020</v>
+      </c>
+      <c r="F830" s="6">
+        <v>208</v>
+      </c>
+      <c r="G830" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="H830" s="3" t="s">
+        <v>1768</v>
+      </c>
     </row>
     <row r="831" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D831" s="6"/>
       <c r="E831" s="6"/>
-      <c r="F831" s="15"/>
-      <c r="G831" s="16"/>
+      <c r="F831" s="6"/>
+      <c r="G831" s="15"/>
     </row>
     <row r="832" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D832" s="6"/>
       <c r="E832" s="6"/>
-      <c r="F832" s="15"/>
-      <c r="G832" s="16"/>
+      <c r="F832" s="6"/>
+      <c r="G832" s="15"/>
     </row>
     <row r="833" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D833" s="6"/>
       <c r="E833" s="6"/>
-      <c r="F833" s="15"/>
-      <c r="G833" s="16"/>
+      <c r="F833" s="6"/>
+      <c r="G833" s="15"/>
     </row>
     <row r="834" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D834" s="6"/>
       <c r="E834" s="6"/>
-      <c r="F834" s="15"/>
-      <c r="G834" s="16"/>
+      <c r="F834" s="6"/>
+      <c r="G834" s="15"/>
     </row>
     <row r="835" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D835" s="6"/>
       <c r="E835" s="6"/>
-      <c r="F835" s="15"/>
-      <c r="G835" s="16"/>
+      <c r="F835" s="6"/>
+      <c r="G835" s="15"/>
     </row>
     <row r="836" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D836" s="6"/>

</xml_diff>

<commit_message>
He Leadeth Me, Version Control
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58273CEE-AB62-1148-8254-1FBCE86DE507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05254858-164A-0D4D-941D-B6F6DAE58928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="191029" calcMode="manual" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3644" uniqueCount="1769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3649" uniqueCount="1772">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5340,6 +5340,15 @@
   </si>
   <si>
     <t>Booth's thesis is that technology is deflationary and accelerating exponentially, but our economy is propped up with debt and our governments have turned capitalism into crony capitalism by becoming lenders of last resort. I agree with many of his observation and found his summaries of quantitative easing, creative destruction, cognitive biases, energy, and AI to be interesting even if a bit full of cliché. He does not present a compelling solution, however, apart from a vague plea to embrace deflation and adopt [[Bitcoin]].</t>
+  </si>
+  <si>
+    <t>He Leadeth Me: An Extraordinary Testament of Faith</t>
+  </si>
+  <si>
+    <t>Walter J. Ciszek, S.J.</t>
+  </si>
+  <si>
+    <t>Jordan and I read this aloud together over a couple of months and it is a beautiful story of faith and perseverance!</t>
   </si>
 </sst>
 </file>
@@ -6972,7 +6981,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A796" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A831" sqref="A831"/>
+      <selection pane="bottomLeft" activeCell="A832" sqref="A832"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25471,10 +25480,30 @@
       </c>
     </row>
     <row r="831" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D831" s="6"/>
-      <c r="E831" s="6"/>
-      <c r="F831" s="6"/>
-      <c r="G831" s="15"/>
+      <c r="A831" s="3" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B831" s="3" t="s">
+        <v>1770</v>
+      </c>
+      <c r="C831" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D831" s="6">
+        <v>2021</v>
+      </c>
+      <c r="E831" s="6">
+        <v>1973</v>
+      </c>
+      <c r="F831" s="6">
+        <v>208</v>
+      </c>
+      <c r="G831" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="H831" s="3" t="s">
+        <v>1771</v>
+      </c>
     </row>
     <row r="832" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D832" s="6"/>

</xml_diff>

<commit_message>
A Man & His Watch
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA03047-AC8F-5746-9188-690FB642C9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E2BD69-D0D6-D44D-8390-461B93CA333B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3700" uniqueCount="1799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3705" uniqueCount="1802">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5430,6 +5430,15 @@
   </si>
   <si>
     <t>Dan mentioned this when talking about classical schools and I had to revisit it in more detail. Such a prophetic book and encouragement to educate our children in the Tao (or Natural Law).</t>
+  </si>
+  <si>
+    <t>A Man &amp; His Watch: Iconic Watches and Stories from the Men Who Wore Them</t>
+  </si>
+  <si>
+    <t>Matt Hranek</t>
+  </si>
+  <si>
+    <t>Jordan gave this to me as a surprise for Christmas and it got me really interested in mechanical watches!</t>
   </si>
 </sst>
 </file>
@@ -7095,7 +7104,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A799" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A842" sqref="A842"/>
+      <selection pane="bottomLeft" activeCell="A844" sqref="A844"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25894,9 +25903,30 @@
       </c>
     </row>
     <row r="843" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D843" s="6"/>
-      <c r="E843" s="6"/>
-      <c r="F843" s="6"/>
+      <c r="A843" s="3" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B843" s="3" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C843" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D843" s="6">
+        <v>2022</v>
+      </c>
+      <c r="E843" s="6">
+        <v>2017</v>
+      </c>
+      <c r="F843" s="6">
+        <v>216</v>
+      </c>
+      <c r="G843" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="H843" s="3" t="s">
+        <v>1801</v>
+      </c>
     </row>
     <row r="844" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D844" s="6"/>

</xml_diff>

<commit_message>
The Shadow of the Wind
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E2BD69-D0D6-D44D-8390-461B93CA333B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4234BF-7F92-FC49-93E2-B240330D023A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="191029" calcMode="manual" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3705" uniqueCount="1802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3710" uniqueCount="1805">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5439,6 +5439,15 @@
   </si>
   <si>
     <t>Jordan gave this to me as a surprise for Christmas and it got me really interested in mechanical watches!</t>
+  </si>
+  <si>
+    <t>The Shadow of the Wind</t>
+  </si>
+  <si>
+    <t>Carlos Ruiz Zafón</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Becca's recommendation which I heartily enjoyed! </t>
   </si>
 </sst>
 </file>
@@ -7104,7 +7113,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A799" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A844" sqref="A844"/>
+      <selection pane="bottomLeft" activeCell="A845" sqref="A845"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25929,9 +25938,30 @@
       </c>
     </row>
     <row r="844" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D844" s="6"/>
-      <c r="E844" s="6"/>
-      <c r="F844" s="6"/>
+      <c r="A844" s="3" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B844" s="3" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C844" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D844" s="6">
+        <v>2022</v>
+      </c>
+      <c r="E844" s="6">
+        <v>2002</v>
+      </c>
+      <c r="F844" s="6">
+        <v>510</v>
+      </c>
+      <c r="G844" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="H844" s="3" t="s">
+        <v>1804</v>
+      </c>
     </row>
     <row r="845" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D845" s="6"/>

</xml_diff>

<commit_message>
purgatorio and ethics of money
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D6EE0F4-7238-1144-A637-7FE2A700AE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A66976FC-7055-5A4B-AE4D-28F6D90CFBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="autoNoTable" iterate="1" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="191029" calcMode="autoNoTable" iterate="1" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3740" uniqueCount="1819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3750" uniqueCount="1823">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5490,6 +5490,18 @@
   </si>
   <si>
     <t>This is from Aftermath and I hope a helpful illustration of one type of outcome we should be preparing (and saving) for.</t>
+  </si>
+  <si>
+    <t>The Ethics of Money Production</t>
+  </si>
+  <si>
+    <t>Jörg Guido Hülsmann</t>
+  </si>
+  <si>
+    <t>Purgatorio</t>
+  </si>
+  <si>
+    <t>Clark Moody recommended this and this book really blew my mind. So much of what I thought I knew about money is wrong, and this book is a beautiful synthesis of the moral and historical aspects of money.</t>
   </si>
 </sst>
 </file>
@@ -26162,14 +26174,56 @@
       </c>
     </row>
     <row r="851" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D851" s="6"/>
-      <c r="E851" s="6"/>
-      <c r="F851" s="6"/>
+      <c r="A851" s="3" t="s">
+        <v>1819</v>
+      </c>
+      <c r="B851" s="3" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C851" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D851" s="6">
+        <v>2022</v>
+      </c>
+      <c r="E851" s="6">
+        <v>2008</v>
+      </c>
+      <c r="F851" s="6">
+        <v>256</v>
+      </c>
+      <c r="G851" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="H851" s="3" t="s">
+        <v>1822</v>
+      </c>
     </row>
     <row r="852" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D852" s="6"/>
-      <c r="E852" s="6"/>
-      <c r="F852" s="6"/>
+      <c r="A852" s="3" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B852" s="3" t="s">
+        <v>1761</v>
+      </c>
+      <c r="C852" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D852" s="6">
+        <v>2022</v>
+      </c>
+      <c r="E852" s="6">
+        <v>1320</v>
+      </c>
+      <c r="F852" s="6">
+        <v>759</v>
+      </c>
+      <c r="G852" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="H852" s="3" t="s">
+        <v>1762</v>
+      </c>
     </row>
     <row r="853" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D853" s="6"/>

</xml_diff>

<commit_message>
Confessions of St. Patrick
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5A5CE4-61B7-B443-B178-27679050E374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A584BFF-2AFF-C84A-9092-C72123A09D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="autoNoTable" iterate="1" calcOnSave="0"/>
+  <calcPr calcId="191029" calcMode="autoNoTable" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3770" uniqueCount="1836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3775" uniqueCount="1839">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5541,6 +5541,15 @@
   </si>
   <si>
     <t>This came from my first CCA lunch and is a principled (though wordy at times) defense of traditional values against wokeness. I especially appreciate his clear articulation of capitalism.</t>
+  </si>
+  <si>
+    <t>The Confession of Saint Patrick</t>
+  </si>
+  <si>
+    <t>St. Patrick</t>
+  </si>
+  <si>
+    <t>I found this at the UA library book sale just in time to read for the week of his feast. It is a beautiful confession so fecund with scripture and so rich in faith.</t>
   </si>
 </sst>
 </file>
@@ -7206,7 +7215,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A820" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A857" sqref="A857"/>
+      <selection pane="bottomLeft" activeCell="A858" sqref="A858"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26369,9 +26378,30 @@
       </c>
     </row>
     <row r="857" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D857" s="6"/>
-      <c r="E857" s="6"/>
-      <c r="F857" s="6"/>
+      <c r="A857" s="3" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B857" s="3" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C857" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D857" s="6">
+        <v>2022</v>
+      </c>
+      <c r="E857" s="6">
+        <v>461</v>
+      </c>
+      <c r="F857" s="6">
+        <v>112</v>
+      </c>
+      <c r="G857" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="H857" s="3" t="s">
+        <v>1838</v>
+      </c>
     </row>
     <row r="858" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D858" s="6"/>

</xml_diff>

<commit_message>
The End and the Beginning, etc.
</commit_message>
<xml_diff>
--- a/reading/reading.xlsx
+++ b/reading/reading.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkudija/Documents/GitHub/mkudija.github.io/reading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481B43A9-2AF1-D147-B21B-9AF3ACF674FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F292F610-496F-6D41-85B7-E46B1CA3CCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1220" windowWidth="20480" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3863" uniqueCount="1881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3868" uniqueCount="1884">
   <si>
     <t>So Good They Can't Ignore You: Why Skills Trump Passion in the Quest for Work You Love</t>
   </si>
@@ -5676,6 +5676,15 @@
   </si>
   <si>
     <t>Fr. Raymund suggested this when he was over. Ultralearning is much better, but this is a good quick read on some basic learning and memorization techniques.</t>
+  </si>
+  <si>
+    <t>The End and the Beginning: Pope John Paul II—The Victory of Freedom, the Last Years, the Legacy</t>
+  </si>
+  <si>
+    <t>https://matthewkudija.com/reading-notes/2022-07-01-The-End-and-the-Beginning.html</t>
+  </si>
+  <si>
+    <t>Here is volume 2 in the John Paul II trilogy! A slog and got me awhile to get around to making my notes, but so wonderful to study and reflect upon his great life.</t>
   </si>
 </sst>
 </file>
@@ -7337,11 +7346,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1175"/>
+  <dimension ref="A1:H1176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A829" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A875" sqref="A875"/>
+      <pane ySplit="1" topLeftCell="A851" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A877" sqref="A877"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26892,85 +26901,85 @@
     </row>
     <row r="872" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A872" s="3" t="s">
-        <v>1871</v>
+        <v>1881</v>
+      </c>
+      <c r="B872" s="3" t="s">
+        <v>759</v>
       </c>
       <c r="C872" s="3" t="s">
-        <v>939</v>
+        <v>196</v>
       </c>
       <c r="D872" s="6">
         <v>2022</v>
       </c>
       <c r="E872" s="6">
-        <v>1954</v>
+        <v>2010</v>
       </c>
       <c r="F872" s="6">
-        <v>30</v>
-      </c>
-      <c r="G872" s="12" t="s">
-        <v>234</v>
+        <v>517</v>
+      </c>
+      <c r="G872" s="14" t="s">
+        <v>1882</v>
       </c>
       <c r="H872" s="3" t="s">
-        <v>1872</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="873" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A873" s="3" t="s">
-        <v>1873</v>
-      </c>
-      <c r="B873" s="3" t="s">
-        <v>1874</v>
+        <v>1871</v>
       </c>
       <c r="C873" s="3" t="s">
-        <v>198</v>
+        <v>939</v>
       </c>
       <c r="D873" s="6">
         <v>2022</v>
       </c>
       <c r="E873" s="6">
-        <v>2022</v>
+        <v>1954</v>
       </c>
       <c r="F873" s="6">
-        <v>272</v>
+        <v>30</v>
       </c>
       <c r="G873" s="12" t="s">
         <v>234</v>
       </c>
       <c r="H873" s="3" t="s">
-        <v>1875</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="874" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A874" s="3" t="s">
-        <v>1876</v>
+        <v>1873</v>
       </c>
       <c r="B874" s="3" t="s">
-        <v>1032</v>
+        <v>1874</v>
       </c>
       <c r="C874" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D874" s="6">
         <v>2022</v>
       </c>
       <c r="E874" s="6">
-        <v>1966</v>
+        <v>2022</v>
       </c>
       <c r="F874" s="6">
-        <v>174</v>
+        <v>272</v>
       </c>
       <c r="G874" s="12" t="s">
         <v>234</v>
       </c>
       <c r="H874" s="3" t="s">
-        <v>1879</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="875" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A875" s="3" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="B875" s="3" t="s">
-        <v>1878</v>
+        <v>1032</v>
       </c>
       <c r="C875" s="3" t="s">
         <v>196</v>
@@ -26979,22 +26988,43 @@
         <v>2022</v>
       </c>
       <c r="E875" s="6">
-        <v>2019</v>
+        <v>1966</v>
       </c>
       <c r="F875" s="6">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="G875" s="12" t="s">
         <v>234</v>
       </c>
       <c r="H875" s="3" t="s">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="876" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A876" s="3" t="s">
+        <v>1877</v>
+      </c>
+      <c r="B876" s="3" t="s">
+        <v>1878</v>
+      </c>
+      <c r="C876" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D876" s="6">
+        <v>2022</v>
+      </c>
+      <c r="E876" s="6">
+        <v>2019</v>
+      </c>
+      <c r="F876" s="6">
+        <v>181</v>
+      </c>
+      <c r="G876" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="H876" s="3" t="s">
         <v>1880</v>
       </c>
-    </row>
-    <row r="876" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D876" s="6"/>
-      <c r="E876" s="6"/>
-      <c r="F876" s="6"/>
     </row>
     <row r="877" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D877" s="6"/>
@@ -28490,6 +28520,11 @@
       <c r="D1175" s="6"/>
       <c r="E1175" s="6"/>
       <c r="F1175" s="6"/>
+    </row>
+    <row r="1176" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D1176" s="6"/>
+      <c r="E1176" s="6"/>
+      <c r="F1176" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G769 G771:G812">
@@ -28521,6 +28556,7 @@
     <hyperlink ref="G826" r:id="rId6" xr:uid="{94B2C2E7-AC2D-7F4F-8C8A-D9BAC34E7F6B}"/>
     <hyperlink ref="G836" r:id="rId7" xr:uid="{4FB1DC9F-1CE5-F848-B510-FD663A1B64DE}"/>
     <hyperlink ref="G851" r:id="rId8" xr:uid="{CF5B95ED-8F4B-B74B-BB2D-482CBDA985F9}"/>
+    <hyperlink ref="G872" r:id="rId9" xr:uid="{D83B6465-FE4D-3C4D-87EE-6C8F1189D33B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>